<commit_message>
Capitalize all spreadsheet column names: easier to track and auto-configure
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glennwood/Documents/PROJECTS/BitCoin/mining/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/opt/git/miners/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1680" windowWidth="25600" windowHeight="11260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2260" windowWidth="25600" windowHeight="9920" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="5" r:id="rId1"/>
-    <sheet name="coin-miners" sheetId="2" r:id="rId2"/>
+    <sheet name="CoinMiners" sheetId="2" r:id="rId2"/>
     <sheet name="Clients" sheetId="4" r:id="rId3"/>
     <sheet name="stats" sheetId="3" r:id="rId4"/>
     <sheet name="Algorithm" sheetId="1" r:id="rId5"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="206">
   <si>
     <t>Algorithm</t>
   </si>
@@ -120,12 +120,6 @@
     <t>eth-proxy</t>
   </si>
   <si>
-    <t>Coin</t>
-  </si>
-  <si>
-    <t>Miner</t>
-  </si>
-  <si>
     <t>ADA</t>
   </si>
   <si>
@@ -270,12 +264,6 @@
     <t>us-east.ethash-hub.miningpoolhub.com:20535</t>
   </si>
   <si>
-    <t>UrlPort</t>
-  </si>
-  <si>
-    <t>Wallet</t>
-  </si>
-  <si>
     <t>ELLA</t>
   </si>
   <si>
@@ -288,9 +276,6 @@
     <t>ethdcrminer64</t>
   </si>
   <si>
-    <t>UserPassword</t>
-  </si>
-  <si>
     <t>albokiadt:RLaA58k3PmwjcLGZ</t>
   </si>
   <si>
@@ -381,9 +366,6 @@
     <t>stratum+tcp://us.hushpool.cloud:5551</t>
   </si>
   <si>
-    <t>Environment</t>
-  </si>
-  <si>
     <t>export GPU_FORCE_64BIT_PTR=1</t>
   </si>
   <si>
@@ -495,15 +477,6 @@
     <t>ETHDCR</t>
   </si>
   <si>
-    <t>Mnemonic</t>
-  </si>
-  <si>
-    <t>Options</t>
-  </si>
-  <si>
-    <t>Executable</t>
-  </si>
-  <si>
     <t>-epool $URL_PORT -ewal $WALLET -epsw x -allpools 1 -allcoins exp -gser 2 -eworker $WORKER_NAME $GPUS $PLATFORM</t>
   </si>
   <si>
@@ -531,20 +504,161 @@
     <t>TEXTBELT_PHN</t>
   </si>
   <si>
-    <t>chdir</t>
-  </si>
-  <si>
     <t>-o $URL_PORT -u $WALLET [-p &lt;OPTIONS&gt;]</t>
   </si>
   <si>
     <t>GPU_FORCE_64BIT_PTR=1</t>
+  </si>
+  <si>
+    <t>stratum+tcp://us.cryptopool.xyz:10000</t>
+  </si>
+  <si>
+    <t>VH8UaPYmDEHgFuyPyGKdkseytnfZvPmqwm</t>
+  </si>
+  <si>
+    <t>us.hushmine.pro:9009</t>
+  </si>
+  <si>
+    <t>us.zclmine.pro:9009</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --server $URL --user $WALLET.ZCL-miner --pass x --port $PORT</t>
+  </si>
+  <si>
+    <t>HUSH-opt</t>
+  </si>
+  <si>
+    <t>t1gshUXiCt1V7LAzc1xxvmZNN4SK6guhGh22eo96sjU7n9okytzYZzbeuQ8AGdevmYyYyu</t>
+  </si>
+  <si>
+    <t>EWBF</t>
+  </si>
+  <si>
+    <t>miner</t>
+  </si>
+  <si>
+    <t>/opt/ewbf</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>KLAUST</t>
+  </si>
+  <si>
+    <t>/opt/ccminer-KlausT</t>
+  </si>
+  <si>
+    <t>NVIDIA</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --server $URL --port $PORT --user $WALLET.ZCL-miner --pass x</t>
+  </si>
+  <si>
+    <t>t1NFZdAYGpVWBuWQcNJnXHZKXpjf18Qn2BX</t>
+  </si>
+  <si>
+    <t>VIVO-NVI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/opt/gatelessgate/Core/gatelessgate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">--gpu-platform 0 --default-config $CONFIG_FILE
+./gatelessgate --gpu-platform 0 --default-config gatelessgate-Vivo.conf
+./gatelessgate --gpu-platform 0 --default-config gatelessgate-Vivo.conf
+</t>
+  </si>
+  <si>
+    <t>VIVO.conf</t>
+  </si>
+  <si>
+    <t>ZCL%AMD</t>
+  </si>
+  <si>
+    <t>ZCL%PRO</t>
+  </si>
+  <si>
+    <t>us-east.equihash-hub.miningpoolhub.com:20575</t>
+  </si>
+  <si>
+    <t>albokiadt:x</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --server $URL --port $PORT --user $USER.$WORKER_NAME --pass $PASSWORD</t>
+  </si>
+  <si>
+    <t>/opt/gatelessgate/Core</t>
+  </si>
+  <si>
+    <t>GATELESSGATE</t>
+  </si>
+  <si>
+    <t>GPU_MAX_HEAP_SIZE=100</t>
+  </si>
+  <si>
+    <t>GPU_USE_SYNC_OBJECTS=1</t>
+  </si>
+  <si>
+    <t>GPU_MAX_ALLOC_PERCENT=100</t>
+  </si>
+  <si>
+    <t>GPU_SINGLE_ALLOC_PERCENT=100</t>
+  </si>
+  <si>
+    <t>SGMINER-PHI</t>
+  </si>
+  <si>
+    <t>/opt/sgminer-phi1612</t>
+  </si>
+  <si>
+    <t>DISPLAY=:0</t>
+  </si>
+  <si>
+    <t>COIN</t>
+  </si>
+  <si>
+    <t>MINER</t>
+  </si>
+  <si>
+    <t>CONFIG_FILE</t>
+  </si>
+  <si>
+    <t>URL_PORT</t>
+  </si>
+  <si>
+    <t>USER_PSW</t>
+  </si>
+  <si>
+    <t>WALLET</t>
+  </si>
+  <si>
+    <t>MNEMONIC</t>
+  </si>
+  <si>
+    <t>PLATFORM</t>
+  </si>
+  <si>
+    <t>EXECUTABLE</t>
+  </si>
+  <si>
+    <t>CHDIR</t>
+  </si>
+  <si>
+    <t>ENVIRONMENT</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -702,6 +816,25 @@
       <color theme="10"/>
       <name val="Microsoft Sans Serif"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="MicrosoftSansSerif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="MicrosoftSansSerif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="MicrosoftSansSerif"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -739,7 +872,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -927,16 +1060,45 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
@@ -952,8 +1114,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1248,23 +1419,23 @@
   <sheetData>
     <row r="1" spans="1:2" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B1" s="64" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="63" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="63" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B3" s="63">
         <v>6502799436</v>
@@ -1277,718 +1448,876 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:Q79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" style="13" customWidth="1"/>
-    <col min="7" max="16384" width="10.7109375" style="13"/>
+    <col min="3" max="3" width="15.5703125" style="71" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.7109375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="26" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>29</v>
+        <v>194</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="26" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="53"/>
+      <c r="D7" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22"/>
+      <c r="B8" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="75"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+    </row>
+    <row r="9" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" s="26" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A15" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="74" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="53" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="D8" s="48" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="65" t="s">
-        <v>167</v>
-      </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="D15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="G15" s="28"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="23"/>
+      <c r="B16" s="77" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="77"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="19" x14ac:dyDescent="0.2">
-      <c r="A15" s="57" t="s">
+      <c r="B17" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="23"/>
+      <c r="B18" s="75" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="75"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="F15" s="28"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="23"/>
-      <c r="B16" s="68" t="s">
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="23"/>
+      <c r="B21" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="23"/>
-      <c r="B18" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="23" t="s">
+      <c r="C21" s="75"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="23"/>
-      <c r="B21" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="23" t="s">
+    <row r="25" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="58" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="58" t="s">
-        <v>48</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="59" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="F25" s="27"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D25" s="59" t="s">
+        <v>145</v>
+      </c>
+      <c r="F25" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="27"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="23"/>
-      <c r="B26" s="68" t="s">
-        <v>149</v>
-      </c>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="27"/>
-    </row>
-    <row r="27" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26" s="77"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="27"/>
+    </row>
+    <row r="27" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B27" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="52" t="s">
+      <c r="C27" s="71"/>
+      <c r="D27" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="F27" s="52"/>
+      <c r="G27" s="50"/>
+    </row>
+    <row r="28" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="23"/>
+      <c r="B28" s="77" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="77"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+    </row>
+    <row r="29" spans="1:17" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="71"/>
+      <c r="D29" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="F29" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" s="47"/>
+    </row>
+    <row r="30" spans="1:17" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="23"/>
+      <c r="B30" s="75" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="75"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="47"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q31" s="69">
+        <v>0.91180555555555554</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="68" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" s="71"/>
+      <c r="D33" s="68" t="s">
+        <v>161</v>
+      </c>
+      <c r="F33" s="68" t="s">
+        <v>165</v>
+      </c>
+      <c r="G33" s="67"/>
+    </row>
+    <row r="34" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="23"/>
+      <c r="B34" s="75" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="75"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="76"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="23"/>
+      <c r="B36" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="75"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G39" s="27"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="23"/>
+      <c r="B40" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="75"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G46" s="27"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="23"/>
+      <c r="B47" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="75"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="76"/>
+      <c r="G47" s="27"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G48" s="27"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="23"/>
+      <c r="B49" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="75"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="76"/>
+      <c r="F49" s="76"/>
+      <c r="G49" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="23"/>
+      <c r="B54" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="75"/>
+      <c r="D54" s="76"/>
+      <c r="E54" s="76"/>
+      <c r="F54" s="76"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G56" s="62" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="23"/>
+      <c r="B57" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="C57" s="77"/>
+      <c r="D57" s="78"/>
+      <c r="E57" s="78"/>
+      <c r="F57" s="78"/>
+      <c r="G57" s="61"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="23"/>
+      <c r="B59" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="75"/>
+      <c r="D59" s="76"/>
+      <c r="E59" s="76"/>
+      <c r="F59" s="76"/>
+    </row>
+    <row r="60" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="71"/>
+      <c r="D60" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="E60" s="51" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="75" t="s">
+        <v>139</v>
+      </c>
+      <c r="C61" s="75"/>
+      <c r="D61" s="76"/>
+      <c r="E61" s="76"/>
+      <c r="F61" s="76"/>
+      <c r="G61" s="76"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="C63" s="72" t="s">
+        <v>179</v>
+      </c>
+      <c r="D63" s="71" t="s">
+        <v>159</v>
+      </c>
+      <c r="F63" s="71" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="23"/>
+      <c r="B64" s="79" t="s">
+        <v>178</v>
+      </c>
+      <c r="C64" s="79"/>
+      <c r="D64" s="78"/>
+      <c r="E64" s="78"/>
+      <c r="F64" s="78"/>
+      <c r="G64" s="78"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A65" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="B65" s="72" t="s">
+        <v>170</v>
+      </c>
+      <c r="C65" s="72"/>
+      <c r="D65" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A66" s="23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A67" s="23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A68" s="23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A69" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A70" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B71" s="74" t="s">
+        <v>166</v>
+      </c>
+      <c r="D71" s="74" t="s">
+        <v>162</v>
+      </c>
+      <c r="F71" s="74" t="s">
+        <v>175</v>
+      </c>
+      <c r="G71" s="73"/>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A72" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="G72" s="47"/>
+    </row>
+    <row r="73" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="23"/>
+      <c r="B73" s="75" t="s">
+        <v>184</v>
+      </c>
+      <c r="C73" s="76"/>
+      <c r="D73" s="76"/>
+      <c r="E73" s="76"/>
+      <c r="F73" s="76"/>
+      <c r="G73" s="73"/>
+    </row>
+    <row r="74" spans="1:17" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="C74" s="71"/>
+      <c r="D74" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="E74" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="G74" s="67"/>
+    </row>
+    <row r="75" spans="1:17" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="23"/>
+      <c r="B75" s="75" t="s">
         <v>146</v>
       </c>
-      <c r="D27" s="52" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="52"/>
-      <c r="F27" s="50"/>
-    </row>
-    <row r="28" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="23"/>
-      <c r="B28" s="68" t="s">
-        <v>150</v>
-      </c>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
-    </row>
-    <row r="29" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="B29" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="C29" t="s">
-        <v>137</v>
-      </c>
-      <c r="D29" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="E29" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="F29" s="47"/>
-    </row>
-    <row r="30" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="23"/>
-      <c r="B30" s="65" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="47"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="23"/>
-      <c r="B34" s="65" t="s">
-        <v>114</v>
-      </c>
-      <c r="C34" s="66"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="66"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F37" s="27"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="23"/>
-      <c r="B38" s="65" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" s="66"/>
-      <c r="D38" s="66"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="61" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="13" t="s">
+      <c r="C75" s="75"/>
+      <c r="D75" s="76"/>
+      <c r="E75" s="76"/>
+      <c r="F75" s="76"/>
+      <c r="G75" s="76"/>
+    </row>
+    <row r="76" spans="1:17" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B76" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="71"/>
+      <c r="D76" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="E76" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="G76" s="67"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
+      <c r="N76" s="13"/>
+      <c r="O76" s="13"/>
+      <c r="P76" s="13"/>
+      <c r="Q76" s="13"/>
+    </row>
+    <row r="77" spans="1:17" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="23"/>
+      <c r="B77" s="75" t="s">
+        <v>96</v>
+      </c>
+      <c r="C77" s="75"/>
+      <c r="D77" s="75"/>
+      <c r="E77" s="75"/>
+      <c r="F77" s="75"/>
+      <c r="G77" s="75"/>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A78" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D78" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F44" s="27"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="23"/>
-      <c r="B45" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="C45" s="66"/>
-      <c r="D45" s="66"/>
-      <c r="E45" s="66"/>
-      <c r="F45" s="27"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F46" s="27"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="23"/>
-      <c r="B47" s="65" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" s="66"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="66"/>
-      <c r="F47" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="23"/>
-      <c r="B52" s="65" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" s="66"/>
-      <c r="D52" s="66"/>
-      <c r="E52" s="66"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A54" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B54" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="C54" s="56" t="s">
-        <v>159</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="F54" s="62" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="23"/>
-      <c r="B55" s="68" t="s">
-        <v>149</v>
-      </c>
-      <c r="C55" s="67"/>
-      <c r="D55" s="67"/>
-      <c r="E55" s="67"/>
-      <c r="F55" s="61"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E56" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="23"/>
-      <c r="B57" s="65" t="s">
-        <v>113</v>
-      </c>
-      <c r="C57" s="66"/>
-      <c r="D57" s="66"/>
-      <c r="E57" s="66"/>
-    </row>
-    <row r="58" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B58" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="C58" s="51" t="s">
-        <v>143</v>
-      </c>
-      <c r="D58" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="65" t="s">
-        <v>145</v>
-      </c>
-      <c r="C59" s="66"/>
-      <c r="D59" s="66"/>
-      <c r="E59" s="66"/>
-      <c r="F59" s="66"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="B67" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C67" s="13" t="s">
+      <c r="E78" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G78" s="27"/>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B79" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="D67" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F67" s="47"/>
-    </row>
-    <row r="68" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="23"/>
-      <c r="B68" s="65" t="s">
-        <v>152</v>
-      </c>
-      <c r="C68" s="66"/>
-      <c r="D68" s="66"/>
-      <c r="E68" s="66"/>
-      <c r="F68" s="66"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="D69" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F69" s="27"/>
-    </row>
-    <row r="70" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="23"/>
-      <c r="B70" s="65" t="s">
-        <v>101</v>
-      </c>
-      <c r="C70" s="66"/>
-      <c r="D70" s="66"/>
-      <c r="E70" s="66"/>
-      <c r="F70" s="66"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="B71" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D71" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F71" s="27"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B72" s="65" t="s">
-        <v>99</v>
-      </c>
-      <c r="C72" s="66"/>
-      <c r="D72" s="66"/>
-      <c r="E72" s="66"/>
-      <c r="F72" s="66"/>
+      <c r="C79" s="75"/>
+      <c r="D79" s="76"/>
+      <c r="E79" s="76"/>
+      <c r="F79" s="76"/>
+      <c r="G79" s="76"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="21">
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B30:F30"/>
     <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B61:G61"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B79:G79"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B75:G75"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B73:F73"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A41" r:id="rId1" display="NMC (Namecoin)"/>
-    <hyperlink ref="A65" r:id="rId2"/>
-    <hyperlink ref="A64" r:id="rId3"/>
-    <hyperlink ref="A62" r:id="rId4"/>
-    <hyperlink ref="A48" r:id="rId5"/>
+    <hyperlink ref="A43" r:id="rId1" display="NMC (Namecoin)"/>
+    <hyperlink ref="A69" r:id="rId2"/>
+    <hyperlink ref="A68" r:id="rId3"/>
+    <hyperlink ref="A66" r:id="rId4"/>
+    <hyperlink ref="A50" r:id="rId5"/>
     <hyperlink ref="A32" r:id="rId6"/>
     <hyperlink ref="A15" r:id="rId7"/>
     <hyperlink ref="A20" r:id="rId8"/>
-    <hyperlink ref="A50" r:id="rId9"/>
+    <hyperlink ref="A52" r:id="rId9"/>
     <hyperlink ref="A31" r:id="rId10"/>
-    <hyperlink ref="A63" r:id="rId11"/>
+    <hyperlink ref="A67" r:id="rId11"/>
     <hyperlink ref="A19" r:id="rId12"/>
-    <hyperlink ref="A61" r:id="rId13"/>
+    <hyperlink ref="A65" r:id="rId13" display="VIVO"/>
     <hyperlink ref="A23" r:id="rId14"/>
-    <hyperlink ref="A67" r:id="rId15"/>
-    <hyperlink ref="A35" r:id="rId16"/>
-    <hyperlink ref="A46" r:id="rId17"/>
+    <hyperlink ref="A72" r:id="rId15"/>
+    <hyperlink ref="A37" r:id="rId16"/>
+    <hyperlink ref="A48" r:id="rId17"/>
     <hyperlink ref="A11" r:id="rId18"/>
-    <hyperlink ref="A36" r:id="rId19"/>
+    <hyperlink ref="A38" r:id="rId19"/>
     <hyperlink ref="A13" r:id="rId20"/>
-    <hyperlink ref="A69" r:id="rId21"/>
-    <hyperlink ref="A71" r:id="rId22"/>
-    <hyperlink ref="A54" r:id="rId23"/>
-    <hyperlink ref="B8" r:id="rId24"/>
-    <hyperlink ref="A8" r:id="rId25"/>
-    <hyperlink ref="A29" r:id="rId26" display="GBX"/>
-    <hyperlink ref="A25" r:id="rId27"/>
-    <hyperlink ref="A56" r:id="rId28" display="UBQ"/>
+    <hyperlink ref="A78" r:id="rId21"/>
+    <hyperlink ref="A56" r:id="rId22"/>
+    <hyperlink ref="B7" r:id="rId23"/>
+    <hyperlink ref="A7" r:id="rId24"/>
+    <hyperlink ref="A29" r:id="rId25" display="GBX"/>
+    <hyperlink ref="A25" r:id="rId26"/>
+    <hyperlink ref="A58" r:id="rId27" display="UBQ"/>
+    <hyperlink ref="A76" r:id="rId28"/>
+    <hyperlink ref="A74" r:id="rId29" display="ZCL"/>
+    <hyperlink ref="A33" r:id="rId30" display="ZCL"/>
+    <hyperlink ref="A63" r:id="rId31"/>
+    <hyperlink ref="A71" r:id="rId32" display="ZCL"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1997,49 +2326,152 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="86" customWidth="1"/>
+    <col min="6" max="6" width="98.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="60" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="60" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" s="60" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="88" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="87" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" s="85" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="60" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" s="60" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="70" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="70" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" s="86" t="s">
         <v>158</v>
       </c>
-      <c r="E2" t="s">
-        <v>157</v>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E6" s="86" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="86" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8" s="86" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E9" s="86" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>192</v>
+      </c>
+      <c r="E10" s="86" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11" s="86" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="86" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2051,9 +2483,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2066,354 +2498,354 @@
   <sheetData>
     <row r="1" spans="1:5" s="38" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
-        <v>29</v>
+        <v>194</v>
       </c>
       <c r="B1" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="38" t="s">
         <v>118</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="29" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="31" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="29" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B6" s="31"/>
       <c r="C6" s="31" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="29" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="31"/>
       <c r="C7" s="31" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="29" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" s="31"/>
       <c r="C8" s="31" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="29" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" s="31"/>
       <c r="C9" s="31" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="30" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="30" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="31" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="30" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="35" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="35" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="35" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="35" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="35" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="42" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="35" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2523,10 +2955,10 @@
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="69"/>
+      <c r="C6" s="80"/>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
@@ -2544,10 +2976,10 @@
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="71"/>
+      <c r="C9" s="82"/>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -2597,21 +3029,21 @@
     </row>
     <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="73"/>
+      <c r="C16" s="84"/>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C17" s="46"/>
       <c r="D17" s="54" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="19" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Reorganize and extend monitor-minors
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="227">
   <si>
     <t>Miners (AMD)</t>
   </si>
@@ -565,9 +565,6 @@
     <t>albokiadt:x</t>
   </si>
   <si>
-    <t xml:space="preserve"> --server $URL --port $PORT --user $USER.$WORKER_NAME --pass $PASSWORD</t>
-  </si>
-  <si>
     <t>/opt/gatelessgate/Core</t>
   </si>
   <si>
@@ -637,9 +634,6 @@
     <t>us-east.equihash-hub.miningpoolhub.com:20570</t>
   </si>
   <si>
-    <t>ETH%mph</t>
-  </si>
-  <si>
     <t>-o  -u &lt;WALLET_ADDRESS&gt; [-p c=&lt;SYMBOL&gt;,&lt;OPTIONS&gt;]</t>
   </si>
   <si>
@@ -707,13 +701,31 @@
   </si>
   <si>
     <t>--server $URL --port $PORT --user $USER.$WORKER_NAME --pass $PASSWORD</t>
+  </si>
+  <si>
+    <t>GRF</t>
+  </si>
+  <si>
+    <t>PROHASH</t>
+  </si>
+  <si>
+    <t>prohashing.com:3333</t>
+  </si>
+  <si>
+    <t>--url $URL --neoscrypt --pass a=scrypt --user $USER</t>
+  </si>
+  <si>
+    <t>ETH%zpool</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="28" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -801,12 +813,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Microsoft Sans Serif"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
       <sz val="11"/>
       <name val="Microsoft Sans Serif"/>
     </font>
@@ -920,7 +926,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -973,10 +979,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -997,22 +1000,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1021,13 +1024,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1059,7 +1062,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
@@ -1102,7 +1105,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1121,13 +1124,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -1140,7 +1143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1157,6 +1160,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1444,41 +1453,41 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.7109375" style="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.7109375" style="55"/>
+    <col min="1" max="1" width="16.5703125" style="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.7109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.7109375" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="56" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:2" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="55" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="54" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="55">
+      <c r="B3" s="54">
         <v>6502799436</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="55" t="s">
-        <v>205</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>206</v>
+      <c r="A4" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1491,7 +1500,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1500,28 +1509,28 @@
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="70" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="69" customWidth="1"/>
     <col min="6" max="6" width="98.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="52" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:6" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="71" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="C1" s="70" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="D1" s="51" t="s">
         <v>194</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="E1" s="68" t="s">
         <v>195</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="F1" s="51" t="s">
         <v>196</v>
-      </c>
-      <c r="F1" s="52" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1532,7 +1541,7 @@
         <v>166</v>
       </c>
       <c r="C2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D2" t="s">
         <v>143</v>
@@ -1549,13 +1558,13 @@
         <v>165</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
         <v>161</v>
       </c>
-      <c r="F3" s="61" t="s">
-        <v>223</v>
+      <c r="F3" s="60" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1566,79 +1575,79 @@
         <v>165</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
         <v>164</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="60" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" s="69" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E6" s="69" t="s">
         <v>178</v>
       </c>
-      <c r="C5" t="s">
-        <v>215</v>
-      </c>
-      <c r="D5" t="s">
-        <v>177</v>
-      </c>
-      <c r="E5" s="70" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E6" s="70" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="69" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E7" s="70" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8" s="69" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E8" s="70" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E9" s="69" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E9" s="70" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B10" t="s">
         <v>166</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E10" s="69" t="s">
         <v>184</v>
       </c>
-      <c r="E10" s="70" t="s">
-        <v>185</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E11" s="70" t="s">
-        <v>181</v>
+      <c r="E11" s="69" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E12" s="70" t="s">
-        <v>180</v>
+      <c r="E12" s="69" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B13" t="s">
         <v>165</v>
@@ -1646,8 +1655,8 @@
       <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="61" t="s">
-        <v>210</v>
+      <c r="F13" s="60" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -1657,18 +1666,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q86"/>
+  <dimension ref="A1:Q89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B77" sqref="B77"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="62" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="61" customWidth="1"/>
     <col min="4" max="4" width="42.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.140625" style="13" customWidth="1"/>
     <col min="6" max="6" width="69.140625" style="13" bestFit="1" customWidth="1"/>
@@ -1676,27 +1685,27 @@
     <col min="8" max="16384" width="10.7109375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:7" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>196</v>
+      <c r="G1" s="19" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1724,33 +1733,33 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>120</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="42" t="s">
+      <c r="C7" s="46"/>
+      <c r="D7" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="41" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="72" t="s">
         <v>151</v>
       </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-    </row>
-    <row r="9" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="72"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+    </row>
+    <row r="9" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>162</v>
       </c>
@@ -1765,7 +1774,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1784,7 +1793,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+      <c r="A13" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1793,59 +1802,59 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="67" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>200</v>
-      </c>
-      <c r="B15" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="67" t="s">
+      <c r="D15" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="67" t="s">
+      <c r="E15" s="66" t="s">
         <v>175</v>
       </c>
-      <c r="F15" s="66"/>
-      <c r="G15" s="68"/>
-    </row>
-    <row r="16" spans="1:7" s="67" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F15" s="65"/>
+      <c r="G15" s="67"/>
+    </row>
+    <row r="16" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
-      <c r="B16" s="76" t="s">
+      <c r="B16" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="76"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>226</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>77</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="E17" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="F17" s="66"/>
-      <c r="G17" s="22"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="21"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
-      <c r="B18" s="76" t="s">
-        <v>201</v>
-      </c>
-      <c r="C18" s="76"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
+      <c r="B18" s="75" t="s">
+        <v>199</v>
+      </c>
+      <c r="C18" s="75"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
@@ -1860,21 +1869,21 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="73"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
+      <c r="A21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
+      <c r="A22" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="13" t="s">
@@ -1889,13 +1898,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="73"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
@@ -1903,7 +1912,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
+      <c r="A25" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1912,717 +1921,721 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>222</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="14"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B28" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="D27" s="51" t="s">
+      <c r="D28" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="F27" s="45" t="s">
+      <c r="F28" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="G27" s="21"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
-      <c r="B28" s="76" t="s">
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="17"/>
+      <c r="B29" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="76"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="21"/>
-    </row>
-    <row r="29" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
+      <c r="C29" s="75"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="20"/>
+    </row>
+    <row r="30" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B30" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="46" t="s">
+      <c r="C30" s="61"/>
+      <c r="D30" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="E29" s="46" t="s">
+      <c r="E30" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="F29" s="46"/>
-      <c r="G29" s="44"/>
-    </row>
-    <row r="30" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-      <c r="B30" s="76" t="s">
+      <c r="F30" s="45"/>
+      <c r="G30" s="43"/>
+    </row>
+    <row r="31" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="17"/>
+      <c r="B31" s="75" t="s">
         <v>138</v>
       </c>
-      <c r="C30" s="76"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
-    </row>
-    <row r="31" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="17" t="s">
+      <c r="C31" s="75"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+    </row>
+    <row r="32" spans="1:7" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>128</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B32" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="C31" s="62"/>
-      <c r="D31" t="s">
+      <c r="C32" s="61"/>
+      <c r="D32" t="s">
         <v>125</v>
       </c>
-      <c r="E31" s="42" t="s">
+      <c r="E32" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="F31" s="42" t="s">
+      <c r="F32" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="G31" s="41"/>
-    </row>
-    <row r="32" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
-      <c r="B32" s="73" t="s">
+      <c r="G32" s="40"/>
+    </row>
+    <row r="33" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="17"/>
+      <c r="B33" s="72" t="s">
         <v>126</v>
       </c>
-      <c r="C32" s="73"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="41"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" s="17" t="s">
+      <c r="C33" s="72"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="40"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>44</v>
       </c>
-      <c r="Q33" s="60"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
+      <c r="Q34" s="59"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="17" t="s">
+    <row r="36" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="59" t="s">
+      <c r="B36" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="C35" s="62"/>
-      <c r="D35" s="59" t="s">
+      <c r="C36" s="61"/>
+      <c r="D36" s="58" t="s">
         <v>155</v>
       </c>
-      <c r="F35" s="59" t="s">
+      <c r="F36" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="G35" s="58"/>
-    </row>
-    <row r="36" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
-      <c r="B36" s="73" t="s">
+      <c r="G36" s="57"/>
+    </row>
+    <row r="37" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="17"/>
+      <c r="B37" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="C36" s="73"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
+      <c r="C37" s="72"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="73"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B38" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D38" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="F38" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
-      <c r="B38" s="73" t="s">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="17"/>
+      <c r="B39" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="73"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39" s="18" t="s">
+      <c r="C39" s="72"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B42" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D42" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E42" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="G41" s="21"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
-      <c r="B42" s="73" t="s">
+      <c r="G42" s="20"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="17"/>
+      <c r="B43" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="C42" s="73"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="53" t="s">
+      <c r="C43" s="72"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="52" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B49" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D49" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E49" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G48" s="21"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="17"/>
-      <c r="B49" s="73" t="s">
+      <c r="G49" s="20"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="17"/>
+      <c r="B50" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="C49" s="73"/>
-      <c r="D49" s="74"/>
-      <c r="E49" s="74"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="21"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
+      <c r="C50" s="72"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="73"/>
+      <c r="F50" s="73"/>
+      <c r="G50" s="20"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B51" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D51" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F50" s="13" t="s">
+      <c r="F51" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="G50" s="21"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="17"/>
-      <c r="B51" s="73" t="s">
+      <c r="G51" s="20"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="17"/>
+      <c r="B52" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="C51" s="73"/>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
-      <c r="F51" s="74"/>
-      <c r="G51" s="21" t="s">
+      <c r="C52" s="72"/>
+      <c r="D52" s="73"/>
+      <c r="E52" s="73"/>
+      <c r="F52" s="73"/>
+      <c r="G52" s="20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="17" t="s">
+    <row r="53" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B53" s="65" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="65"/>
+      <c r="D53" t="s">
+        <v>224</v>
+      </c>
+      <c r="E53" s="66" t="s">
+        <v>210</v>
+      </c>
+      <c r="G53" s="65"/>
+    </row>
+    <row r="54" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="17"/>
+      <c r="B54" s="72" t="s">
+        <v>225</v>
+      </c>
+      <c r="C54" s="74"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="74"/>
+      <c r="F54" s="74"/>
+      <c r="G54" s="65"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="17" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B58" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D58" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="73" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="17"/>
+      <c r="B59" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="C56" s="73"/>
-      <c r="D56" s="74"/>
-      <c r="E56" s="74"/>
-      <c r="F56" s="74"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A58" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B58" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="D58" s="50" t="s">
-        <v>144</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="G58" s="54" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" s="54" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="17"/>
-      <c r="B59" s="76" t="s">
-        <v>137</v>
-      </c>
-      <c r="C59" s="76"/>
-      <c r="D59" s="75"/>
-      <c r="E59" s="75"/>
-      <c r="F59" s="75"/>
-      <c r="G59" s="53"/>
+      <c r="C59" s="72"/>
+      <c r="D59" s="73"/>
+      <c r="E59" s="73"/>
+      <c r="F59" s="73"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D61" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G61" s="53" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="17"/>
+      <c r="B62" s="75" t="s">
+        <v>137</v>
+      </c>
+      <c r="C62" s="75"/>
+      <c r="D62" s="74"/>
+      <c r="E62" s="74"/>
+      <c r="F62" s="74"/>
+      <c r="G62" s="52"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>130</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B63" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="13" t="s">
+      <c r="D63" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F60" s="13" t="s">
+      <c r="F63" s="13" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="17"/>
-      <c r="B61" s="73" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="17"/>
+      <c r="B64" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="C61" s="73"/>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
-      <c r="F61" s="74"/>
-    </row>
-    <row r="62" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="17" t="s">
+      <c r="C64" s="72"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="73"/>
+      <c r="F64" s="73"/>
+    </row>
+    <row r="65" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="45" t="s">
+      <c r="B65" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="62"/>
-      <c r="D62" s="45" t="s">
+      <c r="C65" s="61"/>
+      <c r="D65" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="E62" s="45" t="s">
+      <c r="E65" s="44" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="73" t="s">
+    <row r="66" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="C63" s="73"/>
-      <c r="D63" s="74"/>
-      <c r="E63" s="74"/>
-      <c r="F63" s="74"/>
-      <c r="G63" s="74"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="17" t="s">
+      <c r="C66" s="72"/>
+      <c r="D66" s="73"/>
+      <c r="E66" s="73"/>
+      <c r="F66" s="73"/>
+      <c r="G66" s="73"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="17" t="s">
+    <row r="68" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="63" t="s">
+      <c r="B68" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="C65" s="63" t="s">
+      <c r="C68" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="D65" s="62" t="s">
+      <c r="D68" s="61" t="s">
         <v>153</v>
       </c>
-      <c r="F65" s="62" t="s">
+      <c r="F68" s="61" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="17"/>
-      <c r="B66" s="77" t="s">
+    <row r="69" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="17"/>
+      <c r="B69" s="76" t="s">
         <v>170</v>
       </c>
-      <c r="C66" s="77"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="75"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A67" s="17" t="s">
+      <c r="C69" s="76"/>
+      <c r="D69" s="74"/>
+      <c r="E69" s="74"/>
+      <c r="F69" s="74"/>
+      <c r="G69" s="74"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>168</v>
       </c>
-      <c r="B67" s="63" t="s">
+      <c r="B70" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="C67" s="63"/>
-      <c r="D67" s="57" t="s">
+      <c r="C70" s="62"/>
+      <c r="D70" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="F67" s="13" t="s">
+      <c r="F70" s="13" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="17" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="17" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="17" t="s">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="17" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="17" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="65" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="17" t="s">
+    <row r="76" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>173</v>
       </c>
-      <c r="B73" s="65" t="s">
+      <c r="B76" s="64" t="s">
         <v>160</v>
       </c>
-      <c r="D73" s="65" t="s">
+      <c r="D76" s="64" t="s">
         <v>156</v>
       </c>
-      <c r="F73" s="65" t="s">
+      <c r="F76" s="64" t="s">
         <v>167</v>
       </c>
-      <c r="G73" s="64"/>
-    </row>
-    <row r="74" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="17" t="s">
+      <c r="G76" s="63"/>
+    </row>
+    <row r="77" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>172</v>
       </c>
-      <c r="B74" s="59" t="s">
+      <c r="B77" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="C74" s="62"/>
-      <c r="D74" s="59" t="s">
+      <c r="C77" s="61"/>
+      <c r="D77" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="E74" s="59" t="s">
+      <c r="E77" s="58" t="s">
         <v>175</v>
       </c>
-      <c r="G74" s="58"/>
-    </row>
-    <row r="75" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="17"/>
-      <c r="B75" s="73" t="s">
+      <c r="G77" s="57"/>
+    </row>
+    <row r="78" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="17"/>
+      <c r="B78" s="72" t="s">
         <v>140</v>
       </c>
-      <c r="C75" s="73"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="74"/>
-      <c r="F75" s="74"/>
-      <c r="G75" s="74"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B76" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="D76" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="E76" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="G76" s="41"/>
-    </row>
-    <row r="77" spans="1:7" s="67" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B77" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" s="67" t="s">
-        <v>199</v>
-      </c>
-      <c r="E77" s="67" t="s">
-        <v>212</v>
-      </c>
-      <c r="G77" s="66"/>
-    </row>
-    <row r="78" spans="1:7" s="67" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="17"/>
-      <c r="B78" s="73" t="s">
-        <v>213</v>
-      </c>
-      <c r="C78" s="73"/>
+      <c r="C78" s="72"/>
       <c r="D78" s="73"/>
       <c r="E78" s="73"/>
       <c r="F78" s="73"/>
-      <c r="G78" s="66"/>
-    </row>
-    <row r="79" spans="1:7" s="67" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="17" t="s">
+      <c r="G78" s="73"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>70</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="G79" s="40"/>
+    </row>
+    <row r="80" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>71</v>
+      </c>
+      <c r="B80" s="66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="E80" s="66" t="s">
+        <v>210</v>
+      </c>
+      <c r="G80" s="65"/>
+    </row>
+    <row r="81" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="17"/>
+      <c r="B81" s="72" t="s">
         <v>211</v>
       </c>
-      <c r="B79" s="67" t="s">
-        <v>207</v>
-      </c>
-      <c r="D79" s="67" t="s">
+      <c r="C81" s="72"/>
+      <c r="D81" s="72"/>
+      <c r="E81" s="72"/>
+      <c r="F81" s="72"/>
+      <c r="G81" s="65"/>
+    </row>
+    <row r="82" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>209</v>
+      </c>
+      <c r="B82" s="66" t="s">
+        <v>205</v>
+      </c>
+      <c r="D82" s="66" t="s">
+        <v>202</v>
+      </c>
+      <c r="F82" s="66" t="s">
         <v>204</v>
       </c>
-      <c r="F79" s="67" t="s">
+      <c r="G82" s="65"/>
+    </row>
+    <row r="83" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="17"/>
+      <c r="B83" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="G79" s="66"/>
-    </row>
-    <row r="80" spans="1:7" s="67" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="17"/>
-      <c r="B80" s="73" t="s">
-        <v>208</v>
-      </c>
-      <c r="C80" s="73"/>
-      <c r="D80" s="73"/>
-      <c r="E80" s="73"/>
-      <c r="F80" s="73"/>
-      <c r="G80" s="66"/>
-    </row>
-    <row r="81" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="B81" s="59" t="s">
+      <c r="C83" s="72"/>
+      <c r="D83" s="72"/>
+      <c r="E83" s="72"/>
+      <c r="F83" s="72"/>
+      <c r="G83" s="65"/>
+    </row>
+    <row r="84" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>201</v>
+      </c>
+      <c r="B84" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="C81" s="62"/>
-      <c r="D81" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="E81" s="59" t="s">
+      <c r="C84" s="61"/>
+      <c r="D84" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="E84" s="58" t="s">
         <v>175</v>
       </c>
-      <c r="G81" s="58"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="13"/>
-      <c r="K81" s="13"/>
-      <c r="L81" s="13"/>
-      <c r="M81" s="13"/>
-      <c r="N81" s="13"/>
-      <c r="O81" s="13"/>
-      <c r="P81" s="13"/>
-      <c r="Q81" s="13"/>
-    </row>
-    <row r="82" spans="1:17" s="67" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="17"/>
-      <c r="B82" s="73" t="s">
-        <v>176</v>
-      </c>
-      <c r="C82" s="74"/>
-      <c r="D82" s="74"/>
-      <c r="E82" s="74"/>
-      <c r="F82" s="74"/>
-      <c r="G82" s="66"/>
-    </row>
-    <row r="83" spans="1:17" s="67" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="B83" s="67" t="s">
+      <c r="G84" s="57"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="13"/>
+      <c r="L84" s="13"/>
+      <c r="M84" s="13"/>
+      <c r="N84" s="13"/>
+      <c r="O84" s="13"/>
+      <c r="P84" s="13"/>
+      <c r="Q84" s="13"/>
+    </row>
+    <row r="85" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="17"/>
+      <c r="B85" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="C85" s="73"/>
+      <c r="D85" s="73"/>
+      <c r="E85" s="73"/>
+      <c r="F85" s="73"/>
+      <c r="G85" s="65"/>
+    </row>
+    <row r="86" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>197</v>
+      </c>
+      <c r="B86" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="D83" s="67" t="s">
+      <c r="D86" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="E83" s="67" t="s">
+      <c r="E86" s="66" t="s">
         <v>175</v>
       </c>
-      <c r="G83" s="66"/>
-    </row>
-    <row r="84" spans="1:17" s="67" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="17"/>
-      <c r="B84" s="73" t="s">
+      <c r="G86" s="65"/>
+    </row>
+    <row r="87" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="17"/>
+      <c r="B87" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="C84" s="73"/>
-      <c r="D84" s="73"/>
-      <c r="E84" s="73"/>
-      <c r="F84" s="73"/>
-      <c r="G84" s="73"/>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A85" s="17" t="s">
+      <c r="C87" s="72"/>
+      <c r="D87" s="72"/>
+      <c r="E87" s="72"/>
+      <c r="F87" s="72"/>
+      <c r="G87" s="72"/>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>72</v>
       </c>
-      <c r="B85" s="13" t="s">
+      <c r="B88" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D85" s="13" t="s">
+      <c r="D88" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E85" s="13" t="s">
+      <c r="E88" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="G85" s="21"/>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B86" s="73" t="s">
+      <c r="G88" s="20"/>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B89" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="C86" s="73"/>
-      <c r="D86" s="74"/>
-      <c r="E86" s="74"/>
-      <c r="F86" s="74"/>
-      <c r="G86" s="74"/>
+      <c r="C89" s="72"/>
+      <c r="D89" s="73"/>
+      <c r="E89" s="73"/>
+      <c r="F89" s="73"/>
+      <c r="G89" s="73"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B86:G86"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B75:G75"/>
-    <mergeCell ref="B36:G36"/>
+  <mergeCells count="25">
     <mergeCell ref="B66:G66"/>
-    <mergeCell ref="B84:G84"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B89:G89"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B78:G78"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B54:F54"/>
     <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B64:F64"/>
     <mergeCell ref="B23:F23"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
     <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B52:F52"/>
     <mergeCell ref="B16:G16"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A45" r:id="rId1" display="NMC (Namecoin)"/>
-    <hyperlink ref="A71" r:id="rId2"/>
-    <hyperlink ref="A70" r:id="rId3"/>
-    <hyperlink ref="A68" r:id="rId4"/>
-    <hyperlink ref="A52" r:id="rId5"/>
-    <hyperlink ref="A34" r:id="rId6"/>
-    <hyperlink ref="A22" r:id="rId7"/>
-    <hyperlink ref="A33" r:id="rId8"/>
-    <hyperlink ref="A69" r:id="rId9"/>
-    <hyperlink ref="A21" r:id="rId10"/>
-    <hyperlink ref="A67" r:id="rId11" display="VIVO"/>
-    <hyperlink ref="A25" r:id="rId12"/>
-    <hyperlink ref="A76" r:id="rId13"/>
-    <hyperlink ref="A39" r:id="rId14"/>
-    <hyperlink ref="A50" r:id="rId15"/>
-    <hyperlink ref="A11" r:id="rId16"/>
-    <hyperlink ref="A40" r:id="rId17"/>
-    <hyperlink ref="A13" r:id="rId18"/>
-    <hyperlink ref="A85" r:id="rId19"/>
-    <hyperlink ref="A58" r:id="rId20"/>
-    <hyperlink ref="B7" r:id="rId21"/>
-    <hyperlink ref="A31" r:id="rId22" display="GBX"/>
-    <hyperlink ref="A60" r:id="rId23" display="UBQ"/>
-    <hyperlink ref="A81" r:id="rId24" display="ZEC"/>
-    <hyperlink ref="A74" r:id="rId25" display="ZCL"/>
-    <hyperlink ref="A35" r:id="rId26" display="ZCL"/>
-    <hyperlink ref="A65" r:id="rId27"/>
-    <hyperlink ref="A73" r:id="rId28" display="ZCL"/>
-    <hyperlink ref="A83" r:id="rId29" display="ZEC"/>
-    <hyperlink ref="A79" r:id="rId30" display="ZEC"/>
-    <hyperlink ref="A77" r:id="rId31"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -2641,359 +2654,359 @@
   <cols>
     <col min="1" max="1" width="7" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="91" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="32" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="10.7109375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="32" customFormat="1" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="32" t="s">
+    <row r="1" spans="1:3" s="31" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="29" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="23" customFormat="1" ht="20" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:3" s="22" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="23" customFormat="1" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:3" s="22" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="23" customFormat="1" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+    <row r="7" spans="1:3" s="22" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="23" customFormat="1" ht="20" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:3" s="22" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="23" customFormat="1" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
+    <row r="9" spans="1:3" s="22" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
+    <row r="10" spans="1:3" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
-      </c>
-      <c r="C10" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
+    <row r="11" spans="1:3" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
+    <row r="12" spans="1:3" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>221</v>
-      </c>
-      <c r="C12" s="49" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" s="48" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="42" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="42" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="42" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="29" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="29" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="29" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="28" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="28" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="28" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="28" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="28" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="28" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="28" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="28" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="28" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="30" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="28" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="28" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="28" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="28" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="28" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="35" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="28" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="28" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="28" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="28" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="28" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="28" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="28" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="28" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="29" t="s">
+      <c r="A54" s="28" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="28" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="28" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="29" t="s">
+      <c r="A57" s="28" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="29" t="s">
+      <c r="A58" s="28" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="29" t="s">
+      <c r="A59" s="28" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="28" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3050,14 +3063,14 @@
   <cols>
     <col min="1" max="1" width="14.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="41" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60.7109375" style="14" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="42"/>
+    <col min="5" max="16384" width="10.7109375" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -3066,7 +3079,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="38" x14ac:dyDescent="0.2">
@@ -3076,7 +3089,7 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3085,7 +3098,7 @@
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="36" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3094,28 +3107,28 @@
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="36"/>
     </row>
     <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="36" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="78"/>
+      <c r="C6" s="77"/>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="38" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3124,18 +3137,18 @@
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="37"/>
+      <c r="C8" s="36"/>
     </row>
     <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="80"/>
+      <c r="C9" s="79"/>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
-      <c r="B10" s="38"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
@@ -3147,12 +3160,12 @@
       <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="37"/>
+      <c r="C11" s="36"/>
     </row>
     <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="37"/>
+      <c r="C12" s="36"/>
     </row>
     <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
@@ -3181,10 +3194,10 @@
     </row>
     <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="82"/>
+      <c r="C16" s="81"/>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -3193,8 +3206,8 @@
       <c r="B17" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="48" t="s">
+      <c r="C17" s="39"/>
+      <c r="D17" s="47" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3258,15 +3271,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="71" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="71" t="s">
+    <row r="1" spans="1:3" s="70" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="70" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="71" t="s">
-        <v>220</v>
+      <c r="C1" s="70" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Touchup usability, especially of monitor Fix fiboMeter
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1900" windowWidth="25600" windowHeight="9920" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1900" windowWidth="25600" windowHeight="9920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="230">
   <si>
     <t>Miners (AMD)</t>
   </si>
@@ -527,9 +527,6 @@
   </si>
   <si>
     <t>/opt/ccminer-KlausT</t>
-  </si>
-  <si>
-    <t>NVIDIA</t>
   </si>
   <si>
     <t>AMD</t>
@@ -716,6 +713,18 @@
   </si>
   <si>
     <t>ETH%zpool</t>
+  </si>
+  <si>
+    <t>NVI</t>
+  </si>
+  <si>
+    <t>/opt/silentarmy/silentarmy</t>
+  </si>
+  <si>
+    <t>SILENTARMY</t>
+  </si>
+  <si>
+    <t>ALL</t>
   </si>
 </sst>
 </file>
@@ -877,14 +886,14 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="MicrosoftSansSerif"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <b/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="MicrosoftSansSerif"/>
       <family val="2"/>
@@ -926,7 +935,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1124,13 +1133,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -1166,6 +1172,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1455,7 +1467,7 @@
   <cols>
     <col min="1" max="1" width="16.5703125" style="54" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62.7109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.7109375" style="54"/>
+    <col min="3" max="16384" width="9.28515625" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1484,10 +1496,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="54" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="54" t="s">
         <v>203</v>
-      </c>
-      <c r="B4" s="54" t="s">
-        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1497,51 +1509,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="83" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" style="69" customWidth="1"/>
     <col min="6" max="6" width="98.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="84" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="C1" s="70" t="s">
         <v>192</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="D1" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="E1" s="68" t="s">
         <v>194</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="F1" s="51" t="s">
         <v>195</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>141</v>
       </c>
-      <c r="B2" t="s">
-        <v>166</v>
+      <c r="B2" s="83" t="s">
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D2" t="s">
         <v>143</v>
@@ -1554,28 +1567,28 @@
       <c r="A3" t="s">
         <v>160</v>
       </c>
-      <c r="B3" t="s">
-        <v>165</v>
+      <c r="B3" s="83" t="s">
+        <v>226</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D3" t="s">
         <v>161</v>
       </c>
       <c r="F3" s="60" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>163</v>
       </c>
-      <c r="B4" t="s">
-        <v>165</v>
+      <c r="B4" s="83" t="s">
+        <v>226</v>
       </c>
       <c r="C4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D4" t="s">
         <v>164</v>
@@ -1586,13 +1599,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E5" s="69" t="s">
         <v>152</v>
@@ -1600,44 +1613,50 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E6" s="69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E7" s="69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E8" s="69" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E9" s="69" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" s="83" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="83" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D11" t="s">
         <v>182</v>
       </c>
-      <c r="B10" t="s">
-        <v>166</v>
-      </c>
-      <c r="C10" t="s">
-        <v>214</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E11" s="69" t="s">
         <v>183</v>
-      </c>
-      <c r="E10" s="69" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E11" s="69" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1646,17 +1665,22 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="E13" s="69" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="83" t="s">
+        <v>226</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="60" t="s">
         <v>207</v>
-      </c>
-      <c r="B13" t="s">
-        <v>165</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="60" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -1668,9 +1692,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1682,30 +1706,31 @@
     <col min="5" max="5" width="32.140625" style="13" customWidth="1"/>
     <col min="6" max="6" width="69.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.7109375" style="13"/>
+    <col min="8" max="8" width="10.7109375" style="13"/>
+    <col min="9" max="16384" width="9.28515625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>190</v>
-      </c>
       <c r="G1" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1750,14 +1775,14 @@
     </row>
     <row r="8" spans="1:7" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
@@ -1807,54 +1832,54 @@
         <v>36</v>
       </c>
       <c r="B15" s="66" t="s">
-        <v>77</v>
+        <v>214</v>
       </c>
       <c r="D15" s="66" t="s">
         <v>73</v>
       </c>
       <c r="E15" s="66" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F15" s="65"/>
       <c r="G15" s="67"/>
     </row>
     <row r="16" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="74" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="75"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>77</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F17" s="65"/>
       <c r="G17" s="21"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
-      <c r="B18" s="75" t="s">
-        <v>199</v>
-      </c>
-      <c r="C18" s="75"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
+      <c r="B18" s="74" t="s">
+        <v>198</v>
+      </c>
+      <c r="C18" s="74"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
@@ -1869,13 +1894,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="72"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -1893,18 +1918,18 @@
         <v>93</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
-      <c r="B23" s="72" t="s">
+      <c r="B23" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
@@ -1923,11 +1948,11 @@
     </row>
     <row r="27" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B27" s="14"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="83"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="82"/>
       <c r="E27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1947,13 +1972,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
-      <c r="B29" s="75" t="s">
+      <c r="B29" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="C29" s="75"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="73"/>
+      <c r="F29" s="73"/>
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -1975,14 +2000,14 @@
     </row>
     <row r="31" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
-      <c r="B31" s="75" t="s">
+      <c r="B31" s="74" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="75"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="73"/>
     </row>
     <row r="32" spans="1:7" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -2005,13 +2030,13 @@
     </row>
     <row r="33" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
-      <c r="B33" s="72" t="s">
+      <c r="B33" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="C33" s="72"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="73"/>
+      <c r="E33" s="73"/>
+      <c r="F33" s="73"/>
       <c r="G33" s="40"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
@@ -2043,14 +2068,14 @@
     </row>
     <row r="37" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
-      <c r="B37" s="72" t="s">
+      <c r="B37" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="C37" s="72"/>
-      <c r="D37" s="73"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="73"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
@@ -2068,13 +2093,13 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
-      <c r="B39" s="72" t="s">
+      <c r="B39" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="C39" s="72"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="72"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -2097,19 +2122,19 @@
         <v>79</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G42" s="20"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
-      <c r="B43" s="72" t="s">
+      <c r="B43" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="72"/>
-      <c r="D43" s="73"/>
-      <c r="E43" s="73"/>
-      <c r="F43" s="73"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="72"/>
       <c r="G43" s="52" t="s">
         <v>107</v>
       </c>
@@ -2156,13 +2181,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
-      <c r="B50" s="72" t="s">
+      <c r="B50" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="72"/>
-      <c r="D50" s="73"/>
-      <c r="E50" s="73"/>
-      <c r="F50" s="73"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="72"/>
+      <c r="E50" s="72"/>
+      <c r="F50" s="72"/>
       <c r="G50" s="20"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -2182,42 +2207,42 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
-      <c r="B52" s="72" t="s">
+      <c r="B52" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="C52" s="72"/>
-      <c r="D52" s="73"/>
-      <c r="E52" s="73"/>
-      <c r="F52" s="73"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="72"/>
+      <c r="E52" s="72"/>
+      <c r="F52" s="72"/>
       <c r="G52" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B53" s="65" t="s">
         <v>124</v>
       </c>
       <c r="C53" s="65"/>
       <c r="D53" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E53" s="66" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G53" s="65"/>
     </row>
     <row r="54" spans="1:7" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="17"/>
-      <c r="B54" s="72" t="s">
-        <v>225</v>
-      </c>
-      <c r="C54" s="74"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-      <c r="F54" s="74"/>
+      <c r="B54" s="71" t="s">
+        <v>224</v>
+      </c>
+      <c r="C54" s="73"/>
+      <c r="D54" s="73"/>
+      <c r="E54" s="73"/>
+      <c r="F54" s="73"/>
       <c r="G54" s="65"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -2248,13 +2273,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="17"/>
-      <c r="B59" s="72" t="s">
+      <c r="B59" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="C59" s="72"/>
-      <c r="D59" s="73"/>
-      <c r="E59" s="73"/>
-      <c r="F59" s="73"/>
+      <c r="C59" s="71"/>
+      <c r="D59" s="72"/>
+      <c r="E59" s="72"/>
+      <c r="F59" s="72"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
@@ -2280,13 +2305,13 @@
     </row>
     <row r="62" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="17"/>
-      <c r="B62" s="75" t="s">
+      <c r="B62" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="C62" s="75"/>
-      <c r="D62" s="74"/>
-      <c r="E62" s="74"/>
-      <c r="F62" s="74"/>
+      <c r="C62" s="74"/>
+      <c r="D62" s="73"/>
+      <c r="E62" s="73"/>
+      <c r="F62" s="73"/>
       <c r="G62" s="52"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -2305,13 +2330,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="17"/>
-      <c r="B64" s="72" t="s">
+      <c r="B64" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="C64" s="72"/>
-      <c r="D64" s="73"/>
-      <c r="E64" s="73"/>
-      <c r="F64" s="73"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="72"/>
+      <c r="E64" s="72"/>
+      <c r="F64" s="72"/>
     </row>
     <row r="65" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="17" t="s">
@@ -2329,14 +2354,14 @@
       </c>
     </row>
     <row r="66" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="72" t="s">
+      <c r="B66" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="C66" s="72"/>
-      <c r="D66" s="73"/>
-      <c r="E66" s="73"/>
-      <c r="F66" s="73"/>
-      <c r="G66" s="73"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="72"/>
+      <c r="E66" s="72"/>
+      <c r="F66" s="72"/>
+      <c r="G66" s="72"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="17" t="s">
@@ -2348,10 +2373,10 @@
         <v>64</v>
       </c>
       <c r="B68" s="62" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C68" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D68" s="61" t="s">
         <v>153</v>
@@ -2362,18 +2387,18 @@
     </row>
     <row r="69" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="17"/>
-      <c r="B69" s="76" t="s">
-        <v>170</v>
-      </c>
-      <c r="C69" s="76"/>
-      <c r="D69" s="74"/>
-      <c r="E69" s="74"/>
-      <c r="F69" s="74"/>
-      <c r="G69" s="74"/>
+      <c r="B69" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="C69" s="75"/>
+      <c r="D69" s="73"/>
+      <c r="E69" s="73"/>
+      <c r="F69" s="73"/>
+      <c r="G69" s="73"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B70" s="62" t="s">
         <v>163</v>
@@ -2413,7 +2438,7 @@
     </row>
     <row r="76" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B76" s="64" t="s">
         <v>160</v>
@@ -2422,13 +2447,13 @@
         <v>156</v>
       </c>
       <c r="F76" s="64" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G76" s="63"/>
     </row>
     <row r="77" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B77" s="58" t="s">
         <v>86</v>
@@ -2438,20 +2463,20 @@
         <v>85</v>
       </c>
       <c r="E77" s="58" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G77" s="57"/>
     </row>
     <row r="78" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="17"/>
-      <c r="B78" s="72" t="s">
+      <c r="B78" s="71" t="s">
         <v>140</v>
       </c>
-      <c r="C78" s="72"/>
-      <c r="D78" s="73"/>
-      <c r="E78" s="73"/>
-      <c r="F78" s="73"/>
-      <c r="G78" s="73"/>
+      <c r="C78" s="71"/>
+      <c r="D78" s="72"/>
+      <c r="E78" s="72"/>
+      <c r="F78" s="72"/>
+      <c r="G78" s="72"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
@@ -2461,10 +2486,10 @@
         <v>160</v>
       </c>
       <c r="D79" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E79" s="13" t="s">
         <v>174</v>
-      </c>
-      <c r="E79" s="13" t="s">
-        <v>175</v>
       </c>
       <c r="G79" s="40"/>
     </row>
@@ -2476,63 +2501,63 @@
         <v>14</v>
       </c>
       <c r="D80" s="66" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E80" s="66" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G80" s="65"/>
     </row>
     <row r="81" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="17"/>
-      <c r="B81" s="72" t="s">
-        <v>211</v>
-      </c>
-      <c r="C81" s="72"/>
-      <c r="D81" s="72"/>
-      <c r="E81" s="72"/>
-      <c r="F81" s="72"/>
+      <c r="B81" s="71" t="s">
+        <v>210</v>
+      </c>
+      <c r="C81" s="71"/>
+      <c r="D81" s="71"/>
+      <c r="E81" s="71"/>
+      <c r="F81" s="71"/>
       <c r="G81" s="65"/>
     </row>
     <row r="82" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B82" s="66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D82" s="66" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F82" s="66" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G82" s="65"/>
     </row>
     <row r="83" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="17"/>
-      <c r="B83" s="72" t="s">
-        <v>206</v>
-      </c>
-      <c r="C83" s="72"/>
-      <c r="D83" s="72"/>
-      <c r="E83" s="72"/>
-      <c r="F83" s="72"/>
+      <c r="B83" s="71" t="s">
+        <v>205</v>
+      </c>
+      <c r="C83" s="71"/>
+      <c r="D83" s="71"/>
+      <c r="E83" s="71"/>
+      <c r="F83" s="71"/>
       <c r="G83" s="65"/>
     </row>
     <row r="84" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B84" s="58" t="s">
         <v>160</v>
       </c>
       <c r="C84" s="61"/>
       <c r="D84" s="58" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E84" s="58" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G84" s="57"/>
       <c r="H84" s="13"/>
@@ -2548,18 +2573,18 @@
     </row>
     <row r="85" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="17"/>
-      <c r="B85" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="C85" s="73"/>
-      <c r="D85" s="73"/>
-      <c r="E85" s="73"/>
-      <c r="F85" s="73"/>
+      <c r="B85" s="71" t="s">
+        <v>220</v>
+      </c>
+      <c r="C85" s="72"/>
+      <c r="D85" s="72"/>
+      <c r="E85" s="72"/>
+      <c r="F85" s="72"/>
       <c r="G85" s="65"/>
     </row>
     <row r="86" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B86" s="66" t="s">
         <v>86</v>
@@ -2568,20 +2593,20 @@
         <v>87</v>
       </c>
       <c r="E86" s="66" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G86" s="65"/>
     </row>
     <row r="87" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="17"/>
-      <c r="B87" s="72" t="s">
+      <c r="B87" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="C87" s="72"/>
-      <c r="D87" s="72"/>
-      <c r="E87" s="72"/>
-      <c r="F87" s="72"/>
-      <c r="G87" s="72"/>
+      <c r="C87" s="71"/>
+      <c r="D87" s="71"/>
+      <c r="E87" s="71"/>
+      <c r="F87" s="71"/>
+      <c r="G87" s="71"/>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
@@ -2594,19 +2619,19 @@
         <v>88</v>
       </c>
       <c r="E88" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G88" s="20"/>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B89" s="72" t="s">
+      <c r="B89" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="C89" s="72"/>
-      <c r="D89" s="73"/>
-      <c r="E89" s="73"/>
-      <c r="F89" s="73"/>
-      <c r="G89" s="73"/>
+      <c r="C89" s="71"/>
+      <c r="D89" s="72"/>
+      <c r="E89" s="72"/>
+      <c r="F89" s="72"/>
+      <c r="G89" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -2655,12 +2680,12 @@
     <col min="1" max="1" width="7" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="91" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="13"/>
+    <col min="4" max="16384" width="9.28515625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="31" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>108</v>
@@ -2734,7 +2759,7 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>115</v>
@@ -2754,7 +2779,7 @@
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C12" s="48" t="s">
         <v>129</v>
@@ -3065,12 +3090,12 @@
     <col min="2" max="2" width="18.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" style="41" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60.7109375" style="14" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="41"/>
+    <col min="5" max="16384" width="9.28515625" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -3079,7 +3104,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="38" x14ac:dyDescent="0.2">
@@ -3120,10 +3145,10 @@
     </row>
     <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="77"/>
+      <c r="C6" s="76"/>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
@@ -3141,10 +3166,10 @@
     </row>
     <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="79"/>
+      <c r="C9" s="78"/>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -3194,10 +3219,10 @@
     </row>
     <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="81"/>
+      <c r="C16" s="80"/>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -3273,13 +3298,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="70" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="70" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="70" t="s">
         <v>111</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding some more coins, mapped to more pools with appropriate miner clients
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="1800" windowWidth="25600" windowHeight="13000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="8880" yWindow="2400" windowWidth="25600" windowHeight="13000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="357">
   <si>
     <t>Miners (AMD)</t>
   </si>
@@ -710,12 +710,6 @@
     <t>na-zel.ragnarpool.ovh:2032</t>
   </si>
   <si>
-    <t>--server $URL --user $WALLET.$WORKER_NAME --pass x --port $PORT</t>
-  </si>
-  <si>
-    <t>t1QpiKCkZxybwzN1CX4adbrGQjpmaJj4Ldt:x</t>
-  </si>
-  <si>
     <t>--server $URL --user $USER.$WORKER_NAME --pass x --port $PORT</t>
   </si>
   <si>
@@ -827,12 +821,6 @@
     <t>346u4oMvACtZQK9RASzcgYoZwX4JaAd3Pi</t>
   </si>
   <si>
-    <t>UnderVolt</t>
-  </si>
-  <si>
-    <t>OverClock</t>
-  </si>
-  <si>
     <t>Watts</t>
   </si>
   <si>
@@ -872,9 +860,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Mh/s</t>
   </si>
   <si>
@@ -941,9 +926,6 @@
     <t>iEwW2Phvs7WResQJy3F7kFDpD374erQ5HN</t>
   </si>
   <si>
-    <t>--gpu-platform 0 --algorithm neoscrypt --pool-url &lt;URL_PORT&gt; --default-config $CONFIG_FILE</t>
-  </si>
-  <si>
     <t>INN_PAPER_WALLET</t>
   </si>
   <si>
@@ -965,12 +947,6 @@
     <t>albokiadt</t>
   </si>
   <si>
-    <t>NCEQ</t>
-  </si>
-  <si>
-    <t>NCET</t>
-  </si>
-  <si>
     <t>KMD</t>
   </si>
   <si>
@@ -983,9 +959,6 @@
     <t>RVN</t>
   </si>
   <si>
-    <t>ETH-mph</t>
-  </si>
-  <si>
     <t>eth.suprnova.cc:5005</t>
   </si>
   <si>
@@ -1038,6 +1011,102 @@
   </si>
   <si>
     <t>RIG-NVI</t>
+  </si>
+  <si>
+    <t>stratum+tcp://rvn.suprnova.cc:6667</t>
+  </si>
+  <si>
+    <t>﻿RPifGaVnKCo1eyCEWMtAtsUbC5gpgYpUS4</t>
+  </si>
+  <si>
+    <t>RVN_PAPER_WALLET</t>
+  </si>
+  <si>
+    <t>/opt/suprminer/ccminer</t>
+  </si>
+  <si>
+    <t>ETH-supr</t>
+  </si>
+  <si>
+    <t>ORE</t>
+  </si>
+  <si>
+    <t>stratum+tcp://pool.unimining.net:4533</t>
+  </si>
+  <si>
+    <t>ALGO</t>
+  </si>
+  <si>
+    <t>-o $URL_PORT --algo=$ALGO -u $WALLET -p c=$COIN $GPUS</t>
+  </si>
+  <si>
+    <t>neoscrypt</t>
+  </si>
+  <si>
+    <t>lyra2v2</t>
+  </si>
+  <si>
+    <t>x16r</t>
+  </si>
+  <si>
+    <t>-o $URL_PORT --algo=$ALGO -u $USER.$WORKER_NAME -p password</t>
+  </si>
+  <si>
+    <t>--gpu-platform 0 --algorithm $ALGO --pool-url &lt;URL_PORT&gt; --default-config $CONFIG_FILE</t>
+  </si>
+  <si>
+    <t>--server $URL --port $PORT --user $WALLET.$WORKER_NAME --pass x</t>
+  </si>
+  <si>
+    <t>us.komodominingpool.com:6666</t>
+  </si>
+  <si>
+    <t>--server $URL--user RQPH3ymE1ZJRDedxz2cjW2sUwYx477QsUX --pass x --port $PORT --server backup.komodominingpool.com --user RQPH3ymE1ZJRDedxz2cjW2sUwYx477QsUX --pass x --port $PORT --cuda_device 0</t>
+  </si>
+  <si>
+    <t>KMD-kmp</t>
+  </si>
+  <si>
+    <t>equihash</t>
+  </si>
+  <si>
+    <t>KMD_PAPER_WALLET</t>
+  </si>
+  <si>
+    <t>RKkNi3Vn1Q3LFsuxsE52DQPkcpBLoa1pnM</t>
+  </si>
+  <si>
+    <t>KMD-zpool</t>
+  </si>
+  <si>
+    <t>RKkNi3Vn1Q3LFSuxsE52DQPkcpBLoa1pnM</t>
+  </si>
+  <si>
+    <t>NHEQ</t>
+  </si>
+  <si>
+    <t>NHET</t>
+  </si>
+  <si>
+    <t>OC</t>
+  </si>
+  <si>
+    <t>UV</t>
+  </si>
+  <si>
+    <t>GPU-048ac11c-24be-8e3f-059e-2028689fb9cb</t>
+  </si>
+  <si>
+    <t>GPU-7cac86c5-b598-6294-149c-a53e0df86019</t>
+  </si>
+  <si>
+    <t>GPU-990059da-5633-1178-e4fe-f1f7fc50ad61</t>
+  </si>
+  <si>
+    <t>GPU-3768179a-d438-0c05-de32-7f38e9af63f1</t>
+  </si>
+  <si>
+    <t>Make</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1117,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1281,6 +1350,12 @@
       <name val="MicrosoftSansSerif"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="MicrosoftSansSerif"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1343,7 +1418,7 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1685,44 +1760,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1737,6 +1778,70 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2016,10 +2121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2053,58 +2158,74 @@
         <v>6502799436</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="54" t="s">
-        <v>192</v>
-      </c>
-      <c r="B4" s="54" t="s">
-        <v>193</v>
-      </c>
-    </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="54" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>244</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="54" t="s">
-        <v>302</v>
+        <v>243</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>300</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="54" t="s">
-        <v>256</v>
-      </c>
-      <c r="B7" s="95" t="s">
-        <v>255</v>
+        <v>296</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="54" t="s">
-        <v>237</v>
+        <v>344</v>
       </c>
       <c r="B8" s="54" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="54" t="s">
+        <v>254</v>
+      </c>
+      <c r="B11" s="95" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="54" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="C8" s="54" t="s">
-        <v>236</v>
-      </c>
-      <c r="D8" s="54" t="s">
+      <c r="C12" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="D12" s="54" t="s">
         <v>157</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E12" s="54" t="s">
         <v>213</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2114,8 +2235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2148,19 +2269,19 @@
         <v>186</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="100" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B2" s="110" t="s">
         <v>213</v>
       </c>
       <c r="C2" s="77"/>
       <c r="F2" s="111" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.2">
@@ -2175,7 +2296,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B4" s="72" t="s">
         <v>213</v>
@@ -2184,10 +2305,10 @@
         <v>199</v>
       </c>
       <c r="D4" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2195,7 +2316,7 @@
         <v>137</v>
       </c>
       <c r="B5" s="72" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C5" t="s">
         <v>202</v>
@@ -2254,17 +2375,17 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B10" s="72" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="91"/>
       <c r="F10" s="96" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G10" s="87"/>
       <c r="H10" s="87"/>
@@ -2290,53 +2411,53 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="B12" s="72" t="s">
         <v>213</v>
       </c>
       <c r="C12" t="s">
-        <v>199</v>
-      </c>
-      <c r="D12" t="s">
-        <v>156</v>
-      </c>
-      <c r="F12" s="60" t="s">
-        <v>238</v>
+        <v>279</v>
+      </c>
+      <c r="E12" s="92" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>167</v>
-      </c>
-      <c r="B13" s="72" t="s">
-        <v>213</v>
-      </c>
-      <c r="C13" t="s">
-        <v>284</v>
-      </c>
       <c r="E13" s="92" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E14" s="92" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E15" s="92" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E16" s="92" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E17" s="92" t="s">
-        <v>171</v>
+      <c r="A17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="72" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" t="s">
+        <v>156</v>
+      </c>
+      <c r="F17" s="60" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -2350,10 +2471,10 @@
         <v>14</v>
       </c>
       <c r="F18" s="60" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -2361,7 +2482,7 @@
         <v>215</v>
       </c>
       <c r="B19" s="72" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C19" t="s">
         <v>214</v>
@@ -2396,16 +2517,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B23" s="72" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C23" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D23" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="F23" s="60" t="s">
         <v>89</v>
@@ -2427,7 +2548,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Globals!$C$8:$F$8</xm:f>
+            <xm:f>Globals!$C$12:$F$12</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B20</xm:sqref>
         </x14:dataValidation>
@@ -2439,11 +2560,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R119"/>
+  <dimension ref="A1:S123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B104" sqref="B104:G104"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2451,15 +2572,16 @@
     <col min="1" max="1" width="14.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="83" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="61" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="69.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.7109375" style="13"/>
+    <col min="4" max="4" width="7.140625" style="135" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="61" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="69.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.7109375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="19" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>175</v>
       </c>
@@ -2467,96 +2589,102 @@
         <v>176</v>
       </c>
       <c r="C1" s="93" t="s">
-        <v>242</v>
-      </c>
-      <c r="D1" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1" s="93" t="s">
+        <v>332</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="83"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="13" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
-      <c r="B7" s="123" t="s">
-        <v>249</v>
-      </c>
-      <c r="C7" s="123"/>
-      <c r="D7" s="124"/>
-      <c r="E7" s="124"/>
-      <c r="F7" s="124"/>
-      <c r="G7" s="124"/>
-    </row>
-    <row r="8" spans="1:8" s="118" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="145" t="s">
+        <v>247</v>
+      </c>
+      <c r="C7" s="145"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="146"/>
+      <c r="H7" s="146"/>
+    </row>
+    <row r="8" spans="1:9" s="118" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B8" s="118" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="118" t="s">
-        <v>304</v>
-      </c>
+      <c r="D8" s="135"/>
       <c r="F8" s="118" t="s">
+        <v>298</v>
+      </c>
+      <c r="G8" s="118" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="118" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
-      <c r="B9" s="123" t="s">
-        <v>226</v>
-      </c>
-      <c r="C9" s="123"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
-    </row>
-    <row r="10" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="145" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" s="145"/>
+      <c r="D9" s="145"/>
+      <c r="E9" s="146"/>
+      <c r="F9" s="146"/>
+      <c r="G9" s="146"/>
+      <c r="H9" s="146"/>
+    </row>
+    <row r="10" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="76" t="s">
         <v>116</v>
       </c>
@@ -2564,27 +2692,29 @@
         <v>115</v>
       </c>
       <c r="C10"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="41" t="s">
+      <c r="D10"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="G10" s="41" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
-      <c r="B11" s="123" t="s">
+      <c r="B11" s="145" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="123"/>
-      <c r="D11" s="123"/>
-      <c r="E11" s="124"/>
-      <c r="F11" s="124"/>
-      <c r="G11" s="124"/>
-      <c r="H11" s="124"/>
-    </row>
-    <row r="12" spans="1:8" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="145"/>
+      <c r="D11" s="145"/>
+      <c r="E11" s="145"/>
+      <c r="F11" s="146"/>
+      <c r="G11" s="146"/>
+      <c r="H11" s="146"/>
+      <c r="I11" s="146"/>
+    </row>
+    <row r="12" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>154</v>
       </c>
@@ -2592,123 +2722,133 @@
         <v>155</v>
       </c>
       <c r="C12"/>
-      <c r="D12"/>
-    </row>
-    <row r="13" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="104" t="s">
+        <v>334</v>
+      </c>
+      <c r="E12"/>
+    </row>
+    <row r="13" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B13" t="s">
         <v>155</v>
       </c>
       <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13" s="75" t="s">
-        <v>231</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D13" s="104" t="s">
+        <v>334</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13" s="75" t="s">
+        <v>229</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="76" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>74</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="F16" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="H16" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="76" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="76" t="s">
+        <v>329</v>
+      </c>
+      <c r="B19" s="66" t="s">
+        <v>255</v>
+      </c>
+      <c r="C19" s="83" t="s">
+        <v>234</v>
+      </c>
+      <c r="D19" s="135"/>
+      <c r="F19" s="66" t="s">
+        <v>307</v>
+      </c>
+      <c r="G19" s="66" t="s">
+        <v>302</v>
+      </c>
+      <c r="H19" s="65"/>
+      <c r="I19" s="67"/>
+    </row>
+    <row r="20" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="17"/>
+      <c r="B20" s="148" t="s">
+        <v>308</v>
+      </c>
+      <c r="C20" s="148"/>
+      <c r="D20" s="148"/>
+      <c r="E20" s="148"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="146"/>
+      <c r="H20" s="146"/>
+      <c r="I20" s="146"/>
+    </row>
+    <row r="21" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="76" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" s="66" t="s">
-        <v>257</v>
-      </c>
-      <c r="C19" s="83" t="s">
-        <v>236</v>
-      </c>
-      <c r="E19" s="66" t="s">
-        <v>316</v>
-      </c>
-      <c r="F19" s="66" t="s">
-        <v>308</v>
-      </c>
-      <c r="G19" s="65"/>
-      <c r="H19" s="67"/>
-    </row>
-    <row r="20" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
-      <c r="B20" s="125" t="s">
-        <v>317</v>
-      </c>
-      <c r="C20" s="125"/>
-      <c r="D20" s="125"/>
-      <c r="E20" s="124"/>
-      <c r="F20" s="124"/>
-      <c r="G20" s="124"/>
-      <c r="H20" s="124"/>
-    </row>
-    <row r="21" spans="1:8" s="120" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="76" t="s">
-        <v>315</v>
       </c>
       <c r="B21" s="120" t="s">
         <v>202</v>
       </c>
       <c r="C21" s="120" t="s">
-        <v>236</v>
-      </c>
-      <c r="E21" s="120" t="s">
+        <v>234</v>
+      </c>
+      <c r="D21" s="135"/>
+      <c r="F21" s="120" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="120" t="s">
+      <c r="G21" s="120" t="s">
         <v>166</v>
       </c>
-      <c r="G21" s="119"/>
-      <c r="H21" s="122"/>
-    </row>
-    <row r="22" spans="1:8" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H21" s="119"/>
+      <c r="I21" s="122"/>
+    </row>
+    <row r="22" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
-      <c r="B22" s="125" t="s">
-        <v>247</v>
-      </c>
-      <c r="C22" s="125"/>
-      <c r="D22" s="125"/>
-      <c r="E22" s="124"/>
-      <c r="F22" s="124"/>
-      <c r="G22" s="124"/>
-      <c r="H22" s="124"/>
-    </row>
-    <row r="23" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="148" t="s">
+        <v>245</v>
+      </c>
+      <c r="C22" s="148"/>
+      <c r="D22" s="148"/>
+      <c r="E22" s="148"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="146"/>
+      <c r="I22" s="146"/>
+    </row>
+    <row r="23" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="76" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B23" s="85" t="s">
         <v>202</v>
@@ -2716,192 +2856,204 @@
       <c r="C23" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="E23" s="101" t="s">
-        <v>285</v>
-      </c>
-      <c r="F23" s="85" t="s">
+      <c r="D23" s="135"/>
+      <c r="F23" s="101" t="s">
+        <v>280</v>
+      </c>
+      <c r="G23" s="85" t="s">
         <v>166</v>
       </c>
-      <c r="G23" s="112" t="s">
-        <v>252</v>
-      </c>
-      <c r="H23" s="86"/>
-    </row>
-    <row r="24" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H23" s="112" t="s">
+        <v>250</v>
+      </c>
+      <c r="I23" s="86"/>
+    </row>
+    <row r="24" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
-      <c r="B24" s="125" t="s">
-        <v>286</v>
-      </c>
-      <c r="C24" s="125"/>
-      <c r="D24" s="125"/>
-      <c r="E24" s="124"/>
-      <c r="F24" s="124"/>
-      <c r="G24" s="124"/>
-      <c r="H24" s="124"/>
-    </row>
-    <row r="25" spans="1:8" s="113" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="148" t="s">
+        <v>281</v>
+      </c>
+      <c r="C24" s="148"/>
+      <c r="D24" s="148"/>
+      <c r="E24" s="148"/>
+      <c r="F24" s="146"/>
+      <c r="G24" s="146"/>
+      <c r="H24" s="146"/>
+      <c r="I24" s="146"/>
+    </row>
+    <row r="25" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B25" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="113" t="s">
-        <v>289</v>
-      </c>
+      <c r="D25" s="135"/>
       <c r="F25" s="113" t="s">
+        <v>284</v>
+      </c>
+      <c r="G25" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="G25" s="113" t="s">
-        <v>262</v>
-      </c>
-      <c r="H25" s="112"/>
-    </row>
-    <row r="26" spans="1:8" s="113" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H25" s="113" t="s">
+        <v>260</v>
+      </c>
+      <c r="I25" s="112"/>
+    </row>
+    <row r="26" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
-      <c r="B26" s="123" t="s">
-        <v>288</v>
-      </c>
-      <c r="C26" s="123"/>
-      <c r="D26" s="123"/>
-      <c r="E26" s="124"/>
-      <c r="F26" s="124"/>
-      <c r="G26" s="124"/>
-      <c r="H26" s="112"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="145" t="s">
+        <v>283</v>
+      </c>
+      <c r="C26" s="145"/>
+      <c r="D26" s="145"/>
+      <c r="E26" s="145"/>
+      <c r="F26" s="146"/>
+      <c r="G26" s="146"/>
+      <c r="H26" s="146"/>
+      <c r="I26" s="112"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="F27" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="F27" s="49" t="s">
+      <c r="G27" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="G27" s="65"/>
-      <c r="H27" s="21"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H27" s="65"/>
+      <c r="I27" s="21"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
-      <c r="B28" s="125" t="s">
+      <c r="B28" s="148" t="s">
         <v>189</v>
       </c>
-      <c r="C28" s="125"/>
-      <c r="D28" s="125"/>
-      <c r="E28" s="124"/>
-      <c r="F28" s="124"/>
-      <c r="G28" s="124"/>
-      <c r="H28" s="124"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C28" s="148"/>
+      <c r="D28" s="148"/>
+      <c r="E28" s="148"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="146"/>
+      <c r="I28" s="146"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="F29" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
-      <c r="B30" s="123" t="s">
+      <c r="B30" s="145" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="123"/>
-      <c r="D30" s="123"/>
-      <c r="E30" s="124"/>
-      <c r="F30" s="124"/>
-      <c r="G30" s="124"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C30" s="145"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="146"/>
+      <c r="G30" s="146"/>
+      <c r="H30" s="146"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="F32" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="G32" s="13" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
-      <c r="B33" s="123" t="s">
+      <c r="B33" s="145" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="123"/>
-      <c r="D33" s="123"/>
-      <c r="E33" s="124"/>
-      <c r="F33" s="124"/>
-      <c r="G33" s="124"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C33" s="145"/>
+      <c r="D33" s="145"/>
+      <c r="E33" s="145"/>
+      <c r="F33" s="146"/>
+      <c r="G33" s="146"/>
+      <c r="H33" s="146"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:18" s="66" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>209</v>
       </c>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="71"/>
-      <c r="F37" s="14"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D37" s="14"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="14"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="E38" s="50" t="s">
+      <c r="D38" s="136" t="s">
+        <v>334</v>
+      </c>
+      <c r="F38" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="G38" s="44" t="s">
+      <c r="H38" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="H38" s="20"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I38" s="20"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
-      <c r="B39" s="125" t="s">
-        <v>238</v>
-      </c>
-      <c r="C39" s="125"/>
-      <c r="D39" s="125"/>
-      <c r="E39" s="126"/>
-      <c r="F39" s="126"/>
-      <c r="G39" s="126"/>
-      <c r="H39" s="20"/>
-    </row>
-    <row r="40" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="148" t="s">
+        <v>236</v>
+      </c>
+      <c r="C39" s="148"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="148"/>
+      <c r="F39" s="147"/>
+      <c r="G39" s="147"/>
+      <c r="H39" s="147"/>
+      <c r="I39" s="20"/>
+    </row>
+    <row r="40" spans="1:19" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>132</v>
       </c>
@@ -2909,29 +3061,33 @@
         <v>20</v>
       </c>
       <c r="C40" s="83"/>
-      <c r="D40" s="61"/>
-      <c r="E40" s="45" t="s">
+      <c r="D40" s="136" t="s">
+        <v>334</v>
+      </c>
+      <c r="E40" s="61"/>
+      <c r="F40" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="F40" s="45" t="s">
+      <c r="G40" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="G40" s="45"/>
-      <c r="H40" s="43"/>
-    </row>
-    <row r="41" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H40" s="45"/>
+      <c r="I40" s="43"/>
+    </row>
+    <row r="41" spans="1:19" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
-      <c r="B41" s="125" t="s">
+      <c r="B41" s="148" t="s">
         <v>134</v>
       </c>
-      <c r="C41" s="125"/>
-      <c r="D41" s="125"/>
-      <c r="E41" s="126"/>
-      <c r="F41" s="126"/>
-      <c r="G41" s="126"/>
-      <c r="H41" s="126"/>
-    </row>
-    <row r="42" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="148"/>
+      <c r="D41" s="148"/>
+      <c r="E41" s="148"/>
+      <c r="F41" s="147"/>
+      <c r="G41" s="147"/>
+      <c r="H41" s="147"/>
+      <c r="I41" s="147"/>
+    </row>
+    <row r="42" spans="1:19" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -2939,70 +3095,74 @@
         <v>120</v>
       </c>
       <c r="C42" s="83"/>
-      <c r="D42" s="61"/>
-      <c r="E42" t="s">
+      <c r="D42" s="135"/>
+      <c r="E42" s="61"/>
+      <c r="F42" t="s">
         <v>121</v>
       </c>
-      <c r="F42" s="41" t="s">
+      <c r="G42" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="G42" s="41" t="s">
+      <c r="H42" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="H42" s="40"/>
-    </row>
-    <row r="43" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I42" s="40"/>
+    </row>
+    <row r="43" spans="1:19" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
-      <c r="B43" s="123" t="s">
+      <c r="B43" s="145" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="123"/>
-      <c r="D43" s="123"/>
-      <c r="E43" s="126"/>
-      <c r="F43" s="126"/>
-      <c r="G43" s="126"/>
-      <c r="H43" s="40"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C43" s="145"/>
+      <c r="D43" s="145"/>
+      <c r="E43" s="145"/>
+      <c r="F43" s="147"/>
+      <c r="G43" s="147"/>
+      <c r="H43" s="147"/>
+      <c r="I43" s="40"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
-      <c r="R44" s="59"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S44" s="59"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:18" s="85" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B46" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="E46" s="85" t="s">
-        <v>253</v>
-      </c>
-      <c r="F46" s="137" t="s">
-        <v>312</v>
-      </c>
-      <c r="G46" s="85" t="s">
+      <c r="D46" s="135"/>
+      <c r="F46" s="85" t="s">
+        <v>251</v>
+      </c>
+      <c r="G46" s="125" t="s">
+        <v>304</v>
+      </c>
+      <c r="H46" s="85" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:18" s="85" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
-      <c r="B47" s="123" t="s">
+      <c r="B47" s="145" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="123"/>
-      <c r="D47" s="123"/>
-      <c r="E47" s="124"/>
-      <c r="F47" s="124"/>
-      <c r="G47" s="124"/>
-    </row>
-    <row r="48" spans="1:18" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="145"/>
+      <c r="D47" s="145"/>
+      <c r="E47" s="145"/>
+      <c r="F47" s="146"/>
+      <c r="G47" s="146"/>
+      <c r="H47" s="146"/>
+    </row>
+    <row r="48" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -3010,976 +3170,1107 @@
         <v>152</v>
       </c>
       <c r="C48" s="83"/>
-      <c r="D48" s="61"/>
-      <c r="E48" s="58" t="s">
-        <v>319</v>
-      </c>
-      <c r="F48" s="137" t="s">
-        <v>312</v>
-      </c>
-      <c r="G48" s="58" t="s">
+      <c r="D48" s="135"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="58" t="s">
+        <v>310</v>
+      </c>
+      <c r="G48" s="125" t="s">
+        <v>304</v>
+      </c>
+      <c r="H48" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="H48" s="57"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I48" s="57"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B49" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="F49" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="G49" s="13" t="s">
+      <c r="H49" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
-      <c r="B50" s="123" t="s">
+      <c r="B50" s="145" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="123"/>
-      <c r="D50" s="123"/>
-      <c r="E50" s="124"/>
-      <c r="F50" s="124"/>
-      <c r="G50" s="124"/>
-    </row>
-    <row r="51" spans="1:18" s="117" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A51" s="79" t="s">
-        <v>297</v>
-      </c>
-      <c r="B51" s="62" t="s">
+      <c r="C50" s="145"/>
+      <c r="D50" s="145"/>
+      <c r="E50" s="145"/>
+      <c r="F50" s="146"/>
+      <c r="G50" s="146"/>
+      <c r="H50" s="146"/>
+    </row>
+    <row r="51" spans="1:19" s="144" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A51" s="142" t="s">
+        <v>292</v>
+      </c>
+      <c r="B51" s="143" t="s">
         <v>160</v>
       </c>
-      <c r="C51" s="62" t="s">
+      <c r="C51" s="143" t="s">
         <v>213</v>
       </c>
-      <c r="D51" s="62" t="s">
-        <v>298</v>
-      </c>
-      <c r="E51" s="117" t="s">
-        <v>299</v>
-      </c>
-      <c r="G51" s="117" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" s="117" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D51" s="141" t="s">
+        <v>334</v>
+      </c>
+      <c r="E51" s="143" t="s">
+        <v>293</v>
+      </c>
+      <c r="F51" s="144" t="s">
+        <v>294</v>
+      </c>
+      <c r="H51" s="144" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
-      <c r="B52" s="127" t="s">
-        <v>301</v>
-      </c>
-      <c r="C52" s="127"/>
-      <c r="D52" s="127"/>
-      <c r="E52" s="126"/>
-      <c r="F52" s="126"/>
-      <c r="G52" s="126"/>
-      <c r="H52" s="126"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B52" s="149" t="s">
+        <v>338</v>
+      </c>
+      <c r="C52" s="149"/>
+      <c r="D52" s="149"/>
+      <c r="E52" s="149"/>
+      <c r="F52" s="147"/>
+      <c r="G52" s="147"/>
+      <c r="H52" s="147"/>
+      <c r="I52" s="147"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:18" s="135" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="134" t="s">
-        <v>311</v>
-      </c>
-      <c r="B54" s="135" t="s">
+    <row r="54" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="B54" s="125" t="s">
+        <v>299</v>
+      </c>
+      <c r="E54" s="125" t="s">
+        <v>343</v>
+      </c>
+      <c r="F54" s="125" t="s">
+        <v>191</v>
+      </c>
+      <c r="G54" s="125" t="s">
+        <v>304</v>
+      </c>
+      <c r="H54" s="140" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="17" t="s">
+        <v>342</v>
+      </c>
+      <c r="B55" s="125" t="s">
+        <v>87</v>
+      </c>
+      <c r="F55" s="125" t="s">
+        <v>340</v>
+      </c>
+      <c r="G55" s="125" t="s">
+        <v>304</v>
+      </c>
+      <c r="H55" s="138"/>
+    </row>
+    <row r="56" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="17"/>
+      <c r="B56" s="150" t="s">
+        <v>341</v>
+      </c>
+      <c r="C56" s="146"/>
+      <c r="D56" s="146"/>
+      <c r="E56" s="146"/>
+      <c r="F56" s="146"/>
+      <c r="G56" s="146"/>
+      <c r="H56" s="146"/>
+    </row>
+    <row r="57" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="B57" s="125" t="s">
         <v>152</v>
       </c>
-      <c r="E54" s="135" t="s">
-        <v>313</v>
-      </c>
-      <c r="F54" s="135" t="s">
-        <v>312</v>
-      </c>
-      <c r="G54" s="136"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="F57" s="125" t="s">
+        <v>305</v>
+      </c>
+      <c r="G57" s="125" t="s">
+        <v>304</v>
+      </c>
+      <c r="H57" s="138"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A56" s="17" t="s">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A59" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B59" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E56" s="13" t="s">
+      <c r="F59" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F56" s="13" t="s">
+      <c r="G59" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="H56" s="20"/>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A57" s="17"/>
-      <c r="B57" s="123" t="s">
+      <c r="I59" s="20"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A60" s="17"/>
+      <c r="B60" s="145" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="123"/>
-      <c r="D57" s="123"/>
-      <c r="E57" s="124"/>
-      <c r="F57" s="124"/>
-      <c r="G57" s="124"/>
-      <c r="H57" s="52" t="s">
+      <c r="C60" s="145"/>
+      <c r="D60" s="145"/>
+      <c r="E60" s="145"/>
+      <c r="F60" s="146"/>
+      <c r="G60" s="146"/>
+      <c r="H60" s="146"/>
+      <c r="I60" s="52" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A58" s="17" t="s">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A61" s="17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A59" s="17" t="s">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A62" s="17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:18" s="94" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="133" t="s">
-        <v>309</v>
-      </c>
-      <c r="B60" s="114" t="s">
-        <v>283</v>
-      </c>
-      <c r="C60" s="115"/>
-      <c r="D60" s="115"/>
-      <c r="E60" s="115" t="s">
+    <row r="63" spans="1:19" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="123" t="s">
+        <v>348</v>
+      </c>
+      <c r="B63" s="114" t="s">
+        <v>278</v>
+      </c>
+      <c r="C63" s="115"/>
+      <c r="D63" s="115"/>
+      <c r="E63" s="115"/>
+      <c r="F63" s="115" t="s">
+        <v>258</v>
+      </c>
+      <c r="G63" s="115"/>
+      <c r="H63" s="115" t="s">
         <v>260</v>
       </c>
-      <c r="F60" s="115"/>
-      <c r="G60" s="115" t="s">
-        <v>262</v>
-      </c>
-      <c r="H60" s="115"/>
-      <c r="I60" s="115"/>
-      <c r="J60" s="115"/>
-      <c r="K60" s="115"/>
-      <c r="L60" s="115"/>
-      <c r="M60" s="115"/>
-      <c r="N60" s="115"/>
-      <c r="O60" s="115"/>
-      <c r="P60" s="115"/>
-      <c r="Q60" s="115"/>
-      <c r="R60" s="115"/>
-    </row>
-    <row r="61" spans="1:18" s="85" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="133" t="s">
-        <v>310</v>
-      </c>
-      <c r="B61" s="114" t="s">
-        <v>282</v>
-      </c>
-      <c r="C61" s="115"/>
-      <c r="D61" s="115"/>
-      <c r="E61" s="115" t="s">
-        <v>258</v>
-      </c>
-      <c r="F61" s="115"/>
-      <c r="G61" s="115" t="s">
-        <v>262</v>
-      </c>
-      <c r="H61" s="115"/>
-      <c r="I61" s="115"/>
-      <c r="J61" s="115"/>
-      <c r="K61" s="115"/>
-      <c r="L61" s="115"/>
-      <c r="M61" s="115"/>
-      <c r="N61" s="115"/>
-      <c r="O61" s="115"/>
-      <c r="P61" s="115"/>
-      <c r="Q61" s="115"/>
-      <c r="R61" s="115"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="I63" s="115"/>
+      <c r="J63" s="115"/>
+      <c r="K63" s="115"/>
+      <c r="L63" s="115"/>
+      <c r="M63" s="115"/>
+      <c r="N63" s="115"/>
+      <c r="O63" s="115"/>
+      <c r="P63" s="115"/>
+      <c r="Q63" s="115"/>
+      <c r="R63" s="115"/>
+      <c r="S63" s="115"/>
+    </row>
+    <row r="64" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="123" t="s">
+        <v>349</v>
+      </c>
+      <c r="B64" s="114" t="s">
+        <v>277</v>
+      </c>
+      <c r="C64" s="115"/>
+      <c r="D64" s="115"/>
+      <c r="E64" s="115"/>
+      <c r="F64" s="115" t="s">
+        <v>256</v>
+      </c>
+      <c r="G64" s="115"/>
+      <c r="H64" s="115" t="s">
+        <v>260</v>
+      </c>
+      <c r="I64" s="115"/>
+      <c r="J64" s="115"/>
+      <c r="K64" s="115"/>
+      <c r="L64" s="115"/>
+      <c r="M64" s="115"/>
+      <c r="N64" s="115"/>
+      <c r="O64" s="115"/>
+      <c r="P64" s="115"/>
+      <c r="Q64" s="115"/>
+      <c r="R64" s="115"/>
+      <c r="S64" s="115"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A63" s="17" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="17" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A64" s="17" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="17" t="s">
+    <row r="68" spans="1:9" s="135" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="139" t="s">
+        <v>330</v>
+      </c>
+      <c r="B68" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="D68" s="135" t="s">
+        <v>335</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="H68" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B65" s="85" t="s">
+      <c r="B69" s="85" t="s">
         <v>202</v>
       </c>
-      <c r="E65" s="85" t="s">
+      <c r="D69" s="135"/>
+      <c r="F69" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="F65" s="85" t="s">
+      <c r="G69" s="85" t="s">
         <v>166</v>
       </c>
-      <c r="G65" s="85" t="s">
+      <c r="H69" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="H65" s="84"/>
-    </row>
-    <row r="66" spans="1:8" s="85" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="17"/>
-      <c r="B66" s="123" t="s">
-        <v>254</v>
-      </c>
-      <c r="C66" s="123"/>
-      <c r="D66" s="123"/>
-      <c r="E66" s="124"/>
-      <c r="F66" s="124"/>
-      <c r="G66" s="124"/>
-      <c r="H66" s="84"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="B67" s="13" t="s">
+      <c r="I69" s="84"/>
+    </row>
+    <row r="70" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="17"/>
+      <c r="B70" s="145" t="s">
+        <v>252</v>
+      </c>
+      <c r="C70" s="145"/>
+      <c r="D70" s="145"/>
+      <c r="E70" s="145"/>
+      <c r="F70" s="146"/>
+      <c r="G70" s="146"/>
+      <c r="H70" s="146"/>
+      <c r="I70" s="84"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="B71" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E67" s="13" t="s">
+      <c r="F71" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F67" s="13" t="s">
+      <c r="G71" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="H67" s="20"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="17"/>
-      <c r="B68" s="123" t="s">
+      <c r="I71" s="20"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="17"/>
+      <c r="B72" s="145" t="s">
         <v>83</v>
       </c>
-      <c r="C68" s="123"/>
-      <c r="D68" s="123"/>
-      <c r="E68" s="124"/>
-      <c r="F68" s="124"/>
-      <c r="G68" s="124"/>
-      <c r="H68" s="20"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>295</v>
-      </c>
-      <c r="B69" s="13" t="s">
+      <c r="C72" s="145"/>
+      <c r="D72" s="145"/>
+      <c r="E72" s="145"/>
+      <c r="F72" s="146"/>
+      <c r="G72" s="146"/>
+      <c r="H72" s="146"/>
+      <c r="I72" s="20"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>290</v>
+      </c>
+      <c r="B73" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E69" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="G69" s="13" t="s">
+      <c r="F73" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="H73" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H69" s="20"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="17"/>
-      <c r="B70" s="123" t="s">
-        <v>294</v>
-      </c>
-      <c r="C70" s="123"/>
-      <c r="D70" s="123"/>
-      <c r="E70" s="124"/>
-      <c r="F70" s="124"/>
-      <c r="G70" s="124"/>
-      <c r="H70" s="20" t="s">
+      <c r="I73" s="20"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="17"/>
+      <c r="B74" s="145" t="s">
+        <v>289</v>
+      </c>
+      <c r="C74" s="145"/>
+      <c r="D74" s="145"/>
+      <c r="E74" s="145"/>
+      <c r="F74" s="146"/>
+      <c r="G74" s="146"/>
+      <c r="H74" s="146"/>
+      <c r="I74" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="117" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="75" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>56</v>
       </c>
-      <c r="B71" s="117" t="s">
+      <c r="B75" s="117" t="s">
         <v>202</v>
       </c>
-      <c r="E71" s="117" t="s">
-        <v>296</v>
-      </c>
-      <c r="G71" s="117" t="s">
+      <c r="D75" s="135"/>
+      <c r="F75" s="117" t="s">
+        <v>291</v>
+      </c>
+      <c r="H75" s="117" t="s">
         <v>80</v>
       </c>
-      <c r="H71" s="116"/>
-    </row>
-    <row r="72" spans="1:8" s="117" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="17"/>
-      <c r="B72" s="123" t="s">
+      <c r="I75" s="116"/>
+    </row>
+    <row r="76" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="17"/>
+      <c r="B76" s="145" t="s">
         <v>98</v>
       </c>
-      <c r="C72" s="123"/>
-      <c r="D72" s="123"/>
-      <c r="E72" s="124"/>
-      <c r="F72" s="124"/>
-      <c r="G72" s="124"/>
-      <c r="H72" s="116" t="s">
+      <c r="C76" s="145"/>
+      <c r="D76" s="145"/>
+      <c r="E76" s="145"/>
+      <c r="F76" s="146"/>
+      <c r="G76" s="146"/>
+      <c r="H76" s="146"/>
+      <c r="I76" s="116" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="17" t="s">
+    <row r="77" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="B73" s="65" t="s">
+      <c r="B77" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="C73" s="82"/>
-      <c r="D73" s="65"/>
-      <c r="E73" t="s">
+      <c r="C77" s="82"/>
+      <c r="D77" s="134"/>
+      <c r="E77" s="65"/>
+      <c r="F77" t="s">
         <v>211</v>
       </c>
-      <c r="F73" s="66" t="s">
+      <c r="G77" s="66" t="s">
         <v>198</v>
       </c>
-      <c r="H73" s="65"/>
-    </row>
-    <row r="74" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="17"/>
-      <c r="B74" s="123" t="s">
+      <c r="I77" s="65"/>
+    </row>
+    <row r="78" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="17"/>
+      <c r="B78" s="145" t="s">
         <v>212</v>
       </c>
-      <c r="C74" s="123"/>
-      <c r="D74" s="126"/>
-      <c r="E74" s="126"/>
-      <c r="F74" s="126"/>
-      <c r="G74" s="126"/>
-      <c r="H74" s="65"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="C78" s="145"/>
+      <c r="D78" s="145"/>
+      <c r="E78" s="147"/>
+      <c r="F78" s="147"/>
+      <c r="G78" s="147"/>
+      <c r="H78" s="147"/>
+      <c r="I78" s="65"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:8" s="120" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>314</v>
-      </c>
-      <c r="E76" s="120" t="s">
-        <v>313</v>
-      </c>
-      <c r="G76" s="15" t="s">
+    <row r="80" spans="1:9" s="120" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A80" s="133" t="s">
+        <v>306</v>
+      </c>
+      <c r="B80" s="62" t="s">
+        <v>328</v>
+      </c>
+      <c r="D80" s="135" t="s">
+        <v>336</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="G80" s="120" t="s">
+        <v>302</v>
+      </c>
+      <c r="H80" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="I80" s="120" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="17"/>
+      <c r="B81" s="148" t="s">
+        <v>337</v>
+      </c>
+      <c r="C81" s="148"/>
+      <c r="D81" s="148"/>
+      <c r="E81" s="148"/>
+      <c r="F81" s="147"/>
+      <c r="G81" s="147"/>
+      <c r="H81" s="147"/>
+      <c r="I81" s="119"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F83" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="G83" s="124" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="17"/>
+      <c r="B84" s="145" t="s">
+        <v>96</v>
+      </c>
+      <c r="C84" s="145"/>
+      <c r="D84" s="145"/>
+      <c r="E84" s="145"/>
+      <c r="F84" s="146"/>
+      <c r="G84" s="146"/>
+      <c r="H84" s="146"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>61</v>
+      </c>
+      <c r="B86" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D86" s="136" t="s">
+        <v>334</v>
+      </c>
+      <c r="F86" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="H86" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="H76" s="120" t="s">
+      <c r="I86" s="53" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:8" s="120" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="17"/>
-      <c r="B77" s="125" t="s">
+    <row r="87" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="17"/>
+      <c r="B87" s="148" t="s">
         <v>133</v>
       </c>
-      <c r="C77" s="125"/>
-      <c r="D77" s="125"/>
-      <c r="E77" s="126"/>
-      <c r="F77" s="126"/>
-      <c r="G77" s="126"/>
-      <c r="H77" s="119"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B79" s="13" t="s">
+      <c r="C87" s="148"/>
+      <c r="D87" s="148"/>
+      <c r="E87" s="148"/>
+      <c r="F87" s="147"/>
+      <c r="G87" s="147"/>
+      <c r="H87" s="147"/>
+      <c r="I87" s="52"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>126</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="H88" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="17"/>
+      <c r="B89" s="145" t="s">
+        <v>101</v>
+      </c>
+      <c r="C89" s="145"/>
+      <c r="D89" s="145"/>
+      <c r="E89" s="145"/>
+      <c r="F89" s="146"/>
+      <c r="G89" s="146"/>
+      <c r="H89" s="146"/>
+    </row>
+    <row r="90" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B90" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="E79" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="F79" s="135" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="17"/>
-      <c r="B80" s="123" t="s">
-        <v>96</v>
-      </c>
-      <c r="C80" s="123"/>
-      <c r="D80" s="123"/>
-      <c r="E80" s="124"/>
-      <c r="F80" s="124"/>
-      <c r="G80" s="124"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>61</v>
-      </c>
-      <c r="B82" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="E82" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="G82" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="H82" s="53" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="17"/>
-      <c r="B83" s="125" t="s">
-        <v>133</v>
-      </c>
-      <c r="C83" s="125"/>
-      <c r="D83" s="125"/>
-      <c r="E83" s="126"/>
-      <c r="F83" s="126"/>
-      <c r="G83" s="126"/>
-      <c r="H83" s="52"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>126</v>
-      </c>
-      <c r="B84" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="G84" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="17"/>
-      <c r="B85" s="123" t="s">
-        <v>101</v>
-      </c>
-      <c r="C85" s="123"/>
-      <c r="D85" s="123"/>
-      <c r="E85" s="124"/>
-      <c r="F85" s="124"/>
-      <c r="G85" s="124"/>
-    </row>
-    <row r="86" spans="1:8" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B86" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="C86" s="83"/>
-      <c r="D86" s="61"/>
-      <c r="E86" s="44" t="s">
+      <c r="C90" s="83"/>
+      <c r="D90" s="135"/>
+      <c r="E90" s="61"/>
+      <c r="F90" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="F86" s="44" t="s">
+      <c r="G90" s="44" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B87" s="123" t="s">
+    <row r="91" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B91" s="145" t="s">
         <v>129</v>
       </c>
-      <c r="C87" s="123"/>
-      <c r="D87" s="123"/>
-      <c r="E87" s="124"/>
-      <c r="F87" s="124"/>
-      <c r="G87" s="124"/>
-      <c r="H87" s="124"/>
-    </row>
-    <row r="88" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="81" t="s">
-        <v>233</v>
-      </c>
-      <c r="B88" s="74"/>
-      <c r="C88" s="82"/>
-      <c r="D88" s="74"/>
-      <c r="E88" s="75" t="s">
+      <c r="C91" s="145"/>
+      <c r="D91" s="145"/>
+      <c r="E91" s="145"/>
+      <c r="F91" s="146"/>
+      <c r="G91" s="146"/>
+      <c r="H91" s="146"/>
+      <c r="I91" s="146"/>
+    </row>
+    <row r="92" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="B92" s="74"/>
+      <c r="C92" s="82"/>
+      <c r="D92" s="134"/>
+      <c r="E92" s="74"/>
+      <c r="F92" s="75" t="s">
+        <v>232</v>
+      </c>
+      <c r="H92" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>64</v>
+      </c>
+      <c r="B94" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="C94" s="62"/>
+      <c r="D94" s="62"/>
+      <c r="E94" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="F94" s="61" t="s">
+        <v>148</v>
+      </c>
+      <c r="H94" s="61" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="17"/>
+      <c r="B95" s="149" t="s">
+        <v>161</v>
+      </c>
+      <c r="C95" s="149"/>
+      <c r="D95" s="149"/>
+      <c r="E95" s="149"/>
+      <c r="F95" s="147"/>
+      <c r="G95" s="147"/>
+      <c r="H95" s="147"/>
+      <c r="I95" s="147"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>159</v>
+      </c>
+      <c r="B96" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C96" s="62"/>
+      <c r="D96" s="137" t="s">
+        <v>334</v>
+      </c>
+      <c r="E96" s="62"/>
+      <c r="F96" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="H96" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B102" s="75" t="s">
+        <v>299</v>
+      </c>
+      <c r="C102" s="83"/>
+      <c r="D102" s="135"/>
+      <c r="F102" s="75" t="s">
+        <v>232</v>
+      </c>
+      <c r="H102" s="75" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>164</v>
+      </c>
+      <c r="B103" s="64" t="s">
+        <v>152</v>
+      </c>
+      <c r="C103" s="83"/>
+      <c r="D103" s="135"/>
+      <c r="F103" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="H103" s="64" t="s">
+        <v>158</v>
+      </c>
+      <c r="I103" s="63"/>
+    </row>
+    <row r="104" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>163</v>
+      </c>
+      <c r="B104" s="58" t="s">
+        <v>237</v>
+      </c>
+      <c r="C104" s="83" t="s">
+        <v>157</v>
+      </c>
+      <c r="D104" s="135"/>
+      <c r="E104" s="61"/>
+      <c r="F104" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="G104" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="I104" s="57"/>
+    </row>
+    <row r="105" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="17"/>
+      <c r="B105" s="145" t="s">
+        <v>136</v>
+      </c>
+      <c r="C105" s="145"/>
+      <c r="D105" s="145"/>
+      <c r="E105" s="145"/>
+      <c r="F105" s="146"/>
+      <c r="G105" s="146"/>
+      <c r="H105" s="146"/>
+      <c r="I105" s="146"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>70</v>
+      </c>
+      <c r="B106" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C106" s="83" t="s">
+        <v>213</v>
+      </c>
+      <c r="F106" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G106" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="I106" s="40"/>
+    </row>
+    <row r="107" spans="1:9" s="98" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>70</v>
+      </c>
+      <c r="B107" s="98" t="s">
+        <v>216</v>
+      </c>
+      <c r="C107" s="98" t="s">
         <v>234</v>
       </c>
-      <c r="G88" s="8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>64</v>
-      </c>
-      <c r="B90" s="62" t="s">
-        <v>160</v>
-      </c>
-      <c r="C90" s="62"/>
-      <c r="D90" s="62" t="s">
-        <v>162</v>
-      </c>
-      <c r="E90" s="61" t="s">
-        <v>148</v>
-      </c>
-      <c r="G90" s="61" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="17"/>
-      <c r="B91" s="127" t="s">
-        <v>161</v>
-      </c>
-      <c r="C91" s="127"/>
-      <c r="D91" s="127"/>
-      <c r="E91" s="126"/>
-      <c r="F91" s="126"/>
-      <c r="G91" s="126"/>
-      <c r="H91" s="126"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>159</v>
-      </c>
-      <c r="B92" s="62" t="s">
-        <v>155</v>
-      </c>
-      <c r="C92" s="62"/>
-      <c r="D92" s="62"/>
-      <c r="E92" s="56" t="s">
-        <v>148</v>
-      </c>
-      <c r="G92" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A97" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="B98" s="75" t="s">
-        <v>305</v>
-      </c>
-      <c r="C98" s="83"/>
-      <c r="E98" s="75" t="s">
-        <v>234</v>
-      </c>
-      <c r="G98" s="75" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" s="64" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>164</v>
-      </c>
-      <c r="B99" s="64" t="s">
-        <v>152</v>
-      </c>
-      <c r="C99" s="83"/>
-      <c r="E99" s="64" t="s">
-        <v>151</v>
-      </c>
-      <c r="G99" s="64" t="s">
-        <v>158</v>
-      </c>
-      <c r="H99" s="63"/>
-    </row>
-    <row r="100" spans="1:18" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>163</v>
-      </c>
-      <c r="B100" s="58" t="s">
-        <v>239</v>
-      </c>
-      <c r="C100" s="83" t="s">
-        <v>157</v>
-      </c>
-      <c r="D100" s="61"/>
-      <c r="E100" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="F100" s="58" t="s">
+      <c r="D107" s="135"/>
+      <c r="F107" s="109" t="s">
+        <v>165</v>
+      </c>
+      <c r="G107" s="98" t="s">
         <v>166</v>
       </c>
-      <c r="H100" s="57"/>
-    </row>
-    <row r="101" spans="1:18" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="17"/>
-      <c r="B101" s="123" t="s">
-        <v>136</v>
-      </c>
-      <c r="C101" s="123"/>
-      <c r="D101" s="123"/>
-      <c r="E101" s="124"/>
-      <c r="F101" s="124"/>
-      <c r="G101" s="124"/>
-      <c r="H101" s="124"/>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>70</v>
-      </c>
-      <c r="B102" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C102" s="83" t="s">
-        <v>213</v>
-      </c>
-      <c r="E102" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="F102" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="H102" s="40"/>
-    </row>
-    <row r="103" spans="1:18" s="98" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>70</v>
-      </c>
-      <c r="B103" s="98" t="s">
-        <v>216</v>
-      </c>
-      <c r="C103" s="98" t="s">
-        <v>236</v>
-      </c>
-      <c r="E103" s="109" t="s">
-        <v>165</v>
-      </c>
-      <c r="F103" s="98" t="s">
-        <v>166</v>
-      </c>
-      <c r="H103" s="97"/>
-    </row>
-    <row r="104" spans="1:18" s="98" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="17"/>
-      <c r="B104" s="123" t="s">
-        <v>281</v>
-      </c>
-      <c r="C104" s="123"/>
-      <c r="D104" s="123"/>
-      <c r="E104" s="123"/>
-      <c r="F104" s="123"/>
-      <c r="G104" s="123"/>
-      <c r="H104" s="97"/>
-    </row>
-    <row r="105" spans="1:18" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="I107" s="97"/>
+    </row>
+    <row r="108" spans="1:9" s="98" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="17"/>
+      <c r="B108" s="145" t="s">
+        <v>276</v>
+      </c>
+      <c r="C108" s="145"/>
+      <c r="D108" s="145"/>
+      <c r="E108" s="145"/>
+      <c r="F108" s="145"/>
+      <c r="G108" s="145"/>
+      <c r="H108" s="145"/>
+      <c r="I108" s="97"/>
+    </row>
+    <row r="109" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>71</v>
       </c>
-      <c r="B105" s="66" t="s">
+      <c r="B109" s="66" t="s">
         <v>14</v>
-      </c>
-      <c r="C105" s="83" t="s">
-        <v>213</v>
-      </c>
-      <c r="E105" s="66" t="s">
-        <v>188</v>
-      </c>
-      <c r="F105" s="66" t="s">
-        <v>166</v>
-      </c>
-      <c r="H105" s="65"/>
-    </row>
-    <row r="106" spans="1:18" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="17"/>
-      <c r="B106" s="123" t="s">
-        <v>246</v>
-      </c>
-      <c r="C106" s="123"/>
-      <c r="D106" s="123"/>
-      <c r="E106" s="123"/>
-      <c r="F106" s="123"/>
-      <c r="G106" s="123"/>
-      <c r="H106" s="65"/>
-    </row>
-    <row r="107" spans="1:18" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>197</v>
-      </c>
-      <c r="B107" s="66" t="s">
-        <v>194</v>
-      </c>
-      <c r="C107" s="83"/>
-      <c r="E107" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F107" s="83" t="s">
-        <v>166</v>
-      </c>
-      <c r="G107" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="H107" s="65"/>
-    </row>
-    <row r="108" spans="1:18" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="17"/>
-      <c r="B108" s="123" t="s">
-        <v>195</v>
-      </c>
-      <c r="C108" s="123"/>
-      <c r="D108" s="123"/>
-      <c r="E108" s="123"/>
-      <c r="F108" s="123"/>
-      <c r="G108" s="123"/>
-      <c r="H108" s="65"/>
-    </row>
-    <row r="109" spans="1:18" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>243</v>
-      </c>
-      <c r="B109" s="58" t="s">
-        <v>152</v>
       </c>
       <c r="C109" s="83" t="s">
         <v>213</v>
       </c>
-      <c r="D109" s="61"/>
-      <c r="E109" s="58" t="s">
+      <c r="D109" s="135"/>
+      <c r="F109" s="66" t="s">
         <v>188</v>
       </c>
-      <c r="F109" s="58" t="s">
+      <c r="G109" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="H109" s="57"/>
-      <c r="I109" s="13"/>
-      <c r="J109" s="13"/>
-      <c r="K109" s="13"/>
-      <c r="L109" s="13"/>
-      <c r="M109" s="13"/>
-      <c r="N109" s="13"/>
-      <c r="O109" s="13"/>
-      <c r="P109" s="13"/>
-      <c r="Q109" s="13"/>
-      <c r="R109" s="13"/>
-    </row>
-    <row r="110" spans="1:18" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I109" s="65"/>
+    </row>
+    <row r="110" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="17"/>
-      <c r="B110" s="123" t="s">
+      <c r="B110" s="145" t="s">
+        <v>244</v>
+      </c>
+      <c r="C110" s="145"/>
+      <c r="D110" s="145"/>
+      <c r="E110" s="145"/>
+      <c r="F110" s="145"/>
+      <c r="G110" s="145"/>
+      <c r="H110" s="145"/>
+      <c r="I110" s="65"/>
+    </row>
+    <row r="111" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>197</v>
+      </c>
+      <c r="B111" s="66" t="s">
+        <v>194</v>
+      </c>
+      <c r="C111" s="83"/>
+      <c r="D111" s="136" t="s">
+        <v>334</v>
+      </c>
+      <c r="F111" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="G111" s="83" t="s">
+        <v>166</v>
+      </c>
+      <c r="H111" s="66" t="s">
+        <v>193</v>
+      </c>
+      <c r="I111" s="65"/>
+    </row>
+    <row r="112" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="17"/>
+      <c r="B112" s="145" t="s">
+        <v>195</v>
+      </c>
+      <c r="C112" s="145"/>
+      <c r="D112" s="145"/>
+      <c r="E112" s="145"/>
+      <c r="F112" s="145"/>
+      <c r="G112" s="145"/>
+      <c r="H112" s="145"/>
+      <c r="I112" s="65"/>
+    </row>
+    <row r="113" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>241</v>
+      </c>
+      <c r="B113" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="C113" s="83" t="s">
+        <v>213</v>
+      </c>
+      <c r="D113" s="135"/>
+      <c r="E113" s="61"/>
+      <c r="F113" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="G113" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="I113" s="57"/>
+      <c r="J113" s="13"/>
+      <c r="K113" s="13"/>
+      <c r="L113" s="13"/>
+      <c r="M113" s="13"/>
+      <c r="N113" s="13"/>
+      <c r="O113" s="13"/>
+      <c r="P113" s="13"/>
+      <c r="Q113" s="13"/>
+      <c r="R113" s="13"/>
+      <c r="S113" s="13"/>
+    </row>
+    <row r="114" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="17"/>
+      <c r="B114" s="145" t="s">
         <v>208</v>
       </c>
-      <c r="C110" s="123"/>
-      <c r="D110" s="124"/>
-      <c r="E110" s="124"/>
-      <c r="F110" s="124"/>
-      <c r="G110" s="124"/>
-      <c r="H110" s="65"/>
-    </row>
-    <row r="111" spans="1:18" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="C114" s="145"/>
+      <c r="D114" s="145"/>
+      <c r="E114" s="146"/>
+      <c r="F114" s="146"/>
+      <c r="G114" s="146"/>
+      <c r="H114" s="146"/>
+      <c r="I114" s="65"/>
+    </row>
+    <row r="115" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>187</v>
       </c>
-      <c r="B111" s="66" t="s">
-        <v>290</v>
-      </c>
-      <c r="C111" s="83"/>
-      <c r="E111" s="66" t="s">
+      <c r="B115" s="66" t="s">
+        <v>285</v>
+      </c>
+      <c r="C115" s="83"/>
+      <c r="D115" s="135"/>
+      <c r="F115" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="F111" s="66" t="s">
+      <c r="G115" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="H111" s="65"/>
-    </row>
-    <row r="112" spans="1:18" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="80" t="s">
+      <c r="I115" s="65"/>
+    </row>
+    <row r="116" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="80" t="s">
         <v>219</v>
       </c>
-      <c r="B112" s="75" t="s">
+      <c r="B116" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="C112" s="83"/>
-      <c r="E112" s="75" t="s">
+      <c r="C116" s="83"/>
+      <c r="D116" s="135"/>
+      <c r="F116" s="75" t="s">
         <v>221</v>
       </c>
-      <c r="G112" s="75" t="s">
+      <c r="H116" s="75" t="s">
         <v>220</v>
       </c>
-      <c r="H112" s="74"/>
-    </row>
-    <row r="113" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="16"/>
-      <c r="B113" s="74" t="s">
-        <v>224</v>
-      </c>
-      <c r="C113" s="82"/>
-      <c r="D113" s="74"/>
-    </row>
-    <row r="114" spans="1:8" s="75" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A114" s="79" t="s">
+      <c r="I116" s="74"/>
+    </row>
+    <row r="117" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="16"/>
+      <c r="B117" s="134" t="s">
+        <v>339</v>
+      </c>
+      <c r="C117" s="82"/>
+      <c r="D117" s="134"/>
+      <c r="E117" s="74"/>
+    </row>
+    <row r="118" spans="1:19" s="75" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A118" s="79" t="s">
+        <v>225</v>
+      </c>
+      <c r="B118" s="75" t="s">
+        <v>152</v>
+      </c>
+      <c r="C118" s="83"/>
+      <c r="D118" s="135"/>
+      <c r="F118" s="75" t="s">
+        <v>223</v>
+      </c>
+      <c r="H118" s="75" t="s">
+        <v>220</v>
+      </c>
+      <c r="I118" s="74"/>
+    </row>
+    <row r="119" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="16"/>
+      <c r="B119" s="134" t="s">
+        <v>339</v>
+      </c>
+      <c r="C119" s="82"/>
+      <c r="D119" s="134"/>
+      <c r="E119" s="74"/>
+    </row>
+    <row r="120" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="80" t="s">
         <v>227</v>
       </c>
-      <c r="B114" s="75" t="s">
+      <c r="B120" s="75" t="s">
+        <v>216</v>
+      </c>
+      <c r="C120" s="83"/>
+      <c r="D120" s="135"/>
+      <c r="F120" s="75" t="s">
+        <v>221</v>
+      </c>
+      <c r="H120" s="75" t="s">
+        <v>220</v>
+      </c>
+      <c r="I120" s="74"/>
+    </row>
+    <row r="121" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="16"/>
+      <c r="B121" s="145" t="s">
+        <v>226</v>
+      </c>
+      <c r="C121" s="145"/>
+      <c r="D121" s="145"/>
+      <c r="E121" s="145"/>
+      <c r="F121" s="146"/>
+      <c r="G121" s="146"/>
+      <c r="H121" s="146"/>
+      <c r="I121" s="146"/>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>72</v>
+      </c>
+      <c r="B122" s="120" t="s">
         <v>152</v>
       </c>
-      <c r="C114" s="83"/>
-      <c r="E114" s="75" t="s">
-        <v>223</v>
-      </c>
-      <c r="F114" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="H114" s="74"/>
-    </row>
-    <row r="115" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="16"/>
-      <c r="B115" s="74" t="s">
-        <v>226</v>
-      </c>
-      <c r="C115" s="82"/>
-      <c r="D115" s="74"/>
-    </row>
-    <row r="116" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="80" t="s">
-        <v>229</v>
-      </c>
-      <c r="B116" s="75" t="s">
-        <v>216</v>
-      </c>
-      <c r="C116" s="83"/>
-      <c r="E116" s="75" t="s">
-        <v>221</v>
-      </c>
-      <c r="G116" s="75" t="s">
-        <v>220</v>
-      </c>
-      <c r="H116" s="74"/>
-    </row>
-    <row r="117" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="16"/>
-      <c r="B117" s="123" t="s">
-        <v>228</v>
-      </c>
-      <c r="C117" s="123"/>
-      <c r="D117" s="123"/>
-      <c r="E117" s="124"/>
-      <c r="F117" s="124"/>
-      <c r="G117" s="124"/>
-      <c r="H117" s="124"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>72</v>
-      </c>
-      <c r="B118" s="120" t="s">
+      <c r="F122" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G122" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="I122" s="20"/>
+    </row>
+    <row r="123" spans="1:19" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="80" t="s">
+        <v>314</v>
+      </c>
+      <c r="B123" s="120" t="s">
         <v>152</v>
       </c>
-      <c r="E118" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F118" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="H118" s="20"/>
-    </row>
-    <row r="119" spans="1:8" s="120" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="80" t="s">
-        <v>323</v>
-      </c>
-      <c r="B119" s="120" t="s">
-        <v>152</v>
-      </c>
-      <c r="E119" s="120" t="s">
-        <v>321</v>
-      </c>
-      <c r="F119" s="137" t="s">
+      <c r="D123" s="135"/>
+      <c r="F123" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="G119" s="120" t="s">
-        <v>322</v>
-      </c>
-      <c r="H119" s="119"/>
+      <c r="G123" s="125" t="s">
+        <v>304</v>
+      </c>
+      <c r="H123" s="120" t="s">
+        <v>313</v>
+      </c>
+      <c r="I123" s="119"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B117:H117"/>
+  <mergeCells count="35">
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B121:I121"/>
+    <mergeCell ref="B91:I91"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B70:H70"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B81:H81"/>
+    <mergeCell ref="B76:H76"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B22:I22"/>
     <mergeCell ref="B87:H87"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="B104:G104"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B83:G83"/>
-    <mergeCell ref="B101:H101"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B91:H91"/>
-    <mergeCell ref="B110:G110"/>
-    <mergeCell ref="B108:G108"/>
-    <mergeCell ref="B106:G106"/>
-    <mergeCell ref="B74:G74"/>
-    <mergeCell ref="B85:G85"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B80:G80"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B68:G68"/>
-    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="B105:I105"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B95:I95"/>
+    <mergeCell ref="B50:H50"/>
+    <mergeCell ref="B60:H60"/>
+    <mergeCell ref="B72:H72"/>
+    <mergeCell ref="B74:H74"/>
+    <mergeCell ref="B56:H56"/>
+    <mergeCell ref="B114:H114"/>
+    <mergeCell ref="B112:H112"/>
+    <mergeCell ref="B110:H110"/>
+    <mergeCell ref="B78:H78"/>
+    <mergeCell ref="B89:H89"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B108:H108"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A114" r:id="rId1" display="ZEL"/>
-    <hyperlink ref="A112" r:id="rId2" display="ZEL-CBL"/>
-    <hyperlink ref="A116" r:id="rId3" display="ZEL-CBL"/>
-    <hyperlink ref="G13" r:id="rId4"/>
-    <hyperlink ref="A88" r:id="rId5"/>
-    <hyperlink ref="G88" r:id="rId6"/>
+    <hyperlink ref="A118" r:id="rId1" display="ZEL"/>
+    <hyperlink ref="A116" r:id="rId2" display="ZEL-CBL"/>
+    <hyperlink ref="A120" r:id="rId3" display="ZEL-CBL"/>
+    <hyperlink ref="H13" r:id="rId4"/>
+    <hyperlink ref="A92" r:id="rId5"/>
+    <hyperlink ref="H92" r:id="rId6"/>
     <hyperlink ref="B1" r:id="rId7"/>
-    <hyperlink ref="E23" r:id="rId8" location="/"/>
+    <hyperlink ref="F23" r:id="rId8" location="/"/>
     <hyperlink ref="A51" r:id="rId9"/>
-    <hyperlink ref="A119" r:id="rId10" display="ZEN"/>
+    <hyperlink ref="A123" r:id="rId10" display="ZEN"/>
+    <hyperlink ref="A80" r:id="rId11"/>
+    <hyperlink ref="F80" r:id="rId12"/>
+    <hyperlink ref="F68" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3988,19 +4279,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="106" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="106" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="137" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="106" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" style="106" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" style="99" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.28515625" style="108" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.28515625" style="62" bestFit="1" customWidth="1"/>
@@ -4008,49 +4299,49 @@
   <sheetData>
     <row r="1" spans="1:8" s="102" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="102" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B1" s="102" t="s">
-        <v>278</v>
+        <v>356</v>
       </c>
       <c r="C1" s="102" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D1" s="103" t="s">
-        <v>264</v>
+        <v>350</v>
       </c>
       <c r="E1" s="103" t="s">
-        <v>263</v>
+        <v>351</v>
       </c>
       <c r="F1" s="105" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="G1" s="107" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="H1" s="102" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="144" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="138" t="s">
-        <v>333</v>
-      </c>
-      <c r="B2" s="139"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="140"/>
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="132" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="126" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" s="127"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="128"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="104" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B3" s="104"/>
-      <c r="C3" s="62" t="s">
-        <v>325</v>
+      <c r="C3" s="137" t="s">
+        <v>316</v>
       </c>
       <c r="D3" s="106">
         <v>1400</v>
@@ -4064,47 +4355,27 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="104" t="s">
+        <v>352</v>
+      </c>
+      <c r="C4" s="137" t="s">
         <v>271</v>
-      </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="62" t="s">
-        <v>276</v>
-      </c>
-      <c r="D4" s="106">
-        <v>1350</v>
-      </c>
-      <c r="E4" s="106">
-        <v>160</v>
-      </c>
-      <c r="G4" s="108">
-        <v>31.85</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="104" t="s">
-        <v>270</v>
-      </c>
-      <c r="B5" s="104"/>
-      <c r="C5" s="62" t="s">
-        <v>276</v>
-      </c>
-      <c r="D5" s="106">
-        <v>1350</v>
-      </c>
-      <c r="E5" s="106">
-        <v>160</v>
-      </c>
-      <c r="G5" s="108">
-        <v>31.85</v>
+        <v>353</v>
+      </c>
+      <c r="C5" s="137" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="104" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="104"/>
+      <c r="C6" s="137" t="s">
         <v>272</v>
-      </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="62" t="s">
-        <v>276</v>
       </c>
       <c r="D6" s="106">
         <v>1350</v>
@@ -4118,11 +4389,11 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="104" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B7" s="104"/>
-      <c r="C7" s="62" t="s">
-        <v>276</v>
+      <c r="C7" s="137" t="s">
+        <v>272</v>
       </c>
       <c r="D7" s="106">
         <v>1350</v>
@@ -4135,225 +4406,258 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="104"/>
-      <c r="C8" s="62"/>
-      <c r="F8" s="121"/>
-    </row>
-    <row r="9" spans="1:8" s="144" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="138" t="s">
-        <v>332</v>
-      </c>
-      <c r="B9" s="139"/>
-      <c r="C9" s="140"/>
-      <c r="D9" s="141"/>
-      <c r="E9" s="141"/>
-      <c r="F9" s="142"/>
-      <c r="G9" s="143"/>
-      <c r="H9" s="140"/>
+      <c r="A8" s="104" t="s">
+        <v>268</v>
+      </c>
+      <c r="B8" s="104"/>
+      <c r="C8" s="137" t="s">
+        <v>272</v>
+      </c>
+      <c r="D8" s="106">
+        <v>1350</v>
+      </c>
+      <c r="E8" s="106">
+        <v>160</v>
+      </c>
+      <c r="G8" s="108">
+        <v>31.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="104" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" s="104"/>
+      <c r="C9" s="137" t="s">
+        <v>272</v>
+      </c>
+      <c r="D9" s="106">
+        <v>1350</v>
+      </c>
+      <c r="E9" s="106">
+        <v>160</v>
+      </c>
+      <c r="G9" s="108">
+        <v>31.85</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="104" t="s">
-        <v>267</v>
-      </c>
-      <c r="B10" s="104"/>
-      <c r="C10" s="62" t="s">
-        <v>275</v>
-      </c>
-      <c r="D10" s="106">
-        <v>1150</v>
-      </c>
-      <c r="E10" s="106">
-        <v>160</v>
-      </c>
-      <c r="G10" s="108">
-        <v>31.04</v>
-      </c>
-      <c r="H10" s="62">
-        <v>483.61</v>
+        <v>354</v>
+      </c>
+      <c r="C10" s="137" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="104" t="s">
-        <v>268</v>
-      </c>
-      <c r="B11" s="104"/>
-      <c r="C11" s="62" t="s">
-        <v>275</v>
-      </c>
-      <c r="D11" s="106">
+        <v>355</v>
+      </c>
+      <c r="C11" s="137" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="104"/>
+      <c r="F12" s="121"/>
+    </row>
+    <row r="13" spans="1:8" s="132" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="126" t="s">
+        <v>323</v>
+      </c>
+      <c r="B13" s="127"/>
+      <c r="C13" s="156"/>
+      <c r="D13" s="129"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="130"/>
+      <c r="G13" s="131"/>
+      <c r="H13" s="128"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="104" t="s">
+        <v>263</v>
+      </c>
+      <c r="B14" s="104"/>
+      <c r="C14" s="137" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" s="106">
         <v>1150</v>
       </c>
-      <c r="E11" s="106">
+      <c r="E14" s="106">
         <v>160</v>
       </c>
-      <c r="G11" s="108">
+      <c r="G14" s="108">
+        <v>31.04</v>
+      </c>
+      <c r="H14" s="62">
+        <v>483.61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="104" t="s">
+        <v>264</v>
+      </c>
+      <c r="B15" s="104"/>
+      <c r="C15" s="137" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="106">
+        <v>1150</v>
+      </c>
+      <c r="E15" s="106">
+        <v>160</v>
+      </c>
+      <c r="G15" s="108">
         <v>31.1</v>
       </c>
-      <c r="H11" s="62">
+      <c r="H15" s="62">
         <v>530.94000000000005</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="104" t="s">
-        <v>269</v>
-      </c>
-      <c r="B12" s="104"/>
-      <c r="C12" s="62" t="s">
-        <v>275</v>
-      </c>
-      <c r="D12" s="106">
-        <v>1150</v>
-      </c>
-      <c r="E12" s="106">
-        <v>160</v>
-      </c>
-      <c r="G12" s="108">
-        <v>31.21</v>
-      </c>
-      <c r="H12" s="62">
-        <v>532.42999999999995</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="104" t="s">
-        <v>273</v>
-      </c>
-      <c r="B13" s="104"/>
-      <c r="C13" s="62" t="s">
-        <v>275</v>
-      </c>
-      <c r="D13" s="106">
-        <v>1150</v>
-      </c>
-      <c r="E13" s="106">
-        <v>160</v>
-      </c>
-      <c r="G13" s="108">
-        <v>31.15</v>
-      </c>
-      <c r="H13" s="62">
-        <v>524.54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="104"/>
-      <c r="B14" s="104"/>
-      <c r="C14" s="62"/>
-      <c r="F14" s="121"/>
-    </row>
-    <row r="15" spans="1:8" s="144" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="138" t="s">
-        <v>331</v>
-      </c>
-      <c r="B15" s="139"/>
-      <c r="C15" s="140"/>
-      <c r="D15" s="141"/>
-      <c r="E15" s="141"/>
-      <c r="F15" s="142"/>
-      <c r="G15" s="143"/>
-      <c r="H15" s="140"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="104" t="s">
-        <v>326</v>
-      </c>
-      <c r="C16" s="62" t="s">
-        <v>275</v>
+        <v>265</v>
+      </c>
+      <c r="B16" s="104"/>
+      <c r="C16" s="137" t="s">
+        <v>271</v>
       </c>
       <c r="D16" s="106">
-        <v>1200</v>
+        <v>1150</v>
       </c>
       <c r="E16" s="106">
-        <v>140</v>
-      </c>
-      <c r="F16" s="121">
-        <v>138</v>
+        <v>160</v>
+      </c>
+      <c r="G16" s="108">
+        <v>31.21</v>
       </c>
       <c r="H16" s="62">
-        <v>524.9</v>
+        <v>532.42999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="104" t="s">
-        <v>327</v>
-      </c>
-      <c r="C17" s="62" t="s">
-        <v>275</v>
+        <v>269</v>
+      </c>
+      <c r="B17" s="104"/>
+      <c r="C17" s="137" t="s">
+        <v>271</v>
       </c>
       <c r="D17" s="106">
+        <v>1150</v>
+      </c>
+      <c r="E17" s="106">
+        <v>160</v>
+      </c>
+      <c r="G17" s="108">
+        <v>31.15</v>
+      </c>
+      <c r="H17" s="62">
+        <v>524.54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="104"/>
+      <c r="B18" s="104"/>
+      <c r="F18" s="121"/>
+    </row>
+    <row r="19" spans="1:8" s="132" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="126" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" s="127"/>
+      <c r="C19" s="156"/>
+      <c r="D19" s="129"/>
+      <c r="E19" s="129"/>
+      <c r="F19" s="130"/>
+      <c r="G19" s="131"/>
+      <c r="H19" s="128"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="104" t="s">
+        <v>317</v>
+      </c>
+      <c r="C20" s="137" t="s">
+        <v>271</v>
+      </c>
+      <c r="D20" s="106">
         <v>1200</v>
       </c>
-      <c r="E17" s="106">
+      <c r="E20" s="106">
         <v>140</v>
       </c>
-      <c r="F17" s="121">
+      <c r="F20" s="121">
+        <v>138</v>
+      </c>
+      <c r="H20" s="62">
+        <v>524.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="104" t="s">
+        <v>318</v>
+      </c>
+      <c r="C21" s="137" t="s">
+        <v>271</v>
+      </c>
+      <c r="D21" s="106">
+        <v>1200</v>
+      </c>
+      <c r="E21" s="106">
         <v>140</v>
       </c>
-      <c r="H17" s="62">
+      <c r="F21" s="121">
+        <v>140</v>
+      </c>
+      <c r="H21" s="62">
         <v>520.79999999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="104" t="s">
-        <v>328</v>
-      </c>
-      <c r="C18" s="62" t="s">
-        <v>275</v>
-      </c>
-      <c r="D18" s="106">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="104" t="s">
+        <v>319</v>
+      </c>
+      <c r="C22" s="137" t="s">
+        <v>271</v>
+      </c>
+      <c r="D22" s="106">
         <v>1200</v>
       </c>
-      <c r="E18" s="106">
+      <c r="E22" s="106">
         <v>140</v>
       </c>
-      <c r="F18" s="121">
+      <c r="F22" s="121">
         <v>139</v>
       </c>
-      <c r="H18" s="62">
+      <c r="H22" s="62">
         <v>527.52</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="104" t="s">
-        <v>329</v>
-      </c>
-      <c r="C19" s="62" t="s">
-        <v>275</v>
-      </c>
-      <c r="D19" s="106">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="104" t="s">
+        <v>320</v>
+      </c>
+      <c r="C23" s="137" t="s">
+        <v>271</v>
+      </c>
+      <c r="D23" s="106">
         <v>1200</v>
       </c>
-      <c r="E19" s="106">
+      <c r="E23" s="106">
         <v>140</v>
       </c>
-      <c r="F19" s="121">
+      <c r="F23" s="121">
         <v>135</v>
       </c>
-      <c r="H19" s="62">
+      <c r="H23" s="62">
         <v>480.8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="104"/>
-      <c r="B20" s="104"/>
-      <c r="C20" s="62"/>
-      <c r="F20" s="121"/>
-    </row>
-    <row r="21" spans="1:8" s="144" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="138"/>
-      <c r="B21" s="139"/>
-      <c r="C21" s="140"/>
-      <c r="D21" s="141"/>
-      <c r="E21" s="141"/>
-      <c r="F21" s="142"/>
-      <c r="G21" s="143"/>
-      <c r="H21" s="140"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="104"/>
-      <c r="B22" s="104"/>
-      <c r="C22" s="62"/>
-      <c r="F22" s="121"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="104"/>
+      <c r="B24" s="104"/>
+      <c r="F24" s="121"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4365,7 +4669,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -4839,10 +5143,10 @@
     </row>
     <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="128"/>
+      <c r="C6" s="151"/>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
@@ -4860,10 +5164,10 @@
     </row>
     <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="129" t="s">
+      <c r="B9" s="152" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="130"/>
+      <c r="C9" s="153"/>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -4913,10 +5217,10 @@
     </row>
     <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
-      <c r="B16" s="131" t="s">
+      <c r="B16" s="154" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="132"/>
+      <c r="C16" s="155"/>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">

</xml_diff>

<commit_message>
Add CoinMiner for BTX.
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/opt/git/miners/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/opt/git/mining/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8880" yWindow="2400" windowWidth="25600" windowHeight="13000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="25600" windowHeight="13000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="361">
   <si>
     <t>Miners (AMD)</t>
   </si>
@@ -1107,6 +1107,18 @@
   </si>
   <si>
     <t>Make</t>
+  </si>
+  <si>
+    <t>BTX</t>
+  </si>
+  <si>
+    <t>TimeTravel10</t>
+  </si>
+  <si>
+    <t>stratum+tcp://btx.suprnova.cc:3629</t>
+  </si>
+  <si>
+    <t>﻿1Cmt7oj41SzYdmk2q5AuMYFGoUG3P56Np</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1430,7 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1810,16 +1822,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1841,7 +1857,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2560,11 +2576,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S123"/>
+  <dimension ref="A1:S124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A51:XFD51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2647,15 +2663,15 @@
     </row>
     <row r="7" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
-      <c r="B7" s="145" t="s">
+      <c r="B7" s="147" t="s">
         <v>247</v>
       </c>
-      <c r="C7" s="145"/>
-      <c r="D7" s="145"/>
-      <c r="E7" s="146"/>
-      <c r="F7" s="146"/>
-      <c r="G7" s="146"/>
-      <c r="H7" s="146"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="148"/>
+      <c r="F7" s="148"/>
+      <c r="G7" s="148"/>
+      <c r="H7" s="148"/>
     </row>
     <row r="8" spans="1:9" s="118" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
@@ -2674,62 +2690,71 @@
     </row>
     <row r="9" spans="1:9" s="118" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
-      <c r="B9" s="145" t="s">
+      <c r="B9" s="147" t="s">
         <v>224</v>
       </c>
-      <c r="C9" s="145"/>
-      <c r="D9" s="145"/>
-      <c r="E9" s="146"/>
-      <c r="F9" s="146"/>
-      <c r="G9" s="146"/>
-      <c r="H9" s="146"/>
-    </row>
-    <row r="10" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="76" t="s">
+      <c r="C9" s="147"/>
+      <c r="D9" s="147"/>
+      <c r="E9" s="148"/>
+      <c r="F9" s="148"/>
+      <c r="G9" s="148"/>
+      <c r="H9" s="148"/>
+    </row>
+    <row r="10" spans="1:9" s="145" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="158" t="s">
+        <v>357</v>
+      </c>
+      <c r="B10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10" s="104" t="s">
+        <v>358</v>
+      </c>
+      <c r="E10" s="46"/>
+      <c r="F10" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="G10" s="145" t="s">
+        <v>302</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="76" t="s">
         <v>116</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>115</v>
       </c>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="41" t="s">
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="G10" s="41" t="s">
+      <c r="G11" s="41" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="145" t="s">
+    <row r="12" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="16"/>
+      <c r="B12" s="147" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="145"/>
-      <c r="D11" s="145"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="146"/>
-      <c r="G11" s="146"/>
-      <c r="H11" s="146"/>
-      <c r="I11" s="146"/>
-    </row>
-    <row r="12" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
+      <c r="C12" s="147"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="147"/>
+      <c r="F12" s="148"/>
+      <c r="G12" s="148"/>
+      <c r="H12" s="148"/>
+      <c r="I12" s="148"/>
+    </row>
+    <row r="13" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
         <v>154</v>
-      </c>
-      <c r="B12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C12"/>
-      <c r="D12" s="104" t="s">
-        <v>334</v>
-      </c>
-      <c r="E12"/>
-    </row>
-    <row r="13" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
-        <v>228</v>
       </c>
       <c r="B13" t="s">
         <v>155</v>
@@ -2739,665 +2764,649 @@
         <v>334</v>
       </c>
       <c r="E13"/>
-      <c r="F13" s="75" t="s">
+    </row>
+    <row r="14" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14" s="104" t="s">
+        <v>334</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14" s="75" t="s">
         <v>229</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A15" s="76" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" s="76" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B17" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F17" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H17" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A17" s="76" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" s="76" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="76" t="s">
+    <row r="20" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="76" t="s">
         <v>329</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="B20" s="66" t="s">
         <v>255</v>
       </c>
-      <c r="C19" s="83" t="s">
+      <c r="C20" s="83" t="s">
         <v>234</v>
       </c>
-      <c r="D19" s="135"/>
-      <c r="F19" s="66" t="s">
+      <c r="D20" s="135"/>
+      <c r="F20" s="66" t="s">
         <v>307</v>
       </c>
-      <c r="G19" s="66" t="s">
+      <c r="G20" s="66" t="s">
         <v>302</v>
       </c>
-      <c r="H19" s="65"/>
-      <c r="I19" s="67"/>
-    </row>
-    <row r="20" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
-      <c r="B20" s="148" t="s">
+      <c r="H20" s="65"/>
+      <c r="I20" s="67"/>
+    </row>
+    <row r="21" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="17"/>
+      <c r="B21" s="149" t="s">
         <v>308</v>
       </c>
-      <c r="C20" s="148"/>
-      <c r="D20" s="148"/>
-      <c r="E20" s="148"/>
-      <c r="F20" s="146"/>
-      <c r="G20" s="146"/>
-      <c r="H20" s="146"/>
-      <c r="I20" s="146"/>
-    </row>
-    <row r="21" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="76" t="s">
+      <c r="C21" s="149"/>
+      <c r="D21" s="149"/>
+      <c r="E21" s="149"/>
+      <c r="F21" s="148"/>
+      <c r="G21" s="148"/>
+      <c r="H21" s="148"/>
+      <c r="I21" s="148"/>
+    </row>
+    <row r="22" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="120" t="s">
+      <c r="B22" s="120" t="s">
         <v>202</v>
       </c>
-      <c r="C21" s="120" t="s">
+      <c r="C22" s="120" t="s">
         <v>234</v>
       </c>
-      <c r="D21" s="135"/>
-      <c r="F21" s="120" t="s">
+      <c r="D22" s="135"/>
+      <c r="F22" s="120" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="120" t="s">
+      <c r="G22" s="120" t="s">
         <v>166</v>
       </c>
-      <c r="H21" s="119"/>
-      <c r="I21" s="122"/>
-    </row>
-    <row r="22" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
-      <c r="B22" s="148" t="s">
+      <c r="H22" s="119"/>
+      <c r="I22" s="122"/>
+    </row>
+    <row r="23" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="17"/>
+      <c r="B23" s="149" t="s">
         <v>245</v>
       </c>
-      <c r="C22" s="148"/>
-      <c r="D22" s="148"/>
-      <c r="E22" s="148"/>
-      <c r="F22" s="146"/>
-      <c r="G22" s="146"/>
-      <c r="H22" s="146"/>
-      <c r="I22" s="146"/>
-    </row>
-    <row r="23" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="76" t="s">
+      <c r="C23" s="149"/>
+      <c r="D23" s="149"/>
+      <c r="E23" s="149"/>
+      <c r="F23" s="148"/>
+      <c r="G23" s="148"/>
+      <c r="H23" s="148"/>
+      <c r="I23" s="148"/>
+    </row>
+    <row r="24" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="76" t="s">
         <v>249</v>
       </c>
-      <c r="B23" s="85" t="s">
+      <c r="B24" s="85" t="s">
         <v>202</v>
       </c>
-      <c r="C23" s="85" t="s">
+      <c r="C24" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="D23" s="135"/>
-      <c r="F23" s="101" t="s">
+      <c r="D24" s="135"/>
+      <c r="F24" s="101" t="s">
         <v>280</v>
       </c>
-      <c r="G23" s="85" t="s">
+      <c r="G24" s="85" t="s">
         <v>166</v>
       </c>
-      <c r="H23" s="112" t="s">
+      <c r="H24" s="112" t="s">
         <v>250</v>
       </c>
-      <c r="I23" s="86"/>
-    </row>
-    <row r="24" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="17"/>
-      <c r="B24" s="148" t="s">
+      <c r="I24" s="86"/>
+    </row>
+    <row r="25" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="17"/>
+      <c r="B25" s="149" t="s">
         <v>281</v>
       </c>
-      <c r="C24" s="148"/>
-      <c r="D24" s="148"/>
-      <c r="E24" s="148"/>
-      <c r="F24" s="146"/>
-      <c r="G24" s="146"/>
-      <c r="H24" s="146"/>
-      <c r="I24" s="146"/>
-    </row>
-    <row r="25" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
+      <c r="C25" s="149"/>
+      <c r="D25" s="149"/>
+      <c r="E25" s="149"/>
+      <c r="F25" s="148"/>
+      <c r="G25" s="148"/>
+      <c r="H25" s="148"/>
+      <c r="I25" s="148"/>
+    </row>
+    <row r="26" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="B25" s="113" t="s">
+      <c r="B26" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="135"/>
-      <c r="F25" s="113" t="s">
+      <c r="D26" s="135"/>
+      <c r="F26" s="113" t="s">
         <v>284</v>
       </c>
-      <c r="G25" s="113" t="s">
+      <c r="G26" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="H25" s="113" t="s">
+      <c r="H26" s="113" t="s">
         <v>260</v>
       </c>
-      <c r="I25" s="112"/>
-    </row>
-    <row r="26" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="17"/>
-      <c r="B26" s="145" t="s">
+      <c r="I26" s="112"/>
+    </row>
+    <row r="27" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="17"/>
+      <c r="B27" s="147" t="s">
         <v>283</v>
       </c>
-      <c r="C26" s="145"/>
-      <c r="D26" s="145"/>
-      <c r="E26" s="145"/>
-      <c r="F26" s="146"/>
-      <c r="G26" s="146"/>
-      <c r="H26" s="146"/>
-      <c r="I26" s="112"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="C27" s="147"/>
+      <c r="D27" s="147"/>
+      <c r="E27" s="147"/>
+      <c r="F27" s="148"/>
+      <c r="G27" s="148"/>
+      <c r="H27" s="148"/>
+      <c r="I27" s="112"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>309</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B28" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F28" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="G27" s="49" t="s">
+      <c r="G28" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="H27" s="65"/>
-      <c r="I27" s="21"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
-      <c r="B28" s="148" t="s">
+      <c r="H28" s="65"/>
+      <c r="I28" s="21"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="17"/>
+      <c r="B29" s="149" t="s">
         <v>189</v>
       </c>
-      <c r="C28" s="148"/>
-      <c r="D28" s="148"/>
-      <c r="E28" s="148"/>
-      <c r="F28" s="146"/>
-      <c r="G28" s="146"/>
-      <c r="H28" s="146"/>
-      <c r="I28" s="146"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
+      <c r="C29" s="149"/>
+      <c r="D29" s="149"/>
+      <c r="E29" s="149"/>
+      <c r="F29" s="148"/>
+      <c r="G29" s="148"/>
+      <c r="H29" s="148"/>
+      <c r="I29" s="148"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B30" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F30" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-      <c r="B30" s="145" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="17"/>
+      <c r="B31" s="147" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="145"/>
-      <c r="D30" s="145"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="146"/>
-      <c r="G30" s="146"/>
-      <c r="H30" s="146"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
+      <c r="C31" s="147"/>
+      <c r="D31" s="147"/>
+      <c r="E31" s="147"/>
+      <c r="F31" s="148"/>
+      <c r="G31" s="148"/>
+      <c r="H31" s="148"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B33" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F33" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G33" s="13" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
-      <c r="B33" s="145" t="s">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A34" s="17"/>
+      <c r="B34" s="147" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="145"/>
-      <c r="D33" s="145"/>
-      <c r="E33" s="145"/>
-      <c r="F33" s="146"/>
-      <c r="G33" s="146"/>
-      <c r="H33" s="146"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
+      <c r="C34" s="147"/>
+      <c r="D34" s="147"/>
+      <c r="E34" s="147"/>
+      <c r="F34" s="148"/>
+      <c r="G34" s="148"/>
+      <c r="H34" s="148"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="38" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>209</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="71"/>
-      <c r="G37" s="14"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="14"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B39" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="D38" s="136" t="s">
+      <c r="D39" s="136" t="s">
         <v>334</v>
       </c>
-      <c r="F38" s="50" t="s">
+      <c r="F39" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="H38" s="44" t="s">
+      <c r="H39" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="I38" s="20"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
-      <c r="B39" s="148" t="s">
+      <c r="I39" s="20"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A40" s="17"/>
+      <c r="B40" s="149" t="s">
         <v>236</v>
       </c>
-      <c r="C39" s="148"/>
-      <c r="D39" s="148"/>
-      <c r="E39" s="148"/>
-      <c r="F39" s="147"/>
-      <c r="G39" s="147"/>
-      <c r="H39" s="147"/>
-      <c r="I39" s="20"/>
-    </row>
-    <row r="40" spans="1:19" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
+      <c r="C40" s="149"/>
+      <c r="D40" s="149"/>
+      <c r="E40" s="149"/>
+      <c r="F40" s="150"/>
+      <c r="G40" s="150"/>
+      <c r="H40" s="150"/>
+      <c r="I40" s="20"/>
+    </row>
+    <row r="41" spans="1:19" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B40" s="44" t="s">
+      <c r="B41" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="83"/>
-      <c r="D40" s="136" t="s">
+      <c r="C41" s="83"/>
+      <c r="D41" s="136" t="s">
         <v>334</v>
       </c>
-      <c r="E40" s="61"/>
-      <c r="F40" s="45" t="s">
+      <c r="E41" s="61"/>
+      <c r="F41" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="G40" s="45" t="s">
+      <c r="G41" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="H40" s="45"/>
-      <c r="I40" s="43"/>
-    </row>
-    <row r="41" spans="1:19" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
-      <c r="B41" s="148" t="s">
+      <c r="H41" s="45"/>
+      <c r="I41" s="43"/>
+    </row>
+    <row r="42" spans="1:19" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="17"/>
+      <c r="B42" s="149" t="s">
         <v>134</v>
       </c>
-      <c r="C41" s="148"/>
-      <c r="D41" s="148"/>
-      <c r="E41" s="148"/>
-      <c r="F41" s="147"/>
-      <c r="G41" s="147"/>
-      <c r="H41" s="147"/>
-      <c r="I41" s="147"/>
-    </row>
-    <row r="42" spans="1:19" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="C42" s="149"/>
+      <c r="D42" s="149"/>
+      <c r="E42" s="149"/>
+      <c r="F42" s="150"/>
+      <c r="G42" s="150"/>
+      <c r="H42" s="150"/>
+      <c r="I42" s="150"/>
+    </row>
+    <row r="43" spans="1:19" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>124</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B43" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="C42" s="83"/>
-      <c r="D42" s="135"/>
-      <c r="E42" s="61"/>
-      <c r="F42" t="s">
+      <c r="C43" s="83"/>
+      <c r="D43" s="135"/>
+      <c r="E43" s="61"/>
+      <c r="F43" t="s">
         <v>121</v>
       </c>
-      <c r="G42" s="41" t="s">
+      <c r="G43" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="H42" s="41" t="s">
+      <c r="H43" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="I42" s="40"/>
-    </row>
-    <row r="43" spans="1:19" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
-      <c r="B43" s="145" t="s">
+      <c r="I43" s="40"/>
+    </row>
+    <row r="44" spans="1:19" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="17"/>
+      <c r="B44" s="147" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="145"/>
-      <c r="D43" s="145"/>
-      <c r="E43" s="145"/>
-      <c r="F43" s="147"/>
-      <c r="G43" s="147"/>
-      <c r="H43" s="147"/>
-      <c r="I43" s="40"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>44</v>
-      </c>
-      <c r="S44" s="59"/>
+      <c r="C44" s="147"/>
+      <c r="D44" s="147"/>
+      <c r="E44" s="147"/>
+      <c r="F44" s="150"/>
+      <c r="G44" s="150"/>
+      <c r="H44" s="150"/>
+      <c r="I44" s="40"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="S45" s="59"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
+    <row r="47" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="B46" s="85" t="s">
+      <c r="B47" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="D46" s="135"/>
-      <c r="F46" s="85" t="s">
+      <c r="D47" s="135"/>
+      <c r="F47" s="85" t="s">
         <v>251</v>
       </c>
-      <c r="G46" s="125" t="s">
+      <c r="G47" s="125" t="s">
         <v>304</v>
       </c>
-      <c r="H46" s="85" t="s">
+      <c r="H47" s="85" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="17"/>
-      <c r="B47" s="145" t="s">
+    <row r="48" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="17"/>
+      <c r="B48" s="147" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="145"/>
-      <c r="D47" s="145"/>
-      <c r="E47" s="145"/>
-      <c r="F47" s="146"/>
-      <c r="G47" s="146"/>
-      <c r="H47" s="146"/>
-    </row>
-    <row r="48" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="C48" s="147"/>
+      <c r="D48" s="147"/>
+      <c r="E48" s="147"/>
+      <c r="F48" s="148"/>
+      <c r="G48" s="148"/>
+      <c r="H48" s="148"/>
+    </row>
+    <row r="49" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="58" t="s">
+      <c r="B49" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="C48" s="83"/>
-      <c r="D48" s="135"/>
-      <c r="E48" s="61"/>
-      <c r="F48" s="58" t="s">
+      <c r="C49" s="83"/>
+      <c r="D49" s="135"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="G48" s="125" t="s">
+      <c r="G49" s="125" t="s">
         <v>304</v>
       </c>
-      <c r="H48" s="58" t="s">
+      <c r="H49" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="I48" s="57"/>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
+      <c r="I49" s="57"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A50" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B50" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F49" s="13" t="s">
+      <c r="F50" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="H49" s="13" t="s">
+      <c r="H50" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A50" s="17"/>
-      <c r="B50" s="145" t="s">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A51" s="17"/>
+      <c r="B51" s="147" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="145"/>
-      <c r="D50" s="145"/>
-      <c r="E50" s="145"/>
-      <c r="F50" s="146"/>
-      <c r="G50" s="146"/>
-      <c r="H50" s="146"/>
-    </row>
-    <row r="51" spans="1:19" s="144" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A51" s="142" t="s">
+      <c r="C51" s="147"/>
+      <c r="D51" s="147"/>
+      <c r="E51" s="147"/>
+      <c r="F51" s="148"/>
+      <c r="G51" s="148"/>
+      <c r="H51" s="148"/>
+    </row>
+    <row r="52" spans="1:19" s="144" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A52" s="142" t="s">
         <v>292</v>
       </c>
-      <c r="B51" s="143" t="s">
+      <c r="B52" s="143" t="s">
         <v>160</v>
       </c>
-      <c r="C51" s="143" t="s">
+      <c r="C52" s="143" t="s">
         <v>213</v>
       </c>
-      <c r="D51" s="141" t="s">
+      <c r="D52" s="141" t="s">
         <v>334</v>
       </c>
-      <c r="E51" s="143" t="s">
+      <c r="E52" s="143" t="s">
         <v>293</v>
       </c>
-      <c r="F51" s="144" t="s">
+      <c r="F52" s="144" t="s">
         <v>294</v>
       </c>
-      <c r="H51" s="144" t="s">
+      <c r="H52" s="144" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="52" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="17"/>
-      <c r="B52" s="149" t="s">
+    <row r="53" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="17"/>
+      <c r="B53" s="151" t="s">
         <v>338</v>
       </c>
-      <c r="C52" s="149"/>
-      <c r="D52" s="149"/>
-      <c r="E52" s="149"/>
-      <c r="F52" s="147"/>
-      <c r="G52" s="147"/>
-      <c r="H52" s="147"/>
-      <c r="I52" s="147"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="C53" s="151"/>
+      <c r="D53" s="151"/>
+      <c r="E53" s="151"/>
+      <c r="F53" s="150"/>
+      <c r="G53" s="150"/>
+      <c r="H53" s="150"/>
+      <c r="I53" s="150"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="17" t="s">
-        <v>346</v>
-      </c>
-      <c r="B54" s="125" t="s">
-        <v>299</v>
-      </c>
-      <c r="E54" s="125" t="s">
-        <v>343</v>
-      </c>
-      <c r="F54" s="125" t="s">
-        <v>191</v>
-      </c>
-      <c r="G54" s="125" t="s">
-        <v>304</v>
-      </c>
-      <c r="H54" s="140" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="55" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="B55" s="125" t="s">
-        <v>87</v>
+        <v>299</v>
+      </c>
+      <c r="E55" s="125" t="s">
+        <v>343</v>
       </c>
       <c r="F55" s="125" t="s">
-        <v>340</v>
+        <v>191</v>
       </c>
       <c r="G55" s="125" t="s">
         <v>304</v>
       </c>
-      <c r="H55" s="138"/>
+      <c r="H55" s="140" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="56" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="150" t="s">
+      <c r="A56" s="17" t="s">
+        <v>342</v>
+      </c>
+      <c r="B56" s="125" t="s">
+        <v>87</v>
+      </c>
+      <c r="F56" s="125" t="s">
+        <v>340</v>
+      </c>
+      <c r="G56" s="125" t="s">
+        <v>304</v>
+      </c>
+      <c r="H56" s="138"/>
+    </row>
+    <row r="57" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="17"/>
+      <c r="B57" s="152" t="s">
         <v>341</v>
       </c>
-      <c r="C56" s="146"/>
-      <c r="D56" s="146"/>
-      <c r="E56" s="146"/>
-      <c r="F56" s="146"/>
-      <c r="G56" s="146"/>
-      <c r="H56" s="146"/>
-    </row>
-    <row r="57" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="17" t="s">
+      <c r="C57" s="148"/>
+      <c r="D57" s="148"/>
+      <c r="E57" s="148"/>
+      <c r="F57" s="148"/>
+      <c r="G57" s="148"/>
+      <c r="H57" s="148"/>
+    </row>
+    <row r="58" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="B57" s="125" t="s">
+      <c r="B58" s="125" t="s">
         <v>152</v>
       </c>
-      <c r="F57" s="125" t="s">
+      <c r="F58" s="125" t="s">
         <v>305</v>
       </c>
-      <c r="G57" s="125" t="s">
+      <c r="G58" s="125" t="s">
         <v>304</v>
       </c>
-      <c r="H57" s="138"/>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="H58" s="138"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A59" s="17" t="s">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A60" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B60" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F59" s="13" t="s">
+      <c r="F60" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="G59" s="13" t="s">
+      <c r="G60" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="I59" s="20"/>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A60" s="17"/>
-      <c r="B60" s="145" t="s">
+      <c r="I60" s="20"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A61" s="17"/>
+      <c r="B61" s="147" t="s">
         <v>97</v>
       </c>
-      <c r="C60" s="145"/>
-      <c r="D60" s="145"/>
-      <c r="E60" s="145"/>
-      <c r="F60" s="146"/>
-      <c r="G60" s="146"/>
-      <c r="H60" s="146"/>
-      <c r="I60" s="52" t="s">
+      <c r="C61" s="147"/>
+      <c r="D61" s="147"/>
+      <c r="E61" s="147"/>
+      <c r="F61" s="148"/>
+      <c r="G61" s="148"/>
+      <c r="H61" s="148"/>
+      <c r="I61" s="52" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A61" s="17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A63" s="17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="63" spans="1:19" s="94" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="123" t="s">
+    <row r="64" spans="1:19" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="123" t="s">
         <v>348</v>
       </c>
-      <c r="B63" s="114" t="s">
+      <c r="B64" s="114" t="s">
         <v>278</v>
-      </c>
-      <c r="C63" s="115"/>
-      <c r="D63" s="115"/>
-      <c r="E63" s="115"/>
-      <c r="F63" s="115" t="s">
-        <v>258</v>
-      </c>
-      <c r="G63" s="115"/>
-      <c r="H63" s="115" t="s">
-        <v>260</v>
-      </c>
-      <c r="I63" s="115"/>
-      <c r="J63" s="115"/>
-      <c r="K63" s="115"/>
-      <c r="L63" s="115"/>
-      <c r="M63" s="115"/>
-      <c r="N63" s="115"/>
-      <c r="O63" s="115"/>
-      <c r="P63" s="115"/>
-      <c r="Q63" s="115"/>
-      <c r="R63" s="115"/>
-      <c r="S63" s="115"/>
-    </row>
-    <row r="64" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="123" t="s">
-        <v>349</v>
-      </c>
-      <c r="B64" s="114" t="s">
-        <v>277</v>
       </c>
       <c r="C64" s="115"/>
       <c r="D64" s="115"/>
       <c r="E64" s="115"/>
       <c r="F64" s="115" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G64" s="115"/>
       <c r="H64" s="115" t="s">
@@ -3415,862 +3424,894 @@
       <c r="R64" s="115"/>
       <c r="S64" s="115"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="65" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="123" t="s">
+        <v>349</v>
+      </c>
+      <c r="B65" s="114" t="s">
+        <v>277</v>
+      </c>
+      <c r="C65" s="115"/>
+      <c r="D65" s="115"/>
+      <c r="E65" s="115"/>
+      <c r="F65" s="115" t="s">
+        <v>256</v>
+      </c>
+      <c r="G65" s="115"/>
+      <c r="H65" s="115" t="s">
+        <v>260</v>
+      </c>
+      <c r="I65" s="115"/>
+      <c r="J65" s="115"/>
+      <c r="K65" s="115"/>
+      <c r="L65" s="115"/>
+      <c r="M65" s="115"/>
+      <c r="N65" s="115"/>
+      <c r="O65" s="115"/>
+      <c r="P65" s="115"/>
+      <c r="Q65" s="115"/>
+      <c r="R65" s="115"/>
+      <c r="S65" s="115"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="17" t="s">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A67" s="17" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="17" t="s">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A68" s="17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="1:9" s="135" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="139" t="s">
+    <row r="69" spans="1:19" s="135" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="139" t="s">
         <v>330</v>
       </c>
-      <c r="B68" s="62" t="s">
+      <c r="B69" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="D68" s="135" t="s">
+      <c r="D69" s="135" t="s">
         <v>335</v>
       </c>
-      <c r="F68" s="8" t="s">
+      <c r="F69" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="H68" s="15" t="s">
+      <c r="H69" s="15" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="17" t="s">
+    <row r="70" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B69" s="85" t="s">
+      <c r="B70" s="85" t="s">
         <v>202</v>
       </c>
-      <c r="D69" s="135"/>
-      <c r="F69" s="85" t="s">
+      <c r="D70" s="135"/>
+      <c r="F70" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="G69" s="85" t="s">
+      <c r="G70" s="85" t="s">
         <v>166</v>
       </c>
-      <c r="H69" s="85" t="s">
+      <c r="H70" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="I69" s="84"/>
-    </row>
-    <row r="70" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="17"/>
-      <c r="B70" s="145" t="s">
+      <c r="I70" s="84"/>
+    </row>
+    <row r="71" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="17"/>
+      <c r="B71" s="147" t="s">
         <v>252</v>
       </c>
-      <c r="C70" s="145"/>
-      <c r="D70" s="145"/>
-      <c r="E70" s="145"/>
-      <c r="F70" s="146"/>
-      <c r="G70" s="146"/>
-      <c r="H70" s="146"/>
-      <c r="I70" s="84"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="17" t="s">
+      <c r="C71" s="147"/>
+      <c r="D71" s="147"/>
+      <c r="E71" s="147"/>
+      <c r="F71" s="148"/>
+      <c r="G71" s="148"/>
+      <c r="H71" s="148"/>
+      <c r="I71" s="84"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A72" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B72" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F71" s="13" t="s">
+      <c r="F72" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="G71" s="13" t="s">
+      <c r="G72" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="I71" s="20"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" s="17"/>
-      <c r="B72" s="145" t="s">
+      <c r="I72" s="20"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A73" s="17"/>
+      <c r="B73" s="147" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="145"/>
-      <c r="D72" s="145"/>
-      <c r="E72" s="145"/>
-      <c r="F72" s="146"/>
-      <c r="G72" s="146"/>
-      <c r="H72" s="146"/>
-      <c r="I72" s="20"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="C73" s="147"/>
+      <c r="D73" s="147"/>
+      <c r="E73" s="147"/>
+      <c r="F73" s="148"/>
+      <c r="G73" s="148"/>
+      <c r="H73" s="148"/>
+      <c r="I73" s="20"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>290</v>
       </c>
-      <c r="B73" s="13" t="s">
+      <c r="B74" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F73" s="13" t="s">
+      <c r="F74" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="H73" s="13" t="s">
+      <c r="H74" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="I73" s="20"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="17"/>
-      <c r="B74" s="145" t="s">
+      <c r="I74" s="20"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A75" s="17"/>
+      <c r="B75" s="147" t="s">
         <v>289</v>
       </c>
-      <c r="C74" s="145"/>
-      <c r="D74" s="145"/>
-      <c r="E74" s="145"/>
-      <c r="F74" s="146"/>
-      <c r="G74" s="146"/>
-      <c r="H74" s="146"/>
-      <c r="I74" s="20" t="s">
+      <c r="C75" s="147"/>
+      <c r="D75" s="147"/>
+      <c r="E75" s="147"/>
+      <c r="F75" s="148"/>
+      <c r="G75" s="148"/>
+      <c r="H75" s="148"/>
+      <c r="I75" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    <row r="76" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>56</v>
       </c>
-      <c r="B75" s="117" t="s">
+      <c r="B76" s="117" t="s">
         <v>202</v>
       </c>
-      <c r="D75" s="135"/>
-      <c r="F75" s="117" t="s">
+      <c r="D76" s="135"/>
+      <c r="F76" s="117" t="s">
         <v>291</v>
       </c>
-      <c r="H75" s="117" t="s">
+      <c r="H76" s="117" t="s">
         <v>80</v>
       </c>
-      <c r="I75" s="116"/>
-    </row>
-    <row r="76" spans="1:9" s="117" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="17"/>
-      <c r="B76" s="145" t="s">
+      <c r="I76" s="116"/>
+    </row>
+    <row r="77" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="17"/>
+      <c r="B77" s="147" t="s">
         <v>98</v>
       </c>
-      <c r="C76" s="145"/>
-      <c r="D76" s="145"/>
-      <c r="E76" s="145"/>
-      <c r="F76" s="146"/>
-      <c r="G76" s="146"/>
-      <c r="H76" s="146"/>
-      <c r="I76" s="116" t="s">
+      <c r="C77" s="147"/>
+      <c r="D77" s="147"/>
+      <c r="E77" s="147"/>
+      <c r="F77" s="148"/>
+      <c r="G77" s="148"/>
+      <c r="H77" s="148"/>
+      <c r="I77" s="116" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="17" t="s">
+    <row r="78" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="B77" s="65" t="s">
+      <c r="B78" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="C77" s="82"/>
-      <c r="D77" s="134"/>
-      <c r="E77" s="65"/>
-      <c r="F77" t="s">
+      <c r="C78" s="82"/>
+      <c r="D78" s="134"/>
+      <c r="E78" s="65"/>
+      <c r="F78" t="s">
         <v>211</v>
       </c>
-      <c r="G77" s="66" t="s">
+      <c r="G78" s="66" t="s">
         <v>198</v>
       </c>
-      <c r="I77" s="65"/>
-    </row>
-    <row r="78" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="17"/>
-      <c r="B78" s="145" t="s">
+      <c r="I78" s="65"/>
+    </row>
+    <row r="79" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="17"/>
+      <c r="B79" s="147" t="s">
         <v>212</v>
       </c>
-      <c r="C78" s="145"/>
-      <c r="D78" s="145"/>
-      <c r="E78" s="147"/>
-      <c r="F78" s="147"/>
-      <c r="G78" s="147"/>
-      <c r="H78" s="147"/>
-      <c r="I78" s="65"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="C79" s="147"/>
+      <c r="D79" s="147"/>
+      <c r="E79" s="150"/>
+      <c r="F79" s="150"/>
+      <c r="G79" s="150"/>
+      <c r="H79" s="150"/>
+      <c r="I79" s="65"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:9" s="120" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A80" s="133" t="s">
+    <row r="81" spans="1:9" s="120" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A81" s="133" t="s">
         <v>306</v>
       </c>
-      <c r="B80" s="62" t="s">
+      <c r="B81" s="62" t="s">
         <v>328</v>
       </c>
-      <c r="D80" s="135" t="s">
+      <c r="D81" s="135" t="s">
         <v>336</v>
       </c>
-      <c r="F80" s="8" t="s">
+      <c r="F81" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="G80" s="120" t="s">
+      <c r="G81" s="120" t="s">
         <v>302</v>
       </c>
-      <c r="H80" s="15" t="s">
+      <c r="H81" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="I80" s="120" t="s">
+      <c r="I81" s="120" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="81" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="17"/>
-      <c r="B81" s="148" t="s">
+    <row r="82" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="17"/>
+      <c r="B82" s="149" t="s">
         <v>337</v>
       </c>
-      <c r="C81" s="148"/>
-      <c r="D81" s="148"/>
-      <c r="E81" s="148"/>
-      <c r="F81" s="147"/>
-      <c r="G81" s="147"/>
-      <c r="H81" s="147"/>
-      <c r="I81" s="119"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="C82" s="149"/>
+      <c r="D82" s="149"/>
+      <c r="E82" s="149"/>
+      <c r="F82" s="150"/>
+      <c r="G82" s="150"/>
+      <c r="H82" s="150"/>
+      <c r="I82" s="119"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" s="17" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B83" s="13" t="s">
+      <c r="B84" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F83" s="13" t="s">
+      <c r="F84" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G83" s="124" t="s">
+      <c r="G84" s="124" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="17"/>
-      <c r="B84" s="145" t="s">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="17"/>
+      <c r="B85" s="147" t="s">
         <v>96</v>
       </c>
-      <c r="C84" s="145"/>
-      <c r="D84" s="145"/>
-      <c r="E84" s="145"/>
-      <c r="F84" s="146"/>
-      <c r="G84" s="146"/>
-      <c r="H84" s="146"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="17" t="s">
+      <c r="C85" s="147"/>
+      <c r="D85" s="147"/>
+      <c r="E85" s="147"/>
+      <c r="F85" s="148"/>
+      <c r="G85" s="148"/>
+      <c r="H85" s="148"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>61</v>
       </c>
-      <c r="B86" s="49" t="s">
+      <c r="B87" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="D86" s="136" t="s">
+      <c r="D87" s="136" t="s">
         <v>334</v>
       </c>
-      <c r="F86" s="49" t="s">
+      <c r="F87" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="H86" s="15" t="s">
+      <c r="H87" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="I86" s="53" t="s">
+      <c r="I87" s="53" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="87" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="17"/>
-      <c r="B87" s="148" t="s">
+    <row r="88" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="17"/>
+      <c r="B88" s="149" t="s">
         <v>133</v>
       </c>
-      <c r="C87" s="148"/>
-      <c r="D87" s="148"/>
-      <c r="E87" s="148"/>
-      <c r="F87" s="147"/>
-      <c r="G87" s="147"/>
-      <c r="H87" s="147"/>
-      <c r="I87" s="52"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="C88" s="149"/>
+      <c r="D88" s="149"/>
+      <c r="E88" s="149"/>
+      <c r="F88" s="150"/>
+      <c r="G88" s="150"/>
+      <c r="H88" s="150"/>
+      <c r="I88" s="52"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>126</v>
       </c>
-      <c r="B88" s="13" t="s">
+      <c r="B89" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F88" s="13" t="s">
+      <c r="F89" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="H88" s="13" t="s">
+      <c r="H89" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" s="17"/>
-      <c r="B89" s="145" t="s">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="17"/>
+      <c r="B90" s="147" t="s">
         <v>101</v>
       </c>
-      <c r="C89" s="145"/>
-      <c r="D89" s="145"/>
-      <c r="E89" s="145"/>
-      <c r="F89" s="146"/>
-      <c r="G89" s="146"/>
-      <c r="H89" s="146"/>
-    </row>
-    <row r="90" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="17" t="s">
+      <c r="C90" s="147"/>
+      <c r="D90" s="147"/>
+      <c r="E90" s="147"/>
+      <c r="F90" s="148"/>
+      <c r="G90" s="148"/>
+      <c r="H90" s="148"/>
+    </row>
+    <row r="91" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B90" s="44" t="s">
+      <c r="B91" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="C90" s="83"/>
-      <c r="D90" s="135"/>
-      <c r="E90" s="61"/>
-      <c r="F90" s="44" t="s">
+      <c r="C91" s="83"/>
+      <c r="D91" s="135"/>
+      <c r="E91" s="61"/>
+      <c r="F91" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="G90" s="44" t="s">
+      <c r="G91" s="44" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="91" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="145" t="s">
+    <row r="92" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B92" s="147" t="s">
         <v>129</v>
       </c>
-      <c r="C91" s="145"/>
-      <c r="D91" s="145"/>
-      <c r="E91" s="145"/>
-      <c r="F91" s="146"/>
-      <c r="G91" s="146"/>
-      <c r="H91" s="146"/>
-      <c r="I91" s="146"/>
-    </row>
-    <row r="92" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="81" t="s">
+      <c r="C92" s="147"/>
+      <c r="D92" s="147"/>
+      <c r="E92" s="147"/>
+      <c r="F92" s="148"/>
+      <c r="G92" s="148"/>
+      <c r="H92" s="148"/>
+      <c r="I92" s="148"/>
+    </row>
+    <row r="93" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="81" t="s">
         <v>231</v>
       </c>
-      <c r="B92" s="74"/>
-      <c r="C92" s="82"/>
-      <c r="D92" s="134"/>
-      <c r="E92" s="74"/>
-      <c r="F92" s="75" t="s">
+      <c r="B93" s="74"/>
+      <c r="C93" s="82"/>
+      <c r="D93" s="134"/>
+      <c r="E93" s="74"/>
+      <c r="F93" s="75" t="s">
         <v>232</v>
       </c>
-      <c r="H92" s="8" t="s">
+      <c r="H93" s="8" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" s="17" t="s">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="94" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+    <row r="95" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>64</v>
       </c>
-      <c r="B94" s="62" t="s">
+      <c r="B95" s="62" t="s">
         <v>160</v>
       </c>
-      <c r="C94" s="62"/>
-      <c r="D94" s="62"/>
-      <c r="E94" s="62" t="s">
+      <c r="C95" s="62"/>
+      <c r="D95" s="62"/>
+      <c r="E95" s="62" t="s">
         <v>162</v>
       </c>
-      <c r="F94" s="61" t="s">
+      <c r="F95" s="61" t="s">
         <v>148</v>
       </c>
-      <c r="H94" s="61" t="s">
+      <c r="H95" s="61" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="95" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="17"/>
-      <c r="B95" s="149" t="s">
+    <row r="96" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="17"/>
+      <c r="B96" s="151" t="s">
         <v>161</v>
       </c>
-      <c r="C95" s="149"/>
-      <c r="D95" s="149"/>
-      <c r="E95" s="149"/>
-      <c r="F95" s="147"/>
-      <c r="G95" s="147"/>
-      <c r="H95" s="147"/>
-      <c r="I95" s="147"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>159</v>
-      </c>
-      <c r="B96" s="62" t="s">
-        <v>155</v>
-      </c>
-      <c r="C96" s="62"/>
-      <c r="D96" s="137" t="s">
-        <v>334</v>
-      </c>
-      <c r="E96" s="62"/>
-      <c r="F96" s="56" t="s">
-        <v>148</v>
-      </c>
-      <c r="H96" s="13" t="s">
-        <v>149</v>
-      </c>
+      <c r="C96" s="151"/>
+      <c r="D96" s="151"/>
+      <c r="E96" s="151"/>
+      <c r="F96" s="150"/>
+      <c r="G96" s="150"/>
+      <c r="H96" s="150"/>
+      <c r="I96" s="150"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>65</v>
+        <v>159</v>
+      </c>
+      <c r="B97" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C97" s="62"/>
+      <c r="D97" s="137" t="s">
+        <v>334</v>
+      </c>
+      <c r="E97" s="62"/>
+      <c r="F97" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="H97" s="13" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A101" s="17" t="s">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" s="17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="17" t="s">
+    <row r="103" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="B102" s="75" t="s">
+      <c r="B103" s="75" t="s">
         <v>299</v>
-      </c>
-      <c r="C102" s="83"/>
-      <c r="D102" s="135"/>
-      <c r="F102" s="75" t="s">
-        <v>232</v>
-      </c>
-      <c r="H102" s="75" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" s="64" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>164</v>
-      </c>
-      <c r="B103" s="64" t="s">
-        <v>152</v>
       </c>
       <c r="C103" s="83"/>
       <c r="D103" s="135"/>
-      <c r="F103" s="64" t="s">
+      <c r="F103" s="75" t="s">
+        <v>232</v>
+      </c>
+      <c r="H103" s="75" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>164</v>
+      </c>
+      <c r="B104" s="64" t="s">
+        <v>152</v>
+      </c>
+      <c r="C104" s="83"/>
+      <c r="D104" s="135"/>
+      <c r="F104" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="H103" s="64" t="s">
+      <c r="H104" s="64" t="s">
         <v>158</v>
       </c>
-      <c r="I103" s="63"/>
-    </row>
-    <row r="104" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="I104" s="63"/>
+    </row>
+    <row r="105" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>163</v>
       </c>
-      <c r="B104" s="58" t="s">
+      <c r="B105" s="58" t="s">
         <v>237</v>
       </c>
-      <c r="C104" s="83" t="s">
+      <c r="C105" s="83" t="s">
         <v>157</v>
       </c>
-      <c r="D104" s="135"/>
-      <c r="E104" s="61"/>
-      <c r="F104" s="58" t="s">
+      <c r="D105" s="135"/>
+      <c r="E105" s="61"/>
+      <c r="F105" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="G104" s="58" t="s">
+      <c r="G105" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="I104" s="57"/>
-    </row>
-    <row r="105" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="17"/>
-      <c r="B105" s="145" t="s">
+      <c r="I105" s="57"/>
+    </row>
+    <row r="106" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="17"/>
+      <c r="B106" s="147" t="s">
         <v>136</v>
       </c>
-      <c r="C105" s="145"/>
-      <c r="D105" s="145"/>
-      <c r="E105" s="145"/>
-      <c r="F105" s="146"/>
-      <c r="G105" s="146"/>
-      <c r="H105" s="146"/>
-      <c r="I105" s="146"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>70</v>
-      </c>
-      <c r="B106" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C106" s="83" t="s">
-        <v>213</v>
-      </c>
-      <c r="F106" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="G106" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="I106" s="40"/>
-    </row>
-    <row r="107" spans="1:9" s="98" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C106" s="147"/>
+      <c r="D106" s="147"/>
+      <c r="E106" s="147"/>
+      <c r="F106" s="148"/>
+      <c r="G106" s="148"/>
+      <c r="H106" s="148"/>
+      <c r="I106" s="148"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>70</v>
       </c>
-      <c r="B107" s="98" t="s">
+      <c r="B107" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C107" s="83" t="s">
+        <v>213</v>
+      </c>
+      <c r="F107" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G107" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="I107" s="40"/>
+    </row>
+    <row r="108" spans="1:9" s="98" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>70</v>
+      </c>
+      <c r="B108" s="98" t="s">
         <v>216</v>
       </c>
-      <c r="C107" s="98" t="s">
+      <c r="C108" s="98" t="s">
         <v>234</v>
       </c>
-      <c r="D107" s="135"/>
-      <c r="F107" s="109" t="s">
+      <c r="D108" s="135"/>
+      <c r="F108" s="109" t="s">
         <v>165</v>
       </c>
-      <c r="G107" s="98" t="s">
+      <c r="G108" s="98" t="s">
         <v>166</v>
       </c>
-      <c r="I107" s="97"/>
-    </row>
-    <row r="108" spans="1:9" s="98" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="17"/>
-      <c r="B108" s="145" t="s">
+      <c r="I108" s="97"/>
+    </row>
+    <row r="109" spans="1:9" s="98" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="17"/>
+      <c r="B109" s="147" t="s">
         <v>276</v>
       </c>
-      <c r="C108" s="145"/>
-      <c r="D108" s="145"/>
-      <c r="E108" s="145"/>
-      <c r="F108" s="145"/>
-      <c r="G108" s="145"/>
-      <c r="H108" s="145"/>
-      <c r="I108" s="97"/>
-    </row>
-    <row r="109" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+      <c r="C109" s="147"/>
+      <c r="D109" s="147"/>
+      <c r="E109" s="147"/>
+      <c r="F109" s="147"/>
+      <c r="G109" s="147"/>
+      <c r="H109" s="147"/>
+      <c r="I109" s="97"/>
+    </row>
+    <row r="110" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>71</v>
       </c>
-      <c r="B109" s="66" t="s">
+      <c r="B110" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C109" s="83" t="s">
+      <c r="C110" s="83" t="s">
         <v>213</v>
       </c>
-      <c r="D109" s="135"/>
-      <c r="F109" s="66" t="s">
+      <c r="D110" s="135"/>
+      <c r="F110" s="66" t="s">
         <v>188</v>
       </c>
-      <c r="G109" s="66" t="s">
+      <c r="G110" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="I109" s="65"/>
-    </row>
-    <row r="110" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="17"/>
-      <c r="B110" s="145" t="s">
+      <c r="I110" s="65"/>
+    </row>
+    <row r="111" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="17"/>
+      <c r="B111" s="147" t="s">
         <v>244</v>
       </c>
-      <c r="C110" s="145"/>
-      <c r="D110" s="145"/>
-      <c r="E110" s="145"/>
-      <c r="F110" s="145"/>
-      <c r="G110" s="145"/>
-      <c r="H110" s="145"/>
-      <c r="I110" s="65"/>
-    </row>
-    <row r="111" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="C111" s="147"/>
+      <c r="D111" s="147"/>
+      <c r="E111" s="147"/>
+      <c r="F111" s="147"/>
+      <c r="G111" s="147"/>
+      <c r="H111" s="147"/>
+      <c r="I111" s="65"/>
+    </row>
+    <row r="112" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>197</v>
       </c>
-      <c r="B111" s="66" t="s">
+      <c r="B112" s="66" t="s">
         <v>194</v>
       </c>
-      <c r="C111" s="83"/>
-      <c r="D111" s="136" t="s">
+      <c r="C112" s="83"/>
+      <c r="D112" s="136" t="s">
         <v>334</v>
       </c>
-      <c r="F111" s="66" t="s">
+      <c r="F112" s="66" t="s">
         <v>191</v>
       </c>
-      <c r="G111" s="83" t="s">
+      <c r="G112" s="83" t="s">
         <v>166</v>
       </c>
-      <c r="H111" s="66" t="s">
+      <c r="H112" s="66" t="s">
         <v>193</v>
       </c>
-      <c r="I111" s="65"/>
-    </row>
-    <row r="112" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="17"/>
-      <c r="B112" s="145" t="s">
+      <c r="I112" s="65"/>
+    </row>
+    <row r="113" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="17"/>
+      <c r="B113" s="147" t="s">
         <v>195</v>
       </c>
-      <c r="C112" s="145"/>
-      <c r="D112" s="145"/>
-      <c r="E112" s="145"/>
-      <c r="F112" s="145"/>
-      <c r="G112" s="145"/>
-      <c r="H112" s="145"/>
-      <c r="I112" s="65"/>
-    </row>
-    <row r="113" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="C113" s="147"/>
+      <c r="D113" s="147"/>
+      <c r="E113" s="147"/>
+      <c r="F113" s="147"/>
+      <c r="G113" s="147"/>
+      <c r="H113" s="147"/>
+      <c r="I113" s="65"/>
+    </row>
+    <row r="114" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>241</v>
       </c>
-      <c r="B113" s="58" t="s">
+      <c r="B114" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="C113" s="83" t="s">
+      <c r="C114" s="83" t="s">
         <v>213</v>
       </c>
-      <c r="D113" s="135"/>
-      <c r="E113" s="61"/>
-      <c r="F113" s="58" t="s">
+      <c r="D114" s="135"/>
+      <c r="E114" s="61"/>
+      <c r="F114" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="G113" s="58" t="s">
+      <c r="G114" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="I113" s="57"/>
-      <c r="J113" s="13"/>
-      <c r="K113" s="13"/>
-      <c r="L113" s="13"/>
-      <c r="M113" s="13"/>
-      <c r="N113" s="13"/>
-      <c r="O113" s="13"/>
-      <c r="P113" s="13"/>
-      <c r="Q113" s="13"/>
-      <c r="R113" s="13"/>
-      <c r="S113" s="13"/>
-    </row>
-    <row r="114" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="17"/>
-      <c r="B114" s="145" t="s">
+      <c r="I114" s="57"/>
+      <c r="J114" s="13"/>
+      <c r="K114" s="13"/>
+      <c r="L114" s="13"/>
+      <c r="M114" s="13"/>
+      <c r="N114" s="13"/>
+      <c r="O114" s="13"/>
+      <c r="P114" s="13"/>
+      <c r="Q114" s="13"/>
+      <c r="R114" s="13"/>
+      <c r="S114" s="13"/>
+    </row>
+    <row r="115" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="17"/>
+      <c r="B115" s="147" t="s">
         <v>208</v>
       </c>
-      <c r="C114" s="145"/>
-      <c r="D114" s="145"/>
-      <c r="E114" s="146"/>
-      <c r="F114" s="146"/>
-      <c r="G114" s="146"/>
-      <c r="H114" s="146"/>
-      <c r="I114" s="65"/>
-    </row>
-    <row r="115" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="C115" s="147"/>
+      <c r="D115" s="147"/>
+      <c r="E115" s="148"/>
+      <c r="F115" s="148"/>
+      <c r="G115" s="148"/>
+      <c r="H115" s="148"/>
+      <c r="I115" s="65"/>
+    </row>
+    <row r="116" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>187</v>
       </c>
-      <c r="B115" s="66" t="s">
+      <c r="B116" s="66" t="s">
         <v>285</v>
-      </c>
-      <c r="C115" s="83"/>
-      <c r="D115" s="135"/>
-      <c r="F115" s="66" t="s">
-        <v>85</v>
-      </c>
-      <c r="G115" s="66" t="s">
-        <v>166</v>
-      </c>
-      <c r="I115" s="65"/>
-    </row>
-    <row r="116" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="80" t="s">
-        <v>219</v>
-      </c>
-      <c r="B116" s="75" t="s">
-        <v>152</v>
       </c>
       <c r="C116" s="83"/>
       <c r="D116" s="135"/>
-      <c r="F116" s="75" t="s">
+      <c r="F116" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="G116" s="66" t="s">
+        <v>166</v>
+      </c>
+      <c r="I116" s="65"/>
+    </row>
+    <row r="117" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="80" t="s">
+        <v>219</v>
+      </c>
+      <c r="B117" s="75" t="s">
+        <v>152</v>
+      </c>
+      <c r="C117" s="83"/>
+      <c r="D117" s="135"/>
+      <c r="F117" s="75" t="s">
         <v>221</v>
       </c>
-      <c r="H116" s="75" t="s">
+      <c r="H117" s="75" t="s">
         <v>220</v>
       </c>
-      <c r="I116" s="74"/>
-    </row>
-    <row r="117" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="16"/>
-      <c r="B117" s="134" t="s">
+      <c r="I117" s="74"/>
+    </row>
+    <row r="118" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="16"/>
+      <c r="B118" s="134" t="s">
         <v>339</v>
       </c>
-      <c r="C117" s="82"/>
-      <c r="D117" s="134"/>
-      <c r="E117" s="74"/>
-    </row>
-    <row r="118" spans="1:19" s="75" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A118" s="79" t="s">
+      <c r="C118" s="82"/>
+      <c r="D118" s="134"/>
+      <c r="E118" s="74"/>
+    </row>
+    <row r="119" spans="1:19" s="75" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A119" s="79" t="s">
         <v>225</v>
       </c>
-      <c r="B118" s="75" t="s">
+      <c r="B119" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="C118" s="83"/>
-      <c r="D118" s="135"/>
-      <c r="F118" s="75" t="s">
+      <c r="C119" s="83"/>
+      <c r="D119" s="135"/>
+      <c r="F119" s="75" t="s">
         <v>223</v>
       </c>
-      <c r="H118" s="75" t="s">
+      <c r="H119" s="75" t="s">
         <v>220</v>
       </c>
-      <c r="I118" s="74"/>
-    </row>
-    <row r="119" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="16"/>
-      <c r="B119" s="134" t="s">
+      <c r="I119" s="74"/>
+    </row>
+    <row r="120" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="16"/>
+      <c r="B120" s="134" t="s">
         <v>339</v>
       </c>
-      <c r="C119" s="82"/>
-      <c r="D119" s="134"/>
-      <c r="E119" s="74"/>
-    </row>
-    <row r="120" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="80" t="s">
+      <c r="C120" s="82"/>
+      <c r="D120" s="134"/>
+      <c r="E120" s="74"/>
+    </row>
+    <row r="121" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="80" t="s">
         <v>227</v>
       </c>
-      <c r="B120" s="75" t="s">
+      <c r="B121" s="75" t="s">
         <v>216</v>
       </c>
-      <c r="C120" s="83"/>
-      <c r="D120" s="135"/>
-      <c r="F120" s="75" t="s">
+      <c r="C121" s="83"/>
+      <c r="D121" s="135"/>
+      <c r="F121" s="75" t="s">
         <v>221</v>
       </c>
-      <c r="H120" s="75" t="s">
+      <c r="H121" s="75" t="s">
         <v>220</v>
       </c>
-      <c r="I120" s="74"/>
-    </row>
-    <row r="121" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="16"/>
-      <c r="B121" s="145" t="s">
+      <c r="I121" s="74"/>
+    </row>
+    <row r="122" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="16"/>
+      <c r="B122" s="147" t="s">
         <v>226</v>
       </c>
-      <c r="C121" s="145"/>
-      <c r="D121" s="145"/>
-      <c r="E121" s="145"/>
-      <c r="F121" s="146"/>
-      <c r="G121" s="146"/>
-      <c r="H121" s="146"/>
-      <c r="I121" s="146"/>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+      <c r="C122" s="147"/>
+      <c r="D122" s="147"/>
+      <c r="E122" s="147"/>
+      <c r="F122" s="148"/>
+      <c r="G122" s="148"/>
+      <c r="H122" s="148"/>
+      <c r="I122" s="148"/>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
         <v>72</v>
-      </c>
-      <c r="B122" s="120" t="s">
-        <v>152</v>
-      </c>
-      <c r="F122" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="G122" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="I122" s="20"/>
-    </row>
-    <row r="123" spans="1:19" s="120" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="80" t="s">
-        <v>314</v>
       </c>
       <c r="B123" s="120" t="s">
         <v>152</v>
       </c>
-      <c r="D123" s="135"/>
-      <c r="F123" s="120" t="s">
+      <c r="F123" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G123" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="I123" s="20"/>
+    </row>
+    <row r="124" spans="1:19" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="80" t="s">
+        <v>314</v>
+      </c>
+      <c r="B124" s="120" t="s">
+        <v>152</v>
+      </c>
+      <c r="D124" s="135"/>
+      <c r="F124" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="G123" s="125" t="s">
+      <c r="G124" s="125" t="s">
         <v>304</v>
       </c>
-      <c r="H123" s="120" t="s">
+      <c r="H124" s="120" t="s">
         <v>313</v>
       </c>
-      <c r="I123" s="119"/>
+      <c r="I124" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B115:H115"/>
+    <mergeCell ref="B113:H113"/>
+    <mergeCell ref="B111:H111"/>
+    <mergeCell ref="B79:H79"/>
+    <mergeCell ref="B90:H90"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="B109:H109"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B88:H88"/>
+    <mergeCell ref="B106:I106"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B96:I96"/>
+    <mergeCell ref="B51:H51"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B73:H73"/>
+    <mergeCell ref="B75:H75"/>
+    <mergeCell ref="B57:H57"/>
     <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B121:I121"/>
-    <mergeCell ref="B91:I91"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B70:H70"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B81:H81"/>
-    <mergeCell ref="B76:H76"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B87:H87"/>
-    <mergeCell ref="B105:I105"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B95:I95"/>
-    <mergeCell ref="B50:H50"/>
-    <mergeCell ref="B60:H60"/>
-    <mergeCell ref="B72:H72"/>
-    <mergeCell ref="B74:H74"/>
-    <mergeCell ref="B56:H56"/>
-    <mergeCell ref="B114:H114"/>
-    <mergeCell ref="B112:H112"/>
-    <mergeCell ref="B110:H110"/>
-    <mergeCell ref="B78:H78"/>
-    <mergeCell ref="B89:H89"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B108:H108"/>
+    <mergeCell ref="B122:I122"/>
+    <mergeCell ref="B92:I92"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B71:H71"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B82:H82"/>
+    <mergeCell ref="B77:H77"/>
+    <mergeCell ref="B53:I53"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A118" r:id="rId1" display="ZEL"/>
-    <hyperlink ref="A116" r:id="rId2" display="ZEL-CBL"/>
-    <hyperlink ref="A120" r:id="rId3" display="ZEL-CBL"/>
-    <hyperlink ref="H13" r:id="rId4"/>
-    <hyperlink ref="A92" r:id="rId5"/>
-    <hyperlink ref="H92" r:id="rId6"/>
+    <hyperlink ref="A119" r:id="rId1" display="ZEL"/>
+    <hyperlink ref="A117" r:id="rId2" display="ZEL-CBL"/>
+    <hyperlink ref="A121" r:id="rId3" display="ZEL-CBL"/>
+    <hyperlink ref="H14" r:id="rId4"/>
+    <hyperlink ref="A93" r:id="rId5"/>
+    <hyperlink ref="H93" r:id="rId6"/>
     <hyperlink ref="B1" r:id="rId7"/>
-    <hyperlink ref="F23" r:id="rId8" location="/"/>
-    <hyperlink ref="A51" r:id="rId9"/>
-    <hyperlink ref="A123" r:id="rId10" display="ZEN"/>
-    <hyperlink ref="A80" r:id="rId11"/>
-    <hyperlink ref="F80" r:id="rId12"/>
-    <hyperlink ref="F68" r:id="rId13"/>
+    <hyperlink ref="F24" r:id="rId8" location="/"/>
+    <hyperlink ref="A52" r:id="rId9"/>
+    <hyperlink ref="A124" r:id="rId10" display="ZEN"/>
+    <hyperlink ref="A81" r:id="rId11"/>
+    <hyperlink ref="F81" r:id="rId12"/>
+    <hyperlink ref="F69" r:id="rId13"/>
+    <hyperlink ref="A10" r:id="rId14"/>
+    <hyperlink ref="H10" r:id="rId15" display="Desktop Wallet"/>
+    <hyperlink ref="F10" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4281,7 +4322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4328,7 +4369,7 @@
         <v>324</v>
       </c>
       <c r="B2" s="127"/>
-      <c r="C2" s="156"/>
+      <c r="C2" s="146"/>
       <c r="D2" s="129"/>
       <c r="E2" s="129"/>
       <c r="F2" s="130"/>
@@ -4466,7 +4507,7 @@
         <v>323</v>
       </c>
       <c r="B13" s="127"/>
-      <c r="C13" s="156"/>
+      <c r="C13" s="146"/>
       <c r="D13" s="129"/>
       <c r="E13" s="129"/>
       <c r="F13" s="130"/>
@@ -4567,7 +4608,7 @@
         <v>322</v>
       </c>
       <c r="B19" s="127"/>
-      <c r="C19" s="156"/>
+      <c r="C19" s="146"/>
       <c r="D19" s="129"/>
       <c r="E19" s="129"/>
       <c r="F19" s="130"/>
@@ -5143,10 +5184,10 @@
     </row>
     <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
-      <c r="B6" s="151" t="s">
+      <c r="B6" s="153" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="151"/>
+      <c r="C6" s="153"/>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
@@ -5164,10 +5205,10 @@
     </row>
     <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="152" t="s">
+      <c r="B9" s="154" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="153"/>
+      <c r="C9" s="155"/>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -5217,10 +5258,10 @@
     </row>
     <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
-      <c r="B16" s="154" t="s">
+      <c r="B16" s="156" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="155"/>
+      <c r="C16" s="157"/>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">

</xml_diff>

<commit_message>
Adding avermore and sgminer-gm-x16r miners
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="365">
   <si>
     <t>Miners (AMD)</t>
   </si>
@@ -1119,6 +1119,18 @@
   </si>
   <si>
     <t>﻿1Cmt7oj41SzYdmk2q5AuMYFGoUG3P56Np</t>
+  </si>
+  <si>
+    <t>GPU_MAX_ALLOC_PERCENT=100 GPU_USE_SYNC_OBJECTS=1</t>
+  </si>
+  <si>
+    <t>-k $ALGO -o $URL_PORT -u $USER.$WORKER_NAME -p $PASSWORD -w 64 -X 256</t>
+  </si>
+  <si>
+    <t>RVN-amd</t>
+  </si>
+  <si>
+    <t>/opt/avermore-miner/sgminer</t>
   </si>
 </sst>
 </file>
@@ -1430,7 +1442,7 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1832,10 +1844,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1857,7 +1876,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2576,11 +2594,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S124"/>
+  <dimension ref="A1:S126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2663,15 +2681,15 @@
     </row>
     <row r="7" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
-      <c r="B7" s="147" t="s">
+      <c r="B7" s="150" t="s">
         <v>247</v>
       </c>
-      <c r="C7" s="147"/>
-      <c r="D7" s="147"/>
-      <c r="E7" s="148"/>
-      <c r="F7" s="148"/>
-      <c r="G7" s="148"/>
-      <c r="H7" s="148"/>
+      <c r="C7" s="150"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="151"/>
+      <c r="F7" s="151"/>
+      <c r="G7" s="151"/>
+      <c r="H7" s="151"/>
     </row>
     <row r="8" spans="1:9" s="118" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
@@ -2690,18 +2708,18 @@
     </row>
     <row r="9" spans="1:9" s="118" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
-      <c r="B9" s="147" t="s">
+      <c r="B9" s="150" t="s">
         <v>224</v>
       </c>
-      <c r="C9" s="147"/>
-      <c r="D9" s="147"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="148"/>
-      <c r="H9" s="148"/>
+      <c r="C9" s="150"/>
+      <c r="D9" s="150"/>
+      <c r="E9" s="151"/>
+      <c r="F9" s="151"/>
+      <c r="G9" s="151"/>
+      <c r="H9" s="151"/>
     </row>
     <row r="10" spans="1:9" s="145" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="158" t="s">
+      <c r="A10" s="149" t="s">
         <v>357</v>
       </c>
       <c r="B10" t="s">
@@ -2741,16 +2759,16 @@
     </row>
     <row r="12" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
-      <c r="B12" s="147" t="s">
+      <c r="B12" s="150" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="147"/>
-      <c r="D12" s="147"/>
-      <c r="E12" s="147"/>
-      <c r="F12" s="148"/>
-      <c r="G12" s="148"/>
-      <c r="H12" s="148"/>
-      <c r="I12" s="148"/>
+      <c r="C12" s="150"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="150"/>
+      <c r="F12" s="151"/>
+      <c r="G12" s="151"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="151"/>
     </row>
     <row r="13" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
@@ -2840,16 +2858,16 @@
     </row>
     <row r="21" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
-      <c r="B21" s="149" t="s">
+      <c r="B21" s="153" t="s">
         <v>308</v>
       </c>
-      <c r="C21" s="149"/>
-      <c r="D21" s="149"/>
-      <c r="E21" s="149"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="148"/>
-      <c r="H21" s="148"/>
-      <c r="I21" s="148"/>
+      <c r="C21" s="153"/>
+      <c r="D21" s="153"/>
+      <c r="E21" s="153"/>
+      <c r="F21" s="151"/>
+      <c r="G21" s="151"/>
+      <c r="H21" s="151"/>
+      <c r="I21" s="151"/>
     </row>
     <row r="22" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="76" t="s">
@@ -2873,16 +2891,16 @@
     </row>
     <row r="23" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
-      <c r="B23" s="149" t="s">
+      <c r="B23" s="153" t="s">
         <v>245</v>
       </c>
-      <c r="C23" s="149"/>
-      <c r="D23" s="149"/>
-      <c r="E23" s="149"/>
-      <c r="F23" s="148"/>
-      <c r="G23" s="148"/>
-      <c r="H23" s="148"/>
-      <c r="I23" s="148"/>
+      <c r="C23" s="153"/>
+      <c r="D23" s="153"/>
+      <c r="E23" s="153"/>
+      <c r="F23" s="151"/>
+      <c r="G23" s="151"/>
+      <c r="H23" s="151"/>
+      <c r="I23" s="151"/>
     </row>
     <row r="24" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="76" t="s">
@@ -2908,16 +2926,16 @@
     </row>
     <row r="25" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
-      <c r="B25" s="149" t="s">
+      <c r="B25" s="153" t="s">
         <v>281</v>
       </c>
-      <c r="C25" s="149"/>
-      <c r="D25" s="149"/>
-      <c r="E25" s="149"/>
-      <c r="F25" s="148"/>
-      <c r="G25" s="148"/>
-      <c r="H25" s="148"/>
-      <c r="I25" s="148"/>
+      <c r="C25" s="153"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="153"/>
+      <c r="F25" s="151"/>
+      <c r="G25" s="151"/>
+      <c r="H25" s="151"/>
+      <c r="I25" s="151"/>
     </row>
     <row r="26" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
@@ -2940,15 +2958,15 @@
     </row>
     <row r="27" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
-      <c r="B27" s="147" t="s">
+      <c r="B27" s="150" t="s">
         <v>283</v>
       </c>
-      <c r="C27" s="147"/>
-      <c r="D27" s="147"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="148"/>
-      <c r="G27" s="148"/>
-      <c r="H27" s="148"/>
+      <c r="C27" s="150"/>
+      <c r="D27" s="150"/>
+      <c r="E27" s="150"/>
+      <c r="F27" s="151"/>
+      <c r="G27" s="151"/>
+      <c r="H27" s="151"/>
       <c r="I27" s="112"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -2969,16 +2987,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
-      <c r="B29" s="149" t="s">
+      <c r="B29" s="153" t="s">
         <v>189</v>
       </c>
-      <c r="C29" s="149"/>
-      <c r="D29" s="149"/>
-      <c r="E29" s="149"/>
-      <c r="F29" s="148"/>
-      <c r="G29" s="148"/>
-      <c r="H29" s="148"/>
-      <c r="I29" s="148"/>
+      <c r="C29" s="153"/>
+      <c r="D29" s="153"/>
+      <c r="E29" s="153"/>
+      <c r="F29" s="151"/>
+      <c r="G29" s="151"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
@@ -2993,15 +3011,15 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
-      <c r="B31" s="147" t="s">
+      <c r="B31" s="150" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="147"/>
-      <c r="D31" s="147"/>
-      <c r="E31" s="147"/>
-      <c r="F31" s="148"/>
-      <c r="G31" s="148"/>
-      <c r="H31" s="148"/>
+      <c r="C31" s="150"/>
+      <c r="D31" s="150"/>
+      <c r="E31" s="150"/>
+      <c r="F31" s="151"/>
+      <c r="G31" s="151"/>
+      <c r="H31" s="151"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -3024,15 +3042,15 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
-      <c r="B34" s="147" t="s">
+      <c r="B34" s="150" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="147"/>
-      <c r="D34" s="147"/>
-      <c r="E34" s="147"/>
-      <c r="F34" s="148"/>
-      <c r="G34" s="148"/>
-      <c r="H34" s="148"/>
+      <c r="C34" s="150"/>
+      <c r="D34" s="150"/>
+      <c r="E34" s="150"/>
+      <c r="F34" s="151"/>
+      <c r="G34" s="151"/>
+      <c r="H34" s="151"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
@@ -3080,15 +3098,15 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
-      <c r="B40" s="149" t="s">
+      <c r="B40" s="153" t="s">
         <v>236</v>
       </c>
-      <c r="C40" s="149"/>
-      <c r="D40" s="149"/>
-      <c r="E40" s="149"/>
-      <c r="F40" s="150"/>
-      <c r="G40" s="150"/>
-      <c r="H40" s="150"/>
+      <c r="C40" s="153"/>
+      <c r="D40" s="153"/>
+      <c r="E40" s="153"/>
+      <c r="F40" s="152"/>
+      <c r="G40" s="152"/>
+      <c r="H40" s="152"/>
       <c r="I40" s="20"/>
     </row>
     <row r="41" spans="1:19" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -3114,16 +3132,16 @@
     </row>
     <row r="42" spans="1:19" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
-      <c r="B42" s="149" t="s">
+      <c r="B42" s="153" t="s">
         <v>134</v>
       </c>
-      <c r="C42" s="149"/>
-      <c r="D42" s="149"/>
-      <c r="E42" s="149"/>
-      <c r="F42" s="150"/>
-      <c r="G42" s="150"/>
-      <c r="H42" s="150"/>
-      <c r="I42" s="150"/>
+      <c r="C42" s="153"/>
+      <c r="D42" s="153"/>
+      <c r="E42" s="153"/>
+      <c r="F42" s="152"/>
+      <c r="G42" s="152"/>
+      <c r="H42" s="152"/>
+      <c r="I42" s="152"/>
     </row>
     <row r="43" spans="1:19" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -3148,15 +3166,15 @@
     </row>
     <row r="44" spans="1:19" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
-      <c r="B44" s="147" t="s">
+      <c r="B44" s="150" t="s">
         <v>122</v>
       </c>
-      <c r="C44" s="147"/>
-      <c r="D44" s="147"/>
-      <c r="E44" s="147"/>
-      <c r="F44" s="150"/>
-      <c r="G44" s="150"/>
-      <c r="H44" s="150"/>
+      <c r="C44" s="150"/>
+      <c r="D44" s="150"/>
+      <c r="E44" s="150"/>
+      <c r="F44" s="152"/>
+      <c r="G44" s="152"/>
+      <c r="H44" s="152"/>
       <c r="I44" s="40"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
@@ -3190,15 +3208,15 @@
     </row>
     <row r="48" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
-      <c r="B48" s="147" t="s">
+      <c r="B48" s="150" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="147"/>
-      <c r="D48" s="147"/>
-      <c r="E48" s="147"/>
-      <c r="F48" s="148"/>
-      <c r="G48" s="148"/>
-      <c r="H48" s="148"/>
+      <c r="C48" s="150"/>
+      <c r="D48" s="150"/>
+      <c r="E48" s="150"/>
+      <c r="F48" s="151"/>
+      <c r="G48" s="151"/>
+      <c r="H48" s="151"/>
     </row>
     <row r="49" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -3237,15 +3255,15 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
-      <c r="B51" s="147" t="s">
+      <c r="B51" s="150" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="147"/>
-      <c r="D51" s="147"/>
-      <c r="E51" s="147"/>
-      <c r="F51" s="148"/>
-      <c r="G51" s="148"/>
-      <c r="H51" s="148"/>
+      <c r="C51" s="150"/>
+      <c r="D51" s="150"/>
+      <c r="E51" s="150"/>
+      <c r="F51" s="151"/>
+      <c r="G51" s="151"/>
+      <c r="H51" s="151"/>
     </row>
     <row r="52" spans="1:19" s="144" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A52" s="142" t="s">
@@ -3272,16 +3290,16 @@
     </row>
     <row r="53" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
-      <c r="B53" s="151" t="s">
+      <c r="B53" s="154" t="s">
         <v>338</v>
       </c>
-      <c r="C53" s="151"/>
-      <c r="D53" s="151"/>
-      <c r="E53" s="151"/>
-      <c r="F53" s="150"/>
-      <c r="G53" s="150"/>
-      <c r="H53" s="150"/>
-      <c r="I53" s="150"/>
+      <c r="C53" s="154"/>
+      <c r="D53" s="154"/>
+      <c r="E53" s="154"/>
+      <c r="F53" s="152"/>
+      <c r="G53" s="152"/>
+      <c r="H53" s="152"/>
+      <c r="I53" s="152"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
@@ -3325,15 +3343,15 @@
     </row>
     <row r="57" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
-      <c r="B57" s="152" t="s">
+      <c r="B57" s="155" t="s">
         <v>341</v>
       </c>
-      <c r="C57" s="148"/>
-      <c r="D57" s="148"/>
-      <c r="E57" s="148"/>
-      <c r="F57" s="148"/>
-      <c r="G57" s="148"/>
-      <c r="H57" s="148"/>
+      <c r="C57" s="151"/>
+      <c r="D57" s="151"/>
+      <c r="E57" s="151"/>
+      <c r="F57" s="151"/>
+      <c r="G57" s="151"/>
+      <c r="H57" s="151"/>
     </row>
     <row r="58" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
@@ -3372,15 +3390,15 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" s="17"/>
-      <c r="B61" s="147" t="s">
+      <c r="B61" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C61" s="147"/>
-      <c r="D61" s="147"/>
-      <c r="E61" s="147"/>
-      <c r="F61" s="148"/>
-      <c r="G61" s="148"/>
-      <c r="H61" s="148"/>
+      <c r="C61" s="150"/>
+      <c r="D61" s="150"/>
+      <c r="E61" s="150"/>
+      <c r="F61" s="151"/>
+      <c r="G61" s="151"/>
+      <c r="H61" s="151"/>
       <c r="I61" s="52" t="s">
         <v>103</v>
       </c>
@@ -3506,15 +3524,15 @@
     </row>
     <row r="71" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="17"/>
-      <c r="B71" s="147" t="s">
+      <c r="B71" s="150" t="s">
         <v>252</v>
       </c>
-      <c r="C71" s="147"/>
-      <c r="D71" s="147"/>
-      <c r="E71" s="147"/>
-      <c r="F71" s="148"/>
-      <c r="G71" s="148"/>
-      <c r="H71" s="148"/>
+      <c r="C71" s="150"/>
+      <c r="D71" s="150"/>
+      <c r="E71" s="150"/>
+      <c r="F71" s="151"/>
+      <c r="G71" s="151"/>
+      <c r="H71" s="151"/>
       <c r="I71" s="84"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.2">
@@ -3534,15 +3552,15 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73" s="17"/>
-      <c r="B73" s="147" t="s">
+      <c r="B73" s="150" t="s">
         <v>83</v>
       </c>
-      <c r="C73" s="147"/>
-      <c r="D73" s="147"/>
-      <c r="E73" s="147"/>
-      <c r="F73" s="148"/>
-      <c r="G73" s="148"/>
-      <c r="H73" s="148"/>
+      <c r="C73" s="150"/>
+      <c r="D73" s="150"/>
+      <c r="E73" s="150"/>
+      <c r="F73" s="151"/>
+      <c r="G73" s="151"/>
+      <c r="H73" s="151"/>
       <c r="I73" s="20"/>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.2">
@@ -3562,15 +3580,15 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75" s="17"/>
-      <c r="B75" s="147" t="s">
+      <c r="B75" s="150" t="s">
         <v>289</v>
       </c>
-      <c r="C75" s="147"/>
-      <c r="D75" s="147"/>
-      <c r="E75" s="147"/>
-      <c r="F75" s="148"/>
-      <c r="G75" s="148"/>
-      <c r="H75" s="148"/>
+      <c r="C75" s="150"/>
+      <c r="D75" s="150"/>
+      <c r="E75" s="150"/>
+      <c r="F75" s="151"/>
+      <c r="G75" s="151"/>
+      <c r="H75" s="151"/>
       <c r="I75" s="20" t="s">
         <v>103</v>
       </c>
@@ -3593,15 +3611,15 @@
     </row>
     <row r="77" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="17"/>
-      <c r="B77" s="147" t="s">
+      <c r="B77" s="150" t="s">
         <v>98</v>
       </c>
-      <c r="C77" s="147"/>
-      <c r="D77" s="147"/>
-      <c r="E77" s="147"/>
-      <c r="F77" s="148"/>
-      <c r="G77" s="148"/>
-      <c r="H77" s="148"/>
+      <c r="C77" s="150"/>
+      <c r="D77" s="150"/>
+      <c r="E77" s="150"/>
+      <c r="F77" s="151"/>
+      <c r="G77" s="151"/>
+      <c r="H77" s="151"/>
       <c r="I77" s="116" t="s">
         <v>103</v>
       </c>
@@ -3626,15 +3644,15 @@
     </row>
     <row r="79" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="17"/>
-      <c r="B79" s="147" t="s">
+      <c r="B79" s="150" t="s">
         <v>212</v>
       </c>
-      <c r="C79" s="147"/>
-      <c r="D79" s="147"/>
-      <c r="E79" s="150"/>
-      <c r="F79" s="150"/>
-      <c r="G79" s="150"/>
-      <c r="H79" s="150"/>
+      <c r="C79" s="150"/>
+      <c r="D79" s="150"/>
+      <c r="E79" s="152"/>
+      <c r="F79" s="152"/>
+      <c r="G79" s="152"/>
+      <c r="H79" s="152"/>
       <c r="I79" s="65"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.2">
@@ -3642,534 +3660,550 @@
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:9" s="120" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" s="148" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A81" s="133" t="s">
-        <v>306</v>
+        <v>363</v>
       </c>
       <c r="B81" s="62" t="s">
-        <v>328</v>
-      </c>
-      <c r="D81" s="135" t="s">
+        <v>364</v>
+      </c>
+      <c r="C81" s="148" t="s">
+        <v>157</v>
+      </c>
+      <c r="D81" s="148" t="s">
         <v>336</v>
       </c>
       <c r="F81" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="G81" s="120" t="s">
-        <v>302</v>
+      <c r="G81" s="148" t="s">
+        <v>304</v>
       </c>
       <c r="H81" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="I81" s="120" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I81" s="148" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" s="148" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="17"/>
-      <c r="B82" s="149" t="s">
+      <c r="B82" s="153" t="s">
+        <v>362</v>
+      </c>
+      <c r="C82" s="153"/>
+      <c r="D82" s="153"/>
+      <c r="E82" s="153"/>
+      <c r="F82" s="152"/>
+      <c r="G82" s="152"/>
+      <c r="H82" s="152"/>
+      <c r="I82" s="147"/>
+    </row>
+    <row r="83" spans="1:9" s="120" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A83" s="133" t="s">
+        <v>306</v>
+      </c>
+      <c r="B83" s="62" t="s">
+        <v>328</v>
+      </c>
+      <c r="C83" s="120" t="s">
+        <v>213</v>
+      </c>
+      <c r="D83" s="135" t="s">
+        <v>336</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="G83" s="120" t="s">
+        <v>304</v>
+      </c>
+      <c r="H83" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="I83" s="148" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="17"/>
+      <c r="B84" s="153" t="s">
         <v>337</v>
       </c>
-      <c r="C82" s="149"/>
-      <c r="D82" s="149"/>
-      <c r="E82" s="149"/>
-      <c r="F82" s="150"/>
-      <c r="G82" s="150"/>
-      <c r="H82" s="150"/>
-      <c r="I82" s="119"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="C84" s="153"/>
+      <c r="D84" s="153"/>
+      <c r="E84" s="153"/>
+      <c r="F84" s="152"/>
+      <c r="G84" s="152"/>
+      <c r="H84" s="152"/>
+      <c r="I84" s="119"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B84" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F84" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="G84" s="124" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="17"/>
-      <c r="B85" s="147" t="s">
-        <v>96</v>
-      </c>
-      <c r="C85" s="147"/>
-      <c r="D85" s="147"/>
-      <c r="E85" s="147"/>
-      <c r="F85" s="148"/>
-      <c r="G85" s="148"/>
-      <c r="H85" s="148"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F86" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="G86" s="124" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="17"/>
+      <c r="B87" s="150" t="s">
+        <v>96</v>
+      </c>
+      <c r="C87" s="150"/>
+      <c r="D87" s="150"/>
+      <c r="E87" s="150"/>
+      <c r="F87" s="151"/>
+      <c r="G87" s="151"/>
+      <c r="H87" s="151"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>61</v>
-      </c>
-      <c r="B87" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="D87" s="136" t="s">
-        <v>334</v>
-      </c>
-      <c r="F87" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="H87" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="I87" s="53" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="17"/>
-      <c r="B88" s="149" t="s">
-        <v>133</v>
-      </c>
-      <c r="C88" s="149"/>
-      <c r="D88" s="149"/>
-      <c r="E88" s="149"/>
-      <c r="F88" s="150"/>
-      <c r="G88" s="150"/>
-      <c r="H88" s="150"/>
-      <c r="I88" s="52"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>61</v>
+      </c>
+      <c r="B89" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D89" s="136" t="s">
+        <v>334</v>
+      </c>
+      <c r="F89" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="H89" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="I89" s="53" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="17"/>
+      <c r="B90" s="153" t="s">
+        <v>133</v>
+      </c>
+      <c r="C90" s="153"/>
+      <c r="D90" s="153"/>
+      <c r="E90" s="153"/>
+      <c r="F90" s="152"/>
+      <c r="G90" s="152"/>
+      <c r="H90" s="152"/>
+      <c r="I90" s="52"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>126</v>
       </c>
-      <c r="B89" s="13" t="s">
+      <c r="B91" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F89" s="13" t="s">
+      <c r="F91" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="H89" s="13" t="s">
+      <c r="H91" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" s="17"/>
-      <c r="B90" s="147" t="s">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" s="17"/>
+      <c r="B92" s="150" t="s">
         <v>101</v>
       </c>
-      <c r="C90" s="147"/>
-      <c r="D90" s="147"/>
-      <c r="E90" s="147"/>
-      <c r="F90" s="148"/>
-      <c r="G90" s="148"/>
-      <c r="H90" s="148"/>
-    </row>
-    <row r="91" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="17" t="s">
+      <c r="C92" s="150"/>
+      <c r="D92" s="150"/>
+      <c r="E92" s="150"/>
+      <c r="F92" s="151"/>
+      <c r="G92" s="151"/>
+      <c r="H92" s="151"/>
+    </row>
+    <row r="93" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B91" s="44" t="s">
+      <c r="B93" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="C91" s="83"/>
-      <c r="D91" s="135"/>
-      <c r="E91" s="61"/>
-      <c r="F91" s="44" t="s">
+      <c r="C93" s="83"/>
+      <c r="D93" s="135"/>
+      <c r="E93" s="61"/>
+      <c r="F93" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="G91" s="44" t="s">
+      <c r="G93" s="44" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="92" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="147" t="s">
+    <row r="94" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B94" s="150" t="s">
         <v>129</v>
       </c>
-      <c r="C92" s="147"/>
-      <c r="D92" s="147"/>
-      <c r="E92" s="147"/>
-      <c r="F92" s="148"/>
-      <c r="G92" s="148"/>
-      <c r="H92" s="148"/>
-      <c r="I92" s="148"/>
-    </row>
-    <row r="93" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="81" t="s">
+      <c r="C94" s="150"/>
+      <c r="D94" s="150"/>
+      <c r="E94" s="150"/>
+      <c r="F94" s="151"/>
+      <c r="G94" s="151"/>
+      <c r="H94" s="151"/>
+      <c r="I94" s="151"/>
+    </row>
+    <row r="95" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="81" t="s">
         <v>231</v>
       </c>
-      <c r="B93" s="74"/>
-      <c r="C93" s="82"/>
-      <c r="D93" s="134"/>
-      <c r="E93" s="74"/>
-      <c r="F93" s="75" t="s">
+      <c r="B95" s="74"/>
+      <c r="C95" s="82"/>
+      <c r="D95" s="134"/>
+      <c r="E95" s="74"/>
+      <c r="F95" s="75" t="s">
         <v>232</v>
       </c>
-      <c r="H93" s="8" t="s">
+      <c r="H95" s="8" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" s="17" t="s">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="95" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+    <row r="97" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>64</v>
       </c>
-      <c r="B95" s="62" t="s">
+      <c r="B97" s="62" t="s">
         <v>160</v>
       </c>
-      <c r="C95" s="62"/>
-      <c r="D95" s="62"/>
-      <c r="E95" s="62" t="s">
+      <c r="C97" s="62"/>
+      <c r="D97" s="62"/>
+      <c r="E97" s="62" t="s">
         <v>162</v>
       </c>
-      <c r="F95" s="61" t="s">
+      <c r="F97" s="61" t="s">
         <v>148</v>
       </c>
-      <c r="H95" s="61" t="s">
+      <c r="H97" s="61" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="96" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="17"/>
-      <c r="B96" s="151" t="s">
+    <row r="98" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="17"/>
+      <c r="B98" s="154" t="s">
         <v>161</v>
       </c>
-      <c r="C96" s="151"/>
-      <c r="D96" s="151"/>
-      <c r="E96" s="151"/>
-      <c r="F96" s="150"/>
-      <c r="G96" s="150"/>
-      <c r="H96" s="150"/>
-      <c r="I96" s="150"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>159</v>
-      </c>
-      <c r="B97" s="62" t="s">
-        <v>155</v>
-      </c>
-      <c r="C97" s="62"/>
-      <c r="D97" s="137" t="s">
-        <v>334</v>
-      </c>
-      <c r="E97" s="62"/>
-      <c r="F97" s="56" t="s">
-        <v>148</v>
-      </c>
-      <c r="H97" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>65</v>
-      </c>
+      <c r="C98" s="154"/>
+      <c r="D98" s="154"/>
+      <c r="E98" s="154"/>
+      <c r="F98" s="152"/>
+      <c r="G98" s="152"/>
+      <c r="H98" s="152"/>
+      <c r="I98" s="152"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>66</v>
+        <v>159</v>
+      </c>
+      <c r="B99" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C99" s="62"/>
+      <c r="D99" s="137" t="s">
+        <v>334</v>
+      </c>
+      <c r="E99" s="62"/>
+      <c r="F99" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="H99" s="13" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A102" s="17" t="s">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" s="17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="17" t="s">
+    <row r="105" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="B103" s="75" t="s">
+      <c r="B105" s="75" t="s">
         <v>299</v>
       </c>
-      <c r="C103" s="83"/>
-      <c r="D103" s="135"/>
-      <c r="F103" s="75" t="s">
+      <c r="C105" s="83"/>
+      <c r="D105" s="135"/>
+      <c r="F105" s="75" t="s">
         <v>232</v>
       </c>
-      <c r="H103" s="75" t="s">
+      <c r="H105" s="75" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="104" spans="1:9" s="64" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+    <row r="106" spans="1:9" s="64" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>164</v>
       </c>
-      <c r="B104" s="64" t="s">
+      <c r="B106" s="64" t="s">
         <v>152</v>
       </c>
-      <c r="C104" s="83"/>
-      <c r="D104" s="135"/>
-      <c r="F104" s="64" t="s">
+      <c r="C106" s="83"/>
+      <c r="D106" s="135"/>
+      <c r="F106" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="H104" s="64" t="s">
+      <c r="H106" s="64" t="s">
         <v>158</v>
       </c>
-      <c r="I104" s="63"/>
-    </row>
-    <row r="105" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="I106" s="63"/>
+    </row>
+    <row r="107" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>163</v>
       </c>
-      <c r="B105" s="58" t="s">
+      <c r="B107" s="58" t="s">
         <v>237</v>
       </c>
-      <c r="C105" s="83" t="s">
+      <c r="C107" s="83" t="s">
         <v>157</v>
       </c>
-      <c r="D105" s="135"/>
-      <c r="E105" s="61"/>
-      <c r="F105" s="58" t="s">
+      <c r="D107" s="135"/>
+      <c r="E107" s="61"/>
+      <c r="F107" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="G105" s="58" t="s">
+      <c r="G107" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="I105" s="57"/>
-    </row>
-    <row r="106" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="17"/>
-      <c r="B106" s="147" t="s">
+      <c r="I107" s="57"/>
+    </row>
+    <row r="108" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="17"/>
+      <c r="B108" s="150" t="s">
         <v>136</v>
       </c>
-      <c r="C106" s="147"/>
-      <c r="D106" s="147"/>
-      <c r="E106" s="147"/>
-      <c r="F106" s="148"/>
-      <c r="G106" s="148"/>
-      <c r="H106" s="148"/>
-      <c r="I106" s="148"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="C108" s="150"/>
+      <c r="D108" s="150"/>
+      <c r="E108" s="150"/>
+      <c r="F108" s="151"/>
+      <c r="G108" s="151"/>
+      <c r="H108" s="151"/>
+      <c r="I108" s="151"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>70</v>
       </c>
-      <c r="B107" s="13" t="s">
+      <c r="B109" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="C107" s="83" t="s">
+      <c r="C109" s="83" t="s">
         <v>213</v>
       </c>
-      <c r="F107" s="13" t="s">
+      <c r="F109" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="G107" s="13" t="s">
+      <c r="G109" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="I107" s="40"/>
-    </row>
-    <row r="108" spans="1:9" s="98" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="I109" s="40"/>
+    </row>
+    <row r="110" spans="1:9" s="98" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>70</v>
       </c>
-      <c r="B108" s="98" t="s">
+      <c r="B110" s="98" t="s">
         <v>216</v>
       </c>
-      <c r="C108" s="98" t="s">
+      <c r="C110" s="98" t="s">
         <v>234</v>
       </c>
-      <c r="D108" s="135"/>
-      <c r="F108" s="109" t="s">
+      <c r="D110" s="135"/>
+      <c r="F110" s="109" t="s">
         <v>165</v>
       </c>
-      <c r="G108" s="98" t="s">
+      <c r="G110" s="98" t="s">
         <v>166</v>
       </c>
-      <c r="I108" s="97"/>
-    </row>
-    <row r="109" spans="1:9" s="98" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="17"/>
-      <c r="B109" s="147" t="s">
+      <c r="I110" s="97"/>
+    </row>
+    <row r="111" spans="1:9" s="98" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="17"/>
+      <c r="B111" s="150" t="s">
         <v>276</v>
       </c>
-      <c r="C109" s="147"/>
-      <c r="D109" s="147"/>
-      <c r="E109" s="147"/>
-      <c r="F109" s="147"/>
-      <c r="G109" s="147"/>
-      <c r="H109" s="147"/>
-      <c r="I109" s="97"/>
-    </row>
-    <row r="110" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>71</v>
-      </c>
-      <c r="B110" s="66" t="s">
-        <v>14</v>
-      </c>
-      <c r="C110" s="83" t="s">
-        <v>213</v>
-      </c>
-      <c r="D110" s="135"/>
-      <c r="F110" s="66" t="s">
-        <v>188</v>
-      </c>
-      <c r="G110" s="66" t="s">
-        <v>166</v>
-      </c>
-      <c r="I110" s="65"/>
-    </row>
-    <row r="111" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="17"/>
-      <c r="B111" s="147" t="s">
-        <v>244</v>
-      </c>
-      <c r="C111" s="147"/>
-      <c r="D111" s="147"/>
-      <c r="E111" s="147"/>
-      <c r="F111" s="147"/>
-      <c r="G111" s="147"/>
-      <c r="H111" s="147"/>
-      <c r="I111" s="65"/>
+      <c r="C111" s="150"/>
+      <c r="D111" s="150"/>
+      <c r="E111" s="150"/>
+      <c r="F111" s="150"/>
+      <c r="G111" s="150"/>
+      <c r="H111" s="150"/>
+      <c r="I111" s="97"/>
     </row>
     <row r="112" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>197</v>
+        <v>71</v>
       </c>
       <c r="B112" s="66" t="s">
-        <v>194</v>
-      </c>
-      <c r="C112" s="83"/>
-      <c r="D112" s="136" t="s">
-        <v>334</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C112" s="83" t="s">
+        <v>213</v>
+      </c>
+      <c r="D112" s="135"/>
       <c r="F112" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="G112" s="83" t="s">
+        <v>188</v>
+      </c>
+      <c r="G112" s="66" t="s">
         <v>166</v>
-      </c>
-      <c r="H112" s="66" t="s">
-        <v>193</v>
       </c>
       <c r="I112" s="65"/>
     </row>
     <row r="113" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="17"/>
-      <c r="B113" s="147" t="s">
-        <v>195</v>
-      </c>
-      <c r="C113" s="147"/>
-      <c r="D113" s="147"/>
-      <c r="E113" s="147"/>
-      <c r="F113" s="147"/>
-      <c r="G113" s="147"/>
-      <c r="H113" s="147"/>
+      <c r="B113" s="150" t="s">
+        <v>244</v>
+      </c>
+      <c r="C113" s="150"/>
+      <c r="D113" s="150"/>
+      <c r="E113" s="150"/>
+      <c r="F113" s="150"/>
+      <c r="G113" s="150"/>
+      <c r="H113" s="150"/>
       <c r="I113" s="65"/>
     </row>
-    <row r="114" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>241</v>
-      </c>
-      <c r="B114" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="C114" s="83" t="s">
-        <v>213</v>
-      </c>
-      <c r="D114" s="135"/>
-      <c r="E114" s="61"/>
-      <c r="F114" s="58" t="s">
-        <v>188</v>
-      </c>
-      <c r="G114" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="B114" s="66" t="s">
+        <v>194</v>
+      </c>
+      <c r="C114" s="83"/>
+      <c r="D114" s="136" t="s">
+        <v>334</v>
+      </c>
+      <c r="F114" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="G114" s="83" t="s">
         <v>166</v>
       </c>
-      <c r="I114" s="57"/>
-      <c r="J114" s="13"/>
-      <c r="K114" s="13"/>
-      <c r="L114" s="13"/>
-      <c r="M114" s="13"/>
-      <c r="N114" s="13"/>
-      <c r="O114" s="13"/>
-      <c r="P114" s="13"/>
-      <c r="Q114" s="13"/>
-      <c r="R114" s="13"/>
-      <c r="S114" s="13"/>
+      <c r="H114" s="66" t="s">
+        <v>193</v>
+      </c>
+      <c r="I114" s="65"/>
     </row>
     <row r="115" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="17"/>
-      <c r="B115" s="147" t="s">
+      <c r="B115" s="150" t="s">
+        <v>195</v>
+      </c>
+      <c r="C115" s="150"/>
+      <c r="D115" s="150"/>
+      <c r="E115" s="150"/>
+      <c r="F115" s="150"/>
+      <c r="G115" s="150"/>
+      <c r="H115" s="150"/>
+      <c r="I115" s="65"/>
+    </row>
+    <row r="116" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>241</v>
+      </c>
+      <c r="B116" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="C116" s="83" t="s">
+        <v>213</v>
+      </c>
+      <c r="D116" s="135"/>
+      <c r="E116" s="61"/>
+      <c r="F116" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="G116" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="I116" s="57"/>
+      <c r="J116" s="13"/>
+      <c r="K116" s="13"/>
+      <c r="L116" s="13"/>
+      <c r="M116" s="13"/>
+      <c r="N116" s="13"/>
+      <c r="O116" s="13"/>
+      <c r="P116" s="13"/>
+      <c r="Q116" s="13"/>
+      <c r="R116" s="13"/>
+      <c r="S116" s="13"/>
+    </row>
+    <row r="117" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="17"/>
+      <c r="B117" s="150" t="s">
         <v>208</v>
       </c>
-      <c r="C115" s="147"/>
-      <c r="D115" s="147"/>
-      <c r="E115" s="148"/>
-      <c r="F115" s="148"/>
-      <c r="G115" s="148"/>
-      <c r="H115" s="148"/>
-      <c r="I115" s="65"/>
-    </row>
-    <row r="116" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="C117" s="150"/>
+      <c r="D117" s="150"/>
+      <c r="E117" s="151"/>
+      <c r="F117" s="151"/>
+      <c r="G117" s="151"/>
+      <c r="H117" s="151"/>
+      <c r="I117" s="65"/>
+    </row>
+    <row r="118" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>187</v>
       </c>
-      <c r="B116" s="66" t="s">
+      <c r="B118" s="66" t="s">
         <v>285</v>
       </c>
-      <c r="C116" s="83"/>
-      <c r="D116" s="135"/>
-      <c r="F116" s="66" t="s">
+      <c r="C118" s="83"/>
+      <c r="D118" s="135"/>
+      <c r="F118" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G116" s="66" t="s">
+      <c r="G118" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="I116" s="65"/>
-    </row>
-    <row r="117" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="80" t="s">
+      <c r="I118" s="65"/>
+    </row>
+    <row r="119" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="80" t="s">
         <v>219</v>
-      </c>
-      <c r="B117" s="75" t="s">
-        <v>152</v>
-      </c>
-      <c r="C117" s="83"/>
-      <c r="D117" s="135"/>
-      <c r="F117" s="75" t="s">
-        <v>221</v>
-      </c>
-      <c r="H117" s="75" t="s">
-        <v>220</v>
-      </c>
-      <c r="I117" s="74"/>
-    </row>
-    <row r="118" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="16"/>
-      <c r="B118" s="134" t="s">
-        <v>339</v>
-      </c>
-      <c r="C118" s="82"/>
-      <c r="D118" s="134"/>
-      <c r="E118" s="74"/>
-    </row>
-    <row r="119" spans="1:19" s="75" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A119" s="79" t="s">
-        <v>225</v>
       </c>
       <c r="B119" s="75" t="s">
         <v>152</v>
@@ -4177,7 +4211,7 @@
       <c r="C119" s="83"/>
       <c r="D119" s="135"/>
       <c r="F119" s="75" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H119" s="75" t="s">
         <v>220</v>
@@ -4193,17 +4227,17 @@
       <c r="D120" s="134"/>
       <c r="E120" s="74"/>
     </row>
-    <row r="121" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="80" t="s">
-        <v>227</v>
+    <row r="121" spans="1:19" s="75" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A121" s="79" t="s">
+        <v>225</v>
       </c>
       <c r="B121" s="75" t="s">
-        <v>216</v>
+        <v>152</v>
       </c>
       <c r="C121" s="83"/>
       <c r="D121" s="135"/>
       <c r="F121" s="75" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="H121" s="75" t="s">
         <v>220</v>
@@ -4212,75 +4246,82 @@
     </row>
     <row r="122" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="16"/>
-      <c r="B122" s="147" t="s">
+      <c r="B122" s="134" t="s">
+        <v>339</v>
+      </c>
+      <c r="C122" s="82"/>
+      <c r="D122" s="134"/>
+      <c r="E122" s="74"/>
+    </row>
+    <row r="123" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="80" t="s">
+        <v>227</v>
+      </c>
+      <c r="B123" s="75" t="s">
+        <v>216</v>
+      </c>
+      <c r="C123" s="83"/>
+      <c r="D123" s="135"/>
+      <c r="F123" s="75" t="s">
+        <v>221</v>
+      </c>
+      <c r="H123" s="75" t="s">
+        <v>220</v>
+      </c>
+      <c r="I123" s="74"/>
+    </row>
+    <row r="124" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="16"/>
+      <c r="B124" s="150" t="s">
         <v>226</v>
       </c>
-      <c r="C122" s="147"/>
-      <c r="D122" s="147"/>
-      <c r="E122" s="147"/>
-      <c r="F122" s="148"/>
-      <c r="G122" s="148"/>
-      <c r="H122" s="148"/>
-      <c r="I122" s="148"/>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+      <c r="C124" s="150"/>
+      <c r="D124" s="150"/>
+      <c r="E124" s="150"/>
+      <c r="F124" s="151"/>
+      <c r="G124" s="151"/>
+      <c r="H124" s="151"/>
+      <c r="I124" s="151"/>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
         <v>72</v>
       </c>
-      <c r="B123" s="120" t="s">
+      <c r="B125" s="120" t="s">
         <v>152</v>
       </c>
-      <c r="F123" s="13" t="s">
+      <c r="F125" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G123" s="13" t="s">
+      <c r="G125" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="I123" s="20"/>
-    </row>
-    <row r="124" spans="1:19" s="120" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="80" t="s">
+      <c r="I125" s="20"/>
+    </row>
+    <row r="126" spans="1:19" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="80" t="s">
         <v>314</v>
       </c>
-      <c r="B124" s="120" t="s">
+      <c r="B126" s="120" t="s">
         <v>152</v>
       </c>
-      <c r="D124" s="135"/>
-      <c r="F124" s="120" t="s">
+      <c r="D126" s="135"/>
+      <c r="F126" s="120" t="s">
         <v>312</v>
       </c>
-      <c r="G124" s="125" t="s">
+      <c r="G126" s="125" t="s">
         <v>304</v>
       </c>
-      <c r="H124" s="120" t="s">
+      <c r="H126" s="120" t="s">
         <v>313</v>
       </c>
-      <c r="I124" s="119"/>
+      <c r="I126" s="119"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="B115:H115"/>
-    <mergeCell ref="B113:H113"/>
-    <mergeCell ref="B111:H111"/>
-    <mergeCell ref="B79:H79"/>
-    <mergeCell ref="B90:H90"/>
-    <mergeCell ref="B85:H85"/>
-    <mergeCell ref="B109:H109"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B88:H88"/>
-    <mergeCell ref="B106:I106"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B96:I96"/>
-    <mergeCell ref="B51:H51"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="B73:H73"/>
-    <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B57:H57"/>
+  <mergeCells count="36">
     <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B122:I122"/>
-    <mergeCell ref="B92:I92"/>
+    <mergeCell ref="B124:I124"/>
+    <mergeCell ref="B94:I94"/>
     <mergeCell ref="B42:I42"/>
     <mergeCell ref="B12:I12"/>
     <mergeCell ref="B44:H44"/>
@@ -4291,27 +4332,49 @@
     <mergeCell ref="B21:I21"/>
     <mergeCell ref="B71:H71"/>
     <mergeCell ref="B25:I25"/>
-    <mergeCell ref="B82:H82"/>
+    <mergeCell ref="B84:H84"/>
     <mergeCell ref="B77:H77"/>
     <mergeCell ref="B53:I53"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B90:H90"/>
+    <mergeCell ref="B108:I108"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B98:I98"/>
+    <mergeCell ref="B51:H51"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B73:H73"/>
+    <mergeCell ref="B75:H75"/>
+    <mergeCell ref="B57:H57"/>
+    <mergeCell ref="B82:H82"/>
+    <mergeCell ref="B117:H117"/>
+    <mergeCell ref="B115:H115"/>
+    <mergeCell ref="B113:H113"/>
+    <mergeCell ref="B79:H79"/>
+    <mergeCell ref="B92:H92"/>
+    <mergeCell ref="B87:H87"/>
+    <mergeCell ref="B111:H111"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A119" r:id="rId1" display="ZEL"/>
-    <hyperlink ref="A117" r:id="rId2" display="ZEL-CBL"/>
-    <hyperlink ref="A121" r:id="rId3" display="ZEL-CBL"/>
+    <hyperlink ref="A121" r:id="rId1" display="ZEL"/>
+    <hyperlink ref="A119" r:id="rId2" display="ZEL-CBL"/>
+    <hyperlink ref="A123" r:id="rId3" display="ZEL-CBL"/>
     <hyperlink ref="H14" r:id="rId4"/>
-    <hyperlink ref="A93" r:id="rId5"/>
-    <hyperlink ref="H93" r:id="rId6"/>
+    <hyperlink ref="A95" r:id="rId5"/>
+    <hyperlink ref="H95" r:id="rId6"/>
     <hyperlink ref="B1" r:id="rId7"/>
     <hyperlink ref="F24" r:id="rId8" location="/"/>
     <hyperlink ref="A52" r:id="rId9"/>
-    <hyperlink ref="A124" r:id="rId10" display="ZEN"/>
-    <hyperlink ref="A81" r:id="rId11"/>
-    <hyperlink ref="F81" r:id="rId12"/>
+    <hyperlink ref="A126" r:id="rId10" display="ZEN"/>
+    <hyperlink ref="A83" r:id="rId11"/>
+    <hyperlink ref="F83" r:id="rId12"/>
     <hyperlink ref="F69" r:id="rId13"/>
     <hyperlink ref="A10" r:id="rId14"/>
     <hyperlink ref="H10" r:id="rId15" display="Desktop Wallet"/>
     <hyperlink ref="F10" r:id="rId16"/>
+    <hyperlink ref="F81" r:id="rId17"/>
+    <hyperlink ref="A81" r:id="rId18" display="RVN"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5184,10 +5247,10 @@
     </row>
     <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
-      <c r="B6" s="153" t="s">
+      <c r="B6" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="153"/>
+      <c r="C6" s="156"/>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
@@ -5205,10 +5268,10 @@
     </row>
     <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="154" t="s">
+      <c r="B9" s="157" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="155"/>
+      <c r="C9" s="158"/>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -5258,10 +5321,10 @@
     </row>
     <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
-      <c r="B16" s="156" t="s">
+      <c r="B16" s="159" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="157"/>
+      <c r="C16" s="160"/>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">

</xml_diff>

<commit_message>
Better matching of CoinMiner to PLATFORM; improved 'miners status' performance.
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="25600" windowHeight="13000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="25600" windowHeight="13000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="367">
   <si>
     <t>Miners (AMD)</t>
   </si>
@@ -821,9 +821,6 @@
     <t>346u4oMvACtZQK9RASzcgYoZwX4JaAd3Pi</t>
   </si>
   <si>
-    <t>Watts</t>
-  </si>
-  <si>
     <t>UUID</t>
   </si>
   <si>
@@ -860,9 +857,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Mh/s</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -uri &lt;PROTOCOL&gt;://&lt;USER&gt;.$WORKER_NAME:&lt;PASSWORD&gt;@&lt;URL_PORT&gt; $GPUS</t>
   </si>
   <si>
@@ -1001,9 +995,6 @@
     <t>GPU-0547b4d4-3354-32a0-eb63-e6013ca68ab8</t>
   </si>
   <si>
-    <t>Sol/s</t>
-  </si>
-  <si>
     <t>RIG-BORG-B</t>
   </si>
   <si>
@@ -1131,15 +1122,29 @@
   </si>
   <si>
     <t>/opt/avermore-miner/sgminer</t>
+  </si>
+  <si>
+    <t>OC-RVN</t>
+  </si>
+  <si>
+    <t>UV-RVN</t>
+  </si>
+  <si>
+    <t>RIG-LAB</t>
+  </si>
+  <si>
+    <t>GPU-ce1df382-1fb6-119e-5048-15c524f28cf8</t>
+  </si>
+  <si>
+    <t>GPU-87638278-4aec-d992-0acb-f67662ebce2d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="40" x14ac:knownFonts="1">
     <font>
@@ -1442,7 +1447,7 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1720,7 +1725,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
@@ -1730,20 +1734,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1780,7 +1774,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1795,12 +1788,9 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -2210,26 +2200,26 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="54" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B7" s="54" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="54" t="s">
+        <v>341</v>
+      </c>
+      <c r="B8" s="54" t="s">
         <v>344</v>
-      </c>
-      <c r="B8" s="54" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="54" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B9" s="54" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2307,22 +2297,22 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="99" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="105" t="s">
         <v>213</v>
       </c>
       <c r="C2" s="77"/>
-      <c r="F2" s="111" t="s">
-        <v>275</v>
+      <c r="F2" s="106" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="99" t="s">
         <v>222</v>
       </c>
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="105" t="s">
         <v>213</v>
       </c>
       <c r="C3" s="77"/>
@@ -2330,7 +2320,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B4" s="72" t="s">
         <v>213</v>
@@ -2339,10 +2329,10 @@
         <v>199</v>
       </c>
       <c r="D4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2451,7 +2441,7 @@
         <v>213</v>
       </c>
       <c r="C12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E12" s="92" t="s">
         <v>147</v>
@@ -2491,7 +2481,7 @@
         <v>156</v>
       </c>
       <c r="F17" s="60" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -2551,16 +2541,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B23" s="72" t="s">
         <v>234</v>
       </c>
       <c r="C23" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F23" s="60" t="s">
         <v>89</v>
@@ -2596,7 +2586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
     </sheetView>
@@ -2606,7 +2596,7 @@
     <col min="1" max="1" width="14.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="83" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="135" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="126" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" style="61" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" style="13" customWidth="1"/>
@@ -2626,7 +2616,7 @@
         <v>240</v>
       </c>
       <c r="D1" s="93" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>177</v>
@@ -2681,63 +2671,63 @@
     </row>
     <row r="7" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
-      <c r="B7" s="150" t="s">
+      <c r="B7" s="141" t="s">
         <v>247</v>
       </c>
-      <c r="C7" s="150"/>
-      <c r="D7" s="150"/>
-      <c r="E7" s="151"/>
-      <c r="F7" s="151"/>
-      <c r="G7" s="151"/>
-      <c r="H7" s="151"/>
-    </row>
-    <row r="8" spans="1:9" s="118" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="141"/>
+      <c r="D7" s="141"/>
+      <c r="E7" s="142"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="142"/>
+      <c r="H7" s="142"/>
+    </row>
+    <row r="8" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="B8" s="118" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8" s="113" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="135"/>
-      <c r="F8" s="118" t="s">
-        <v>298</v>
-      </c>
-      <c r="G8" s="118" t="s">
+      <c r="D8" s="126"/>
+      <c r="F8" s="113" t="s">
+        <v>296</v>
+      </c>
+      <c r="G8" s="113" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="118" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
-      <c r="B9" s="150" t="s">
+      <c r="B9" s="141" t="s">
         <v>224</v>
       </c>
-      <c r="C9" s="150"/>
-      <c r="D9" s="150"/>
-      <c r="E9" s="151"/>
-      <c r="F9" s="151"/>
-      <c r="G9" s="151"/>
-      <c r="H9" s="151"/>
-    </row>
-    <row r="10" spans="1:9" s="145" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="149" t="s">
-        <v>357</v>
+      <c r="C9" s="141"/>
+      <c r="D9" s="141"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="142"/>
+      <c r="G9" s="142"/>
+      <c r="H9" s="142"/>
+    </row>
+    <row r="10" spans="1:9" s="136" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="140" t="s">
+        <v>354</v>
       </c>
       <c r="B10" t="s">
         <v>155</v>
       </c>
       <c r="C10"/>
-      <c r="D10" s="104" t="s">
-        <v>358</v>
+      <c r="D10" s="102" t="s">
+        <v>355</v>
       </c>
       <c r="E10" s="46"/>
       <c r="F10" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="G10" s="145" t="s">
-        <v>302</v>
+        <v>356</v>
+      </c>
+      <c r="G10" s="136" t="s">
+        <v>300</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
@@ -2759,16 +2749,16 @@
     </row>
     <row r="12" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
-      <c r="B12" s="150" t="s">
+      <c r="B12" s="141" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="150"/>
-      <c r="D12" s="150"/>
-      <c r="E12" s="150"/>
-      <c r="F12" s="151"/>
-      <c r="G12" s="151"/>
-      <c r="H12" s="151"/>
-      <c r="I12" s="151"/>
+      <c r="C12" s="141"/>
+      <c r="D12" s="141"/>
+      <c r="E12" s="141"/>
+      <c r="F12" s="142"/>
+      <c r="G12" s="142"/>
+      <c r="H12" s="142"/>
+      <c r="I12" s="142"/>
     </row>
     <row r="13" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
@@ -2778,8 +2768,8 @@
         <v>155</v>
       </c>
       <c r="C13"/>
-      <c r="D13" s="104" t="s">
-        <v>334</v>
+      <c r="D13" s="102" t="s">
+        <v>331</v>
       </c>
       <c r="E13"/>
     </row>
@@ -2791,8 +2781,8 @@
         <v>155</v>
       </c>
       <c r="C14"/>
-      <c r="D14" s="104" t="s">
-        <v>334</v>
+      <c r="D14" s="102" t="s">
+        <v>331</v>
       </c>
       <c r="E14"/>
       <c r="F14" s="75" t="s">
@@ -2838,7 +2828,7 @@
     </row>
     <row r="20" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="76" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B20" s="66" t="s">
         <v>255</v>
@@ -2846,61 +2836,61 @@
       <c r="C20" s="83" t="s">
         <v>234</v>
       </c>
-      <c r="D20" s="135"/>
+      <c r="D20" s="126"/>
       <c r="F20" s="66" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G20" s="66" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H20" s="65"/>
       <c r="I20" s="67"/>
     </row>
     <row r="21" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
-      <c r="B21" s="153" t="s">
-        <v>308</v>
-      </c>
-      <c r="C21" s="153"/>
-      <c r="D21" s="153"/>
-      <c r="E21" s="153"/>
-      <c r="F21" s="151"/>
-      <c r="G21" s="151"/>
-      <c r="H21" s="151"/>
-      <c r="I21" s="151"/>
-    </row>
-    <row r="22" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="144" t="s">
+        <v>306</v>
+      </c>
+      <c r="C21" s="144"/>
+      <c r="D21" s="144"/>
+      <c r="E21" s="144"/>
+      <c r="F21" s="142"/>
+      <c r="G21" s="142"/>
+      <c r="H21" s="142"/>
+      <c r="I21" s="142"/>
+    </row>
+    <row r="22" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="120" t="s">
+      <c r="B22" s="115" t="s">
         <v>202</v>
       </c>
-      <c r="C22" s="120" t="s">
+      <c r="C22" s="115" t="s">
         <v>234</v>
       </c>
-      <c r="D22" s="135"/>
-      <c r="F22" s="120" t="s">
+      <c r="D22" s="126"/>
+      <c r="F22" s="115" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="120" t="s">
+      <c r="G22" s="115" t="s">
         <v>166</v>
       </c>
-      <c r="H22" s="119"/>
-      <c r="I22" s="122"/>
-    </row>
-    <row r="23" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="114"/>
+      <c r="I22" s="116"/>
+    </row>
+    <row r="23" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
-      <c r="B23" s="153" t="s">
+      <c r="B23" s="144" t="s">
         <v>245</v>
       </c>
-      <c r="C23" s="153"/>
-      <c r="D23" s="153"/>
-      <c r="E23" s="153"/>
-      <c r="F23" s="151"/>
-      <c r="G23" s="151"/>
-      <c r="H23" s="151"/>
-      <c r="I23" s="151"/>
+      <c r="C23" s="144"/>
+      <c r="D23" s="144"/>
+      <c r="E23" s="144"/>
+      <c r="F23" s="142"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="142"/>
+      <c r="I23" s="142"/>
     </row>
     <row r="24" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="76" t="s">
@@ -2912,66 +2902,66 @@
       <c r="C24" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="D24" s="135"/>
-      <c r="F24" s="101" t="s">
-        <v>280</v>
+      <c r="D24" s="126"/>
+      <c r="F24" s="100" t="s">
+        <v>278</v>
       </c>
       <c r="G24" s="85" t="s">
         <v>166</v>
       </c>
-      <c r="H24" s="112" t="s">
+      <c r="H24" s="107" t="s">
         <v>250</v>
       </c>
       <c r="I24" s="86"/>
     </row>
     <row r="25" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
-      <c r="B25" s="153" t="s">
+      <c r="B25" s="144" t="s">
+        <v>279</v>
+      </c>
+      <c r="C25" s="144"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="144"/>
+      <c r="F25" s="142"/>
+      <c r="G25" s="142"/>
+      <c r="H25" s="142"/>
+      <c r="I25" s="142"/>
+    </row>
+    <row r="26" spans="1:9" s="108" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="B26" s="108" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="126"/>
+      <c r="F26" s="108" t="s">
+        <v>282</v>
+      </c>
+      <c r="G26" s="108" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="108" t="s">
+        <v>260</v>
+      </c>
+      <c r="I26" s="107"/>
+    </row>
+    <row r="27" spans="1:9" s="108" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="17"/>
+      <c r="B27" s="141" t="s">
         <v>281</v>
       </c>
-      <c r="C25" s="153"/>
-      <c r="D25" s="153"/>
-      <c r="E25" s="153"/>
-      <c r="F25" s="151"/>
-      <c r="G25" s="151"/>
-      <c r="H25" s="151"/>
-      <c r="I25" s="151"/>
-    </row>
-    <row r="26" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="B26" s="113" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="135"/>
-      <c r="F26" s="113" t="s">
-        <v>284</v>
-      </c>
-      <c r="G26" s="113" t="s">
-        <v>82</v>
-      </c>
-      <c r="H26" s="113" t="s">
-        <v>260</v>
-      </c>
-      <c r="I26" s="112"/>
-    </row>
-    <row r="27" spans="1:9" s="113" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
-      <c r="B27" s="150" t="s">
-        <v>283</v>
-      </c>
-      <c r="C27" s="150"/>
-      <c r="D27" s="150"/>
-      <c r="E27" s="150"/>
-      <c r="F27" s="151"/>
-      <c r="G27" s="151"/>
-      <c r="H27" s="151"/>
-      <c r="I27" s="112"/>
+      <c r="C27" s="141"/>
+      <c r="D27" s="141"/>
+      <c r="E27" s="141"/>
+      <c r="F27" s="142"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="142"/>
+      <c r="I27" s="107"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>77</v>
@@ -2987,16 +2977,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
-      <c r="B29" s="153" t="s">
+      <c r="B29" s="144" t="s">
         <v>189</v>
       </c>
-      <c r="C29" s="153"/>
-      <c r="D29" s="153"/>
-      <c r="E29" s="153"/>
-      <c r="F29" s="151"/>
-      <c r="G29" s="151"/>
-      <c r="H29" s="151"/>
-      <c r="I29" s="151"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="142"/>
+      <c r="G29" s="142"/>
+      <c r="H29" s="142"/>
+      <c r="I29" s="142"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
@@ -3011,15 +3001,15 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
-      <c r="B31" s="150" t="s">
+      <c r="B31" s="141" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="150"/>
-      <c r="D31" s="150"/>
-      <c r="E31" s="150"/>
-      <c r="F31" s="151"/>
-      <c r="G31" s="151"/>
-      <c r="H31" s="151"/>
+      <c r="C31" s="141"/>
+      <c r="D31" s="141"/>
+      <c r="E31" s="141"/>
+      <c r="F31" s="142"/>
+      <c r="G31" s="142"/>
+      <c r="H31" s="142"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -3042,15 +3032,15 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
-      <c r="B34" s="150" t="s">
+      <c r="B34" s="141" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="150"/>
-      <c r="D34" s="150"/>
-      <c r="E34" s="150"/>
-      <c r="F34" s="151"/>
-      <c r="G34" s="151"/>
-      <c r="H34" s="151"/>
+      <c r="C34" s="141"/>
+      <c r="D34" s="141"/>
+      <c r="E34" s="141"/>
+      <c r="F34" s="142"/>
+      <c r="G34" s="142"/>
+      <c r="H34" s="142"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
@@ -3085,8 +3075,8 @@
       <c r="B39" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="D39" s="136" t="s">
-        <v>334</v>
+      <c r="D39" s="127" t="s">
+        <v>331</v>
       </c>
       <c r="F39" s="50" t="s">
         <v>135</v>
@@ -3098,15 +3088,15 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
-      <c r="B40" s="153" t="s">
+      <c r="B40" s="144" t="s">
         <v>236</v>
       </c>
-      <c r="C40" s="153"/>
-      <c r="D40" s="153"/>
-      <c r="E40" s="153"/>
-      <c r="F40" s="152"/>
-      <c r="G40" s="152"/>
-      <c r="H40" s="152"/>
+      <c r="C40" s="144"/>
+      <c r="D40" s="144"/>
+      <c r="E40" s="144"/>
+      <c r="F40" s="143"/>
+      <c r="G40" s="143"/>
+      <c r="H40" s="143"/>
       <c r="I40" s="20"/>
     </row>
     <row r="41" spans="1:19" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -3117,8 +3107,8 @@
         <v>20</v>
       </c>
       <c r="C41" s="83"/>
-      <c r="D41" s="136" t="s">
-        <v>334</v>
+      <c r="D41" s="127" t="s">
+        <v>331</v>
       </c>
       <c r="E41" s="61"/>
       <c r="F41" s="45" t="s">
@@ -3132,16 +3122,16 @@
     </row>
     <row r="42" spans="1:19" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
-      <c r="B42" s="153" t="s">
+      <c r="B42" s="144" t="s">
         <v>134</v>
       </c>
-      <c r="C42" s="153"/>
-      <c r="D42" s="153"/>
-      <c r="E42" s="153"/>
-      <c r="F42" s="152"/>
-      <c r="G42" s="152"/>
-      <c r="H42" s="152"/>
-      <c r="I42" s="152"/>
+      <c r="C42" s="144"/>
+      <c r="D42" s="144"/>
+      <c r="E42" s="144"/>
+      <c r="F42" s="143"/>
+      <c r="G42" s="143"/>
+      <c r="H42" s="143"/>
+      <c r="I42" s="143"/>
     </row>
     <row r="43" spans="1:19" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -3151,7 +3141,7 @@
         <v>120</v>
       </c>
       <c r="C43" s="83"/>
-      <c r="D43" s="135"/>
+      <c r="D43" s="126"/>
       <c r="E43" s="61"/>
       <c r="F43" t="s">
         <v>121</v>
@@ -3166,15 +3156,15 @@
     </row>
     <row r="44" spans="1:19" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
-      <c r="B44" s="150" t="s">
+      <c r="B44" s="141" t="s">
         <v>122</v>
       </c>
-      <c r="C44" s="150"/>
-      <c r="D44" s="150"/>
-      <c r="E44" s="150"/>
-      <c r="F44" s="152"/>
-      <c r="G44" s="152"/>
-      <c r="H44" s="152"/>
+      <c r="C44" s="141"/>
+      <c r="D44" s="141"/>
+      <c r="E44" s="141"/>
+      <c r="F44" s="143"/>
+      <c r="G44" s="143"/>
+      <c r="H44" s="143"/>
       <c r="I44" s="40"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
@@ -3190,17 +3180,17 @@
     </row>
     <row r="47" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B47" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="135"/>
+      <c r="D47" s="126"/>
       <c r="F47" s="85" t="s">
         <v>251</v>
       </c>
-      <c r="G47" s="125" t="s">
-        <v>304</v>
+      <c r="G47" s="119" t="s">
+        <v>302</v>
       </c>
       <c r="H47" s="85" t="s">
         <v>91</v>
@@ -3208,15 +3198,15 @@
     </row>
     <row r="48" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
-      <c r="B48" s="150" t="s">
+      <c r="B48" s="141" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="150"/>
-      <c r="D48" s="150"/>
-      <c r="E48" s="150"/>
-      <c r="F48" s="151"/>
-      <c r="G48" s="151"/>
-      <c r="H48" s="151"/>
+      <c r="C48" s="141"/>
+      <c r="D48" s="141"/>
+      <c r="E48" s="141"/>
+      <c r="F48" s="142"/>
+      <c r="G48" s="142"/>
+      <c r="H48" s="142"/>
     </row>
     <row r="49" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -3226,13 +3216,13 @@
         <v>152</v>
       </c>
       <c r="C49" s="83"/>
-      <c r="D49" s="135"/>
+      <c r="D49" s="126"/>
       <c r="E49" s="61"/>
       <c r="F49" s="58" t="s">
-        <v>310</v>
-      </c>
-      <c r="G49" s="125" t="s">
-        <v>304</v>
+        <v>308</v>
+      </c>
+      <c r="G49" s="119" t="s">
+        <v>302</v>
       </c>
       <c r="H49" s="58" t="s">
         <v>91</v>
@@ -3255,118 +3245,118 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
-      <c r="B51" s="150" t="s">
+      <c r="B51" s="141" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="150"/>
-      <c r="D51" s="150"/>
-      <c r="E51" s="150"/>
-      <c r="F51" s="151"/>
-      <c r="G51" s="151"/>
-      <c r="H51" s="151"/>
-    </row>
-    <row r="52" spans="1:19" s="144" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A52" s="142" t="s">
+      <c r="C51" s="141"/>
+      <c r="D51" s="141"/>
+      <c r="E51" s="141"/>
+      <c r="F51" s="142"/>
+      <c r="G51" s="142"/>
+      <c r="H51" s="142"/>
+    </row>
+    <row r="52" spans="1:19" s="135" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A52" s="133" t="s">
+        <v>290</v>
+      </c>
+      <c r="B52" s="134" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="134" t="s">
+        <v>213</v>
+      </c>
+      <c r="D52" s="132" t="s">
+        <v>331</v>
+      </c>
+      <c r="E52" s="134" t="s">
+        <v>291</v>
+      </c>
+      <c r="F52" s="135" t="s">
         <v>292</v>
       </c>
-      <c r="B52" s="143" t="s">
-        <v>160</v>
-      </c>
-      <c r="C52" s="143" t="s">
-        <v>213</v>
-      </c>
-      <c r="D52" s="141" t="s">
-        <v>334</v>
-      </c>
-      <c r="E52" s="143" t="s">
+      <c r="H52" s="135" t="s">
         <v>293</v>
       </c>
-      <c r="F52" s="144" t="s">
-        <v>294</v>
-      </c>
-      <c r="H52" s="144" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:19" s="112" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
-      <c r="B53" s="154" t="s">
-        <v>338</v>
-      </c>
-      <c r="C53" s="154"/>
-      <c r="D53" s="154"/>
-      <c r="E53" s="154"/>
-      <c r="F53" s="152"/>
-      <c r="G53" s="152"/>
-      <c r="H53" s="152"/>
-      <c r="I53" s="152"/>
+      <c r="B53" s="145" t="s">
+        <v>335</v>
+      </c>
+      <c r="C53" s="145"/>
+      <c r="D53" s="145"/>
+      <c r="E53" s="145"/>
+      <c r="F53" s="143"/>
+      <c r="G53" s="143"/>
+      <c r="H53" s="143"/>
+      <c r="I53" s="143"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
-        <v>346</v>
-      </c>
-      <c r="B55" s="125" t="s">
-        <v>299</v>
-      </c>
-      <c r="E55" s="125" t="s">
         <v>343</v>
       </c>
-      <c r="F55" s="125" t="s">
+      <c r="B55" s="119" t="s">
+        <v>297</v>
+      </c>
+      <c r="E55" s="119" t="s">
+        <v>340</v>
+      </c>
+      <c r="F55" s="119" t="s">
         <v>191</v>
       </c>
-      <c r="G55" s="125" t="s">
-        <v>304</v>
-      </c>
-      <c r="H55" s="140" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G55" s="119" t="s">
+        <v>302</v>
+      </c>
+      <c r="H55" s="131" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
-        <v>342</v>
-      </c>
-      <c r="B56" s="125" t="s">
+        <v>339</v>
+      </c>
+      <c r="B56" s="119" t="s">
         <v>87</v>
       </c>
-      <c r="F56" s="125" t="s">
-        <v>340</v>
-      </c>
-      <c r="G56" s="125" t="s">
-        <v>304</v>
-      </c>
-      <c r="H56" s="138"/>
-    </row>
-    <row r="57" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F56" s="119" t="s">
+        <v>337</v>
+      </c>
+      <c r="G56" s="119" t="s">
+        <v>302</v>
+      </c>
+      <c r="H56" s="129"/>
+    </row>
+    <row r="57" spans="1:19" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
-      <c r="B57" s="155" t="s">
-        <v>341</v>
-      </c>
-      <c r="C57" s="151"/>
-      <c r="D57" s="151"/>
-      <c r="E57" s="151"/>
-      <c r="F57" s="151"/>
-      <c r="G57" s="151"/>
-      <c r="H57" s="151"/>
-    </row>
-    <row r="58" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="146" t="s">
+        <v>338</v>
+      </c>
+      <c r="C57" s="142"/>
+      <c r="D57" s="142"/>
+      <c r="E57" s="142"/>
+      <c r="F57" s="142"/>
+      <c r="G57" s="142"/>
+      <c r="H57" s="142"/>
+    </row>
+    <row r="58" spans="1:19" s="119" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="B58" s="119" t="s">
+        <v>152</v>
+      </c>
+      <c r="F58" s="119" t="s">
         <v>303</v>
       </c>
-      <c r="B58" s="125" t="s">
-        <v>152</v>
-      </c>
-      <c r="F58" s="125" t="s">
-        <v>305</v>
-      </c>
-      <c r="G58" s="125" t="s">
-        <v>304</v>
-      </c>
-      <c r="H58" s="138"/>
+      <c r="G58" s="119" t="s">
+        <v>302</v>
+      </c>
+      <c r="H58" s="129"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
@@ -3390,15 +3380,15 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" s="17"/>
-      <c r="B61" s="150" t="s">
+      <c r="B61" s="141" t="s">
         <v>97</v>
       </c>
-      <c r="C61" s="150"/>
-      <c r="D61" s="150"/>
-      <c r="E61" s="150"/>
-      <c r="F61" s="151"/>
-      <c r="G61" s="151"/>
-      <c r="H61" s="151"/>
+      <c r="C61" s="141"/>
+      <c r="D61" s="141"/>
+      <c r="E61" s="141"/>
+      <c r="F61" s="142"/>
+      <c r="G61" s="142"/>
+      <c r="H61" s="142"/>
       <c r="I61" s="52" t="s">
         <v>103</v>
       </c>
@@ -3414,62 +3404,62 @@
       </c>
     </row>
     <row r="64" spans="1:19" s="94" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="123" t="s">
-        <v>348</v>
-      </c>
-      <c r="B64" s="114" t="s">
-        <v>278</v>
-      </c>
-      <c r="C64" s="115"/>
-      <c r="D64" s="115"/>
-      <c r="E64" s="115"/>
-      <c r="F64" s="115" t="s">
+      <c r="A64" s="117" t="s">
+        <v>345</v>
+      </c>
+      <c r="B64" s="109" t="s">
+        <v>276</v>
+      </c>
+      <c r="C64" s="110"/>
+      <c r="D64" s="110"/>
+      <c r="E64" s="110"/>
+      <c r="F64" s="110" t="s">
         <v>258</v>
       </c>
-      <c r="G64" s="115"/>
-      <c r="H64" s="115" t="s">
+      <c r="G64" s="110"/>
+      <c r="H64" s="110" t="s">
         <v>260</v>
       </c>
-      <c r="I64" s="115"/>
-      <c r="J64" s="115"/>
-      <c r="K64" s="115"/>
-      <c r="L64" s="115"/>
-      <c r="M64" s="115"/>
-      <c r="N64" s="115"/>
-      <c r="O64" s="115"/>
-      <c r="P64" s="115"/>
-      <c r="Q64" s="115"/>
-      <c r="R64" s="115"/>
-      <c r="S64" s="115"/>
+      <c r="I64" s="110"/>
+      <c r="J64" s="110"/>
+      <c r="K64" s="110"/>
+      <c r="L64" s="110"/>
+      <c r="M64" s="110"/>
+      <c r="N64" s="110"/>
+      <c r="O64" s="110"/>
+      <c r="P64" s="110"/>
+      <c r="Q64" s="110"/>
+      <c r="R64" s="110"/>
+      <c r="S64" s="110"/>
     </row>
     <row r="65" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="123" t="s">
-        <v>349</v>
-      </c>
-      <c r="B65" s="114" t="s">
-        <v>277</v>
-      </c>
-      <c r="C65" s="115"/>
-      <c r="D65" s="115"/>
-      <c r="E65" s="115"/>
-      <c r="F65" s="115" t="s">
+      <c r="A65" s="117" t="s">
+        <v>346</v>
+      </c>
+      <c r="B65" s="109" t="s">
+        <v>275</v>
+      </c>
+      <c r="C65" s="110"/>
+      <c r="D65" s="110"/>
+      <c r="E65" s="110"/>
+      <c r="F65" s="110" t="s">
         <v>256</v>
       </c>
-      <c r="G65" s="115"/>
-      <c r="H65" s="115" t="s">
+      <c r="G65" s="110"/>
+      <c r="H65" s="110" t="s">
         <v>260</v>
       </c>
-      <c r="I65" s="115"/>
-      <c r="J65" s="115"/>
-      <c r="K65" s="115"/>
-      <c r="L65" s="115"/>
-      <c r="M65" s="115"/>
-      <c r="N65" s="115"/>
-      <c r="O65" s="115"/>
-      <c r="P65" s="115"/>
-      <c r="Q65" s="115"/>
-      <c r="R65" s="115"/>
-      <c r="S65" s="115"/>
+      <c r="I65" s="110"/>
+      <c r="J65" s="110"/>
+      <c r="K65" s="110"/>
+      <c r="L65" s="110"/>
+      <c r="M65" s="110"/>
+      <c r="N65" s="110"/>
+      <c r="O65" s="110"/>
+      <c r="P65" s="110"/>
+      <c r="Q65" s="110"/>
+      <c r="R65" s="110"/>
+      <c r="S65" s="110"/>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
@@ -3486,18 +3476,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="1:19" s="135" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="139" t="s">
-        <v>330</v>
+    <row r="69" spans="1:19" s="126" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="130" t="s">
+        <v>327</v>
       </c>
       <c r="B69" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="D69" s="135" t="s">
-        <v>335</v>
+      <c r="D69" s="126" t="s">
+        <v>332</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H69" s="15" t="s">
         <v>140</v>
@@ -3510,7 +3500,7 @@
       <c r="B70" s="85" t="s">
         <v>202</v>
       </c>
-      <c r="D70" s="135"/>
+      <c r="D70" s="126"/>
       <c r="F70" s="85" t="s">
         <v>73</v>
       </c>
@@ -3524,15 +3514,15 @@
     </row>
     <row r="71" spans="1:19" s="85" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="17"/>
-      <c r="B71" s="150" t="s">
+      <c r="B71" s="141" t="s">
         <v>252</v>
       </c>
-      <c r="C71" s="150"/>
-      <c r="D71" s="150"/>
-      <c r="E71" s="150"/>
-      <c r="F71" s="151"/>
-      <c r="G71" s="151"/>
-      <c r="H71" s="151"/>
+      <c r="C71" s="141"/>
+      <c r="D71" s="141"/>
+      <c r="E71" s="141"/>
+      <c r="F71" s="142"/>
+      <c r="G71" s="142"/>
+      <c r="H71" s="142"/>
       <c r="I71" s="84"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.2">
@@ -3552,26 +3542,26 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73" s="17"/>
-      <c r="B73" s="150" t="s">
+      <c r="B73" s="141" t="s">
         <v>83</v>
       </c>
-      <c r="C73" s="150"/>
-      <c r="D73" s="150"/>
-      <c r="E73" s="150"/>
-      <c r="F73" s="151"/>
-      <c r="G73" s="151"/>
-      <c r="H73" s="151"/>
+      <c r="C73" s="141"/>
+      <c r="D73" s="141"/>
+      <c r="E73" s="141"/>
+      <c r="F73" s="142"/>
+      <c r="G73" s="142"/>
+      <c r="H73" s="142"/>
       <c r="I73" s="20"/>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>9</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H74" s="13" t="s">
         <v>80</v>
@@ -3580,47 +3570,47 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75" s="17"/>
-      <c r="B75" s="150" t="s">
-        <v>289</v>
-      </c>
-      <c r="C75" s="150"/>
-      <c r="D75" s="150"/>
-      <c r="E75" s="150"/>
-      <c r="F75" s="151"/>
-      <c r="G75" s="151"/>
-      <c r="H75" s="151"/>
+      <c r="B75" s="141" t="s">
+        <v>287</v>
+      </c>
+      <c r="C75" s="141"/>
+      <c r="D75" s="141"/>
+      <c r="E75" s="141"/>
+      <c r="F75" s="142"/>
+      <c r="G75" s="142"/>
+      <c r="H75" s="142"/>
       <c r="I75" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:19" s="112" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>56</v>
       </c>
-      <c r="B76" s="117" t="s">
+      <c r="B76" s="112" t="s">
         <v>202</v>
       </c>
-      <c r="D76" s="135"/>
-      <c r="F76" s="117" t="s">
-        <v>291</v>
-      </c>
-      <c r="H76" s="117" t="s">
+      <c r="D76" s="126"/>
+      <c r="F76" s="112" t="s">
+        <v>289</v>
+      </c>
+      <c r="H76" s="112" t="s">
         <v>80</v>
       </c>
-      <c r="I76" s="116"/>
-    </row>
-    <row r="77" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I76" s="111"/>
+    </row>
+    <row r="77" spans="1:19" s="112" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="17"/>
-      <c r="B77" s="150" t="s">
+      <c r="B77" s="141" t="s">
         <v>98</v>
       </c>
-      <c r="C77" s="150"/>
-      <c r="D77" s="150"/>
-      <c r="E77" s="150"/>
-      <c r="F77" s="151"/>
-      <c r="G77" s="151"/>
-      <c r="H77" s="151"/>
-      <c r="I77" s="116" t="s">
+      <c r="C77" s="141"/>
+      <c r="D77" s="141"/>
+      <c r="E77" s="141"/>
+      <c r="F77" s="142"/>
+      <c r="G77" s="142"/>
+      <c r="H77" s="142"/>
+      <c r="I77" s="111" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3632,7 +3622,7 @@
         <v>120</v>
       </c>
       <c r="C78" s="82"/>
-      <c r="D78" s="134"/>
+      <c r="D78" s="125"/>
       <c r="E78" s="65"/>
       <c r="F78" t="s">
         <v>211</v>
@@ -3644,15 +3634,15 @@
     </row>
     <row r="79" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="17"/>
-      <c r="B79" s="150" t="s">
+      <c r="B79" s="141" t="s">
         <v>212</v>
       </c>
-      <c r="C79" s="150"/>
-      <c r="D79" s="150"/>
-      <c r="E79" s="152"/>
-      <c r="F79" s="152"/>
-      <c r="G79" s="152"/>
-      <c r="H79" s="152"/>
+      <c r="C79" s="141"/>
+      <c r="D79" s="141"/>
+      <c r="E79" s="143"/>
+      <c r="F79" s="143"/>
+      <c r="G79" s="143"/>
+      <c r="H79" s="143"/>
       <c r="I79" s="65"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.2">
@@ -3660,83 +3650,83 @@
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:9" s="148" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A81" s="133" t="s">
-        <v>363</v>
+    <row r="81" spans="1:9" s="139" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A81" s="124" t="s">
+        <v>360</v>
       </c>
       <c r="B81" s="62" t="s">
-        <v>364</v>
-      </c>
-      <c r="C81" s="148" t="s">
+        <v>361</v>
+      </c>
+      <c r="C81" s="139" t="s">
         <v>157</v>
       </c>
-      <c r="D81" s="148" t="s">
-        <v>336</v>
+      <c r="D81" s="139" t="s">
+        <v>333</v>
       </c>
       <c r="F81" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="G81" s="139" t="s">
+        <v>302</v>
+      </c>
+      <c r="H81" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="I81" s="139" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" s="139" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="17"/>
+      <c r="B82" s="144" t="s">
+        <v>359</v>
+      </c>
+      <c r="C82" s="144"/>
+      <c r="D82" s="144"/>
+      <c r="E82" s="144"/>
+      <c r="F82" s="143"/>
+      <c r="G82" s="143"/>
+      <c r="H82" s="143"/>
+      <c r="I82" s="138"/>
+    </row>
+    <row r="83" spans="1:9" s="115" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A83" s="124" t="s">
+        <v>304</v>
+      </c>
+      <c r="B83" s="62" t="s">
         <v>325</v>
       </c>
-      <c r="G81" s="148" t="s">
-        <v>304</v>
-      </c>
-      <c r="H81" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="I81" s="148" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" s="148" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="17"/>
-      <c r="B82" s="153" t="s">
-        <v>362</v>
-      </c>
-      <c r="C82" s="153"/>
-      <c r="D82" s="153"/>
-      <c r="E82" s="153"/>
-      <c r="F82" s="152"/>
-      <c r="G82" s="152"/>
-      <c r="H82" s="152"/>
-      <c r="I82" s="147"/>
-    </row>
-    <row r="83" spans="1:9" s="120" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A83" s="133" t="s">
-        <v>306</v>
-      </c>
-      <c r="B83" s="62" t="s">
-        <v>328</v>
-      </c>
-      <c r="C83" s="120" t="s">
+      <c r="C83" s="115" t="s">
         <v>213</v>
       </c>
-      <c r="D83" s="135" t="s">
-        <v>336</v>
+      <c r="D83" s="126" t="s">
+        <v>333</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="G83" s="120" t="s">
-        <v>304</v>
+        <v>322</v>
+      </c>
+      <c r="G83" s="115" t="s">
+        <v>302</v>
       </c>
       <c r="H83" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="I83" s="148" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+      <c r="I83" s="139" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="17"/>
-      <c r="B84" s="153" t="s">
-        <v>337</v>
-      </c>
-      <c r="C84" s="153"/>
-      <c r="D84" s="153"/>
-      <c r="E84" s="153"/>
-      <c r="F84" s="152"/>
-      <c r="G84" s="152"/>
-      <c r="H84" s="152"/>
-      <c r="I84" s="119"/>
+      <c r="B84" s="144" t="s">
+        <v>334</v>
+      </c>
+      <c r="C84" s="144"/>
+      <c r="D84" s="144"/>
+      <c r="E84" s="144"/>
+      <c r="F84" s="143"/>
+      <c r="G84" s="143"/>
+      <c r="H84" s="143"/>
+      <c r="I84" s="114"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
@@ -3753,21 +3743,21 @@
       <c r="F86" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G86" s="124" t="s">
-        <v>304</v>
+      <c r="G86" s="118" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="17"/>
-      <c r="B87" s="150" t="s">
+      <c r="B87" s="141" t="s">
         <v>96</v>
       </c>
-      <c r="C87" s="150"/>
-      <c r="D87" s="150"/>
-      <c r="E87" s="150"/>
-      <c r="F87" s="151"/>
-      <c r="G87" s="151"/>
-      <c r="H87" s="151"/>
+      <c r="C87" s="141"/>
+      <c r="D87" s="141"/>
+      <c r="E87" s="141"/>
+      <c r="F87" s="142"/>
+      <c r="G87" s="142"/>
+      <c r="H87" s="142"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="17" t="s">
@@ -3781,8 +3771,8 @@
       <c r="B89" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="D89" s="136" t="s">
-        <v>334</v>
+      <c r="D89" s="127" t="s">
+        <v>331</v>
       </c>
       <c r="F89" s="49" t="s">
         <v>139</v>
@@ -3796,15 +3786,15 @@
     </row>
     <row r="90" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="17"/>
-      <c r="B90" s="153" t="s">
+      <c r="B90" s="144" t="s">
         <v>133</v>
       </c>
-      <c r="C90" s="153"/>
-      <c r="D90" s="153"/>
-      <c r="E90" s="153"/>
-      <c r="F90" s="152"/>
-      <c r="G90" s="152"/>
-      <c r="H90" s="152"/>
+      <c r="C90" s="144"/>
+      <c r="D90" s="144"/>
+      <c r="E90" s="144"/>
+      <c r="F90" s="143"/>
+      <c r="G90" s="143"/>
+      <c r="H90" s="143"/>
       <c r="I90" s="52"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -3823,15 +3813,15 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="17"/>
-      <c r="B92" s="150" t="s">
+      <c r="B92" s="141" t="s">
         <v>101</v>
       </c>
-      <c r="C92" s="150"/>
-      <c r="D92" s="150"/>
-      <c r="E92" s="150"/>
-      <c r="F92" s="151"/>
-      <c r="G92" s="151"/>
-      <c r="H92" s="151"/>
+      <c r="C92" s="141"/>
+      <c r="D92" s="141"/>
+      <c r="E92" s="141"/>
+      <c r="F92" s="142"/>
+      <c r="G92" s="142"/>
+      <c r="H92" s="142"/>
     </row>
     <row r="93" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
@@ -3841,7 +3831,7 @@
         <v>77</v>
       </c>
       <c r="C93" s="83"/>
-      <c r="D93" s="135"/>
+      <c r="D93" s="126"/>
       <c r="E93" s="61"/>
       <c r="F93" s="44" t="s">
         <v>127</v>
@@ -3851,16 +3841,16 @@
       </c>
     </row>
     <row r="94" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B94" s="150" t="s">
+      <c r="B94" s="141" t="s">
         <v>129</v>
       </c>
-      <c r="C94" s="150"/>
-      <c r="D94" s="150"/>
-      <c r="E94" s="150"/>
-      <c r="F94" s="151"/>
-      <c r="G94" s="151"/>
-      <c r="H94" s="151"/>
-      <c r="I94" s="151"/>
+      <c r="C94" s="141"/>
+      <c r="D94" s="141"/>
+      <c r="E94" s="141"/>
+      <c r="F94" s="142"/>
+      <c r="G94" s="142"/>
+      <c r="H94" s="142"/>
+      <c r="I94" s="142"/>
     </row>
     <row r="95" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="81" t="s">
@@ -3868,7 +3858,7 @@
       </c>
       <c r="B95" s="74"/>
       <c r="C95" s="82"/>
-      <c r="D95" s="134"/>
+      <c r="D95" s="125"/>
       <c r="E95" s="74"/>
       <c r="F95" s="75" t="s">
         <v>232</v>
@@ -3903,16 +3893,16 @@
     </row>
     <row r="98" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="17"/>
-      <c r="B98" s="154" t="s">
+      <c r="B98" s="145" t="s">
         <v>161</v>
       </c>
-      <c r="C98" s="154"/>
-      <c r="D98" s="154"/>
-      <c r="E98" s="154"/>
-      <c r="F98" s="152"/>
-      <c r="G98" s="152"/>
-      <c r="H98" s="152"/>
-      <c r="I98" s="152"/>
+      <c r="C98" s="145"/>
+      <c r="D98" s="145"/>
+      <c r="E98" s="145"/>
+      <c r="F98" s="143"/>
+      <c r="G98" s="143"/>
+      <c r="H98" s="143"/>
+      <c r="I98" s="143"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
@@ -3922,8 +3912,8 @@
         <v>155</v>
       </c>
       <c r="C99" s="62"/>
-      <c r="D99" s="137" t="s">
-        <v>334</v>
+      <c r="D99" s="128" t="s">
+        <v>331</v>
       </c>
       <c r="E99" s="62"/>
       <c r="F99" s="56" t="s">
@@ -3963,15 +3953,15 @@
         <v>218</v>
       </c>
       <c r="B105" s="75" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C105" s="83"/>
-      <c r="D105" s="135"/>
+      <c r="D105" s="126"/>
       <c r="F105" s="75" t="s">
         <v>232</v>
       </c>
       <c r="H105" s="75" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="64" customFormat="1" x14ac:dyDescent="0.2">
@@ -3982,7 +3972,7 @@
         <v>152</v>
       </c>
       <c r="C106" s="83"/>
-      <c r="D106" s="135"/>
+      <c r="D106" s="126"/>
       <c r="F106" s="64" t="s">
         <v>151</v>
       </c>
@@ -4001,7 +3991,7 @@
       <c r="C107" s="83" t="s">
         <v>157</v>
       </c>
-      <c r="D107" s="135"/>
+      <c r="D107" s="126"/>
       <c r="E107" s="61"/>
       <c r="F107" s="58" t="s">
         <v>84</v>
@@ -4013,16 +4003,16 @@
     </row>
     <row r="108" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="17"/>
-      <c r="B108" s="150" t="s">
+      <c r="B108" s="141" t="s">
         <v>136</v>
       </c>
-      <c r="C108" s="150"/>
-      <c r="D108" s="150"/>
-      <c r="E108" s="150"/>
-      <c r="F108" s="151"/>
-      <c r="G108" s="151"/>
-      <c r="H108" s="151"/>
-      <c r="I108" s="151"/>
+      <c r="C108" s="141"/>
+      <c r="D108" s="141"/>
+      <c r="E108" s="141"/>
+      <c r="F108" s="142"/>
+      <c r="G108" s="142"/>
+      <c r="H108" s="142"/>
+      <c r="I108" s="142"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
@@ -4052,8 +4042,8 @@
       <c r="C110" s="98" t="s">
         <v>234</v>
       </c>
-      <c r="D110" s="135"/>
-      <c r="F110" s="109" t="s">
+      <c r="D110" s="126"/>
+      <c r="F110" s="104" t="s">
         <v>165</v>
       </c>
       <c r="G110" s="98" t="s">
@@ -4063,15 +4053,15 @@
     </row>
     <row r="111" spans="1:9" s="98" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="17"/>
-      <c r="B111" s="150" t="s">
-        <v>276</v>
-      </c>
-      <c r="C111" s="150"/>
-      <c r="D111" s="150"/>
-      <c r="E111" s="150"/>
-      <c r="F111" s="150"/>
-      <c r="G111" s="150"/>
-      <c r="H111" s="150"/>
+      <c r="B111" s="141" t="s">
+        <v>274</v>
+      </c>
+      <c r="C111" s="141"/>
+      <c r="D111" s="141"/>
+      <c r="E111" s="141"/>
+      <c r="F111" s="141"/>
+      <c r="G111" s="141"/>
+      <c r="H111" s="141"/>
       <c r="I111" s="97"/>
     </row>
     <row r="112" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
@@ -4084,7 +4074,7 @@
       <c r="C112" s="83" t="s">
         <v>213</v>
       </c>
-      <c r="D112" s="135"/>
+      <c r="D112" s="126"/>
       <c r="F112" s="66" t="s">
         <v>188</v>
       </c>
@@ -4095,15 +4085,15 @@
     </row>
     <row r="113" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="17"/>
-      <c r="B113" s="150" t="s">
+      <c r="B113" s="141" t="s">
         <v>244</v>
       </c>
-      <c r="C113" s="150"/>
-      <c r="D113" s="150"/>
-      <c r="E113" s="150"/>
-      <c r="F113" s="150"/>
-      <c r="G113" s="150"/>
-      <c r="H113" s="150"/>
+      <c r="C113" s="141"/>
+      <c r="D113" s="141"/>
+      <c r="E113" s="141"/>
+      <c r="F113" s="141"/>
+      <c r="G113" s="141"/>
+      <c r="H113" s="141"/>
       <c r="I113" s="65"/>
     </row>
     <row r="114" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
@@ -4114,8 +4104,8 @@
         <v>194</v>
       </c>
       <c r="C114" s="83"/>
-      <c r="D114" s="136" t="s">
-        <v>334</v>
+      <c r="D114" s="127" t="s">
+        <v>331</v>
       </c>
       <c r="F114" s="66" t="s">
         <v>191</v>
@@ -4130,15 +4120,15 @@
     </row>
     <row r="115" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="17"/>
-      <c r="B115" s="150" t="s">
+      <c r="B115" s="141" t="s">
         <v>195</v>
       </c>
-      <c r="C115" s="150"/>
-      <c r="D115" s="150"/>
-      <c r="E115" s="150"/>
-      <c r="F115" s="150"/>
-      <c r="G115" s="150"/>
-      <c r="H115" s="150"/>
+      <c r="C115" s="141"/>
+      <c r="D115" s="141"/>
+      <c r="E115" s="141"/>
+      <c r="F115" s="141"/>
+      <c r="G115" s="141"/>
+      <c r="H115" s="141"/>
       <c r="I115" s="65"/>
     </row>
     <row r="116" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.2">
@@ -4151,7 +4141,7 @@
       <c r="C116" s="83" t="s">
         <v>213</v>
       </c>
-      <c r="D116" s="135"/>
+      <c r="D116" s="126"/>
       <c r="E116" s="61"/>
       <c r="F116" s="58" t="s">
         <v>188</v>
@@ -4173,15 +4163,15 @@
     </row>
     <row r="117" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="17"/>
-      <c r="B117" s="150" t="s">
+      <c r="B117" s="141" t="s">
         <v>208</v>
       </c>
-      <c r="C117" s="150"/>
-      <c r="D117" s="150"/>
-      <c r="E117" s="151"/>
-      <c r="F117" s="151"/>
-      <c r="G117" s="151"/>
-      <c r="H117" s="151"/>
+      <c r="C117" s="141"/>
+      <c r="D117" s="141"/>
+      <c r="E117" s="142"/>
+      <c r="F117" s="142"/>
+      <c r="G117" s="142"/>
+      <c r="H117" s="142"/>
       <c r="I117" s="65"/>
     </row>
     <row r="118" spans="1:19" s="66" customFormat="1" x14ac:dyDescent="0.2">
@@ -4189,10 +4179,10 @@
         <v>187</v>
       </c>
       <c r="B118" s="66" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C118" s="83"/>
-      <c r="D118" s="135"/>
+      <c r="D118" s="126"/>
       <c r="F118" s="66" t="s">
         <v>85</v>
       </c>
@@ -4209,7 +4199,7 @@
         <v>152</v>
       </c>
       <c r="C119" s="83"/>
-      <c r="D119" s="135"/>
+      <c r="D119" s="126"/>
       <c r="F119" s="75" t="s">
         <v>221</v>
       </c>
@@ -4220,11 +4210,11 @@
     </row>
     <row r="120" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="16"/>
-      <c r="B120" s="134" t="s">
-        <v>339</v>
+      <c r="B120" s="125" t="s">
+        <v>336</v>
       </c>
       <c r="C120" s="82"/>
-      <c r="D120" s="134"/>
+      <c r="D120" s="125"/>
       <c r="E120" s="74"/>
     </row>
     <row r="121" spans="1:19" s="75" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -4235,7 +4225,7 @@
         <v>152</v>
       </c>
       <c r="C121" s="83"/>
-      <c r="D121" s="135"/>
+      <c r="D121" s="126"/>
       <c r="F121" s="75" t="s">
         <v>223</v>
       </c>
@@ -4246,11 +4236,11 @@
     </row>
     <row r="122" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="16"/>
-      <c r="B122" s="134" t="s">
-        <v>339</v>
+      <c r="B122" s="125" t="s">
+        <v>336</v>
       </c>
       <c r="C122" s="82"/>
-      <c r="D122" s="134"/>
+      <c r="D122" s="125"/>
       <c r="E122" s="74"/>
     </row>
     <row r="123" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -4261,7 +4251,7 @@
         <v>216</v>
       </c>
       <c r="C123" s="83"/>
-      <c r="D123" s="135"/>
+      <c r="D123" s="126"/>
       <c r="F123" s="75" t="s">
         <v>221</v>
       </c>
@@ -4272,22 +4262,22 @@
     </row>
     <row r="124" spans="1:19" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="16"/>
-      <c r="B124" s="150" t="s">
+      <c r="B124" s="141" t="s">
         <v>226</v>
       </c>
-      <c r="C124" s="150"/>
-      <c r="D124" s="150"/>
-      <c r="E124" s="150"/>
-      <c r="F124" s="151"/>
-      <c r="G124" s="151"/>
-      <c r="H124" s="151"/>
-      <c r="I124" s="151"/>
+      <c r="C124" s="141"/>
+      <c r="D124" s="141"/>
+      <c r="E124" s="141"/>
+      <c r="F124" s="142"/>
+      <c r="G124" s="142"/>
+      <c r="H124" s="142"/>
+      <c r="I124" s="142"/>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>72</v>
       </c>
-      <c r="B125" s="120" t="s">
+      <c r="B125" s="115" t="s">
         <v>152</v>
       </c>
       <c r="F125" s="13" t="s">
@@ -4298,24 +4288,24 @@
       </c>
       <c r="I125" s="20"/>
     </row>
-    <row r="126" spans="1:19" s="120" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:19" s="115" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="80" t="s">
-        <v>314</v>
-      </c>
-      <c r="B126" s="120" t="s">
+        <v>312</v>
+      </c>
+      <c r="B126" s="115" t="s">
         <v>152</v>
       </c>
-      <c r="D126" s="135"/>
-      <c r="F126" s="120" t="s">
-        <v>312</v>
-      </c>
-      <c r="G126" s="125" t="s">
-        <v>304</v>
-      </c>
-      <c r="H126" s="120" t="s">
-        <v>313</v>
-      </c>
-      <c r="I126" s="119"/>
+      <c r="D126" s="126"/>
+      <c r="F126" s="115" t="s">
+        <v>310</v>
+      </c>
+      <c r="G126" s="119" t="s">
+        <v>302</v>
+      </c>
+      <c r="H126" s="115" t="s">
+        <v>311</v>
+      </c>
+      <c r="I126" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="36">
@@ -4383,385 +4373,443 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="137" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" style="106" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4" style="106" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" style="99" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" style="108" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="62" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="128" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="103" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" style="103" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="103" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="103" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="102" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+    <row r="1" spans="1:7" s="101" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="101" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="101" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1" s="101" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="101" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1" s="101" t="s">
+        <v>348</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>362</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="123" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="120" t="s">
+        <v>321</v>
+      </c>
+      <c r="B2" s="121"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="102" t="s">
+        <v>313</v>
+      </c>
+      <c r="B3" s="102"/>
+      <c r="C3" s="128" t="s">
+        <v>314</v>
+      </c>
+      <c r="D3" s="103">
+        <v>1400</v>
+      </c>
+      <c r="E3" s="103">
+        <v>250</v>
+      </c>
+      <c r="F3" s="103">
+        <v>1400</v>
+      </c>
+      <c r="G3" s="103">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="102" t="s">
+        <v>349</v>
+      </c>
+      <c r="C4" s="128" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="102" t="s">
+        <v>350</v>
+      </c>
+      <c r="C5" s="128" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="102" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="102"/>
+      <c r="C6" s="128" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" s="103">
+        <v>1350</v>
+      </c>
+      <c r="E6" s="103">
+        <v>160</v>
+      </c>
+      <c r="F6" s="103">
+        <v>1350</v>
+      </c>
+      <c r="G6" s="103">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="102" t="s">
+        <v>265</v>
+      </c>
+      <c r="B7" s="102"/>
+      <c r="C7" s="128" t="s">
+        <v>271</v>
+      </c>
+      <c r="D7" s="103">
+        <v>1350</v>
+      </c>
+      <c r="E7" s="103">
+        <v>160</v>
+      </c>
+      <c r="F7" s="103">
+        <v>1350</v>
+      </c>
+      <c r="G7" s="103">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="102" t="s">
+        <v>267</v>
+      </c>
+      <c r="B8" s="102"/>
+      <c r="C8" s="128" t="s">
+        <v>271</v>
+      </c>
+      <c r="D8" s="103">
+        <v>1350</v>
+      </c>
+      <c r="E8" s="103">
+        <v>160</v>
+      </c>
+      <c r="F8" s="103">
+        <v>1350</v>
+      </c>
+      <c r="G8" s="103">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="102" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" s="102"/>
+      <c r="C9" s="128" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" s="103">
+        <v>1350</v>
+      </c>
+      <c r="E9" s="103">
+        <v>160</v>
+      </c>
+      <c r="F9" s="103">
+        <v>1350</v>
+      </c>
+      <c r="G9" s="103">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="102" t="s">
+        <v>351</v>
+      </c>
+      <c r="C10" s="128" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="102" t="s">
+        <v>352</v>
+      </c>
+      <c r="C11" s="128" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="102"/>
+    </row>
+    <row r="13" spans="1:7" s="123" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="120" t="s">
+        <v>320</v>
+      </c>
+      <c r="B13" s="121"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="102" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="102" t="s">
-        <v>356</v>
-      </c>
-      <c r="C1" s="102" t="s">
-        <v>273</v>
-      </c>
-      <c r="D1" s="103" t="s">
-        <v>350</v>
-      </c>
-      <c r="E1" s="103" t="s">
-        <v>351</v>
-      </c>
-      <c r="F1" s="105" t="s">
-        <v>261</v>
-      </c>
-      <c r="G1" s="107" t="s">
-        <v>274</v>
-      </c>
-      <c r="H1" s="102" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="132" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="126" t="s">
-        <v>324</v>
-      </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="146"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="128"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="104" t="s">
+      <c r="B14" s="102"/>
+      <c r="C14" s="128" t="s">
+        <v>270</v>
+      </c>
+      <c r="D14" s="103">
+        <v>1150</v>
+      </c>
+      <c r="E14" s="103">
+        <v>160</v>
+      </c>
+      <c r="F14" s="103">
+        <v>1150</v>
+      </c>
+      <c r="G14" s="103">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="102" t="s">
+        <v>263</v>
+      </c>
+      <c r="B15" s="102"/>
+      <c r="C15" s="128" t="s">
+        <v>270</v>
+      </c>
+      <c r="D15" s="103">
+        <v>1150</v>
+      </c>
+      <c r="E15" s="103">
+        <v>160</v>
+      </c>
+      <c r="F15" s="103">
+        <v>1150</v>
+      </c>
+      <c r="G15" s="103">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="102" t="s">
+        <v>264</v>
+      </c>
+      <c r="B16" s="102"/>
+      <c r="C16" s="128" t="s">
+        <v>270</v>
+      </c>
+      <c r="D16" s="103">
+        <v>1150</v>
+      </c>
+      <c r="E16" s="103">
+        <v>160</v>
+      </c>
+      <c r="F16" s="103">
+        <v>1150</v>
+      </c>
+      <c r="G16" s="103">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="102" t="s">
+        <v>268</v>
+      </c>
+      <c r="B17" s="102"/>
+      <c r="C17" s="128" t="s">
+        <v>270</v>
+      </c>
+      <c r="D17" s="103">
+        <v>1150</v>
+      </c>
+      <c r="E17" s="103">
+        <v>160</v>
+      </c>
+      <c r="F17" s="103">
+        <v>1150</v>
+      </c>
+      <c r="G17" s="103">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="102"/>
+      <c r="B18" s="102"/>
+    </row>
+    <row r="19" spans="1:7" s="123" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="120" t="s">
+        <v>319</v>
+      </c>
+      <c r="B19" s="121"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="122"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="122"/>
+      <c r="G19" s="122"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="102" t="s">
         <v>315</v>
       </c>
-      <c r="B3" s="104"/>
-      <c r="C3" s="137" t="s">
+      <c r="C20" s="128" t="s">
+        <v>270</v>
+      </c>
+      <c r="D20" s="103">
+        <v>1200</v>
+      </c>
+      <c r="E20" s="103">
+        <v>140</v>
+      </c>
+      <c r="F20" s="103">
+        <v>1200</v>
+      </c>
+      <c r="G20" s="103">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="102" t="s">
         <v>316</v>
       </c>
-      <c r="D3" s="106">
+      <c r="C21" s="128" t="s">
+        <v>270</v>
+      </c>
+      <c r="D21" s="103">
+        <v>1200</v>
+      </c>
+      <c r="E21" s="103">
+        <v>140</v>
+      </c>
+      <c r="F21" s="103">
+        <v>1200</v>
+      </c>
+      <c r="G21" s="103">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="102" t="s">
+        <v>317</v>
+      </c>
+      <c r="C22" s="128" t="s">
+        <v>270</v>
+      </c>
+      <c r="D22" s="103">
+        <v>1200</v>
+      </c>
+      <c r="E22" s="103">
+        <v>140</v>
+      </c>
+      <c r="F22" s="103">
+        <v>1200</v>
+      </c>
+      <c r="G22" s="103">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="102" t="s">
+        <v>318</v>
+      </c>
+      <c r="C23" s="128" t="s">
+        <v>270</v>
+      </c>
+      <c r="D23" s="103">
+        <v>1200</v>
+      </c>
+      <c r="E23" s="103">
+        <v>140</v>
+      </c>
+      <c r="F23" s="103">
+        <v>1200</v>
+      </c>
+      <c r="G23" s="103">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="102"/>
+      <c r="B24" s="102"/>
+    </row>
+    <row r="25" spans="1:7" s="123" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="120" t="s">
+        <v>364</v>
+      </c>
+      <c r="B25" s="121"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="122"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="122"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="102" t="s">
+        <v>366</v>
+      </c>
+      <c r="B26" s="102"/>
+      <c r="C26" s="128" t="s">
+        <v>314</v>
+      </c>
+      <c r="D26" s="103">
         <v>1400</v>
       </c>
-      <c r="E3" s="106">
+      <c r="E26" s="103">
         <v>250</v>
       </c>
-      <c r="F3" s="99">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="104" t="s">
-        <v>352</v>
-      </c>
-      <c r="C4" s="137" t="s">
+      <c r="F26" s="103">
+        <v>1100</v>
+      </c>
+      <c r="G26" s="103">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="102" t="s">
+        <v>365</v>
+      </c>
+      <c r="C27" s="128" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="104" t="s">
-        <v>353</v>
-      </c>
-      <c r="C5" s="137" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="104" t="s">
-        <v>267</v>
-      </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="137" t="s">
-        <v>272</v>
-      </c>
-      <c r="D6" s="106">
-        <v>1350</v>
-      </c>
-      <c r="E6" s="106">
-        <v>160</v>
-      </c>
-      <c r="G6" s="108">
-        <v>31.85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="104" t="s">
-        <v>266</v>
-      </c>
-      <c r="B7" s="104"/>
-      <c r="C7" s="137" t="s">
-        <v>272</v>
-      </c>
-      <c r="D7" s="106">
-        <v>1350</v>
-      </c>
-      <c r="E7" s="106">
-        <v>160</v>
-      </c>
-      <c r="G7" s="108">
-        <v>31.85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="104" t="s">
-        <v>268</v>
-      </c>
-      <c r="B8" s="104"/>
-      <c r="C8" s="137" t="s">
-        <v>272</v>
-      </c>
-      <c r="D8" s="106">
-        <v>1350</v>
-      </c>
-      <c r="E8" s="106">
-        <v>160</v>
-      </c>
-      <c r="G8" s="108">
-        <v>31.85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="104" t="s">
-        <v>270</v>
-      </c>
-      <c r="B9" s="104"/>
-      <c r="C9" s="137" t="s">
-        <v>272</v>
-      </c>
-      <c r="D9" s="106">
-        <v>1350</v>
-      </c>
-      <c r="E9" s="106">
-        <v>160</v>
-      </c>
-      <c r="G9" s="108">
-        <v>31.85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="104" t="s">
-        <v>354</v>
-      </c>
-      <c r="C10" s="137" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="104" t="s">
-        <v>355</v>
-      </c>
-      <c r="C11" s="137" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="104"/>
-      <c r="F12" s="121"/>
-    </row>
-    <row r="13" spans="1:8" s="132" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="126" t="s">
-        <v>323</v>
-      </c>
-      <c r="B13" s="127"/>
-      <c r="C13" s="146"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="130"/>
-      <c r="G13" s="131"/>
-      <c r="H13" s="128"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="104" t="s">
-        <v>263</v>
-      </c>
-      <c r="B14" s="104"/>
-      <c r="C14" s="137" t="s">
-        <v>271</v>
-      </c>
-      <c r="D14" s="106">
-        <v>1150</v>
-      </c>
-      <c r="E14" s="106">
-        <v>160</v>
-      </c>
-      <c r="G14" s="108">
-        <v>31.04</v>
-      </c>
-      <c r="H14" s="62">
-        <v>483.61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="104" t="s">
-        <v>264</v>
-      </c>
-      <c r="B15" s="104"/>
-      <c r="C15" s="137" t="s">
-        <v>271</v>
-      </c>
-      <c r="D15" s="106">
-        <v>1150</v>
-      </c>
-      <c r="E15" s="106">
-        <v>160</v>
-      </c>
-      <c r="G15" s="108">
-        <v>31.1</v>
-      </c>
-      <c r="H15" s="62">
-        <v>530.94000000000005</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="104" t="s">
-        <v>265</v>
-      </c>
-      <c r="B16" s="104"/>
-      <c r="C16" s="137" t="s">
-        <v>271</v>
-      </c>
-      <c r="D16" s="106">
-        <v>1150</v>
-      </c>
-      <c r="E16" s="106">
-        <v>160</v>
-      </c>
-      <c r="G16" s="108">
-        <v>31.21</v>
-      </c>
-      <c r="H16" s="62">
-        <v>532.42999999999995</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="104" t="s">
-        <v>269</v>
-      </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="137" t="s">
-        <v>271</v>
-      </c>
-      <c r="D17" s="106">
-        <v>1150</v>
-      </c>
-      <c r="E17" s="106">
-        <v>160</v>
-      </c>
-      <c r="G17" s="108">
-        <v>31.15</v>
-      </c>
-      <c r="H17" s="62">
-        <v>524.54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="104"/>
-      <c r="B18" s="104"/>
-      <c r="F18" s="121"/>
-    </row>
-    <row r="19" spans="1:8" s="132" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="126" t="s">
-        <v>322</v>
-      </c>
-      <c r="B19" s="127"/>
-      <c r="C19" s="146"/>
-      <c r="D19" s="129"/>
-      <c r="E19" s="129"/>
-      <c r="F19" s="130"/>
-      <c r="G19" s="131"/>
-      <c r="H19" s="128"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="104" t="s">
-        <v>317</v>
-      </c>
-      <c r="C20" s="137" t="s">
-        <v>271</v>
-      </c>
-      <c r="D20" s="106">
+      <c r="D27" s="103">
         <v>1200</v>
       </c>
-      <c r="E20" s="106">
-        <v>140</v>
-      </c>
-      <c r="F20" s="121">
-        <v>138</v>
-      </c>
-      <c r="H20" s="62">
-        <v>524.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="104" t="s">
-        <v>318</v>
-      </c>
-      <c r="C21" s="137" t="s">
-        <v>271</v>
-      </c>
-      <c r="D21" s="106">
+      <c r="E27" s="103">
+        <v>120</v>
+      </c>
+      <c r="F27" s="103">
         <v>1200</v>
       </c>
-      <c r="E21" s="106">
-        <v>140</v>
-      </c>
-      <c r="F21" s="121">
-        <v>140</v>
-      </c>
-      <c r="H21" s="62">
-        <v>520.79999999999995</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="104" t="s">
-        <v>319</v>
-      </c>
-      <c r="C22" s="137" t="s">
-        <v>271</v>
-      </c>
-      <c r="D22" s="106">
-        <v>1200</v>
-      </c>
-      <c r="E22" s="106">
-        <v>140</v>
-      </c>
-      <c r="F22" s="121">
-        <v>139</v>
-      </c>
-      <c r="H22" s="62">
-        <v>527.52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="104" t="s">
-        <v>320</v>
-      </c>
-      <c r="C23" s="137" t="s">
-        <v>271</v>
-      </c>
-      <c r="D23" s="106">
-        <v>1200</v>
-      </c>
-      <c r="E23" s="106">
-        <v>140</v>
-      </c>
-      <c r="F23" s="121">
-        <v>135</v>
-      </c>
-      <c r="H23" s="62">
-        <v>480.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="104"/>
-      <c r="B24" s="104"/>
-      <c r="F24" s="121"/>
+      <c r="G27" s="103">
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5247,10 +5295,10 @@
     </row>
     <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
-      <c r="B6" s="156" t="s">
+      <c r="B6" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="156"/>
+      <c r="C6" s="147"/>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
@@ -5268,10 +5316,10 @@
     </row>
     <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="157" t="s">
+      <c r="B9" s="148" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="158"/>
+      <c r="C9" s="149"/>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -5321,10 +5369,10 @@
     </row>
     <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
-      <c r="B16" s="159" t="s">
+      <c r="B16" s="150" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="160"/>
+      <c r="C16" s="151"/>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">

</xml_diff>

<commit_message>
Restore 'MINER'=>Clients/MNEMONIC mapping that regressed recently.
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="25600" windowHeight="13000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-20" yWindow="2400" windowWidth="25600" windowHeight="13000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="5" r:id="rId1"/>
@@ -1841,10 +1841,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2260,7 +2260,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2586,9 +2586,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B73" sqref="B73:H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2848,12 +2848,12 @@
     </row>
     <row r="21" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
-      <c r="B21" s="144" t="s">
+      <c r="B21" s="143" t="s">
         <v>306</v>
       </c>
-      <c r="C21" s="144"/>
-      <c r="D21" s="144"/>
-      <c r="E21" s="144"/>
+      <c r="C21" s="143"/>
+      <c r="D21" s="143"/>
+      <c r="E21" s="143"/>
       <c r="F21" s="142"/>
       <c r="G21" s="142"/>
       <c r="H21" s="142"/>
@@ -2881,12 +2881,12 @@
     </row>
     <row r="23" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
-      <c r="B23" s="144" t="s">
+      <c r="B23" s="143" t="s">
         <v>245</v>
       </c>
-      <c r="C23" s="144"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
+      <c r="C23" s="143"/>
+      <c r="D23" s="143"/>
+      <c r="E23" s="143"/>
       <c r="F23" s="142"/>
       <c r="G23" s="142"/>
       <c r="H23" s="142"/>
@@ -2916,12 +2916,12 @@
     </row>
     <row r="25" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
-      <c r="B25" s="144" t="s">
+      <c r="B25" s="143" t="s">
         <v>279</v>
       </c>
-      <c r="C25" s="144"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="144"/>
+      <c r="C25" s="143"/>
+      <c r="D25" s="143"/>
+      <c r="E25" s="143"/>
       <c r="F25" s="142"/>
       <c r="G25" s="142"/>
       <c r="H25" s="142"/>
@@ -2977,12 +2977,12 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
-      <c r="B29" s="144" t="s">
+      <c r="B29" s="143" t="s">
         <v>189</v>
       </c>
-      <c r="C29" s="144"/>
-      <c r="D29" s="144"/>
-      <c r="E29" s="144"/>
+      <c r="C29" s="143"/>
+      <c r="D29" s="143"/>
+      <c r="E29" s="143"/>
       <c r="F29" s="142"/>
       <c r="G29" s="142"/>
       <c r="H29" s="142"/>
@@ -3088,15 +3088,15 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
-      <c r="B40" s="144" t="s">
+      <c r="B40" s="143" t="s">
         <v>236</v>
       </c>
-      <c r="C40" s="144"/>
-      <c r="D40" s="144"/>
-      <c r="E40" s="144"/>
-      <c r="F40" s="143"/>
-      <c r="G40" s="143"/>
-      <c r="H40" s="143"/>
+      <c r="C40" s="143"/>
+      <c r="D40" s="143"/>
+      <c r="E40" s="143"/>
+      <c r="F40" s="144"/>
+      <c r="G40" s="144"/>
+      <c r="H40" s="144"/>
       <c r="I40" s="20"/>
     </row>
     <row r="41" spans="1:19" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -3122,16 +3122,16 @@
     </row>
     <row r="42" spans="1:19" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
-      <c r="B42" s="144" t="s">
+      <c r="B42" s="143" t="s">
         <v>134</v>
       </c>
-      <c r="C42" s="144"/>
-      <c r="D42" s="144"/>
-      <c r="E42" s="144"/>
-      <c r="F42" s="143"/>
-      <c r="G42" s="143"/>
-      <c r="H42" s="143"/>
-      <c r="I42" s="143"/>
+      <c r="C42" s="143"/>
+      <c r="D42" s="143"/>
+      <c r="E42" s="143"/>
+      <c r="F42" s="144"/>
+      <c r="G42" s="144"/>
+      <c r="H42" s="144"/>
+      <c r="I42" s="144"/>
     </row>
     <row r="43" spans="1:19" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -3162,9 +3162,9 @@
       <c r="C44" s="141"/>
       <c r="D44" s="141"/>
       <c r="E44" s="141"/>
-      <c r="F44" s="143"/>
-      <c r="G44" s="143"/>
-      <c r="H44" s="143"/>
+      <c r="F44" s="144"/>
+      <c r="G44" s="144"/>
+      <c r="H44" s="144"/>
       <c r="I44" s="40"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
@@ -3286,10 +3286,10 @@
       <c r="C53" s="145"/>
       <c r="D53" s="145"/>
       <c r="E53" s="145"/>
-      <c r="F53" s="143"/>
-      <c r="G53" s="143"/>
-      <c r="H53" s="143"/>
-      <c r="I53" s="143"/>
+      <c r="F53" s="144"/>
+      <c r="G53" s="144"/>
+      <c r="H53" s="144"/>
+      <c r="I53" s="144"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
@@ -3476,11 +3476,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="1:19" s="126" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:19" s="126" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="130" t="s">
         <v>327</v>
       </c>
-      <c r="B69" s="62" t="s">
+      <c r="B69" t="s">
         <v>155</v>
       </c>
       <c r="D69" s="126" t="s">
@@ -3639,10 +3639,10 @@
       </c>
       <c r="C79" s="141"/>
       <c r="D79" s="141"/>
-      <c r="E79" s="143"/>
-      <c r="F79" s="143"/>
-      <c r="G79" s="143"/>
-      <c r="H79" s="143"/>
+      <c r="E79" s="144"/>
+      <c r="F79" s="144"/>
+      <c r="G79" s="144"/>
+      <c r="H79" s="144"/>
       <c r="I79" s="65"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.2">
@@ -3678,15 +3678,15 @@
     </row>
     <row r="82" spans="1:9" s="139" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="17"/>
-      <c r="B82" s="144" t="s">
+      <c r="B82" s="143" t="s">
         <v>359</v>
       </c>
-      <c r="C82" s="144"/>
-      <c r="D82" s="144"/>
-      <c r="E82" s="144"/>
-      <c r="F82" s="143"/>
-      <c r="G82" s="143"/>
-      <c r="H82" s="143"/>
+      <c r="C82" s="143"/>
+      <c r="D82" s="143"/>
+      <c r="E82" s="143"/>
+      <c r="F82" s="144"/>
+      <c r="G82" s="144"/>
+      <c r="H82" s="144"/>
       <c r="I82" s="138"/>
     </row>
     <row r="83" spans="1:9" s="115" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -3717,15 +3717,15 @@
     </row>
     <row r="84" spans="1:9" s="115" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="17"/>
-      <c r="B84" s="144" t="s">
+      <c r="B84" s="143" t="s">
         <v>334</v>
       </c>
-      <c r="C84" s="144"/>
-      <c r="D84" s="144"/>
-      <c r="E84" s="144"/>
-      <c r="F84" s="143"/>
-      <c r="G84" s="143"/>
-      <c r="H84" s="143"/>
+      <c r="C84" s="143"/>
+      <c r="D84" s="143"/>
+      <c r="E84" s="143"/>
+      <c r="F84" s="144"/>
+      <c r="G84" s="144"/>
+      <c r="H84" s="144"/>
       <c r="I84" s="114"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -3786,15 +3786,15 @@
     </row>
     <row r="90" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="17"/>
-      <c r="B90" s="144" t="s">
+      <c r="B90" s="143" t="s">
         <v>133</v>
       </c>
-      <c r="C90" s="144"/>
-      <c r="D90" s="144"/>
-      <c r="E90" s="144"/>
-      <c r="F90" s="143"/>
-      <c r="G90" s="143"/>
-      <c r="H90" s="143"/>
+      <c r="C90" s="143"/>
+      <c r="D90" s="143"/>
+      <c r="E90" s="143"/>
+      <c r="F90" s="144"/>
+      <c r="G90" s="144"/>
+      <c r="H90" s="144"/>
       <c r="I90" s="52"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -3899,10 +3899,10 @@
       <c r="C98" s="145"/>
       <c r="D98" s="145"/>
       <c r="E98" s="145"/>
-      <c r="F98" s="143"/>
-      <c r="G98" s="143"/>
-      <c r="H98" s="143"/>
-      <c r="I98" s="143"/>
+      <c r="F98" s="144"/>
+      <c r="G98" s="144"/>
+      <c r="H98" s="144"/>
+      <c r="I98" s="144"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
@@ -4309,6 +4309,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B117:H117"/>
+    <mergeCell ref="B115:H115"/>
+    <mergeCell ref="B113:H113"/>
+    <mergeCell ref="B79:H79"/>
+    <mergeCell ref="B92:H92"/>
+    <mergeCell ref="B87:H87"/>
+    <mergeCell ref="B111:H111"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B90:H90"/>
+    <mergeCell ref="B108:I108"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B98:I98"/>
+    <mergeCell ref="B51:H51"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B73:H73"/>
+    <mergeCell ref="B75:H75"/>
+    <mergeCell ref="B57:H57"/>
+    <mergeCell ref="B82:H82"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B124:I124"/>
     <mergeCell ref="B94:I94"/>
@@ -4325,26 +4345,6 @@
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B77:H77"/>
     <mergeCell ref="B53:I53"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B90:H90"/>
-    <mergeCell ref="B108:I108"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B98:I98"/>
-    <mergeCell ref="B51:H51"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="B73:H73"/>
-    <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B57:H57"/>
-    <mergeCell ref="B82:H82"/>
-    <mergeCell ref="B117:H117"/>
-    <mergeCell ref="B115:H115"/>
-    <mergeCell ref="B113:H113"/>
-    <mergeCell ref="B79:H79"/>
-    <mergeCell ref="B92:H92"/>
-    <mergeCell ref="B87:H87"/>
-    <mergeCell ref="B111:H111"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A121" r:id="rId1" display="ZEL"/>
@@ -4375,7 +4375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>

</xml_diff>

<commit_message>
Introducing --scope option to 'miners status'.
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="522">
   <si>
     <t>Miners (AMD)</t>
   </si>
@@ -1602,16 +1602,7 @@
     <t>GUuefiwUDznDnyWD9rfixw1vo5Xeo7wqEk</t>
   </si>
   <si>
-    <t>RIG_TAGS</t>
-  </si>
-  <si>
-    <t>AMD,BORG,NVI,LAB-W</t>
-  </si>
-  <si>
-    <t>RIG_IPS</t>
-  </si>
-  <si>
-    <t>10.0.0.4,10.0.0.7,10.0.0.2,10.0.0.5</t>
+    <t>MINERS_USER</t>
   </si>
 </sst>
 </file>
@@ -1932,7 +1923,7 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2398,6 +2389,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2678,10 +2672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2702,106 +2696,99 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+    <row r="2" spans="1:5" s="168" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="168" t="s">
         <v>521</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="54" t="s">
-        <v>523</v>
-      </c>
-      <c r="B3" s="54" t="s">
-        <v>524</v>
+      <c r="B2" s="168" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="54" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="54" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="54" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B5" s="54">
         <v>6502799436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="54" t="s">
-        <v>191</v>
+        <v>241</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>192</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="54" t="s">
-        <v>241</v>
+        <v>292</v>
       </c>
       <c r="B9" s="54" t="s">
-        <v>240</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="54" t="s">
-        <v>292</v>
+        <v>338</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>291</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="54" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="B11" s="54" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="54" t="s">
-        <v>322</v>
-      </c>
-      <c r="B12" s="54" t="s">
         <v>321</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="54" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13" s="95" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="54" t="s">
-        <v>252</v>
-      </c>
-      <c r="B14" s="95" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="54" t="s">
         <v>234</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B14" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C14" s="54" t="s">
         <v>233</v>
       </c>
-      <c r="D15" s="54" t="s">
+      <c r="D14" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="E15" s="54" t="s">
+      <c r="E14" s="54" t="s">
         <v>212</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1"/>
+    <hyperlink ref="B13" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3124,7 +3111,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Globals!$C$15:$F$15</xm:f>
+            <xm:f>Globals!$C$14:$F$14</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B20</xm:sqref>
         </x14:dataValidation>
@@ -3139,7 +3126,7 @@
   <dimension ref="A1:S131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
More python3, "a bytes-like object is required", et.al.
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1620" windowWidth="20620" windowHeight="12740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="640" yWindow="1620" windowWidth="20620" windowHeight="12740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="641">
   <si>
     <t>Miners (AMD)</t>
   </si>
@@ -1953,6 +1953,12 @@
   </si>
   <si>
     <t>RVN-ice</t>
+  </si>
+  <si>
+    <t>Gos</t>
+  </si>
+  <si>
+    <t>XMN,RVN, etc.</t>
   </si>
 </sst>
 </file>
@@ -2423,7 +2429,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2713,7 +2719,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2892,6 +2897,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3220,18 +3227,18 @@
       <c r="B2" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="140"/>
-      <c r="H2" s="140"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="140"/>
-      <c r="K2" s="140"/>
-      <c r="L2" s="140"/>
-      <c r="M2" s="140"/>
-      <c r="N2" s="140"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="139"/>
+      <c r="J2" s="139"/>
+      <c r="K2" s="139"/>
+      <c r="L2" s="139"/>
+      <c r="M2" s="139"/>
+      <c r="N2" s="139"/>
     </row>
     <row r="3" spans="1:14" s="67" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="67" t="s">
@@ -3240,6 +3247,187 @@
       <c r="B3" s="67" t="s">
         <v>571</v>
       </c>
+      <c r="C3" s="139"/>
+      <c r="D3" s="139"/>
+      <c r="E3" s="139"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="139"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="139"/>
+      <c r="K3" s="139"/>
+      <c r="L3" s="139"/>
+      <c r="M3" s="139"/>
+      <c r="N3" s="139"/>
+    </row>
+    <row r="4" spans="1:14" s="67" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="139"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="139"/>
+      <c r="J4" s="139"/>
+      <c r="K4" s="139"/>
+      <c r="L4" s="139"/>
+      <c r="M4" s="139"/>
+      <c r="N4" s="139"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="57" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="37" t="s">
+        <v>289</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>616</v>
+      </c>
+      <c r="D6" s="57" t="s">
+        <v>547</v>
+      </c>
+      <c r="E6" s="57" t="s">
+        <v>299</v>
+      </c>
+      <c r="F6" s="57" t="s">
+        <v>545</v>
+      </c>
+      <c r="G6" s="57" t="s">
+        <v>292</v>
+      </c>
+      <c r="H6" s="57" t="s">
+        <v>524</v>
+      </c>
+      <c r="I6" s="57" t="s">
+        <v>291</v>
+      </c>
+      <c r="J6" s="57" t="s">
+        <v>617</v>
+      </c>
+      <c r="K6" s="57" t="s">
+        <v>293</v>
+      </c>
+      <c r="L6" s="57" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L7" s="57" t="s">
+        <v>619</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6" style="143" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="142" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" style="142" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="142" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="142" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="142" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="142" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="142" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" style="142" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" style="142" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="142" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" style="142" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" style="142" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.7109375" style="142"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="151" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1" s="151" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="153" t="s">
+        <v>573</v>
+      </c>
+      <c r="C1" s="153" t="s">
+        <v>576</v>
+      </c>
+      <c r="D1" s="153" t="s">
+        <v>575</v>
+      </c>
+      <c r="E1" s="152" t="s">
+        <v>580</v>
+      </c>
+      <c r="F1" s="152" t="s">
+        <v>579</v>
+      </c>
+      <c r="G1" s="154" t="s">
+        <v>577</v>
+      </c>
+      <c r="H1" s="153" t="s">
+        <v>622</v>
+      </c>
+      <c r="I1" s="152" t="s">
+        <v>574</v>
+      </c>
+      <c r="J1" s="152" t="s">
+        <v>620</v>
+      </c>
+      <c r="K1" s="163" t="s">
+        <v>626</v>
+      </c>
+      <c r="L1" s="154" t="s">
+        <v>623</v>
+      </c>
+      <c r="M1" s="152" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="155" customFormat="1" ht="33" x14ac:dyDescent="0.2">
+      <c r="A2" s="148" t="s">
+        <v>614</v>
+      </c>
+      <c r="B2" s="149" t="s">
+        <v>613</v>
+      </c>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150"/>
+      <c r="J2" s="150"/>
+      <c r="K2" s="150"/>
+      <c r="L2" s="150"/>
+      <c r="M2" s="150"/>
+    </row>
+    <row r="3" spans="1:13" s="143" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="143" t="s">
+        <v>582</v>
+      </c>
+      <c r="B3" s="142"/>
       <c r="C3" s="140"/>
       <c r="D3" s="140"/>
       <c r="E3" s="140"/>
@@ -3251,9 +3439,12 @@
       <c r="K3" s="140"/>
       <c r="L3" s="140"/>
       <c r="M3" s="140"/>
-      <c r="N3" s="140"/>
-    </row>
-    <row r="4" spans="1:14" s="67" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:13" s="143" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="143" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="142"/>
       <c r="C4" s="140"/>
       <c r="D4" s="140"/>
       <c r="E4" s="140"/>
@@ -3265,468 +3456,284 @@
       <c r="K4" s="140"/>
       <c r="L4" s="140"/>
       <c r="M4" s="140"/>
-      <c r="N4" s="140"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>211</v>
-      </c>
-      <c r="D5" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="E5" s="57" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B6" s="37" t="s">
-        <v>289</v>
-      </c>
-      <c r="C6" s="57" t="s">
-        <v>616</v>
-      </c>
-      <c r="D6" s="57" t="s">
-        <v>547</v>
-      </c>
-      <c r="E6" s="57" t="s">
-        <v>299</v>
-      </c>
-      <c r="F6" s="57" t="s">
-        <v>545</v>
-      </c>
-      <c r="G6" s="57" t="s">
-        <v>292</v>
-      </c>
-      <c r="H6" s="57" t="s">
-        <v>524</v>
-      </c>
-      <c r="I6" s="57" t="s">
-        <v>291</v>
-      </c>
-      <c r="J6" s="57" t="s">
-        <v>617</v>
-      </c>
-      <c r="K6" s="57" t="s">
-        <v>293</v>
-      </c>
-      <c r="L6" s="57" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L7" s="57" t="s">
-        <v>619</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M44"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6" style="144" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="143" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" style="143" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" style="143" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="143" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="143" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="143" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="143" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6" style="143" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" style="143" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="143" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" style="143" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5" style="143" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.7109375" style="143"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="152" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="152" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="154" t="s">
-        <v>573</v>
-      </c>
-      <c r="C1" s="154" t="s">
-        <v>576</v>
-      </c>
-      <c r="D1" s="154" t="s">
-        <v>575</v>
-      </c>
-      <c r="E1" s="153" t="s">
-        <v>580</v>
-      </c>
-      <c r="F1" s="153" t="s">
-        <v>579</v>
-      </c>
-      <c r="G1" s="155" t="s">
-        <v>577</v>
-      </c>
-      <c r="H1" s="154" t="s">
-        <v>622</v>
-      </c>
-      <c r="I1" s="153" t="s">
-        <v>574</v>
-      </c>
-      <c r="J1" s="153" t="s">
-        <v>620</v>
-      </c>
-      <c r="K1" s="164" t="s">
-        <v>626</v>
-      </c>
-      <c r="L1" s="155" t="s">
-        <v>623</v>
-      </c>
-      <c r="M1" s="153" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="156" customFormat="1" ht="33" x14ac:dyDescent="0.2">
-      <c r="A2" s="149" t="s">
-        <v>614</v>
-      </c>
-      <c r="B2" s="150" t="s">
-        <v>613</v>
-      </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
-      <c r="K2" s="151"/>
-      <c r="L2" s="151"/>
-      <c r="M2" s="151"/>
-    </row>
-    <row r="3" spans="1:13" s="144" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="144" t="s">
-        <v>582</v>
-      </c>
-      <c r="B3" s="143"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="141"/>
-      <c r="K3" s="141"/>
-      <c r="L3" s="141"/>
-      <c r="M3" s="141"/>
-    </row>
-    <row r="4" spans="1:13" s="144" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="144" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="143"/>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="141"/>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="L4" s="141"/>
-      <c r="M4" s="141"/>
-    </row>
-    <row r="5" spans="1:13" s="147" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="147" t="s">
+    </row>
+    <row r="5" spans="1:13" s="146" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="146" t="s">
         <v>615</v>
       </c>
-      <c r="B5" s="148"/>
-      <c r="D5" s="147" t="s">
+      <c r="B5" s="147"/>
+      <c r="D5" s="146" t="s">
         <v>621</v>
       </c>
-      <c r="H5" s="147" t="s">
+      <c r="H5" s="146" t="s">
         <v>621</v>
       </c>
-      <c r="I5" s="147" t="s">
+      <c r="I5" s="146" t="s">
         <v>621</v>
       </c>
-      <c r="J5" s="147" t="s">
+      <c r="J5" s="146" t="s">
         <v>621</v>
       </c>
-      <c r="L5" s="147" t="s">
+      <c r="L5" s="146" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="144" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="144" t="s">
+    <row r="6" spans="1:13" s="143" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="143" t="s">
         <v>583</v>
       </c>
-      <c r="B6" s="143"/>
-      <c r="C6" s="141"/>
-      <c r="D6" s="141"/>
-      <c r="E6" s="141"/>
-      <c r="F6" s="141"/>
-      <c r="G6" s="141"/>
-      <c r="H6" s="141"/>
-      <c r="I6" s="141"/>
-      <c r="J6" s="141"/>
-      <c r="K6" s="141"/>
-      <c r="L6" s="141"/>
-      <c r="M6" s="141"/>
-    </row>
-    <row r="7" spans="1:13" s="144" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="144" t="s">
+      <c r="B6" s="142"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
+      <c r="G6" s="140"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="140"/>
+      <c r="L6" s="140"/>
+      <c r="M6" s="140"/>
+    </row>
+    <row r="7" spans="1:13" s="143" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="143" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="143"/>
-      <c r="C7" s="141"/>
-      <c r="D7" s="141"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="141"/>
-      <c r="G7" s="141"/>
-      <c r="H7" s="141"/>
-      <c r="I7" s="141"/>
-      <c r="J7" s="141"/>
-      <c r="K7" s="141"/>
-      <c r="L7" s="141"/>
-      <c r="M7" s="141"/>
-    </row>
-    <row r="8" spans="1:13" s="144" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="144" t="s">
+      <c r="B7" s="142"/>
+      <c r="C7" s="140"/>
+      <c r="D7" s="140"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="140"/>
+      <c r="G7" s="140"/>
+      <c r="H7" s="140"/>
+      <c r="I7" s="140"/>
+      <c r="J7" s="140"/>
+      <c r="K7" s="140"/>
+      <c r="L7" s="140"/>
+      <c r="M7" s="140"/>
+    </row>
+    <row r="8" spans="1:13" s="143" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="143" t="s">
         <v>584</v>
       </c>
-      <c r="B8" s="143"/>
-      <c r="C8" s="141"/>
-      <c r="D8" s="141"/>
-      <c r="E8" s="141"/>
-      <c r="F8" s="141"/>
-      <c r="G8" s="141"/>
-      <c r="H8" s="141"/>
-      <c r="I8" s="141"/>
-      <c r="J8" s="141"/>
-      <c r="K8" s="141"/>
-      <c r="L8" s="141"/>
-      <c r="M8" s="141"/>
+      <c r="B8" s="142"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="140"/>
+      <c r="E8" s="140"/>
+      <c r="F8" s="140"/>
+      <c r="G8" s="140"/>
+      <c r="H8" s="140"/>
+      <c r="I8" s="140"/>
+      <c r="J8" s="140"/>
+      <c r="K8" s="140"/>
+      <c r="L8" s="140"/>
+      <c r="M8" s="140"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="144" t="s">
+      <c r="A9" s="143" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="144" t="s">
+      <c r="B9" s="143" t="s">
         <v>621</v>
       </c>
-      <c r="C9" s="142" t="s">
+      <c r="C9" s="141" t="s">
         <v>621</v>
       </c>
-      <c r="D9" s="142" t="s">
+      <c r="D9" s="141" t="s">
         <v>621</v>
       </c>
-      <c r="E9" s="142" t="s">
+      <c r="E9" s="141" t="s">
         <v>621</v>
       </c>
-      <c r="F9" s="142" t="s">
+      <c r="F9" s="141" t="s">
         <v>621</v>
       </c>
-      <c r="G9" s="142" t="s">
+      <c r="G9" s="141" t="s">
         <v>581</v>
       </c>
-      <c r="H9" s="142"/>
-      <c r="I9" s="142" t="s">
+      <c r="H9" s="141"/>
+      <c r="I9" s="141" t="s">
         <v>621</v>
       </c>
-      <c r="J9" s="142"/>
-      <c r="K9" s="142"/>
-      <c r="L9" s="142"/>
-      <c r="M9" s="142" t="s">
+      <c r="J9" s="141"/>
+      <c r="K9" s="141"/>
+      <c r="L9" s="141"/>
+      <c r="M9" s="141" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="144" t="s">
+      <c r="A10" s="143" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="144" t="s">
+      <c r="A11" s="143" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="144" t="s">
+      <c r="A12" s="143" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="144" t="s">
+      <c r="A13" s="143" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="144" t="s">
+      <c r="A14" s="143" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="144" t="s">
+      <c r="A15" s="143" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="143" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="144" t="s">
+      <c r="A17" s="143" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="144" t="s">
+      <c r="A18" s="143" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="144" t="s">
+      <c r="A19" s="143" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="144" t="s">
+      <c r="A20" s="143" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="144" t="s">
+      <c r="A21" s="143" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="144" t="s">
+      <c r="A22" s="143" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="144" t="s">
+      <c r="A23" s="143" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="144" t="s">
+      <c r="A24" s="143" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="144" t="s">
+      <c r="A25" s="143" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="145" t="s">
+      <c r="A26" s="144" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="144" t="s">
+      <c r="A27" s="143" t="s">
         <v>596</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="144" t="s">
+      <c r="A28" s="143" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="144" t="s">
+      <c r="A29" s="143" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="144" t="s">
+      <c r="A30" s="143" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="144" t="s">
+      <c r="A31" s="143" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="144" t="s">
+      <c r="A32" s="143" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="144" t="s">
+      <c r="A33" s="143" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="144" t="s">
+      <c r="A34" s="143" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="144" t="s">
+      <c r="A35" s="143" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="146" t="s">
+      <c r="A36" s="145" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="145" t="s">
+      <c r="A37" s="144" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="144" t="s">
+      <c r="A38" s="143" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="144" t="s">
+      <c r="A39" s="143" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="144" t="s">
+      <c r="A40" s="143" t="s">
         <v>608</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="144" t="s">
+      <c r="A41" s="143" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="144" t="s">
+      <c r="A42" s="143" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="144" t="s">
+      <c r="A43" s="143" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="144" t="s">
+      <c r="A44" s="143" t="s">
         <v>612</v>
       </c>
     </row>
@@ -3753,7 +3760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1:O1048576"/>
     </sheetView>
   </sheetViews>
@@ -3980,10 +3987,10 @@
         <v>637</v>
       </c>
       <c r="E13" s="85"/>
-      <c r="F13" s="165" t="s">
+      <c r="F13" s="164" t="s">
         <v>457</v>
       </c>
-      <c r="G13" s="165"/>
+      <c r="G13" s="164"/>
     </row>
     <row r="14" spans="1:7" s="103" customFormat="1" ht="55" x14ac:dyDescent="0.2">
       <c r="A14" s="103" t="s">
@@ -4054,10 +4061,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4082,7 +4089,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="165" t="s">
         <v>535</v>
       </c>
       <c r="B2" t="s">
@@ -4093,7 +4100,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="166" t="s">
         <v>538</v>
       </c>
       <c r="B3" t="s">
@@ -4104,11 +4111,20 @@
       </c>
       <c r="D3" t="s">
         <v>541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="166" t="s">
+        <v>639</v>
+      </c>
+      <c r="B4" t="s">
+        <v>640</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="CryptoPools"/>
+    <hyperlink ref="A4" r:id="rId2" display="Gox"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4126,15 +4142,15 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="92" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="106" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="106" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="106" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="106" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" style="106" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" style="106" customWidth="1"/>
-    <col min="8" max="8" width="69.140625" style="106" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="106" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.7109375" style="106"/>
+    <col min="2" max="2" width="15.5703125" style="105" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="105" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="105" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="105" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" style="105" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="105" customWidth="1"/>
+    <col min="8" max="8" width="69.140625" style="105" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="105" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.7109375" style="105"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="43" customFormat="1" ht="19" x14ac:dyDescent="0.2">
@@ -4167,31 +4183,31 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="105" t="s">
         <v>515</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="105" t="s">
         <v>520</v>
       </c>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="106" t="s">
         <v>521</v>
       </c>
-      <c r="F2" s="106" t="s">
+      <c r="F2" s="105" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="96"/>
-      <c r="B3" s="133" t="s">
+      <c r="B3" s="132" t="s">
         <v>516</v>
       </c>
-      <c r="C3" s="133"/>
-      <c r="D3" s="133"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="132"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="92" t="s">
@@ -4203,16 +4219,16 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="130" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="92" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="139" t="s">
+      <c r="A7" s="138" t="s">
         <v>615</v>
       </c>
-      <c r="D7" s="108" t="s">
+      <c r="D7" s="107" t="s">
         <v>299</v>
       </c>
     </row>
@@ -4225,129 +4241,129 @@
       <c r="A9" s="93" t="s">
         <v>465</v>
       </c>
-      <c r="B9" s="106" t="s">
+      <c r="B9" s="105" t="s">
         <v>193</v>
       </c>
-      <c r="D9" s="108" t="s">
+      <c r="D9" s="107" t="s">
         <v>299</v>
       </c>
-      <c r="F9" s="106" t="s">
+      <c r="F9" s="105" t="s">
         <v>467</v>
       </c>
-      <c r="G9" s="106" t="s">
+      <c r="G9" s="105" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="133" t="s">
+      <c r="B10" s="132" t="s">
         <v>221</v>
       </c>
-      <c r="C10" s="133"/>
-      <c r="D10" s="133"/>
-      <c r="E10" s="134"/>
-      <c r="F10" s="134"/>
-      <c r="G10" s="134"/>
-      <c r="H10" s="134"/>
+      <c r="C10" s="132"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="133"/>
+      <c r="H10" s="133"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="93" t="s">
         <v>464</v>
       </c>
-      <c r="B11" s="106" t="s">
+      <c r="B11" s="105" t="s">
         <v>193</v>
       </c>
-      <c r="D11" s="108" t="s">
+      <c r="D11" s="107" t="s">
         <v>299</v>
       </c>
-      <c r="F11" s="106" t="s">
+      <c r="F11" s="105" t="s">
         <v>466</v>
       </c>
-      <c r="G11" s="106" t="s">
+      <c r="G11" s="105" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="133" t="s">
+      <c r="B12" s="132" t="s">
         <v>221</v>
       </c>
-      <c r="C12" s="133"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="134"/>
-      <c r="G12" s="134"/>
-      <c r="H12" s="134"/>
+      <c r="C12" s="132"/>
+      <c r="D12" s="132"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="133"/>
+      <c r="H12" s="133"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="106" t="s">
+      <c r="B13" s="105" t="s">
         <v>193</v>
       </c>
-      <c r="D13" s="108" t="s">
+      <c r="D13" s="107" t="s">
         <v>299</v>
       </c>
-      <c r="F13" s="106" t="s">
+      <c r="F13" s="105" t="s">
         <v>194</v>
       </c>
-      <c r="G13" s="106" t="s">
+      <c r="G13" s="105" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="133" t="s">
+      <c r="B14" s="132" t="s">
         <v>221</v>
       </c>
-      <c r="C14" s="133"/>
-      <c r="D14" s="133"/>
-      <c r="E14" s="134"/>
-      <c r="F14" s="134"/>
-      <c r="G14" s="134"/>
-      <c r="H14" s="134"/>
+      <c r="C14" s="132"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="133"/>
+      <c r="H14" s="133"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="92" t="s">
         <v>260</v>
       </c>
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="105" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="106" t="s">
+      <c r="F15" s="105" t="s">
         <v>261</v>
       </c>
-      <c r="G15" s="106" t="s">
+      <c r="G15" s="105" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="133" t="s">
+      <c r="B16" s="132" t="s">
         <v>201</v>
       </c>
-      <c r="C16" s="133"/>
-      <c r="D16" s="133"/>
-      <c r="E16" s="134"/>
-      <c r="F16" s="134"/>
-      <c r="G16" s="134"/>
-      <c r="H16" s="134"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
+      <c r="G16" s="133"/>
+      <c r="H16" s="133"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="94" t="s">
         <v>310</v>
       </c>
-      <c r="B17" s="106" t="s">
+      <c r="B17" s="105" t="s">
         <v>142</v>
       </c>
-      <c r="D17" s="108" t="s">
+      <c r="D17" s="107" t="s">
         <v>311</v>
       </c>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109" t="s">
+      <c r="E17" s="108"/>
+      <c r="F17" s="108" t="s">
         <v>312</v>
       </c>
-      <c r="G17" s="106" t="s">
+      <c r="G17" s="105" t="s">
         <v>263</v>
       </c>
-      <c r="H17" s="109" t="s">
+      <c r="H17" s="108" t="s">
         <v>313</v>
       </c>
     </row>
@@ -4355,37 +4371,37 @@
       <c r="A18" s="95" t="s">
         <v>110</v>
       </c>
-      <c r="B18" s="106" t="s">
+      <c r="B18" s="105" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="109"/>
-      <c r="F18" s="106" t="s">
+      <c r="E18" s="108"/>
+      <c r="F18" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="106" t="s">
+      <c r="G18" s="105" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="133" t="s">
+      <c r="B19" s="132" t="s">
         <v>133</v>
       </c>
-      <c r="C19" s="133"/>
-      <c r="D19" s="133"/>
-      <c r="E19" s="133"/>
-      <c r="F19" s="134"/>
-      <c r="G19" s="134"/>
-      <c r="H19" s="134"/>
-      <c r="I19" s="134"/>
+      <c r="C19" s="132"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="132"/>
+      <c r="F19" s="133"/>
+      <c r="G19" s="133"/>
+      <c r="H19" s="133"/>
+      <c r="I19" s="133"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="92" t="s">
         <v>141</v>
       </c>
-      <c r="B20" s="106" t="s">
+      <c r="B20" s="105" t="s">
         <v>532</v>
       </c>
-      <c r="D20" s="108" t="s">
+      <c r="D20" s="107" t="s">
         <v>291</v>
       </c>
       <c r="F20" s="104" t="s">
@@ -4396,13 +4412,13 @@
       <c r="A21" s="92" t="s">
         <v>537</v>
       </c>
-      <c r="B21" s="106" t="s">
+      <c r="B21" s="105" t="s">
         <v>532</v>
       </c>
-      <c r="D21" s="108" t="s">
+      <c r="D21" s="107" t="s">
         <v>291</v>
       </c>
-      <c r="F21" s="106" t="s">
+      <c r="F21" s="105" t="s">
         <v>530</v>
       </c>
     </row>
@@ -4410,13 +4426,13 @@
       <c r="A22" s="92" t="s">
         <v>529</v>
       </c>
-      <c r="B22" s="106" t="s">
+      <c r="B22" s="105" t="s">
         <v>142</v>
       </c>
-      <c r="D22" s="108" t="s">
+      <c r="D22" s="107" t="s">
         <v>291</v>
       </c>
-      <c r="F22" s="106" t="s">
+      <c r="F22" s="105" t="s">
         <v>527</v>
       </c>
     </row>
@@ -4424,16 +4440,16 @@
       <c r="A23" s="92" t="s">
         <v>205</v>
       </c>
-      <c r="B23" s="106" t="s">
+      <c r="B23" s="105" t="s">
         <v>142</v>
       </c>
-      <c r="D23" s="108" t="s">
+      <c r="D23" s="107" t="s">
         <v>291</v>
       </c>
-      <c r="F23" s="106" t="s">
+      <c r="F23" s="105" t="s">
         <v>206</v>
       </c>
-      <c r="H23" s="109" t="s">
+      <c r="H23" s="108" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4451,13 +4467,13 @@
       <c r="A26" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="106" t="s">
+      <c r="B26" s="105" t="s">
         <v>127</v>
       </c>
-      <c r="F26" s="106" t="s">
+      <c r="F26" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="H26" s="106" t="s">
+      <c r="H26" s="105" t="s">
         <v>75</v>
       </c>
     </row>
@@ -4475,213 +4491,213 @@
       <c r="A29" s="95" t="s">
         <v>286</v>
       </c>
-      <c r="B29" s="106" t="s">
+      <c r="B29" s="105" t="s">
         <v>226</v>
       </c>
-      <c r="C29" s="106" t="s">
+      <c r="C29" s="105" t="s">
         <v>211</v>
       </c>
-      <c r="F29" s="106" t="s">
+      <c r="F29" s="105" t="s">
         <v>268</v>
       </c>
-      <c r="G29" s="106" t="s">
+      <c r="G29" s="105" t="s">
         <v>263</v>
       </c>
-      <c r="H29" s="110"/>
-      <c r="I29" s="111"/>
+      <c r="H29" s="109"/>
+      <c r="I29" s="110"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="96"/>
-      <c r="B30" s="135" t="s">
+      <c r="B30" s="134" t="s">
         <v>269</v>
       </c>
-      <c r="C30" s="135"/>
-      <c r="D30" s="135"/>
-      <c r="E30" s="135"/>
-      <c r="F30" s="134"/>
-      <c r="G30" s="134"/>
-      <c r="H30" s="134"/>
-      <c r="I30" s="134"/>
+      <c r="C30" s="134"/>
+      <c r="D30" s="134"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="133"/>
+      <c r="G30" s="133"/>
+      <c r="H30" s="133"/>
+      <c r="I30" s="133"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="106" t="s">
+      <c r="B31" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="C31" s="106" t="s">
+      <c r="C31" s="105" t="s">
         <v>191</v>
       </c>
-      <c r="F31" s="106" t="s">
+      <c r="F31" s="105" t="s">
         <v>72</v>
       </c>
-      <c r="G31" s="106" t="s">
+      <c r="G31" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="H31" s="110"/>
-      <c r="I31" s="111"/>
+      <c r="H31" s="109"/>
+      <c r="I31" s="110"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="96"/>
-      <c r="B32" s="135" t="s">
+      <c r="B32" s="134" t="s">
         <v>506</v>
       </c>
-      <c r="C32" s="135"/>
-      <c r="D32" s="135"/>
-      <c r="E32" s="135"/>
-      <c r="F32" s="134"/>
-      <c r="G32" s="134"/>
-      <c r="H32" s="134"/>
-      <c r="I32" s="134"/>
+      <c r="C32" s="134"/>
+      <c r="D32" s="134"/>
+      <c r="E32" s="134"/>
+      <c r="F32" s="133"/>
+      <c r="G32" s="133"/>
+      <c r="H32" s="133"/>
+      <c r="I32" s="133"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="95" t="s">
         <v>223</v>
       </c>
-      <c r="B33" s="106" t="s">
+      <c r="B33" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="C33" s="106" t="s">
+      <c r="C33" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="F33" s="112" t="s">
+      <c r="F33" s="111" t="s">
         <v>245</v>
       </c>
-      <c r="G33" s="106" t="s">
+      <c r="G33" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="H33" s="110" t="s">
+      <c r="H33" s="109" t="s">
         <v>224</v>
       </c>
-      <c r="I33" s="111"/>
+      <c r="I33" s="110"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="96"/>
-      <c r="B34" s="135" t="s">
+      <c r="B34" s="134" t="s">
         <v>246</v>
       </c>
-      <c r="C34" s="135"/>
-      <c r="D34" s="135"/>
-      <c r="E34" s="135"/>
-      <c r="F34" s="134"/>
-      <c r="G34" s="134"/>
-      <c r="H34" s="134"/>
-      <c r="I34" s="134"/>
+      <c r="C34" s="134"/>
+      <c r="D34" s="134"/>
+      <c r="E34" s="134"/>
+      <c r="F34" s="133"/>
+      <c r="G34" s="133"/>
+      <c r="H34" s="133"/>
+      <c r="I34" s="133"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="96" t="s">
         <v>247</v>
       </c>
-      <c r="B35" s="106" t="s">
+      <c r="B35" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="106" t="s">
+      <c r="F35" s="105" t="s">
         <v>249</v>
       </c>
-      <c r="G35" s="106" t="s">
+      <c r="G35" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="H35" s="106" t="s">
+      <c r="H35" s="105" t="s">
         <v>229</v>
       </c>
-      <c r="I35" s="110"/>
+      <c r="I35" s="109"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="96"/>
-      <c r="B36" s="133" t="s">
+      <c r="B36" s="132" t="s">
         <v>248</v>
       </c>
-      <c r="C36" s="133"/>
-      <c r="D36" s="133"/>
-      <c r="E36" s="133"/>
-      <c r="F36" s="134"/>
-      <c r="G36" s="134"/>
-      <c r="H36" s="134"/>
-      <c r="I36" s="110"/>
+      <c r="C36" s="132"/>
+      <c r="D36" s="132"/>
+      <c r="E36" s="132"/>
+      <c r="F36" s="133"/>
+      <c r="G36" s="133"/>
+      <c r="H36" s="133"/>
+      <c r="I36" s="109"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="106" t="s">
+      <c r="A37" s="105" t="s">
         <v>270</v>
       </c>
-      <c r="B37" s="106" t="s">
+      <c r="B37" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="F37" s="106" t="s">
+      <c r="F37" s="105" t="s">
         <v>171</v>
       </c>
-      <c r="G37" s="106" t="s">
+      <c r="G37" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="H37" s="110"/>
-      <c r="I37" s="111"/>
+      <c r="H37" s="109"/>
+      <c r="I37" s="110"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="96"/>
-      <c r="B38" s="135" t="s">
+      <c r="B38" s="134" t="s">
         <v>170</v>
       </c>
-      <c r="C38" s="135"/>
-      <c r="D38" s="135"/>
-      <c r="E38" s="135"/>
-      <c r="F38" s="134"/>
-      <c r="G38" s="134"/>
-      <c r="H38" s="134"/>
-      <c r="I38" s="134"/>
+      <c r="C38" s="134"/>
+      <c r="D38" s="134"/>
+      <c r="E38" s="134"/>
+      <c r="F38" s="133"/>
+      <c r="G38" s="133"/>
+      <c r="H38" s="133"/>
+      <c r="I38" s="133"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="106" t="s">
+      <c r="B39" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="F39" s="106" t="s">
+      <c r="F39" s="105" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="96"/>
-      <c r="B40" s="133" t="s">
+      <c r="B40" s="132" t="s">
         <v>507</v>
       </c>
-      <c r="C40" s="133"/>
-      <c r="D40" s="133"/>
-      <c r="E40" s="133"/>
-      <c r="F40" s="134"/>
-      <c r="G40" s="134"/>
-      <c r="H40" s="134"/>
+      <c r="C40" s="132"/>
+      <c r="D40" s="132"/>
+      <c r="E40" s="132"/>
+      <c r="F40" s="133"/>
+      <c r="G40" s="133"/>
+      <c r="H40" s="133"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="106" t="s">
+      <c r="A41" s="105" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="106" t="s">
+      <c r="A42" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="106" t="s">
+      <c r="B42" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="F42" s="106" t="s">
+      <c r="F42" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="G42" s="106" t="s">
+      <c r="G42" s="105" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="96"/>
-      <c r="B43" s="133" t="s">
+      <c r="B43" s="132" t="s">
         <v>507</v>
       </c>
-      <c r="C43" s="133"/>
-      <c r="D43" s="133"/>
-      <c r="E43" s="133"/>
-      <c r="F43" s="134"/>
-      <c r="G43" s="134"/>
-      <c r="H43" s="134"/>
+      <c r="C43" s="132"/>
+      <c r="D43" s="132"/>
+      <c r="E43" s="132"/>
+      <c r="F43" s="133"/>
+      <c r="G43" s="133"/>
+      <c r="H43" s="133"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="96" t="s">
@@ -4689,7 +4705,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="106" t="s">
+      <c r="A45" s="105" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4699,117 +4715,117 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="106" t="s">
+      <c r="A47" s="105" t="s">
         <v>188</v>
       </c>
-      <c r="B47" s="113"/>
-      <c r="C47" s="113"/>
-      <c r="D47" s="113"/>
-      <c r="E47" s="114"/>
-      <c r="F47" s="115"/>
-      <c r="G47" s="113"/>
+      <c r="B47" s="112"/>
+      <c r="C47" s="112"/>
+      <c r="D47" s="112"/>
+      <c r="E47" s="113"/>
+      <c r="F47" s="114"/>
+      <c r="G47" s="112"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="106" t="s">
+      <c r="A48" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="B48" s="106" t="s">
+      <c r="B48" s="105" t="s">
         <v>142</v>
       </c>
-      <c r="D48" s="108" t="s">
+      <c r="D48" s="107" t="s">
         <v>291</v>
       </c>
-      <c r="F48" s="113" t="s">
+      <c r="F48" s="112" t="s">
         <v>125</v>
       </c>
-      <c r="H48" s="106" t="s">
+      <c r="H48" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="I48" s="110"/>
+      <c r="I48" s="109"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="96"/>
-      <c r="B49" s="135" t="s">
+      <c r="B49" s="134" t="s">
         <v>213</v>
       </c>
-      <c r="C49" s="135"/>
-      <c r="D49" s="135"/>
-      <c r="E49" s="135"/>
-      <c r="F49" s="134"/>
-      <c r="G49" s="134"/>
-      <c r="H49" s="134"/>
-      <c r="I49" s="110"/>
+      <c r="C49" s="134"/>
+      <c r="D49" s="134"/>
+      <c r="E49" s="134"/>
+      <c r="F49" s="133"/>
+      <c r="G49" s="133"/>
+      <c r="H49" s="133"/>
+      <c r="I49" s="109"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="B50" s="106" t="s">
+      <c r="B50" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="D50" s="108" t="s">
+      <c r="D50" s="107" t="s">
         <v>291</v>
       </c>
-      <c r="F50" s="106" t="s">
+      <c r="F50" s="105" t="s">
         <v>122</v>
       </c>
-      <c r="G50" s="106" t="s">
+      <c r="G50" s="105" t="s">
         <v>123</v>
       </c>
-      <c r="I50" s="110"/>
+      <c r="I50" s="109"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="96"/>
-      <c r="B51" s="135" t="s">
+      <c r="B51" s="134" t="s">
         <v>508</v>
       </c>
-      <c r="C51" s="135"/>
-      <c r="D51" s="135"/>
-      <c r="E51" s="135"/>
-      <c r="F51" s="134"/>
-      <c r="G51" s="134"/>
-      <c r="H51" s="134"/>
-      <c r="I51" s="134"/>
+      <c r="C51" s="134"/>
+      <c r="D51" s="134"/>
+      <c r="E51" s="134"/>
+      <c r="F51" s="133"/>
+      <c r="G51" s="133"/>
+      <c r="H51" s="133"/>
+      <c r="I51" s="133"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="106" t="s">
+      <c r="B52" s="105" t="s">
         <v>114</v>
       </c>
-      <c r="F52" s="106" t="s">
+      <c r="F52" s="105" t="s">
         <v>115</v>
       </c>
-      <c r="G52" s="106" t="s">
+      <c r="G52" s="105" t="s">
         <v>116</v>
       </c>
-      <c r="H52" s="106" t="s">
+      <c r="H52" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="I52" s="110"/>
+      <c r="I52" s="109"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="96"/>
-      <c r="B53" s="133" t="s">
+      <c r="B53" s="132" t="s">
         <v>509</v>
       </c>
-      <c r="C53" s="133"/>
-      <c r="D53" s="133"/>
-      <c r="E53" s="133"/>
-      <c r="F53" s="134"/>
-      <c r="G53" s="134"/>
-      <c r="H53" s="134"/>
-      <c r="I53" s="110"/>
+      <c r="C53" s="132"/>
+      <c r="D53" s="132"/>
+      <c r="E53" s="132"/>
+      <c r="F53" s="133"/>
+      <c r="G53" s="133"/>
+      <c r="H53" s="133"/>
+      <c r="I53" s="109"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A54" s="106" t="s">
+      <c r="A54" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="S54" s="116"/>
+      <c r="S54" s="115"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A55" s="106" t="s">
+      <c r="A55" s="105" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4817,74 +4833,74 @@
       <c r="A56" s="96" t="s">
         <v>272</v>
       </c>
-      <c r="B56" s="106" t="s">
+      <c r="B56" s="105" t="s">
         <v>89</v>
       </c>
-      <c r="F56" s="106" t="s">
+      <c r="F56" s="105" t="s">
         <v>225</v>
       </c>
-      <c r="G56" s="117" t="s">
+      <c r="G56" s="116" t="s">
         <v>265</v>
       </c>
-      <c r="H56" s="106" t="s">
+      <c r="H56" s="105" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" s="96"/>
-      <c r="B57" s="133" t="s">
+      <c r="B57" s="132" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="133"/>
-      <c r="D57" s="133"/>
-      <c r="E57" s="133"/>
-      <c r="F57" s="134"/>
-      <c r="G57" s="134"/>
-      <c r="H57" s="134"/>
+      <c r="C57" s="132"/>
+      <c r="D57" s="132"/>
+      <c r="E57" s="132"/>
+      <c r="F57" s="133"/>
+      <c r="G57" s="133"/>
+      <c r="H57" s="133"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A58" s="106" t="s">
+      <c r="A58" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="B58" s="106" t="s">
+      <c r="B58" s="105" t="s">
         <v>139</v>
       </c>
-      <c r="F58" s="106" t="s">
+      <c r="F58" s="105" t="s">
         <v>271</v>
       </c>
-      <c r="G58" s="117" t="s">
+      <c r="G58" s="116" t="s">
         <v>265</v>
       </c>
-      <c r="H58" s="106" t="s">
+      <c r="H58" s="105" t="s">
         <v>88</v>
       </c>
-      <c r="I58" s="110"/>
+      <c r="I58" s="109"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" s="96" t="s">
         <v>210</v>
       </c>
-      <c r="B59" s="106" t="s">
+      <c r="B59" s="105" t="s">
         <v>89</v>
       </c>
-      <c r="F59" s="106" t="s">
+      <c r="F59" s="105" t="s">
         <v>137</v>
       </c>
-      <c r="H59" s="106" t="s">
+      <c r="H59" s="105" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" s="96"/>
-      <c r="B60" s="133" t="s">
+      <c r="B60" s="132" t="s">
         <v>97</v>
       </c>
-      <c r="C60" s="133"/>
-      <c r="D60" s="133"/>
-      <c r="E60" s="133"/>
-      <c r="F60" s="134"/>
-      <c r="G60" s="134"/>
-      <c r="H60" s="134"/>
+      <c r="C60" s="132"/>
+      <c r="D60" s="132"/>
+      <c r="E60" s="132"/>
+      <c r="F60" s="133"/>
+      <c r="G60" s="133"/>
+      <c r="H60" s="133"/>
     </row>
     <row r="61" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A61" s="99" t="s">
@@ -4896,141 +4912,141 @@
       <c r="C61" s="95" t="s">
         <v>191</v>
       </c>
-      <c r="D61" s="118" t="s">
+      <c r="D61" s="117" t="s">
         <v>291</v>
       </c>
       <c r="E61" s="95" t="s">
         <v>257</v>
       </c>
-      <c r="F61" s="106" t="s">
+      <c r="F61" s="105" t="s">
         <v>258</v>
       </c>
-      <c r="H61" s="106" t="s">
+      <c r="H61" s="105" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" s="96"/>
-      <c r="B62" s="136" t="s">
+      <c r="B62" s="135" t="s">
         <v>294</v>
       </c>
-      <c r="C62" s="136"/>
-      <c r="D62" s="136"/>
-      <c r="E62" s="136"/>
-      <c r="F62" s="134"/>
-      <c r="G62" s="134"/>
-      <c r="H62" s="134"/>
-      <c r="I62" s="134"/>
+      <c r="C62" s="135"/>
+      <c r="D62" s="135"/>
+      <c r="E62" s="135"/>
+      <c r="F62" s="133"/>
+      <c r="G62" s="133"/>
+      <c r="H62" s="133"/>
+      <c r="I62" s="133"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A63" s="106" t="s">
+      <c r="A63" s="105" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="96" t="s">
         <v>301</v>
       </c>
-      <c r="B64" s="117" t="s">
+      <c r="B64" s="116" t="s">
         <v>532</v>
       </c>
-      <c r="E64" s="117" t="s">
+      <c r="E64" s="116" t="s">
         <v>299</v>
       </c>
-      <c r="F64" s="117" t="s">
+      <c r="F64" s="116" t="s">
         <v>172</v>
       </c>
-      <c r="G64" s="117" t="s">
+      <c r="G64" s="116" t="s">
         <v>265</v>
       </c>
-      <c r="H64" s="119" t="s">
+      <c r="H64" s="118" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="65" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:19" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="96" t="s">
         <v>298</v>
       </c>
-      <c r="B65" s="117" t="s">
+      <c r="B65" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="F65" s="117" t="s">
+      <c r="F65" s="116" t="s">
         <v>296</v>
       </c>
-      <c r="G65" s="117" t="s">
+      <c r="G65" s="116" t="s">
         <v>265</v>
       </c>
       <c r="H65" s="97"/>
     </row>
-    <row r="66" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:19" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="96"/>
-      <c r="B66" s="137" t="s">
+      <c r="B66" s="136" t="s">
         <v>297</v>
       </c>
-      <c r="C66" s="134"/>
-      <c r="D66" s="134"/>
-      <c r="E66" s="134"/>
-      <c r="F66" s="134"/>
-      <c r="G66" s="134"/>
-      <c r="H66" s="134"/>
-    </row>
-    <row r="67" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C66" s="133"/>
+      <c r="D66" s="133"/>
+      <c r="E66" s="133"/>
+      <c r="F66" s="133"/>
+      <c r="G66" s="133"/>
+      <c r="H66" s="133"/>
+    </row>
+    <row r="67" spans="1:19" s="116" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="96" t="s">
         <v>264</v>
       </c>
-      <c r="B67" s="117" t="s">
+      <c r="B67" s="116" t="s">
         <v>139</v>
       </c>
-      <c r="F67" s="117" t="s">
+      <c r="F67" s="116" t="s">
         <v>266</v>
       </c>
-      <c r="G67" s="117" t="s">
+      <c r="G67" s="116" t="s">
         <v>265</v>
       </c>
       <c r="H67" s="97"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A68" s="106" t="s">
+      <c r="A68" s="105" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:19" s="130" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="126" t="s">
+    <row r="69" spans="1:19" s="129" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="125" t="s">
         <v>625</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A70" s="106" t="s">
+      <c r="A70" s="105" t="s">
         <v>496</v>
       </c>
-      <c r="B70" s="106" t="s">
+      <c r="B70" s="105" t="s">
         <v>532</v>
       </c>
-      <c r="D70" s="106" t="s">
+      <c r="D70" s="105" t="s">
         <v>498</v>
       </c>
-      <c r="F70" s="106" t="s">
+      <c r="F70" s="105" t="s">
         <v>499</v>
       </c>
-      <c r="G70" s="106" t="s">
+      <c r="G70" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="H70" s="106" t="s">
+      <c r="H70" s="105" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71" s="96"/>
-      <c r="B71" s="133" t="s">
+      <c r="B71" s="132" t="s">
         <v>501</v>
       </c>
-      <c r="C71" s="133"/>
-      <c r="D71" s="133"/>
-      <c r="E71" s="133"/>
-      <c r="F71" s="134"/>
-      <c r="G71" s="134"/>
-      <c r="H71" s="134"/>
-      <c r="I71" s="110" t="s">
+      <c r="C71" s="132"/>
+      <c r="D71" s="132"/>
+      <c r="E71" s="132"/>
+      <c r="F71" s="133"/>
+      <c r="G71" s="133"/>
+      <c r="H71" s="133"/>
+      <c r="I71" s="109" t="s">
         <v>134</v>
       </c>
     </row>
@@ -5038,29 +5054,29 @@
       <c r="A72" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="B72" s="106" t="s">
+      <c r="B72" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="F72" s="106" t="s">
+      <c r="F72" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="G72" s="106" t="s">
+      <c r="G72" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="I72" s="110"/>
+      <c r="I72" s="109"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73" s="96"/>
-      <c r="B73" s="133" t="s">
+      <c r="B73" s="132" t="s">
         <v>510</v>
       </c>
-      <c r="C73" s="133"/>
-      <c r="D73" s="133"/>
-      <c r="E73" s="133"/>
-      <c r="F73" s="134"/>
-      <c r="G73" s="134"/>
-      <c r="H73" s="134"/>
-      <c r="I73" s="110" t="s">
+      <c r="C73" s="132"/>
+      <c r="D73" s="132"/>
+      <c r="E73" s="132"/>
+      <c r="F73" s="133"/>
+      <c r="G73" s="133"/>
+      <c r="H73" s="133"/>
+      <c r="I73" s="109" t="s">
         <v>134</v>
       </c>
     </row>
@@ -5078,41 +5094,41 @@
       <c r="A76" s="98" t="s">
         <v>548</v>
       </c>
-      <c r="B76" s="120" t="s">
+      <c r="B76" s="119" t="s">
         <v>546</v>
       </c>
-      <c r="C76" s="121"/>
-      <c r="D76" s="127" t="s">
+      <c r="C76" s="120"/>
+      <c r="D76" s="126" t="s">
         <v>547</v>
       </c>
-      <c r="E76" s="121"/>
-      <c r="F76" s="121"/>
-      <c r="G76" s="121"/>
-      <c r="H76" s="121" t="s">
+      <c r="E76" s="120"/>
+      <c r="F76" s="120"/>
+      <c r="G76" s="120"/>
+      <c r="H76" s="120" t="s">
         <v>229</v>
       </c>
-      <c r="I76" s="121"/>
-      <c r="J76" s="121"/>
-      <c r="K76" s="121"/>
-      <c r="L76" s="121"/>
-      <c r="M76" s="121"/>
-      <c r="N76" s="121"/>
-      <c r="O76" s="121"/>
-      <c r="P76" s="121"/>
-      <c r="Q76" s="121"/>
-      <c r="R76" s="121"/>
-      <c r="S76" s="121"/>
+      <c r="I76" s="120"/>
+      <c r="J76" s="120"/>
+      <c r="K76" s="120"/>
+      <c r="L76" s="120"/>
+      <c r="M76" s="120"/>
+      <c r="N76" s="120"/>
+      <c r="O76" s="120"/>
+      <c r="P76" s="120"/>
+      <c r="Q76" s="120"/>
+      <c r="R76" s="120"/>
+      <c r="S76" s="120"/>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A77" s="96"/>
-      <c r="B77" s="133"/>
-      <c r="C77" s="133"/>
-      <c r="D77" s="133"/>
-      <c r="E77" s="133"/>
-      <c r="F77" s="134"/>
-      <c r="G77" s="134"/>
-      <c r="H77" s="134"/>
-      <c r="I77" s="110" t="s">
+      <c r="B77" s="132"/>
+      <c r="C77" s="132"/>
+      <c r="D77" s="132"/>
+      <c r="E77" s="132"/>
+      <c r="F77" s="133"/>
+      <c r="G77" s="133"/>
+      <c r="H77" s="133"/>
+      <c r="I77" s="109" t="s">
         <v>134</v>
       </c>
     </row>
@@ -5120,111 +5136,111 @@
       <c r="A78" s="98" t="s">
         <v>549</v>
       </c>
-      <c r="B78" s="106" t="s">
+      <c r="B78" s="105" t="s">
         <v>176</v>
       </c>
-      <c r="C78" s="121"/>
-      <c r="D78" s="121" t="s">
+      <c r="C78" s="120"/>
+      <c r="D78" s="120" t="s">
         <v>299</v>
       </c>
-      <c r="E78" s="121"/>
-      <c r="F78" s="121" t="s">
+      <c r="E78" s="120"/>
+      <c r="F78" s="120" t="s">
         <v>556</v>
       </c>
-      <c r="G78" s="121"/>
-      <c r="H78" s="121" t="s">
+      <c r="G78" s="120"/>
+      <c r="H78" s="120" t="s">
         <v>229</v>
       </c>
-      <c r="I78" s="121"/>
-      <c r="J78" s="121"/>
-      <c r="K78" s="121"/>
-      <c r="L78" s="121"/>
-      <c r="M78" s="121"/>
-      <c r="N78" s="121"/>
-      <c r="O78" s="121"/>
-      <c r="P78" s="121"/>
-      <c r="Q78" s="121"/>
-      <c r="R78" s="121"/>
-      <c r="S78" s="121"/>
+      <c r="I78" s="120"/>
+      <c r="J78" s="120"/>
+      <c r="K78" s="120"/>
+      <c r="L78" s="120"/>
+      <c r="M78" s="120"/>
+      <c r="N78" s="120"/>
+      <c r="O78" s="120"/>
+      <c r="P78" s="120"/>
+      <c r="Q78" s="120"/>
+      <c r="R78" s="120"/>
+      <c r="S78" s="120"/>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79" s="98" t="s">
         <v>550</v>
       </c>
-      <c r="B79" s="130" t="s">
+      <c r="B79" s="129" t="s">
         <v>182</v>
       </c>
-      <c r="C79" s="121" t="s">
+      <c r="C79" s="120" t="s">
         <v>144</v>
       </c>
-      <c r="D79" s="121" t="s">
+      <c r="D79" s="120" t="s">
         <v>545</v>
       </c>
-      <c r="E79" s="121"/>
-      <c r="F79" s="121" t="s">
+      <c r="E79" s="120"/>
+      <c r="F79" s="120" t="s">
         <v>227</v>
       </c>
-      <c r="G79" s="121"/>
-      <c r="H79" s="121" t="s">
+      <c r="G79" s="120"/>
+      <c r="H79" s="120" t="s">
         <v>229</v>
       </c>
-      <c r="I79" s="121"/>
-      <c r="J79" s="121"/>
-      <c r="K79" s="121"/>
-      <c r="L79" s="121"/>
-      <c r="M79" s="121"/>
-      <c r="N79" s="121"/>
-      <c r="O79" s="121"/>
-      <c r="P79" s="121"/>
-      <c r="Q79" s="121"/>
-      <c r="R79" s="121"/>
-      <c r="S79" s="121"/>
-    </row>
-    <row r="80" spans="1:19" s="130" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I79" s="120"/>
+      <c r="J79" s="120"/>
+      <c r="K79" s="120"/>
+      <c r="L79" s="120"/>
+      <c r="M79" s="120"/>
+      <c r="N79" s="120"/>
+      <c r="O79" s="120"/>
+      <c r="P79" s="120"/>
+      <c r="Q79" s="120"/>
+      <c r="R79" s="120"/>
+      <c r="S79" s="120"/>
+    </row>
+    <row r="80" spans="1:19" s="129" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="98" t="s">
         <v>550</v>
       </c>
-      <c r="B80" s="120" t="s">
+      <c r="B80" s="119" t="s">
         <v>226</v>
       </c>
-      <c r="C80" s="121" t="s">
+      <c r="C80" s="120" t="s">
         <v>191</v>
       </c>
-      <c r="D80" s="121" t="s">
+      <c r="D80" s="120" t="s">
         <v>545</v>
       </c>
-      <c r="E80" s="121"/>
-      <c r="F80" s="121" t="s">
+      <c r="E80" s="120"/>
+      <c r="F80" s="120" t="s">
         <v>227</v>
       </c>
-      <c r="G80" s="121"/>
-      <c r="H80" s="121" t="s">
+      <c r="G80" s="120"/>
+      <c r="H80" s="120" t="s">
         <v>229</v>
       </c>
-      <c r="I80" s="121"/>
-      <c r="J80" s="121"/>
-      <c r="K80" s="121"/>
-      <c r="L80" s="121"/>
-      <c r="M80" s="121"/>
-      <c r="N80" s="121"/>
-      <c r="O80" s="121"/>
-      <c r="P80" s="121"/>
-      <c r="Q80" s="121"/>
-      <c r="R80" s="121"/>
-      <c r="S80" s="121"/>
+      <c r="I80" s="120"/>
+      <c r="J80" s="120"/>
+      <c r="K80" s="120"/>
+      <c r="L80" s="120"/>
+      <c r="M80" s="120"/>
+      <c r="N80" s="120"/>
+      <c r="O80" s="120"/>
+      <c r="P80" s="120"/>
+      <c r="Q80" s="120"/>
+      <c r="R80" s="120"/>
+      <c r="S80" s="120"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81" s="96"/>
-      <c r="B81" s="133" t="s">
+      <c r="B81" s="132" t="s">
         <v>564</v>
       </c>
-      <c r="C81" s="133"/>
-      <c r="D81" s="133"/>
-      <c r="E81" s="133"/>
-      <c r="F81" s="134"/>
-      <c r="G81" s="134"/>
-      <c r="H81" s="134"/>
-      <c r="I81" s="110" t="s">
+      <c r="C81" s="132"/>
+      <c r="D81" s="132"/>
+      <c r="E81" s="132"/>
+      <c r="F81" s="133"/>
+      <c r="G81" s="133"/>
+      <c r="H81" s="133"/>
+      <c r="I81" s="109" t="s">
         <v>134</v>
       </c>
     </row>
@@ -5232,50 +5248,50 @@
       <c r="A82" s="98" t="s">
         <v>551</v>
       </c>
-      <c r="B82" s="120" t="s">
+      <c r="B82" s="119" t="s">
         <v>532</v>
       </c>
-      <c r="C82" s="121"/>
-      <c r="D82" s="121" t="s">
+      <c r="C82" s="120"/>
+      <c r="D82" s="120" t="s">
         <v>498</v>
       </c>
-      <c r="E82" s="121"/>
-      <c r="F82" s="121" t="s">
+      <c r="E82" s="120"/>
+      <c r="F82" s="120" t="s">
         <v>563</v>
       </c>
-      <c r="G82" s="121"/>
-      <c r="H82" s="121" t="s">
+      <c r="G82" s="120"/>
+      <c r="H82" s="120" t="s">
         <v>229</v>
       </c>
-      <c r="I82" s="121"/>
-      <c r="J82" s="121"/>
-      <c r="K82" s="121"/>
-      <c r="L82" s="121"/>
-      <c r="M82" s="121"/>
-      <c r="N82" s="121"/>
-      <c r="O82" s="121"/>
-      <c r="P82" s="121"/>
-      <c r="Q82" s="121"/>
-      <c r="R82" s="121"/>
-      <c r="S82" s="121"/>
+      <c r="I82" s="120"/>
+      <c r="J82" s="120"/>
+      <c r="K82" s="120"/>
+      <c r="L82" s="120"/>
+      <c r="M82" s="120"/>
+      <c r="N82" s="120"/>
+      <c r="O82" s="120"/>
+      <c r="P82" s="120"/>
+      <c r="Q82" s="120"/>
+      <c r="R82" s="120"/>
+      <c r="S82" s="120"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83" s="96"/>
-      <c r="B83" s="133" t="s">
+      <c r="B83" s="132" t="s">
         <v>562</v>
       </c>
-      <c r="C83" s="133"/>
-      <c r="D83" s="133"/>
-      <c r="E83" s="133"/>
-      <c r="F83" s="133"/>
-      <c r="G83" s="133"/>
-      <c r="H83" s="133"/>
-      <c r="I83" s="110" t="s">
+      <c r="C83" s="132"/>
+      <c r="D83" s="132"/>
+      <c r="E83" s="132"/>
+      <c r="F83" s="132"/>
+      <c r="G83" s="132"/>
+      <c r="H83" s="132"/>
+      <c r="I83" s="109" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A84" s="106" t="s">
+      <c r="A84" s="105" t="s">
         <v>51</v>
       </c>
     </row>
@@ -5293,34 +5309,34 @@
       <c r="A87" s="95" t="s">
         <v>287</v>
       </c>
-      <c r="B87" s="106" t="s">
+      <c r="B87" s="105" t="s">
         <v>532</v>
       </c>
-      <c r="C87" s="106" t="s">
+      <c r="C87" s="105" t="s">
         <v>191</v>
       </c>
-      <c r="D87" s="106" t="s">
+      <c r="D87" s="105" t="s">
         <v>292</v>
       </c>
-      <c r="F87" s="109" t="s">
+      <c r="F87" s="108" t="s">
         <v>288</v>
       </c>
-      <c r="H87" s="122" t="s">
+      <c r="H87" s="121" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88" s="96"/>
-      <c r="B88" s="133" t="s">
+      <c r="B88" s="132" t="s">
         <v>290</v>
       </c>
-      <c r="C88" s="133"/>
-      <c r="D88" s="133"/>
-      <c r="E88" s="133"/>
-      <c r="F88" s="134"/>
-      <c r="G88" s="134"/>
-      <c r="H88" s="134"/>
-      <c r="I88" s="110" t="s">
+      <c r="C88" s="132"/>
+      <c r="D88" s="132"/>
+      <c r="E88" s="132"/>
+      <c r="F88" s="133"/>
+      <c r="G88" s="133"/>
+      <c r="H88" s="133"/>
+      <c r="I88" s="109" t="s">
         <v>134</v>
       </c>
     </row>
@@ -5328,118 +5344,118 @@
       <c r="A89" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="B89" s="106" t="s">
+      <c r="B89" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="F89" s="106" t="s">
+      <c r="F89" s="105" t="s">
         <v>72</v>
       </c>
-      <c r="G89" s="106" t="s">
+      <c r="G89" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="H89" s="106" t="s">
+      <c r="H89" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="I89" s="110"/>
+      <c r="I89" s="109"/>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90" s="96"/>
-      <c r="B90" s="133" t="s">
+      <c r="B90" s="132" t="s">
         <v>511</v>
       </c>
-      <c r="C90" s="133"/>
-      <c r="D90" s="133"/>
-      <c r="E90" s="133"/>
-      <c r="F90" s="134"/>
-      <c r="G90" s="134"/>
-      <c r="H90" s="134"/>
-      <c r="I90" s="110"/>
+      <c r="C90" s="132"/>
+      <c r="D90" s="132"/>
+      <c r="E90" s="132"/>
+      <c r="F90" s="133"/>
+      <c r="G90" s="133"/>
+      <c r="H90" s="133"/>
+      <c r="I90" s="109"/>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91" s="96" t="s">
         <v>222</v>
       </c>
-      <c r="B91" s="106" t="s">
+      <c r="B91" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="F91" s="106" t="s">
+      <c r="F91" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="G91" s="106" t="s">
+      <c r="G91" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="I91" s="110"/>
+      <c r="I91" s="109"/>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A92" s="96"/>
-      <c r="B92" s="133" t="s">
+      <c r="B92" s="132" t="s">
         <v>82</v>
       </c>
-      <c r="C92" s="133"/>
-      <c r="D92" s="133"/>
-      <c r="E92" s="133"/>
-      <c r="F92" s="134"/>
-      <c r="G92" s="134"/>
-      <c r="H92" s="134"/>
-      <c r="I92" s="110"/>
+      <c r="C92" s="132"/>
+      <c r="D92" s="132"/>
+      <c r="E92" s="132"/>
+      <c r="F92" s="133"/>
+      <c r="G92" s="133"/>
+      <c r="H92" s="133"/>
+      <c r="I92" s="109"/>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A93" s="106" t="s">
+      <c r="A93" s="105" t="s">
         <v>254</v>
       </c>
-      <c r="B93" s="106" t="s">
+      <c r="B93" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="F93" s="106" t="s">
+      <c r="F93" s="105" t="s">
         <v>252</v>
       </c>
-      <c r="H93" s="106" t="s">
+      <c r="H93" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="I93" s="110"/>
+      <c r="I93" s="109"/>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94" s="96"/>
-      <c r="B94" s="133" t="s">
+      <c r="B94" s="132" t="s">
         <v>253</v>
       </c>
-      <c r="C94" s="133"/>
-      <c r="D94" s="133"/>
-      <c r="E94" s="133"/>
-      <c r="F94" s="134"/>
-      <c r="G94" s="134"/>
-      <c r="H94" s="134"/>
-      <c r="I94" s="110" t="s">
+      <c r="C94" s="132"/>
+      <c r="D94" s="132"/>
+      <c r="E94" s="132"/>
+      <c r="F94" s="133"/>
+      <c r="G94" s="133"/>
+      <c r="H94" s="133"/>
+      <c r="I94" s="109" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A95" s="106" t="s">
+      <c r="A95" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="B95" s="106" t="s">
+      <c r="B95" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="F95" s="106" t="s">
+      <c r="F95" s="105" t="s">
         <v>255</v>
       </c>
-      <c r="H95" s="106" t="s">
+      <c r="H95" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="I95" s="110"/>
+      <c r="I95" s="109"/>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A96" s="96"/>
-      <c r="B96" s="133" t="s">
+      <c r="B96" s="132" t="s">
         <v>93</v>
       </c>
-      <c r="C96" s="133"/>
-      <c r="D96" s="133"/>
-      <c r="E96" s="133"/>
-      <c r="F96" s="134"/>
-      <c r="G96" s="134"/>
-      <c r="H96" s="134"/>
-      <c r="I96" s="110" t="s">
+      <c r="C96" s="132"/>
+      <c r="D96" s="132"/>
+      <c r="E96" s="132"/>
+      <c r="F96" s="133"/>
+      <c r="G96" s="133"/>
+      <c r="H96" s="133"/>
+      <c r="I96" s="109" t="s">
         <v>134</v>
       </c>
     </row>
@@ -5447,37 +5463,37 @@
       <c r="A97" s="96" t="s">
         <v>189</v>
       </c>
-      <c r="B97" s="110" t="s">
+      <c r="B97" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="C97" s="110"/>
-      <c r="D97" s="108" t="s">
+      <c r="C97" s="109"/>
+      <c r="D97" s="107" t="s">
         <v>291</v>
       </c>
-      <c r="E97" s="110"/>
-      <c r="F97" s="106" t="s">
+      <c r="E97" s="109"/>
+      <c r="F97" s="105" t="s">
         <v>190</v>
       </c>
-      <c r="G97" s="106" t="s">
+      <c r="G97" s="105" t="s">
         <v>178</v>
       </c>
-      <c r="I97" s="110"/>
+      <c r="I97" s="109"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="96"/>
-      <c r="B98" s="133" t="s">
+      <c r="B98" s="132" t="s">
         <v>635</v>
       </c>
-      <c r="C98" s="133"/>
-      <c r="D98" s="133"/>
-      <c r="E98" s="134"/>
-      <c r="F98" s="134"/>
-      <c r="G98" s="134"/>
-      <c r="H98" s="134"/>
-      <c r="I98" s="110"/>
+      <c r="C98" s="132"/>
+      <c r="D98" s="132"/>
+      <c r="E98" s="133"/>
+      <c r="F98" s="133"/>
+      <c r="G98" s="133"/>
+      <c r="H98" s="133"/>
+      <c r="I98" s="109"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A99" s="106" t="s">
+      <c r="A99" s="105" t="s">
         <v>56</v>
       </c>
     </row>
@@ -5488,37 +5504,37 @@
       <c r="B100" s="95" t="s">
         <v>315</v>
       </c>
-      <c r="C100" s="106" t="s">
+      <c r="C100" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="D100" s="106" t="s">
+      <c r="D100" s="105" t="s">
         <v>293</v>
       </c>
-      <c r="F100" s="109" t="s">
+      <c r="F100" s="108" t="s">
         <v>283</v>
       </c>
-      <c r="G100" s="106" t="s">
+      <c r="G100" s="105" t="s">
         <v>265</v>
       </c>
-      <c r="H100" s="122" t="s">
+      <c r="H100" s="121" t="s">
         <v>284</v>
       </c>
-      <c r="I100" s="106" t="s">
+      <c r="I100" s="105" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="96"/>
-      <c r="B101" s="135" t="s">
+      <c r="B101" s="134" t="s">
         <v>502</v>
       </c>
-      <c r="C101" s="135"/>
-      <c r="D101" s="135"/>
-      <c r="E101" s="135"/>
-      <c r="F101" s="134"/>
-      <c r="G101" s="134"/>
-      <c r="H101" s="134"/>
-      <c r="I101" s="110"/>
+      <c r="C101" s="134"/>
+      <c r="D101" s="134"/>
+      <c r="E101" s="134"/>
+      <c r="F101" s="133"/>
+      <c r="G101" s="133"/>
+      <c r="H101" s="133"/>
+      <c r="I101" s="109"/>
     </row>
     <row r="102" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A102" s="99" t="s">
@@ -5527,22 +5543,22 @@
       <c r="B102" s="95" t="s">
         <v>636</v>
       </c>
-      <c r="C102" s="106" t="s">
+      <c r="C102" s="105" t="s">
         <v>191</v>
       </c>
-      <c r="D102" s="106" t="s">
+      <c r="D102" s="105" t="s">
         <v>293</v>
       </c>
-      <c r="F102" s="109" t="s">
+      <c r="F102" s="108" t="s">
         <v>283</v>
       </c>
-      <c r="G102" s="106" t="s">
+      <c r="G102" s="105" t="s">
         <v>265</v>
       </c>
-      <c r="H102" s="122" t="s">
+      <c r="H102" s="121" t="s">
         <v>284</v>
       </c>
-      <c r="I102" s="106" t="s">
+      <c r="I102" s="105" t="s">
         <v>314</v>
       </c>
     </row>
@@ -5553,40 +5569,40 @@
       <c r="B103" s="95" t="s">
         <v>636</v>
       </c>
-      <c r="C103" s="106" t="s">
+      <c r="C103" s="105" t="s">
         <v>191</v>
       </c>
-      <c r="D103" s="106" t="s">
+      <c r="D103" s="105" t="s">
         <v>293</v>
       </c>
-      <c r="F103" s="109" t="s">
+      <c r="F103" s="108" t="s">
         <v>557</v>
       </c>
-      <c r="G103" s="106" t="s">
+      <c r="G103" s="105" t="s">
         <v>265</v>
       </c>
-      <c r="H103" s="122" t="s">
+      <c r="H103" s="121" t="s">
         <v>284</v>
       </c>
-      <c r="I103" s="106" t="s">
+      <c r="I103" s="105" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="96"/>
-      <c r="B104" s="135" t="s">
+      <c r="B104" s="134" t="s">
         <v>560</v>
       </c>
-      <c r="C104" s="135"/>
-      <c r="D104" s="135"/>
-      <c r="E104" s="135"/>
-      <c r="F104" s="134"/>
-      <c r="G104" s="134"/>
-      <c r="H104" s="134"/>
-      <c r="I104" s="110"/>
+      <c r="C104" s="134"/>
+      <c r="D104" s="134"/>
+      <c r="E104" s="134"/>
+      <c r="F104" s="133"/>
+      <c r="G104" s="133"/>
+      <c r="H104" s="133"/>
+      <c r="I104" s="109"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A105" s="106" t="s">
+      <c r="A105" s="105" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5594,27 +5610,27 @@
       <c r="A106" s="96" t="s">
         <v>90</v>
       </c>
-      <c r="B106" s="106" t="s">
+      <c r="B106" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="F106" s="106" t="s">
+      <c r="F106" s="105" t="s">
         <v>91</v>
       </c>
-      <c r="G106" s="123" t="s">
+      <c r="G106" s="122" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="96"/>
-      <c r="B107" s="133" t="s">
+      <c r="B107" s="132" t="s">
         <v>92</v>
       </c>
-      <c r="C107" s="133"/>
-      <c r="D107" s="133"/>
-      <c r="E107" s="133"/>
-      <c r="F107" s="134"/>
-      <c r="G107" s="134"/>
-      <c r="H107" s="134"/>
+      <c r="C107" s="132"/>
+      <c r="D107" s="132"/>
+      <c r="E107" s="132"/>
+      <c r="F107" s="133"/>
+      <c r="G107" s="133"/>
+      <c r="H107" s="133"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="96" t="s">
@@ -5622,90 +5638,90 @@
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A109" s="106" t="s">
+      <c r="A109" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="B109" s="106" t="s">
+      <c r="B109" s="105" t="s">
         <v>142</v>
       </c>
-      <c r="D109" s="108" t="s">
+      <c r="D109" s="107" t="s">
         <v>291</v>
       </c>
-      <c r="F109" s="106" t="s">
+      <c r="F109" s="105" t="s">
         <v>129</v>
       </c>
-      <c r="H109" s="122" t="s">
+      <c r="H109" s="121" t="s">
         <v>130</v>
       </c>
-      <c r="I109" s="106" t="s">
+      <c r="I109" s="105" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" s="106" t="s">
+      <c r="A110" s="105" t="s">
         <v>119</v>
       </c>
-      <c r="B110" s="106" t="s">
+      <c r="B110" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="F110" s="106" t="s">
+      <c r="F110" s="105" t="s">
         <v>95</v>
       </c>
-      <c r="H110" s="106" t="s">
+      <c r="H110" s="105" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="96"/>
-      <c r="B111" s="133" t="s">
+      <c r="B111" s="132" t="s">
         <v>96</v>
       </c>
-      <c r="C111" s="133"/>
-      <c r="D111" s="133"/>
-      <c r="E111" s="133"/>
-      <c r="F111" s="134"/>
-      <c r="G111" s="134"/>
-      <c r="H111" s="134"/>
+      <c r="C111" s="132"/>
+      <c r="D111" s="132"/>
+      <c r="E111" s="132"/>
+      <c r="F111" s="133"/>
+      <c r="G111" s="133"/>
+      <c r="H111" s="133"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="B112" s="106" t="s">
+      <c r="B112" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="F112" s="106" t="s">
+      <c r="F112" s="105" t="s">
         <v>120</v>
       </c>
-      <c r="G112" s="106" t="s">
+      <c r="G112" s="105" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A113" s="106"/>
-      <c r="B113" s="133" t="s">
+      <c r="A113" s="105"/>
+      <c r="B113" s="132" t="s">
         <v>503</v>
       </c>
-      <c r="C113" s="133"/>
-      <c r="D113" s="133"/>
-      <c r="E113" s="133"/>
-      <c r="F113" s="134"/>
-      <c r="G113" s="134"/>
-      <c r="H113" s="134"/>
-      <c r="I113" s="134"/>
+      <c r="C113" s="132"/>
+      <c r="D113" s="132"/>
+      <c r="E113" s="132"/>
+      <c r="F113" s="133"/>
+      <c r="G113" s="133"/>
+      <c r="H113" s="133"/>
+      <c r="I113" s="133"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="100" t="s">
         <v>208</v>
       </c>
-      <c r="B114" s="110"/>
-      <c r="C114" s="110"/>
-      <c r="D114" s="110"/>
-      <c r="E114" s="110"/>
-      <c r="F114" s="106" t="s">
+      <c r="B114" s="109"/>
+      <c r="C114" s="109"/>
+      <c r="D114" s="109"/>
+      <c r="E114" s="109"/>
+      <c r="F114" s="105" t="s">
         <v>209</v>
       </c>
-      <c r="H114" s="109" t="s">
+      <c r="H114" s="108" t="s">
         <v>161</v>
       </c>
     </row>
@@ -5715,7 +5731,7 @@
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A116" s="106" t="s">
+      <c r="A116" s="105" t="s">
         <v>63</v>
       </c>
       <c r="B116" s="95" t="s">
@@ -5726,262 +5742,262 @@
       <c r="E116" s="95" t="s">
         <v>148</v>
       </c>
-      <c r="F116" s="106" t="s">
+      <c r="F116" s="105" t="s">
         <v>135</v>
       </c>
-      <c r="H116" s="106" t="s">
+      <c r="H116" s="105" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="96"/>
-      <c r="B117" s="136" t="s">
+      <c r="B117" s="135" t="s">
         <v>500</v>
       </c>
-      <c r="C117" s="136"/>
-      <c r="D117" s="136"/>
-      <c r="E117" s="136"/>
-      <c r="F117" s="134"/>
-      <c r="G117" s="134"/>
-      <c r="H117" s="134"/>
-      <c r="I117" s="134"/>
+      <c r="C117" s="135"/>
+      <c r="D117" s="135"/>
+      <c r="E117" s="135"/>
+      <c r="F117" s="133"/>
+      <c r="G117" s="133"/>
+      <c r="H117" s="133"/>
+      <c r="I117" s="133"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A118" s="106" t="s">
+      <c r="A118" s="105" t="s">
         <v>146</v>
       </c>
       <c r="B118" s="95" t="s">
         <v>142</v>
       </c>
       <c r="C118" s="95"/>
-      <c r="D118" s="124" t="s">
+      <c r="D118" s="123" t="s">
         <v>291</v>
       </c>
       <c r="E118" s="95"/>
-      <c r="F118" s="106" t="s">
+      <c r="F118" s="105" t="s">
         <v>135</v>
       </c>
-      <c r="H118" s="106" t="s">
+      <c r="H118" s="105" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A119" s="106" t="s">
+      <c r="A119" s="105" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A120" s="106" t="s">
+      <c r="A120" s="105" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A121" s="106" t="s">
+      <c r="A121" s="105" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A122" s="128" t="s">
+      <c r="A122" s="127" t="s">
         <v>554</v>
       </c>
-      <c r="B122" s="130" t="s">
+      <c r="B122" s="129" t="s">
         <v>629</v>
       </c>
-      <c r="C122" s="106" t="s">
+      <c r="C122" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="D122" s="106" t="s">
+      <c r="D122" s="105" t="s">
         <v>293</v>
       </c>
-      <c r="F122" s="109" t="s">
+      <c r="F122" s="108" t="s">
         <v>630</v>
       </c>
-      <c r="G122" s="106" t="s">
+      <c r="G122" s="105" t="s">
         <v>265</v>
       </c>
-      <c r="H122" s="122" t="s">
+      <c r="H122" s="121" t="s">
         <v>553</v>
       </c>
-      <c r="I122" s="106" t="s">
+      <c r="I122" s="105" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="96"/>
-      <c r="B123" s="135"/>
-      <c r="C123" s="135"/>
-      <c r="D123" s="135"/>
-      <c r="E123" s="135"/>
-      <c r="F123" s="134"/>
-      <c r="G123" s="134"/>
-      <c r="H123" s="134"/>
-      <c r="I123" s="110"/>
-    </row>
-    <row r="124" spans="1:9" s="130" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="128" t="s">
+      <c r="B123" s="134"/>
+      <c r="C123" s="134"/>
+      <c r="D123" s="134"/>
+      <c r="E123" s="134"/>
+      <c r="F123" s="133"/>
+      <c r="G123" s="133"/>
+      <c r="H123" s="133"/>
+      <c r="I123" s="109"/>
+    </row>
+    <row r="124" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="127" t="s">
         <v>631</v>
       </c>
-      <c r="B124" s="130" t="s">
+      <c r="B124" s="129" t="s">
         <v>532</v>
       </c>
-      <c r="C124" s="130" t="s">
+      <c r="C124" s="129" t="s">
         <v>191</v>
       </c>
-      <c r="D124" s="130" t="s">
+      <c r="D124" s="129" t="s">
         <v>293</v>
       </c>
-      <c r="F124" s="109" t="s">
+      <c r="F124" s="108" t="s">
         <v>628</v>
       </c>
-      <c r="G124" s="130" t="s">
+      <c r="G124" s="129" t="s">
         <v>265</v>
       </c>
-      <c r="H124" s="122" t="s">
+      <c r="H124" s="121" t="s">
         <v>553</v>
       </c>
-      <c r="I124" s="130" t="s">
+      <c r="I124" s="129" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="125" spans="1:9" s="130" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="128" t="s">
+    <row r="125" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="127" t="s">
         <v>627</v>
       </c>
       <c r="B125" s="95" t="s">
         <v>285</v>
       </c>
-      <c r="C125" s="130" t="s">
+      <c r="C125" s="129" t="s">
         <v>191</v>
       </c>
-      <c r="D125" s="130" t="s">
+      <c r="D125" s="129" t="s">
         <v>293</v>
       </c>
-      <c r="F125" s="109" t="s">
+      <c r="F125" s="108" t="s">
         <v>561</v>
       </c>
-      <c r="G125" s="130" t="s">
+      <c r="G125" s="129" t="s">
         <v>265</v>
       </c>
-      <c r="H125" s="122" t="s">
+      <c r="H125" s="121" t="s">
         <v>553</v>
       </c>
-      <c r="I125" s="130" t="s">
+      <c r="I125" s="129" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="126" spans="1:9" s="130" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="96"/>
-      <c r="B126" s="135" t="s">
+      <c r="B126" s="134" t="s">
         <v>559</v>
       </c>
-      <c r="C126" s="135"/>
-      <c r="D126" s="135"/>
-      <c r="E126" s="135"/>
-      <c r="F126" s="134"/>
-      <c r="G126" s="134"/>
-      <c r="H126" s="134"/>
-      <c r="I126" s="129"/>
+      <c r="C126" s="134"/>
+      <c r="D126" s="134"/>
+      <c r="E126" s="134"/>
+      <c r="F126" s="133"/>
+      <c r="G126" s="133"/>
+      <c r="H126" s="133"/>
+      <c r="I126" s="128"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A127" s="128" t="s">
+      <c r="A127" s="127" t="s">
         <v>558</v>
       </c>
       <c r="B127" s="95" t="s">
         <v>285</v>
       </c>
-      <c r="C127" s="106" t="s">
+      <c r="C127" s="105" t="s">
         <v>191</v>
       </c>
-      <c r="D127" s="106" t="s">
+      <c r="D127" s="105" t="s">
         <v>293</v>
       </c>
-      <c r="F127" s="109" t="s">
+      <c r="F127" s="108" t="s">
         <v>552</v>
       </c>
-      <c r="G127" s="106" t="s">
+      <c r="G127" s="105" t="s">
         <v>265</v>
       </c>
-      <c r="H127" s="122" t="s">
+      <c r="H127" s="121" t="s">
         <v>553</v>
       </c>
-      <c r="I127" s="106" t="s">
+      <c r="I127" s="105" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="96"/>
-      <c r="B128" s="133" t="s">
+      <c r="B128" s="132" t="s">
         <v>290</v>
       </c>
-      <c r="C128" s="133"/>
-      <c r="D128" s="133"/>
-      <c r="E128" s="133"/>
-      <c r="F128" s="133"/>
-      <c r="G128" s="133"/>
-      <c r="H128" s="133"/>
-      <c r="I128" s="110" t="s">
+      <c r="C128" s="132"/>
+      <c r="D128" s="132"/>
+      <c r="E128" s="132"/>
+      <c r="F128" s="132"/>
+      <c r="G128" s="132"/>
+      <c r="H128" s="132"/>
+      <c r="I128" s="109" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A129" s="106" t="s">
+      <c r="A129" s="105" t="s">
         <v>67</v>
       </c>
-      <c r="B129" s="106" t="s">
+      <c r="B129" s="105" t="s">
         <v>522</v>
       </c>
-      <c r="C129" s="106" t="s">
+      <c r="C129" s="105" t="s">
         <v>211</v>
       </c>
-      <c r="D129" s="108" t="s">
+      <c r="D129" s="107" t="s">
         <v>524</v>
       </c>
-      <c r="F129" s="106" t="s">
+      <c r="F129" s="105" t="s">
         <v>514</v>
       </c>
-      <c r="G129" s="106" t="s">
+      <c r="G129" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="I129" s="106" t="s">
+      <c r="I129" s="105" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="96"/>
-      <c r="B130" s="133" t="s">
+      <c r="B130" s="132" t="s">
         <v>523</v>
       </c>
-      <c r="C130" s="133"/>
-      <c r="D130" s="133"/>
-      <c r="E130" s="133"/>
-      <c r="F130" s="134"/>
-      <c r="G130" s="134"/>
-      <c r="H130" s="134"/>
-      <c r="I130" s="134"/>
+      <c r="C130" s="132"/>
+      <c r="D130" s="132"/>
+      <c r="E130" s="132"/>
+      <c r="F130" s="133"/>
+      <c r="G130" s="133"/>
+      <c r="H130" s="133"/>
+      <c r="I130" s="133"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A131" s="106" t="s">
+      <c r="A131" s="105" t="s">
         <v>519</v>
       </c>
-      <c r="B131" s="106" t="s">
+      <c r="B131" s="105" t="s">
         <v>520</v>
       </c>
-      <c r="F131" s="106" t="s">
+      <c r="F131" s="105" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="96"/>
-      <c r="B132" s="133" t="s">
+      <c r="B132" s="132" t="s">
         <v>518</v>
       </c>
-      <c r="C132" s="133"/>
-      <c r="D132" s="133"/>
-      <c r="E132" s="133"/>
-      <c r="F132" s="134"/>
-      <c r="G132" s="134"/>
-      <c r="H132" s="134"/>
-      <c r="I132" s="134"/>
+      <c r="C132" s="132"/>
+      <c r="D132" s="132"/>
+      <c r="E132" s="132"/>
+      <c r="F132" s="133"/>
+      <c r="G132" s="133"/>
+      <c r="H132" s="133"/>
+      <c r="I132" s="133"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="96" t="s">
@@ -5992,16 +6008,16 @@
       <c r="A134" s="96" t="s">
         <v>195</v>
       </c>
-      <c r="B134" s="106" t="s">
+      <c r="B134" s="105" t="s">
         <v>532</v>
       </c>
-      <c r="D134" s="106" t="s">
+      <c r="D134" s="105" t="s">
         <v>292</v>
       </c>
-      <c r="F134" s="106" t="s">
+      <c r="F134" s="105" t="s">
         <v>544</v>
       </c>
-      <c r="G134" s="106" t="s">
+      <c r="G134" s="105" t="s">
         <v>152</v>
       </c>
       <c r="H134" s="95" t="s">
@@ -6009,307 +6025,307 @@
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A135" s="106" t="s">
+      <c r="A135" s="105" t="s">
         <v>150</v>
       </c>
-      <c r="B135" s="106" t="s">
+      <c r="B135" s="105" t="s">
         <v>139</v>
       </c>
-      <c r="F135" s="106" t="s">
+      <c r="F135" s="105" t="s">
         <v>138</v>
       </c>
-      <c r="H135" s="106" t="s">
+      <c r="H135" s="105" t="s">
         <v>145</v>
       </c>
-      <c r="I135" s="110"/>
+      <c r="I135" s="109"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A136" s="106" t="s">
+      <c r="A136" s="105" t="s">
         <v>149</v>
       </c>
-      <c r="B136" s="106" t="s">
+      <c r="B136" s="105" t="s">
         <v>214</v>
       </c>
-      <c r="C136" s="106" t="s">
+      <c r="C136" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="F136" s="106" t="s">
+      <c r="F136" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="G136" s="106" t="s">
+      <c r="G136" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="I136" s="110"/>
+      <c r="I136" s="109"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="96"/>
-      <c r="B137" s="133" t="s">
+      <c r="B137" s="132" t="s">
         <v>126</v>
       </c>
-      <c r="C137" s="133"/>
-      <c r="D137" s="133"/>
-      <c r="E137" s="133"/>
-      <c r="F137" s="134"/>
-      <c r="G137" s="134"/>
-      <c r="H137" s="134"/>
-      <c r="I137" s="134"/>
+      <c r="C137" s="132"/>
+      <c r="D137" s="132"/>
+      <c r="E137" s="132"/>
+      <c r="F137" s="133"/>
+      <c r="G137" s="133"/>
+      <c r="H137" s="133"/>
+      <c r="I137" s="133"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A138" s="106" t="s">
+      <c r="A138" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="B138" s="106" t="s">
+      <c r="B138" s="105" t="s">
         <v>139</v>
       </c>
-      <c r="C138" s="106" t="s">
+      <c r="C138" s="105" t="s">
         <v>191</v>
       </c>
-      <c r="F138" s="106" t="s">
+      <c r="F138" s="105" t="s">
         <v>151</v>
       </c>
-      <c r="G138" s="106" t="s">
+      <c r="G138" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="I138" s="110"/>
+      <c r="I138" s="109"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A139" s="106" t="s">
+      <c r="A139" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="B139" s="106" t="s">
+      <c r="B139" s="105" t="s">
         <v>193</v>
       </c>
-      <c r="C139" s="106" t="s">
+      <c r="C139" s="105" t="s">
         <v>211</v>
       </c>
-      <c r="F139" s="125" t="s">
+      <c r="F139" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="G139" s="106" t="s">
+      <c r="G139" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="I139" s="110" t="s">
+      <c r="I139" s="109" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="96"/>
-      <c r="B140" s="133" t="s">
+      <c r="B140" s="132" t="s">
         <v>243</v>
       </c>
-      <c r="C140" s="133"/>
-      <c r="D140" s="133"/>
-      <c r="E140" s="133"/>
-      <c r="F140" s="133"/>
-      <c r="G140" s="133"/>
-      <c r="H140" s="133"/>
-      <c r="I140" s="110"/>
+      <c r="C140" s="132"/>
+      <c r="D140" s="132"/>
+      <c r="E140" s="132"/>
+      <c r="F140" s="132"/>
+      <c r="G140" s="132"/>
+      <c r="H140" s="132"/>
+      <c r="I140" s="109"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A141" s="106" t="s">
+      <c r="A141" s="105" t="s">
         <v>458</v>
       </c>
-      <c r="B141" s="106" t="s">
+      <c r="B141" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="C141" s="106" t="s">
+      <c r="C141" s="105" t="s">
         <v>191</v>
       </c>
-      <c r="F141" s="106" t="s">
+      <c r="F141" s="105" t="s">
         <v>169</v>
       </c>
-      <c r="G141" s="106" t="s">
+      <c r="G141" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="I141" s="110"/>
+      <c r="I141" s="109"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="96"/>
-      <c r="B142" s="133" t="s">
+      <c r="B142" s="132" t="s">
         <v>219</v>
       </c>
-      <c r="C142" s="133"/>
-      <c r="D142" s="133"/>
-      <c r="E142" s="133"/>
-      <c r="F142" s="133"/>
-      <c r="G142" s="133"/>
-      <c r="H142" s="133"/>
-      <c r="I142" s="110"/>
+      <c r="C142" s="132"/>
+      <c r="D142" s="132"/>
+      <c r="E142" s="132"/>
+      <c r="F142" s="132"/>
+      <c r="G142" s="132"/>
+      <c r="H142" s="132"/>
+      <c r="I142" s="109"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A143" s="106" t="s">
+      <c r="A143" s="105" t="s">
         <v>177</v>
       </c>
-      <c r="B143" s="106" t="s">
+      <c r="B143" s="105" t="s">
         <v>174</v>
       </c>
-      <c r="D143" s="108" t="s">
+      <c r="D143" s="107" t="s">
         <v>291</v>
       </c>
-      <c r="F143" s="106" t="s">
+      <c r="F143" s="105" t="s">
         <v>172</v>
       </c>
-      <c r="G143" s="106" t="s">
+      <c r="G143" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="H143" s="106" t="s">
+      <c r="H143" s="105" t="s">
         <v>173</v>
       </c>
-      <c r="I143" s="110"/>
+      <c r="I143" s="109"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="96"/>
-      <c r="B144" s="133" t="s">
+      <c r="B144" s="132" t="s">
         <v>175</v>
       </c>
-      <c r="C144" s="133"/>
-      <c r="D144" s="133"/>
-      <c r="E144" s="133"/>
-      <c r="F144" s="133"/>
-      <c r="G144" s="133"/>
-      <c r="H144" s="133"/>
-      <c r="I144" s="110"/>
+      <c r="C144" s="132"/>
+      <c r="D144" s="132"/>
+      <c r="E144" s="132"/>
+      <c r="F144" s="132"/>
+      <c r="G144" s="132"/>
+      <c r="H144" s="132"/>
+      <c r="I144" s="109"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A145" s="106" t="s">
+      <c r="A145" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="B145" s="106" t="s">
+      <c r="B145" s="105" t="s">
         <v>139</v>
       </c>
-      <c r="C145" s="106" t="s">
+      <c r="C145" s="105" t="s">
         <v>191</v>
       </c>
-      <c r="F145" s="106" t="s">
+      <c r="F145" s="105" t="s">
         <v>169</v>
       </c>
-      <c r="G145" s="106" t="s">
+      <c r="G145" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="I145" s="110" t="s">
+      <c r="I145" s="109" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A146" s="106" t="s">
+      <c r="A146" s="105" t="s">
         <v>168</v>
       </c>
-      <c r="B146" s="106" t="s">
+      <c r="B146" s="105" t="s">
         <v>250</v>
       </c>
-      <c r="F146" s="106" t="s">
+      <c r="F146" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="G146" s="106" t="s">
+      <c r="G146" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="I146" s="110"/>
+      <c r="I146" s="109"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A147" s="126" t="s">
+      <c r="A147" s="125" t="s">
         <v>196</v>
       </c>
-      <c r="B147" s="106" t="s">
+      <c r="B147" s="105" t="s">
         <v>139</v>
       </c>
-      <c r="F147" s="106" t="s">
+      <c r="F147" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="H147" s="106" t="s">
+      <c r="H147" s="105" t="s">
         <v>197</v>
       </c>
-      <c r="I147" s="110"/>
+      <c r="I147" s="109"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B148" s="110" t="s">
+      <c r="B148" s="109" t="s">
         <v>295</v>
       </c>
-      <c r="C148" s="110"/>
-      <c r="D148" s="110"/>
-      <c r="E148" s="110"/>
+      <c r="C148" s="109"/>
+      <c r="D148" s="109"/>
+      <c r="E148" s="109"/>
     </row>
     <row r="149" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A149" s="99" t="s">
         <v>202</v>
       </c>
-      <c r="B149" s="106" t="s">
+      <c r="B149" s="105" t="s">
         <v>139</v>
       </c>
-      <c r="F149" s="106" t="s">
+      <c r="F149" s="105" t="s">
         <v>200</v>
       </c>
-      <c r="H149" s="106" t="s">
+      <c r="H149" s="105" t="s">
         <v>197</v>
       </c>
-      <c r="I149" s="110"/>
+      <c r="I149" s="109"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B150" s="110" t="s">
+      <c r="B150" s="109" t="s">
         <v>295</v>
       </c>
-      <c r="C150" s="110"/>
-      <c r="D150" s="110"/>
-      <c r="E150" s="110"/>
+      <c r="C150" s="109"/>
+      <c r="D150" s="109"/>
+      <c r="E150" s="109"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A151" s="126" t="s">
+      <c r="A151" s="125" t="s">
         <v>204</v>
       </c>
-      <c r="B151" s="106" t="s">
+      <c r="B151" s="105" t="s">
         <v>193</v>
       </c>
-      <c r="F151" s="106" t="s">
+      <c r="F151" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="H151" s="106" t="s">
+      <c r="H151" s="105" t="s">
         <v>197</v>
       </c>
-      <c r="I151" s="110"/>
+      <c r="I151" s="109"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B152" s="133" t="s">
+      <c r="B152" s="132" t="s">
         <v>203</v>
       </c>
-      <c r="C152" s="133"/>
-      <c r="D152" s="133"/>
-      <c r="E152" s="133"/>
-      <c r="F152" s="134"/>
-      <c r="G152" s="134"/>
-      <c r="H152" s="134"/>
-      <c r="I152" s="134"/>
+      <c r="C152" s="132"/>
+      <c r="D152" s="132"/>
+      <c r="E152" s="132"/>
+      <c r="F152" s="133"/>
+      <c r="G152" s="133"/>
+      <c r="H152" s="133"/>
+      <c r="I152" s="133"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A153" s="106" t="s">
+      <c r="A153" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="B153" s="106" t="s">
+      <c r="B153" s="105" t="s">
         <v>139</v>
       </c>
-      <c r="F153" s="106" t="s">
+      <c r="F153" s="105" t="s">
         <v>85</v>
       </c>
-      <c r="G153" s="106" t="s">
+      <c r="G153" s="105" t="s">
         <v>152</v>
       </c>
-      <c r="I153" s="110"/>
+      <c r="I153" s="109"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A154" s="126" t="s">
+      <c r="A154" s="125" t="s">
         <v>275</v>
       </c>
-      <c r="B154" s="106" t="s">
+      <c r="B154" s="105" t="s">
         <v>139</v>
       </c>
-      <c r="F154" s="106" t="s">
+      <c r="F154" s="105" t="s">
         <v>273</v>
       </c>
-      <c r="G154" s="117" t="s">
+      <c r="G154" s="116" t="s">
         <v>265</v>
       </c>
-      <c r="H154" s="106" t="s">
+      <c r="H154" s="105" t="s">
         <v>274</v>
       </c>
-      <c r="I154" s="110"/>
+      <c r="I154" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="47">
@@ -7458,7 +7474,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="38" x14ac:dyDescent="0.2">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="156" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -7469,7 +7485,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="38" x14ac:dyDescent="0.2">
-      <c r="A3" s="158"/>
+      <c r="A3" s="157"/>
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
@@ -7485,7 +7501,7 @@
       <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="157" t="s">
+      <c r="A5" s="156" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="5"/>
@@ -7494,32 +7510,32 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="158"/>
-      <c r="B6" s="138" t="s">
+      <c r="A6" s="157"/>
+      <c r="B6" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="138"/>
+      <c r="C6" s="137"/>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="158"/>
+      <c r="A7" s="157"/>
       <c r="B7" s="6"/>
       <c r="C7" s="31" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="158"/>
+      <c r="A8" s="157"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="158"/>
-      <c r="B9" s="160" t="s">
+      <c r="A9" s="157"/>
+      <c r="B9" s="159" t="s">
         <v>624</v>
       </c>
-      <c r="C9" s="161"/>
+      <c r="C9" s="160"/>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -7543,7 +7559,7 @@
       <c r="C12" s="29"/>
     </row>
     <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="159" t="s">
+      <c r="A13" s="158" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -7554,25 +7570,25 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="158"/>
+      <c r="A14" s="157"/>
       <c r="B14" s="5"/>
       <c r="C14" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A15" s="158"/>
+      <c r="A15" s="157"/>
       <c r="B15" s="5"/>
       <c r="C15" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="158"/>
-      <c r="B16" s="162" t="s">
+      <c r="A16" s="157"/>
+      <c r="B16" s="161" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="163"/>
+      <c r="C16" s="162"/>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -7656,23 +7672,23 @@
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="131" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="131" t="s">
+    <row r="1" spans="1:6" s="130" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="130" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="131" t="s">
+      <c r="B1" s="130" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="131" t="s">
+      <c r="C1" s="130" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="131" t="s">
+      <c r="D1" s="130" t="s">
         <v>528</v>
       </c>
-      <c r="E1" s="131" t="s">
+      <c r="E1" s="130" t="s">
         <v>482</v>
       </c>
-      <c r="F1" s="131" t="s">
+      <c r="F1" s="130" t="s">
         <v>572</v>
       </c>
     </row>
@@ -7680,25 +7696,25 @@
       <c r="A2" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="131" t="s">
         <v>173</v>
       </c>
-      <c r="C2" s="132" t="s">
+      <c r="C2" s="131" t="s">
         <v>218</v>
       </c>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>256</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132" t="s">
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131" t="s">
         <v>259</v>
       </c>
     </row>
@@ -7706,11 +7722,11 @@
       <c r="A4" t="s">
         <v>264</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132" t="s">
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131" t="s">
         <v>302</v>
       </c>
     </row>
@@ -7718,11 +7734,11 @@
       <c r="A5" t="s">
         <v>267</v>
       </c>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132"/>
-      <c r="F5" s="132" t="s">
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131" t="s">
         <v>284</v>
       </c>
     </row>
@@ -7730,118 +7746,118 @@
       <c r="A6" t="s">
         <v>554</v>
       </c>
-      <c r="B6" s="132"/>
-      <c r="C6" s="132"/>
-      <c r="D6" s="132"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="132" t="s">
+      <c r="B6" s="131"/>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="132"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="132"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="131"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="132"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="131"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="132"/>
-      <c r="C9" s="132"/>
-      <c r="D9" s="132"/>
-      <c r="E9" s="132"/>
-      <c r="F9" s="132"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="131"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="132"/>
-      <c r="C10" s="132"/>
-      <c r="D10" s="132"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="131"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="131"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="132"/>
-      <c r="C11" s="132"/>
-      <c r="D11" s="132"/>
-      <c r="E11" s="132"/>
-      <c r="F11" s="132"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="131"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="132"/>
-      <c r="C12" s="132"/>
-      <c r="D12" s="132"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="132"/>
+      <c r="B12" s="131"/>
+      <c r="C12" s="131"/>
+      <c r="D12" s="131"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="132"/>
-      <c r="C13" s="132"/>
-      <c r="D13" s="132"/>
-      <c r="E13" s="132"/>
-      <c r="F13" s="132"/>
+      <c r="B13" s="131"/>
+      <c r="C13" s="131"/>
+      <c r="D13" s="131"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="131"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="132"/>
-      <c r="C14" s="132"/>
-      <c r="D14" s="132"/>
-      <c r="E14" s="132"/>
-      <c r="F14" s="132"/>
+      <c r="B14" s="131"/>
+      <c r="C14" s="131"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="131"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="132"/>
-      <c r="C15" s="132"/>
-      <c r="D15" s="132"/>
-      <c r="E15" s="132"/>
-      <c r="F15" s="132"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="131"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="131"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="132"/>
-      <c r="C16" s="132"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="132"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="131"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="132"/>
-      <c r="C17" s="132"/>
-      <c r="D17" s="132"/>
-      <c r="E17" s="132"/>
-      <c r="F17" s="132"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="131"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="132"/>
-      <c r="C18" s="132"/>
-      <c r="D18" s="132"/>
-      <c r="E18" s="132"/>
-      <c r="F18" s="132"/>
+      <c r="B18" s="131"/>
+      <c r="C18" s="131"/>
+      <c r="D18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="131"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="132"/>
-      <c r="C19" s="132"/>
-      <c r="D19" s="132"/>
-      <c r="E19" s="132"/>
-      <c r="F19" s="132"/>
+      <c r="B19" s="131"/>
+      <c r="C19" s="131"/>
+      <c r="D19" s="131"/>
+      <c r="E19" s="131"/>
+      <c r="F19" s="131"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="132"/>
-      <c r="C20" s="132"/>
-      <c r="D20" s="132"/>
-      <c r="E20" s="132"/>
-      <c r="F20" s="132"/>
+      <c r="B20" s="131"/>
+      <c r="C20" s="131"/>
+      <c r="D20" s="131"/>
+      <c r="E20" s="131"/>
+      <c r="F20" s="131"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="132"/>
-      <c r="C21" s="132"/>
-      <c r="D21" s="132"/>
-      <c r="E21" s="132"/>
-      <c r="F21" s="132"/>
+      <c r="B21" s="131"/>
+      <c r="C21" s="131"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="131"/>
+      <c r="F21" s="131"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change in whattomine.com's parsing.
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="707">
   <si>
     <t>Miners (AMD)</t>
   </si>
@@ -1577,9 +1577,6 @@
     <t>Titan</t>
   </si>
   <si>
-    <t>nvidia-smi shows ok, but ethdcrminer64 says "No AMD OPENCL or NVIDIA CUDA GPUs found, exit"</t>
-  </si>
-  <si>
     <t>stratum+tcp://openpool.tech:4233</t>
   </si>
   <si>
@@ -1685,9 +1682,6 @@
     <t>/opt/silentarmy</t>
   </si>
   <si>
-    <t>https://whattomine.com/coins?utf8=%E2%9C%93&amp;adapt_q_280x=0&amp;adapt_q_380=0&amp;adapt_q_fury=0&amp;adapt_q_470=0&amp;adapt_q_480=0&amp;adapt_q_570=0&amp;adapt_q_580=0&amp;adapt_q_vega56=0&amp;adapt_q_vega64=0&amp;adapt_q_750Ti=0&amp;adapt_q_1050Ti=0&amp;adapt_q_10606=0&amp;adapt_q_1070=0&amp;adapt_q_1070Ti=3&amp;adapt_1070Ti=true&amp;adapt_q_1080=1&amp;adapt_1080=true&amp;adapt_q_1080Ti=0&amp;eth=true&amp;factor%5Beth_hr%5D=114.8&amp;factor%5Beth_p%5D=545.0&amp;grof=true&amp;factor%5Bgro_hr%5D=154.0&amp;factor%5Bgro_p%5D=510.0&amp;phi=true&amp;factor%5Bphi_hr%5D=90.0&amp;factor%5Bphi_p%5D=550.0&amp;cn=true&amp;factor%5Bcn_hr%5D=2470.0&amp;factor%5Bcn_p%5D=370.0&amp;cn7=true&amp;factor%5Bcn7_hr%5D=2470.0&amp;factor%5Bcn7_p%5D=370.0&amp;eq=true&amp;factor%5Beq_hr%5D=1960.0&amp;factor%5Beq_p%5D=490.0&amp;lre=true&amp;factor%5Blrev2_hr%5D=169500.0&amp;factor%5Blrev2_p%5D=510.0&amp;ns=true&amp;factor%5Bns_hr%5D=4210.0&amp;factor%5Bns_p%5D=510.0&amp;tt10=true&amp;factor%5Btt10_hr%5D=80.3&amp;factor%5Btt10_p%5D=510.0&amp;x16r=true&amp;factor%5Bx16r_hr%5D=40.5&amp;factor%5Bx16r_p%5D=525.0&amp;skh=true&amp;factor%5Bskh_hr%5D=131.0&amp;factor%5Bskh_p%5D=510.0&amp;n5=true&amp;factor%5Bn5_hr%5D=208.0&amp;factor%5Bn5_p%5D=510.0&amp;xn=true&amp;factor%5Bxn_hr%5D=14.6&amp;factor%5Bxn_p%5D=490.0&amp;factor%5Bcost%5D=0.0945&amp;sort=Profitability24&amp;volume=0&amp;revenue=24h&amp;factor%5Bexchanges%5D%5B%5D=&amp;factor%5Bexchanges%5D%5B%5D=binance&amp;factor%5Bexchanges%5D%5B%5D=bitfinex&amp;factor%5Bexchanges%5D%5B%5D=bittrex&amp;factor%5Bexchanges%5D%5B%5D=cryptobridge&amp;factor%5Bexchanges%5D%5B%5D=cryptopia&amp;factor%5Bexchanges%5D%5B%5D=hitbtc&amp;factor%5Bexchanges%5D%5B%5D=poloniex&amp;factor%5Bexchanges%5D%5B%5D=yobit&amp;dataset=Titans&amp;commit=Calculate</t>
-  </si>
-  <si>
     <t>LOCATION</t>
   </si>
   <si>
@@ -2160,6 +2154,9 @@
   </si>
   <si>
     <t>Motley</t>
+  </si>
+  <si>
+    <t>https://whattomine.com/coins?utf8=%E2%9C%93&amp;adapt_q_280x=0&amp;adapt_q_380=0&amp;adapt_q_fury=0&amp;adapt_q_470=0&amp;adapt_q_480=0&amp;adapt_q_570=0&amp;adapt_q_580=0&amp;adapt_q_vega56=0&amp;adapt_q_vega64=0&amp;adapt_q_750Ti=0&amp;adapt_q_1050Ti=0&amp;adapt_q_10606=0&amp;adapt_q_1070=0&amp;adapt_q_1070Ti=3&amp;adapt_1070Ti=true&amp;adapt_q_1080=0&amp;adapt_q_1080Ti=1&amp;adapt_1080Ti=true&amp;eth=true&amp;factor%5Beth_hr%5D=126.50&amp;factor%5Beth_p%5D=545.00&amp;grof=true&amp;factor%5Bgro_hr%5D=167.50&amp;factor%5Bgro_p%5D=570.00&amp;phi=true&amp;factor%5Bphi_hr%5D=99.00&amp;factor%5Bphi_p%5D=590.00&amp;cn=true&amp;factor%5Bcn_hr%5D=2720.00&amp;factor%5Bcn_p%5D=410.00&amp;cn7=true&amp;factor%5Bcn7_hr%5D=2720.00&amp;factor%5Bcn7_p%5D=410.00&amp;eq=true&amp;factor%5Beq_hr%5D=2095.00&amp;factor%5Beq_p%5D=550.00&amp;lre=true&amp;factor%5Blrev2_hr%5D=187000.00&amp;factor%5Blrev2_p%5D=550.00&amp;ns=true&amp;factor%5Bns_hr%5D=4550.00&amp;factor%5Bns_p%5D=550.00&amp;tt10=true&amp;factor%5Btt10_hr%5D=88.50&amp;factor%5Btt10_p%5D=560.00&amp;x16r=true&amp;factor%5Bx16r_hr%5D=45.00&amp;factor%5Bx16r_p%5D=565.00&amp;factor%5Bl2z_hr%5D=9.00&amp;factor%5Bl2z_p%5D=500.00&amp;n5=true&amp;factor%5Bn5_hr%5D=225.00&amp;factor%5Bn5_p%5D=550.00&amp;xn=true&amp;factor%5Bxn_hr%5D=16.10&amp;factor%5Bxn_p%5D=550.00&amp;factor%5Bcost%5D=0.0945&amp;sort=Profitability24&amp;volume=0&amp;revenue=24h&amp;factor%5Bexchanges%5D%5B%5D=&amp;factor%5Bexchanges%5D%5B%5D=binance&amp;factor%5Bexchanges%5D%5B%5D=bitfinex&amp;factor%5Bexchanges%5D%5B%5D=bittrex&amp;factor%5Bexchanges%5D%5B%5D=cryptobridge&amp;factor%5Bexchanges%5D%5B%5D=cryptopia&amp;factor%5Bexchanges%5D%5B%5D=hitbtc&amp;factor%5Bexchanges%5D%5B%5D=poloniex&amp;factor%5Bexchanges%5D%5B%5D=yobit&amp;dataset=Titans&amp;commit=Calculate</t>
   </si>
 </sst>
 </file>
@@ -3553,10 +3550,10 @@
     </row>
     <row r="3" spans="1:14" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="66" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B3" s="66" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C3" s="129"/>
       <c r="D3" s="129"/>
@@ -3607,16 +3604,16 @@
         <v>281</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D6" s="56" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E6" s="56" t="s">
         <v>291</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G6" s="56" t="s">
         <v>284</v>
@@ -3628,18 +3625,18 @@
         <v>283</v>
       </c>
       <c r="J6" s="56" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="K6" s="56" t="s">
         <v>285</v>
       </c>
       <c r="L6" s="56" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L7" s="56" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
   </sheetData>
@@ -3682,57 +3679,57 @@
         <v>153</v>
       </c>
       <c r="B1" s="143" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1" s="143" t="s">
         <v>552</v>
       </c>
-      <c r="C1" s="143" t="s">
+      <c r="D1" s="143" t="s">
+        <v>551</v>
+      </c>
+      <c r="E1" s="142" t="s">
+        <v>556</v>
+      </c>
+      <c r="F1" s="142" t="s">
+        <v>555</v>
+      </c>
+      <c r="G1" s="144" t="s">
+        <v>553</v>
+      </c>
+      <c r="H1" s="143" t="s">
+        <v>599</v>
+      </c>
+      <c r="I1" s="159" t="s">
+        <v>667</v>
+      </c>
+      <c r="J1" s="165" t="s">
+        <v>646</v>
+      </c>
+      <c r="K1" s="158" t="s">
+        <v>647</v>
+      </c>
+      <c r="L1" s="142" t="s">
+        <v>597</v>
+      </c>
+      <c r="M1" s="146" t="s">
+        <v>603</v>
+      </c>
+      <c r="N1" s="146" t="s">
+        <v>668</v>
+      </c>
+      <c r="O1" s="144" t="s">
+        <v>600</v>
+      </c>
+      <c r="P1" s="143" t="s">
         <v>554</v>
-      </c>
-      <c r="D1" s="143" t="s">
-        <v>553</v>
-      </c>
-      <c r="E1" s="142" t="s">
-        <v>558</v>
-      </c>
-      <c r="F1" s="142" t="s">
-        <v>557</v>
-      </c>
-      <c r="G1" s="144" t="s">
-        <v>555</v>
-      </c>
-      <c r="H1" s="143" t="s">
-        <v>601</v>
-      </c>
-      <c r="I1" s="159" t="s">
-        <v>669</v>
-      </c>
-      <c r="J1" s="165" t="s">
-        <v>648</v>
-      </c>
-      <c r="K1" s="158" t="s">
-        <v>649</v>
-      </c>
-      <c r="L1" s="142" t="s">
-        <v>599</v>
-      </c>
-      <c r="M1" s="146" t="s">
-        <v>605</v>
-      </c>
-      <c r="N1" s="146" t="s">
-        <v>670</v>
-      </c>
-      <c r="O1" s="144" t="s">
-        <v>602</v>
-      </c>
-      <c r="P1" s="143" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="145" customFormat="1" ht="33" x14ac:dyDescent="0.2">
       <c r="A2" s="138" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B2" s="139" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C2" s="140"/>
       <c r="D2" s="140"/>
@@ -3751,7 +3748,7 @@
     </row>
     <row r="3" spans="1:16" s="133" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="133" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B3" s="132"/>
       <c r="C3" s="130"/>
@@ -3791,25 +3788,25 @@
     </row>
     <row r="5" spans="1:16" s="136" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="136" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B5" s="137"/>
       <c r="D5" s="136" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="H5" s="136" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L5" s="136" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="O5" s="136" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="133" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="133" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B6" s="132"/>
       <c r="C6" s="130"/>
@@ -3849,7 +3846,7 @@
     </row>
     <row r="8" spans="1:16" s="133" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="133" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B8" s="132"/>
       <c r="C8" s="130"/>
@@ -3879,7 +3876,7 @@
       <c r="G9" s="130"/>
       <c r="H9" s="130"/>
       <c r="J9" s="131" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="K9" s="130"/>
       <c r="L9" s="130"/>
@@ -3893,22 +3890,22 @@
         <v>30</v>
       </c>
       <c r="B10" s="133" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C10" s="131" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D10" s="131" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E10" s="131" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F10" s="131" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G10" s="131" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="H10" s="131"/>
       <c r="I10" s="131"/>
@@ -3919,12 +3916,12 @@
       <c r="N10" s="131"/>
       <c r="O10" s="131"/>
       <c r="P10" s="131" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="133" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -3939,36 +3936,36 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="133" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="I14" s="132" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="N14" s="132" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="O14" s="132" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="133" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="133" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="160" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="133" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -3978,7 +3975,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="133" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -3986,17 +3983,17 @@
         <v>35</v>
       </c>
       <c r="J21" s="132" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="133" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="133" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -4004,12 +4001,12 @@
         <v>42</v>
       </c>
       <c r="J24" s="132" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="133" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -4017,12 +4014,12 @@
         <v>45</v>
       </c>
       <c r="J26" s="132" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="133" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -4030,17 +4027,17 @@
         <v>249</v>
       </c>
       <c r="J28" s="132" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="133" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="133" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -4055,12 +4052,12 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="133" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="133" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -4070,12 +4067,12 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="133" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="133" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -4083,22 +4080,22 @@
         <v>55</v>
       </c>
       <c r="J38" s="132" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="133" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="133" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="133" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -4106,57 +4103,57 @@
         <v>260</v>
       </c>
       <c r="I42" s="132" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="133" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="135" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="134" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="133" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="133" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="133" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="133" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="133" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="133" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="133" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -4164,7 +4161,7 @@
         <v>69</v>
       </c>
       <c r="J53" s="132" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
   </sheetData>
@@ -4240,52 +4237,52 @@
         <v>188</v>
       </c>
       <c r="C2" s="78" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D2" s="78" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E2" s="80"/>
       <c r="F2" s="81" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="79" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="77" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B3" s="45" t="s">
         <v>141</v>
       </c>
       <c r="C3" s="78" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D3" s="78" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E3" s="80"/>
       <c r="F3" s="81" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="100" customFormat="1" ht="50" x14ac:dyDescent="0.2">
       <c r="A4" s="152" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B4" s="39" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="100" t="s">
+        <v>618</v>
+      </c>
+      <c r="D4" s="100" t="s">
+        <v>619</v>
+      </c>
+      <c r="E4" s="153" t="s">
         <v>620</v>
       </c>
-      <c r="D4" s="100" t="s">
-        <v>621</v>
-      </c>
-      <c r="E4" s="153" t="s">
-        <v>622</v>
-      </c>
       <c r="F4" s="99" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="79" customFormat="1" ht="19" x14ac:dyDescent="0.2">
@@ -4296,16 +4293,16 @@
         <v>188</v>
       </c>
       <c r="C5" s="78" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D5" s="79" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E5" s="82" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="F5" s="79" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="100" customFormat="1" ht="50" x14ac:dyDescent="0.2">
@@ -4340,7 +4337,7 @@
       </c>
       <c r="E7" s="84"/>
       <c r="F7" s="41" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="G7" s="85"/>
     </row>
@@ -4398,7 +4395,7 @@
         <v>140</v>
       </c>
       <c r="F11" s="99" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -4412,7 +4409,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="99" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G12" s="51" t="s">
         <v>212</v>
@@ -4426,10 +4423,10 @@
         <v>208</v>
       </c>
       <c r="C13" s="51" t="s">
+        <v>546</v>
+      </c>
+      <c r="D13" s="51" t="s">
         <v>547</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="33" x14ac:dyDescent="0.2">
@@ -4451,7 +4448,7 @@
     </row>
     <row r="15" spans="1:7" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="100" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B15" s="39" t="s">
         <v>188</v>
@@ -4460,7 +4457,7 @@
         <v>176</v>
       </c>
       <c r="D15" s="100" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E15" s="83"/>
       <c r="F15" s="177" t="s">
@@ -4470,7 +4467,7 @@
     </row>
     <row r="16" spans="1:7" s="100" customFormat="1" ht="50" x14ac:dyDescent="0.2">
       <c r="A16" s="100" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B16" s="39" t="s">
         <v>188</v>
@@ -4485,7 +4482,7 @@
         <v>472</v>
       </c>
       <c r="F16" s="99" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -4559,91 +4556,91 @@
   <sheetData>
     <row r="1" spans="1:12" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="161" t="s">
+        <v>519</v>
+      </c>
+      <c r="B1" s="164" t="s">
+        <v>651</v>
+      </c>
+      <c r="C1" s="149" t="s">
         <v>520</v>
       </c>
-      <c r="B1" s="164" t="s">
+      <c r="D1" s="151" t="s">
+        <v>523</v>
+      </c>
+      <c r="E1" s="148" t="s">
+        <v>616</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>661</v>
+      </c>
+      <c r="G1" s="150" t="s">
         <v>653</v>
       </c>
-      <c r="C1" s="149" t="s">
-        <v>521</v>
-      </c>
-      <c r="D1" s="151" t="s">
-        <v>524</v>
-      </c>
-      <c r="E1" s="148" t="s">
-        <v>618</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>663</v>
-      </c>
-      <c r="G1" s="150" t="s">
-        <v>655</v>
-      </c>
       <c r="H1" s="36" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I1" s="36" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="K1" s="150" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="L1" s="42" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C2" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F2" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="G2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="H2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="I2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="I3" s="162" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="J3" s="162"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D4" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D5" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -4651,7 +4648,7 @@
         <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D6" s="147"/>
       <c r="E6" s="147"/>
@@ -4664,11 +4661,11 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C7" s="147"/>
       <c r="D7" s="147" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E7" s="147"/>
       <c r="F7" s="147"/>
@@ -4680,10 +4677,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>628</v>
+      </c>
+      <c r="D8" t="s">
         <v>630</v>
-      </c>
-      <c r="D8" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -4691,7 +4688,7 @@
         <v>35</v>
       </c>
       <c r="H9" s="162" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="I9" s="162"/>
       <c r="J9" s="162"/>
@@ -4702,7 +4699,7 @@
       </c>
       <c r="C10" s="147"/>
       <c r="D10" s="147" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E10" s="147"/>
       <c r="F10" s="147"/>
@@ -4718,7 +4715,7 @@
       </c>
       <c r="C11" s="147"/>
       <c r="D11" s="147" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E11" s="147"/>
       <c r="F11" s="147"/>
@@ -4734,7 +4731,7 @@
       </c>
       <c r="C12" s="147"/>
       <c r="D12" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="E12" s="147"/>
       <c r="F12" s="147"/>
@@ -4749,19 +4746,19 @@
         <v>55</v>
       </c>
       <c r="B13" s="162" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C13" s="147"/>
       <c r="D13" s="147"/>
       <c r="E13" s="147" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F13" s="147"/>
       <c r="G13" s="162" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="H13" s="162" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="I13" s="162"/>
       <c r="J13" s="162"/>
@@ -4774,20 +4771,20 @@
       <c r="C14" s="147"/>
       <c r="D14" s="147"/>
       <c r="E14" s="147" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F14" s="147"/>
       <c r="G14" s="147"/>
       <c r="H14" s="147"/>
       <c r="I14" s="169" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="J14" s="169"/>
       <c r="K14" s="147"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C15" s="147"/>
       <c r="D15" s="147"/>
@@ -4797,7 +4794,7 @@
       <c r="H15" s="147"/>
       <c r="I15" s="169"/>
       <c r="J15" s="169" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="K15" s="147"/>
     </row>
@@ -4806,18 +4803,18 @@
         <v>63</v>
       </c>
       <c r="D16" s="147" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E17" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="I17" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -4825,37 +4822,37 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D18" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C19" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D20" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C21" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D21" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>
@@ -4975,7 +4972,7 @@
     </row>
     <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="128" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B7" s="125" t="s">
         <v>216</v>
@@ -4984,7 +4981,7 @@
         <v>291</v>
       </c>
       <c r="F7" s="102" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="G7" s="113" t="s">
         <v>258</v>
@@ -5157,32 +5154,32 @@
         <v>138</v>
       </c>
       <c r="B20" s="102" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D20" s="104" t="s">
         <v>283</v>
       </c>
       <c r="F20" s="101" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="89" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B21" s="102" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D21" s="104" t="s">
         <v>283</v>
       </c>
       <c r="F21" s="102" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="89" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B22" s="102" t="s">
         <v>139</v>
@@ -5191,7 +5188,7 @@
         <v>283</v>
       </c>
       <c r="F22" s="102" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -5223,7 +5220,7 @@
     </row>
     <row r="26" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="92" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B26" s="156" t="s">
         <v>139</v>
@@ -5232,7 +5229,7 @@
         <v>283</v>
       </c>
       <c r="F26" s="156" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -5256,7 +5253,7 @@
     </row>
     <row r="29" spans="1:9" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="92" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B29" s="173" t="s">
         <v>179</v>
@@ -5265,16 +5262,16 @@
         <v>188</v>
       </c>
       <c r="D29" s="173" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F29" s="173" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G29" s="173" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H29" s="172" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="I29" s="174" t="s">
         <v>471</v>
@@ -5283,7 +5280,7 @@
     <row r="30" spans="1:9" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="93"/>
       <c r="B30" s="178" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C30" s="178"/>
       <c r="D30" s="178"/>
@@ -5295,7 +5292,7 @@
     </row>
     <row r="31" spans="1:9" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="92" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B31" s="173" t="s">
         <v>124</v>
@@ -5304,16 +5301,16 @@
         <v>188</v>
       </c>
       <c r="D31" s="173" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F31" s="173" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="G31" s="173" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H31" s="172" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="I31" s="174" t="s">
         <v>471</v>
@@ -5321,7 +5318,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="93" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B32" s="156" t="s">
         <v>124</v>
@@ -5330,10 +5327,10 @@
         <v>208</v>
       </c>
       <c r="D32" s="102" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F32" s="125" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="G32" s="125" t="s">
         <v>149</v>
@@ -5350,13 +5347,13 @@
         <v>208</v>
       </c>
       <c r="D33" s="173" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F33" s="173" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="G33" s="173" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H33" s="172"/>
       <c r="I33" s="174" t="s">
@@ -5365,7 +5362,7 @@
     </row>
     <row r="34" spans="1:19" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="92" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B34" s="173" t="s">
         <v>179</v>
@@ -5374,13 +5371,13 @@
         <v>208</v>
       </c>
       <c r="D34" s="173" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F34" s="173" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="G34" s="173" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H34" s="172"/>
       <c r="I34" s="174" t="s">
@@ -5402,7 +5399,7 @@
     </row>
     <row r="36" spans="1:19" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="92" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B36" s="173" t="s">
         <v>179</v>
@@ -5411,7 +5408,7 @@
         <v>208</v>
       </c>
       <c r="F36" s="152" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="G36" s="173" t="s">
         <v>149</v>
@@ -5487,13 +5484,13 @@
         <v>188</v>
       </c>
       <c r="D40" s="102" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F40" s="102" t="s">
         <v>72</v>
       </c>
       <c r="G40" s="102" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H40" s="106"/>
       <c r="I40" s="107" t="s">
@@ -5689,7 +5686,7 @@
     </row>
     <row r="57" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="93" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B57" s="156" t="s">
         <v>139</v>
@@ -5698,7 +5695,7 @@
         <v>283</v>
       </c>
       <c r="F57" s="156" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="G57" s="156" t="s">
         <v>121</v>
@@ -5711,7 +5708,7 @@
     <row r="58" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="93"/>
       <c r="B58" s="178" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C58" s="178"/>
       <c r="D58" s="178"/>
@@ -5732,7 +5729,7 @@
         <v>283</v>
       </c>
       <c r="F59" s="109" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="H59" s="102" t="s">
         <v>77</v>
@@ -5742,7 +5739,7 @@
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="93"/>
       <c r="B60" s="178" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C60" s="178"/>
       <c r="D60" s="178"/>
@@ -5754,7 +5751,7 @@
     </row>
     <row r="61" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="156" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B61" s="156" t="s">
         <v>114</v>
@@ -5763,7 +5760,7 @@
         <v>283</v>
       </c>
       <c r="F61" s="109" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="G61" s="156" t="s">
         <v>115</v>
@@ -5788,7 +5785,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="93" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B63" s="156" t="s">
         <v>139</v>
@@ -5807,7 +5804,7 @@
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="93"/>
       <c r="B64" s="178" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C64" s="178"/>
       <c r="D64" s="178"/>
@@ -5828,7 +5825,7 @@
         <v>283</v>
       </c>
       <c r="F65" s="102" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="G65" s="102" t="s">
         <v>115</v>
@@ -5981,7 +5978,7 @@
         <v>293</v>
       </c>
       <c r="B77" s="113" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E77" s="113" t="s">
         <v>291</v>
@@ -6045,7 +6042,7 @@
     </row>
     <row r="82" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="121" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.2">
@@ -6053,7 +6050,7 @@
         <v>484</v>
       </c>
       <c r="B83" s="102" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D83" s="102" t="s">
         <v>486</v>
@@ -6125,18 +6122,18 @@
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89" s="95" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B89" s="117" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C89" s="117"/>
       <c r="D89" s="122" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E89" s="117"/>
       <c r="F89" s="117" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="G89" s="125" t="s">
         <v>149</v>
@@ -6160,7 +6157,7 @@
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90" s="95" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B90" s="102" t="s">
         <v>173</v>
@@ -6171,7 +6168,7 @@
       </c>
       <c r="E90" s="117"/>
       <c r="F90" s="117" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G90" s="117"/>
       <c r="H90" s="117" t="s">
@@ -6191,7 +6188,7 @@
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91" s="95" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B91" s="125" t="s">
         <v>179</v>
@@ -6200,7 +6197,7 @@
         <v>141</v>
       </c>
       <c r="D91" s="117" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E91" s="117"/>
       <c r="F91" s="117" t="s">
@@ -6224,7 +6221,7 @@
     </row>
     <row r="92" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="95" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B92" s="116" t="s">
         <v>222</v>
@@ -6233,7 +6230,7 @@
         <v>188</v>
       </c>
       <c r="D92" s="117" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E92" s="117"/>
       <c r="F92" s="117" t="s">
@@ -6258,7 +6255,7 @@
     <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93" s="93"/>
       <c r="B93" s="180" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C93" s="180"/>
       <c r="D93" s="180"/>
@@ -6272,10 +6269,10 @@
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94" s="95" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B94" s="116" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C94" s="117"/>
       <c r="D94" s="117" t="s">
@@ -6283,7 +6280,7 @@
       </c>
       <c r="E94" s="117"/>
       <c r="F94" s="117" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G94" s="117"/>
       <c r="H94" s="117" t="s">
@@ -6304,7 +6301,7 @@
     <row r="95" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A95" s="93"/>
       <c r="B95" s="180" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C95" s="180"/>
       <c r="D95" s="180"/>
@@ -6336,7 +6333,7 @@
         <v>279</v>
       </c>
       <c r="B99" s="102" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C99" s="102" t="s">
         <v>188</v>
@@ -6427,7 +6424,7 @@
     </row>
     <row r="105" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="92" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B105" s="156" t="s">
         <v>179</v>
@@ -6436,13 +6433,13 @@
         <v>188</v>
       </c>
       <c r="D105" s="156" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F105" s="156" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="G105" s="156" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H105" s="156" t="s">
         <v>79</v>
@@ -6454,7 +6451,7 @@
     <row r="106" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="93"/>
       <c r="B106" s="178" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C106" s="178"/>
       <c r="D106" s="178"/>
@@ -6472,7 +6469,7 @@
         <v>179</v>
       </c>
       <c r="F107" s="156" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="H107" s="156" t="s">
         <v>79</v>
@@ -6482,7 +6479,7 @@
     <row r="108" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="93"/>
       <c r="B108" s="180" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C108" s="180"/>
       <c r="D108" s="180"/>
@@ -6526,13 +6523,13 @@
     </row>
     <row r="111" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="156" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B111" s="156" t="s">
         <v>179</v>
       </c>
       <c r="F111" s="156" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="H111" s="156" t="s">
         <v>79</v>
@@ -6577,7 +6574,7 @@
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="93"/>
       <c r="B114" s="180" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C114" s="180"/>
       <c r="D114" s="180"/>
@@ -6636,7 +6633,7 @@
         <v>260</v>
       </c>
       <c r="B118" s="92" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C118" s="102" t="s">
         <v>188</v>
@@ -6659,10 +6656,10 @@
     </row>
     <row r="119" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A119" s="96" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B119" s="92" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C119" s="102" t="s">
         <v>188</v>
@@ -6671,7 +6668,7 @@
         <v>285</v>
       </c>
       <c r="F119" s="105" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G119" s="102" t="s">
         <v>258</v>
@@ -6686,7 +6683,7 @@
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="93"/>
       <c r="B120" s="178" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C120" s="178"/>
       <c r="D120" s="178"/>
@@ -6729,10 +6726,10 @@
     </row>
     <row r="124" spans="1:9" s="168" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="93" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B124" s="116" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C124" s="167" t="s">
         <v>188</v>
@@ -6742,7 +6739,7 @@
       </c>
       <c r="E124" s="167"/>
       <c r="F124" s="168" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G124" s="170" t="s">
         <v>258</v>
@@ -6914,10 +6911,10 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="123" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B139" s="125" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C139" s="102" t="s">
         <v>141</v>
@@ -6926,13 +6923,13 @@
         <v>285</v>
       </c>
       <c r="F139" s="105" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="G139" s="102" t="s">
         <v>258</v>
       </c>
       <c r="H139" s="118" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I139" s="102" t="s">
         <v>306</v>
@@ -6951,10 +6948,10 @@
     </row>
     <row r="141" spans="1:9" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="123" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B141" s="125" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C141" s="125" t="s">
         <v>188</v>
@@ -6963,13 +6960,13 @@
         <v>285</v>
       </c>
       <c r="F141" s="105" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="G141" s="125" t="s">
         <v>258</v>
       </c>
       <c r="H141" s="118" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I141" s="125" t="s">
         <v>306</v>
@@ -6977,7 +6974,7 @@
     </row>
     <row r="142" spans="1:9" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="123" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B142" s="92" t="s">
         <v>277</v>
@@ -6989,13 +6986,13 @@
         <v>285</v>
       </c>
       <c r="F142" s="105" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G142" s="125" t="s">
         <v>258</v>
       </c>
       <c r="H142" s="118" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I142" s="125" t="s">
         <v>306</v>
@@ -7004,7 +7001,7 @@
     <row r="143" spans="1:9" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="93"/>
       <c r="B143" s="178" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C143" s="178"/>
       <c r="D143" s="178"/>
@@ -7016,7 +7013,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="123" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B144" s="92" t="s">
         <v>277</v>
@@ -7028,13 +7025,13 @@
         <v>285</v>
       </c>
       <c r="F144" s="105" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G144" s="102" t="s">
         <v>258</v>
       </c>
       <c r="H144" s="118" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I144" s="102" t="s">
         <v>306</v>
@@ -7125,19 +7122,19 @@
         <v>192</v>
       </c>
       <c r="B151" s="102" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D151" s="102" t="s">
         <v>284</v>
       </c>
       <c r="F151" s="102" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G151" s="102" t="s">
         <v>149</v>
       </c>
       <c r="H151" s="92" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
@@ -7544,8 +7541,8 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5:F10"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7562,7 +7559,7 @@
     <col min="10" max="10" width="77.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>225</v>
       </c>
@@ -7579,10 +7576,10 @@
         <v>296</v>
       </c>
       <c r="F1" s="40" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="H1" s="40" t="s">
         <v>308</v>
@@ -7591,9 +7588,9 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B2" s="72"/>
       <c r="C2" s="52"/>
@@ -7604,7 +7601,7 @@
       <c r="H2" s="47"/>
       <c r="I2" s="47"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="43" t="s">
         <v>297</v>
       </c>
@@ -7630,7 +7627,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="43" t="s">
         <v>298</v>
       </c>
@@ -7656,7 +7653,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="43" t="s">
         <v>230</v>
       </c>
@@ -7683,7 +7680,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="43" t="s">
         <v>229</v>
       </c>
@@ -7710,7 +7707,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="43" t="s">
         <v>231</v>
       </c>
@@ -7737,7 +7734,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="43" t="s">
         <v>233</v>
       </c>
@@ -7763,11 +7760,8 @@
       <c r="I8" s="44">
         <v>160</v>
       </c>
-      <c r="J8" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="43" t="s">
         <v>299</v>
       </c>
@@ -7793,7 +7787,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="43" t="s">
         <v>300</v>
       </c>
@@ -7819,10 +7813,10 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="43"/>
     </row>
-    <row r="12" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
         <v>464</v>
       </c>
@@ -7835,7 +7829,7 @@
       <c r="H12" s="47"/>
       <c r="I12" s="47"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="43" t="s">
         <v>226</v>
       </c>
@@ -7862,7 +7856,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="43" t="s">
         <v>227</v>
       </c>
@@ -7889,7 +7883,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="43" t="s">
         <v>228</v>
       </c>
@@ -7916,7 +7910,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="43" t="s">
         <v>232</v>
       </c>
@@ -8114,7 +8108,7 @@
         <v>225</v>
       </c>
       <c r="J26" s="71" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -8123,7 +8117,7 @@
     </row>
     <row r="28" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="46" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B28" s="72"/>
       <c r="C28" s="52"/>
@@ -8148,10 +8142,10 @@
         <v>120</v>
       </c>
       <c r="F29" s="44">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="G29" s="44">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="H29" s="44">
         <v>1200</v>
@@ -8177,10 +8171,10 @@
         <v>140</v>
       </c>
       <c r="F30" s="44">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="G30" s="175">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="H30" s="175">
         <v>1000</v>
@@ -8207,10 +8201,10 @@
         <v>150</v>
       </c>
       <c r="F31" s="44">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="G31" s="175">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="H31" s="175">
         <v>1000</v>
@@ -8237,7 +8231,7 @@
         <v>140</v>
       </c>
       <c r="F32" s="44">
-        <v>1200</v>
+        <v>1150</v>
       </c>
       <c r="G32" s="175">
         <v>130</v>
@@ -8754,7 +8748,7 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="189"/>
       <c r="B9" s="184" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C9" s="185"/>
     </row>
@@ -8904,13 +8898,13 @@
         <v>182</v>
       </c>
       <c r="D1" s="126" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E1" s="126" t="s">
         <v>470</v>
       </c>
       <c r="F1" s="126" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -8965,14 +8959,14 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B6" s="127"/>
       <c r="C6" s="127"/>
       <c r="D6" s="127"/>
       <c r="E6" s="127"/>
       <c r="F6" s="127" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -9122,7 +9116,7 @@
         <v>512</v>
       </c>
       <c r="G1" s="42" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="64" customFormat="1" ht="14" x14ac:dyDescent="0.2">
@@ -9139,10 +9133,10 @@
         <v>478</v>
       </c>
       <c r="F2" s="65" t="s">
-        <v>549</v>
+        <v>706</v>
       </c>
       <c r="G2" s="64" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Use latest gpustat (from github, not PyPi).
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="1600" windowWidth="25540" windowHeight="10900" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="60" yWindow="1740" windowWidth="25540" windowHeight="10900" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="708">
   <si>
     <t>Miners (AMD)</t>
   </si>
@@ -2157,6 +2157,9 @@
   </si>
   <si>
     <t>https://whattomine.com/coins?utf8=%E2%9C%93&amp;adapt_q_280x=0&amp;adapt_q_380=0&amp;adapt_q_fury=0&amp;adapt_q_470=0&amp;adapt_q_480=0&amp;adapt_q_570=0&amp;adapt_q_580=0&amp;adapt_q_vega56=0&amp;adapt_q_vega64=0&amp;adapt_q_750Ti=0&amp;adapt_q_1050Ti=0&amp;adapt_q_10606=0&amp;adapt_q_1070=0&amp;adapt_q_1070Ti=3&amp;adapt_1070Ti=true&amp;adapt_q_1080=0&amp;adapt_q_1080Ti=1&amp;adapt_1080Ti=true&amp;eth=true&amp;factor%5Beth_hr%5D=126.50&amp;factor%5Beth_p%5D=545.00&amp;grof=true&amp;factor%5Bgro_hr%5D=167.50&amp;factor%5Bgro_p%5D=570.00&amp;phi=true&amp;factor%5Bphi_hr%5D=99.00&amp;factor%5Bphi_p%5D=590.00&amp;cn=true&amp;factor%5Bcn_hr%5D=2720.00&amp;factor%5Bcn_p%5D=410.00&amp;cn7=true&amp;factor%5Bcn7_hr%5D=2720.00&amp;factor%5Bcn7_p%5D=410.00&amp;eq=true&amp;factor%5Beq_hr%5D=2095.00&amp;factor%5Beq_p%5D=550.00&amp;lre=true&amp;factor%5Blrev2_hr%5D=187000.00&amp;factor%5Blrev2_p%5D=550.00&amp;ns=true&amp;factor%5Bns_hr%5D=4550.00&amp;factor%5Bns_p%5D=550.00&amp;tt10=true&amp;factor%5Btt10_hr%5D=88.50&amp;factor%5Btt10_p%5D=560.00&amp;x16r=true&amp;factor%5Bx16r_hr%5D=45.00&amp;factor%5Bx16r_p%5D=565.00&amp;factor%5Bl2z_hr%5D=9.00&amp;factor%5Bl2z_p%5D=500.00&amp;n5=true&amp;factor%5Bn5_hr%5D=225.00&amp;factor%5Bn5_p%5D=550.00&amp;xn=true&amp;factor%5Bxn_hr%5D=16.10&amp;factor%5Bxn_p%5D=550.00&amp;factor%5Bcost%5D=0.0945&amp;sort=Profitability24&amp;volume=0&amp;revenue=24h&amp;factor%5Bexchanges%5D%5B%5D=&amp;factor%5Bexchanges%5D%5B%5D=binance&amp;factor%5Bexchanges%5D%5B%5D=bitfinex&amp;factor%5Bexchanges%5D%5B%5D=bittrex&amp;factor%5Bexchanges%5D%5B%5D=cryptobridge&amp;factor%5Bexchanges%5D%5B%5D=cryptopia&amp;factor%5Bexchanges%5D%5B%5D=hitbtc&amp;factor%5Bexchanges%5D%5B%5D=poloniex&amp;factor%5Bexchanges%5D%5B%5D=yobit&amp;dataset=Titans&amp;commit=Calculate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $GPUS -epool $URL_PORT -ewal $WALLET.$WORKER_NAME -eworker $WALLET.$WORKER_NAME -esm 2 -epsw $PSW -allpools 1 -allcoins 1 -mode 1 -lidag 0 -asm 0 -mport 0</t>
   </si>
 </sst>
 </file>
@@ -2667,7 +2670,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3163,24 +3166,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
@@ -3205,8 +3216,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4191,8 +4200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4460,10 +4469,10 @@
         <v>614</v>
       </c>
       <c r="E15" s="83"/>
-      <c r="F15" s="177" t="s">
+      <c r="F15" s="181" t="s">
         <v>449</v>
       </c>
-      <c r="G15" s="177"/>
+      <c r="G15" s="181"/>
     </row>
     <row r="16" spans="1:7" s="100" customFormat="1" ht="50" x14ac:dyDescent="0.2">
       <c r="A16" s="100" t="s">
@@ -4878,11 +4887,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S171"/>
+  <dimension ref="A1:S172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35:I35"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4944,16 +4953,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="93"/>
-      <c r="B3" s="180" t="s">
+      <c r="B3" s="182" t="s">
         <v>503</v>
       </c>
-      <c r="C3" s="180"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="180"/>
-      <c r="F3" s="179"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="179"/>
-      <c r="I3" s="179"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="183"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="89" t="s">
@@ -5010,15 +5019,15 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="180" t="s">
+      <c r="B10" s="182" t="s">
         <v>217</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="180"/>
-      <c r="E10" s="179"/>
-      <c r="F10" s="179"/>
-      <c r="G10" s="179"/>
-      <c r="H10" s="179"/>
+      <c r="C10" s="182"/>
+      <c r="D10" s="182"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="183"/>
+      <c r="H10" s="183"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="90" t="s">
@@ -5038,15 +5047,15 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="180" t="s">
+      <c r="B12" s="182" t="s">
         <v>217</v>
       </c>
-      <c r="C12" s="180"/>
-      <c r="D12" s="180"/>
-      <c r="E12" s="179"/>
-      <c r="F12" s="179"/>
-      <c r="G12" s="179"/>
-      <c r="H12" s="179"/>
+      <c r="C12" s="182"/>
+      <c r="D12" s="182"/>
+      <c r="E12" s="183"/>
+      <c r="F12" s="183"/>
+      <c r="G12" s="183"/>
+      <c r="H12" s="183"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="89" t="s">
@@ -5066,15 +5075,15 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="180" t="s">
+      <c r="B14" s="182" t="s">
         <v>217</v>
       </c>
-      <c r="C14" s="180"/>
-      <c r="D14" s="180"/>
-      <c r="E14" s="179"/>
-      <c r="F14" s="179"/>
-      <c r="G14" s="179"/>
-      <c r="H14" s="179"/>
+      <c r="C14" s="182"/>
+      <c r="D14" s="182"/>
+      <c r="E14" s="183"/>
+      <c r="F14" s="183"/>
+      <c r="G14" s="183"/>
+      <c r="H14" s="183"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="89" t="s">
@@ -5091,15 +5100,15 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="180" t="s">
+      <c r="B16" s="182" t="s">
         <v>198</v>
       </c>
-      <c r="C16" s="180"/>
-      <c r="D16" s="180"/>
-      <c r="E16" s="179"/>
-      <c r="F16" s="179"/>
-      <c r="G16" s="179"/>
-      <c r="H16" s="179"/>
+      <c r="C16" s="182"/>
+      <c r="D16" s="182"/>
+      <c r="E16" s="183"/>
+      <c r="F16" s="183"/>
+      <c r="G16" s="183"/>
+      <c r="H16" s="183"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="91" t="s">
@@ -5138,16 +5147,16 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="180" t="s">
+      <c r="B19" s="182" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="180"/>
-      <c r="D19" s="180"/>
-      <c r="E19" s="180"/>
-      <c r="F19" s="179"/>
-      <c r="G19" s="179"/>
-      <c r="H19" s="179"/>
-      <c r="I19" s="179"/>
+      <c r="C19" s="182"/>
+      <c r="D19" s="182"/>
+      <c r="E19" s="182"/>
+      <c r="F19" s="183"/>
+      <c r="G19" s="183"/>
+      <c r="H19" s="183"/>
+      <c r="I19" s="183"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="89" t="s">
@@ -5279,16 +5288,16 @@
     </row>
     <row r="30" spans="1:9" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="93"/>
-      <c r="B30" s="178" t="s">
+      <c r="B30" s="184" t="s">
         <v>693</v>
       </c>
-      <c r="C30" s="178"/>
-      <c r="D30" s="178"/>
-      <c r="E30" s="178"/>
-      <c r="F30" s="179"/>
-      <c r="G30" s="179"/>
-      <c r="H30" s="179"/>
-      <c r="I30" s="179"/>
+      <c r="C30" s="184"/>
+      <c r="D30" s="184"/>
+      <c r="E30" s="184"/>
+      <c r="F30" s="183"/>
+      <c r="G30" s="183"/>
+      <c r="H30" s="183"/>
+      <c r="I30" s="183"/>
     </row>
     <row r="31" spans="1:9" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="92" t="s">
@@ -5386,16 +5395,16 @@
     </row>
     <row r="35" spans="1:19" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="93"/>
-      <c r="B35" s="178" t="s">
+      <c r="B35" s="184" t="s">
         <v>494</v>
       </c>
-      <c r="C35" s="178"/>
-      <c r="D35" s="178"/>
-      <c r="E35" s="178"/>
-      <c r="F35" s="179"/>
-      <c r="G35" s="179"/>
-      <c r="H35" s="179"/>
-      <c r="I35" s="179"/>
+      <c r="C35" s="184"/>
+      <c r="D35" s="184"/>
+      <c r="E35" s="184"/>
+      <c r="F35" s="183"/>
+      <c r="G35" s="183"/>
+      <c r="H35" s="183"/>
+      <c r="I35" s="183"/>
     </row>
     <row r="36" spans="1:19" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="92" t="s">
@@ -5420,16 +5429,16 @@
     </row>
     <row r="37" spans="1:19" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="93"/>
-      <c r="B37" s="178" t="s">
+      <c r="B37" s="184" t="s">
         <v>240</v>
       </c>
-      <c r="C37" s="178"/>
-      <c r="D37" s="178"/>
-      <c r="E37" s="178"/>
-      <c r="F37" s="179"/>
-      <c r="G37" s="179"/>
-      <c r="H37" s="179"/>
-      <c r="I37" s="179"/>
+      <c r="C37" s="184"/>
+      <c r="D37" s="184"/>
+      <c r="E37" s="184"/>
+      <c r="F37" s="183"/>
+      <c r="G37" s="183"/>
+      <c r="H37" s="183"/>
+      <c r="I37" s="183"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="92" t="s">
@@ -5452,16 +5461,16 @@
     </row>
     <row r="39" spans="1:19" s="156" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="93"/>
-      <c r="B39" s="178" t="s">
+      <c r="B39" s="184" t="s">
         <v>262</v>
       </c>
-      <c r="C39" s="178"/>
-      <c r="D39" s="178"/>
-      <c r="E39" s="178"/>
-      <c r="F39" s="178"/>
-      <c r="G39" s="178"/>
-      <c r="H39" s="178"/>
-      <c r="I39" s="178"/>
+      <c r="C39" s="184"/>
+      <c r="D39" s="184"/>
+      <c r="E39" s="184"/>
+      <c r="F39" s="184"/>
+      <c r="G39" s="184"/>
+      <c r="H39" s="184"/>
+      <c r="I39" s="184"/>
       <c r="J39" s="102"/>
       <c r="K39" s="102"/>
       <c r="L39" s="102"/>
@@ -5481,7 +5490,7 @@
         <v>179</v>
       </c>
       <c r="C40" s="102" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="D40" s="102" t="s">
         <v>526</v>
@@ -5499,16 +5508,16 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="93"/>
-      <c r="B41" s="178" t="s">
+      <c r="B41" s="184" t="s">
         <v>494</v>
       </c>
-      <c r="C41" s="178"/>
-      <c r="D41" s="178"/>
-      <c r="E41" s="178"/>
-      <c r="F41" s="179"/>
-      <c r="G41" s="179"/>
-      <c r="H41" s="179"/>
-      <c r="I41" s="179"/>
+      <c r="C41" s="184"/>
+      <c r="D41" s="184"/>
+      <c r="E41" s="184"/>
+      <c r="F41" s="183"/>
+      <c r="G41" s="183"/>
+      <c r="H41" s="183"/>
+      <c r="I41" s="183"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="92" t="s">
@@ -5533,16 +5542,16 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="93"/>
-      <c r="B43" s="178" t="s">
+      <c r="B43" s="184" t="s">
         <v>240</v>
       </c>
-      <c r="C43" s="178"/>
-      <c r="D43" s="178"/>
-      <c r="E43" s="178"/>
-      <c r="F43" s="179"/>
-      <c r="G43" s="179"/>
-      <c r="H43" s="179"/>
-      <c r="I43" s="179"/>
+      <c r="C43" s="184"/>
+      <c r="D43" s="184"/>
+      <c r="E43" s="184"/>
+      <c r="F43" s="183"/>
+      <c r="G43" s="183"/>
+      <c r="H43" s="183"/>
+      <c r="I43" s="183"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="93" t="s">
@@ -5564,15 +5573,15 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="93"/>
-      <c r="B45" s="180" t="s">
+      <c r="B45" s="182" t="s">
         <v>242</v>
       </c>
-      <c r="C45" s="180"/>
-      <c r="D45" s="180"/>
-      <c r="E45" s="180"/>
-      <c r="F45" s="179"/>
-      <c r="G45" s="179"/>
-      <c r="H45" s="179"/>
+      <c r="C45" s="182"/>
+      <c r="D45" s="182"/>
+      <c r="E45" s="182"/>
+      <c r="F45" s="183"/>
+      <c r="G45" s="183"/>
+      <c r="H45" s="183"/>
       <c r="I45" s="106"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
@@ -5593,16 +5602,16 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="93"/>
-      <c r="B47" s="178" t="s">
+      <c r="B47" s="184" t="s">
         <v>167</v>
       </c>
-      <c r="C47" s="178"/>
-      <c r="D47" s="178"/>
-      <c r="E47" s="178"/>
-      <c r="F47" s="179"/>
-      <c r="G47" s="179"/>
-      <c r="H47" s="179"/>
-      <c r="I47" s="179"/>
+      <c r="C47" s="184"/>
+      <c r="D47" s="184"/>
+      <c r="E47" s="184"/>
+      <c r="F47" s="183"/>
+      <c r="G47" s="183"/>
+      <c r="H47" s="183"/>
+      <c r="I47" s="183"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="93" t="s">
@@ -5617,15 +5626,15 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="93"/>
-      <c r="B49" s="180" t="s">
+      <c r="B49" s="182" t="s">
         <v>495</v>
       </c>
-      <c r="C49" s="180"/>
-      <c r="D49" s="180"/>
-      <c r="E49" s="180"/>
-      <c r="F49" s="179"/>
-      <c r="G49" s="179"/>
-      <c r="H49" s="179"/>
+      <c r="C49" s="182"/>
+      <c r="D49" s="182"/>
+      <c r="E49" s="182"/>
+      <c r="F49" s="183"/>
+      <c r="G49" s="183"/>
+      <c r="H49" s="183"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="102" t="s">
@@ -5648,15 +5657,15 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="93"/>
-      <c r="B52" s="180" t="s">
+      <c r="B52" s="182" t="s">
         <v>495</v>
       </c>
-      <c r="C52" s="180"/>
-      <c r="D52" s="180"/>
-      <c r="E52" s="180"/>
-      <c r="F52" s="179"/>
-      <c r="G52" s="179"/>
-      <c r="H52" s="179"/>
+      <c r="C52" s="182"/>
+      <c r="D52" s="182"/>
+      <c r="E52" s="182"/>
+      <c r="F52" s="183"/>
+      <c r="G52" s="183"/>
+      <c r="H52" s="183"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="93" t="s">
@@ -5707,16 +5716,16 @@
     </row>
     <row r="58" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="93"/>
-      <c r="B58" s="178" t="s">
+      <c r="B58" s="184" t="s">
         <v>676</v>
       </c>
-      <c r="C58" s="178"/>
-      <c r="D58" s="178"/>
-      <c r="E58" s="178"/>
-      <c r="F58" s="179"/>
-      <c r="G58" s="179"/>
-      <c r="H58" s="179"/>
-      <c r="I58" s="179"/>
+      <c r="C58" s="184"/>
+      <c r="D58" s="184"/>
+      <c r="E58" s="184"/>
+      <c r="F58" s="183"/>
+      <c r="G58" s="183"/>
+      <c r="H58" s="183"/>
+      <c r="I58" s="183"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="102" t="s">
@@ -5738,15 +5747,15 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="93"/>
-      <c r="B60" s="178" t="s">
+      <c r="B60" s="184" t="s">
         <v>670</v>
       </c>
-      <c r="C60" s="178"/>
-      <c r="D60" s="178"/>
-      <c r="E60" s="178"/>
-      <c r="F60" s="179"/>
-      <c r="G60" s="179"/>
-      <c r="H60" s="179"/>
+      <c r="C60" s="184"/>
+      <c r="D60" s="184"/>
+      <c r="E60" s="184"/>
+      <c r="F60" s="183"/>
+      <c r="G60" s="183"/>
+      <c r="H60" s="183"/>
       <c r="I60" s="106"/>
     </row>
     <row r="61" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
@@ -5772,15 +5781,15 @@
     </row>
     <row r="62" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="93"/>
-      <c r="B62" s="180" t="s">
+      <c r="B62" s="182" t="s">
         <v>496</v>
       </c>
-      <c r="C62" s="180"/>
-      <c r="D62" s="180"/>
-      <c r="E62" s="180"/>
-      <c r="F62" s="179"/>
-      <c r="G62" s="179"/>
-      <c r="H62" s="179"/>
+      <c r="C62" s="182"/>
+      <c r="D62" s="182"/>
+      <c r="E62" s="182"/>
+      <c r="F62" s="183"/>
+      <c r="G62" s="183"/>
+      <c r="H62" s="183"/>
       <c r="I62" s="155"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -5803,16 +5812,16 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="93"/>
-      <c r="B64" s="178" t="s">
+      <c r="B64" s="184" t="s">
         <v>675</v>
       </c>
-      <c r="C64" s="178"/>
-      <c r="D64" s="178"/>
-      <c r="E64" s="178"/>
-      <c r="F64" s="179"/>
-      <c r="G64" s="179"/>
-      <c r="H64" s="179"/>
-      <c r="I64" s="179"/>
+      <c r="C64" s="184"/>
+      <c r="D64" s="184"/>
+      <c r="E64" s="184"/>
+      <c r="F64" s="183"/>
+      <c r="G64" s="183"/>
+      <c r="H64" s="183"/>
+      <c r="I64" s="183"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65" s="102" t="s">
@@ -5837,15 +5846,15 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66" s="93"/>
-      <c r="B66" s="180" t="s">
+      <c r="B66" s="182" t="s">
         <v>496</v>
       </c>
-      <c r="C66" s="180"/>
-      <c r="D66" s="180"/>
-      <c r="E66" s="180"/>
-      <c r="F66" s="179"/>
-      <c r="G66" s="179"/>
-      <c r="H66" s="179"/>
+      <c r="C66" s="182"/>
+      <c r="D66" s="182"/>
+      <c r="E66" s="182"/>
+      <c r="F66" s="183"/>
+      <c r="G66" s="183"/>
+      <c r="H66" s="183"/>
       <c r="I66" s="106"/>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.2">
@@ -5878,15 +5887,15 @@
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70" s="93"/>
-      <c r="B70" s="180" t="s">
+      <c r="B70" s="182" t="s">
         <v>97</v>
       </c>
-      <c r="C70" s="180"/>
-      <c r="D70" s="180"/>
-      <c r="E70" s="180"/>
-      <c r="F70" s="179"/>
-      <c r="G70" s="179"/>
-      <c r="H70" s="179"/>
+      <c r="C70" s="182"/>
+      <c r="D70" s="182"/>
+      <c r="E70" s="182"/>
+      <c r="F70" s="183"/>
+      <c r="G70" s="183"/>
+      <c r="H70" s="183"/>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71" s="102" t="s">
@@ -5922,15 +5931,15 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73" s="93"/>
-      <c r="B73" s="180" t="s">
+      <c r="B73" s="182" t="s">
         <v>97</v>
       </c>
-      <c r="C73" s="180"/>
-      <c r="D73" s="180"/>
-      <c r="E73" s="180"/>
-      <c r="F73" s="179"/>
-      <c r="G73" s="179"/>
-      <c r="H73" s="179"/>
+      <c r="C73" s="182"/>
+      <c r="D73" s="182"/>
+      <c r="E73" s="182"/>
+      <c r="F73" s="183"/>
+      <c r="G73" s="183"/>
+      <c r="H73" s="183"/>
     </row>
     <row r="74" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A74" s="96" t="s">
@@ -5957,16 +5966,16 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75" s="93"/>
-      <c r="B75" s="182" t="s">
+      <c r="B75" s="185" t="s">
         <v>286</v>
       </c>
-      <c r="C75" s="182"/>
-      <c r="D75" s="182"/>
-      <c r="E75" s="182"/>
-      <c r="F75" s="179"/>
-      <c r="G75" s="179"/>
-      <c r="H75" s="179"/>
-      <c r="I75" s="179"/>
+      <c r="C75" s="185"/>
+      <c r="D75" s="185"/>
+      <c r="E75" s="185"/>
+      <c r="F75" s="183"/>
+      <c r="G75" s="183"/>
+      <c r="H75" s="183"/>
+      <c r="I75" s="183"/>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A76" s="102" t="s">
@@ -6010,15 +6019,15 @@
     </row>
     <row r="79" spans="1:19" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="93"/>
-      <c r="B79" s="181" t="s">
+      <c r="B79" s="186" t="s">
         <v>289</v>
       </c>
-      <c r="C79" s="179"/>
-      <c r="D79" s="179"/>
-      <c r="E79" s="179"/>
-      <c r="F79" s="179"/>
-      <c r="G79" s="179"/>
-      <c r="H79" s="179"/>
+      <c r="C79" s="183"/>
+      <c r="D79" s="183"/>
+      <c r="E79" s="183"/>
+      <c r="F79" s="183"/>
+      <c r="G79" s="183"/>
+      <c r="H79" s="183"/>
     </row>
     <row r="80" spans="1:19" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="93" t="s">
@@ -6067,15 +6076,15 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84" s="93"/>
-      <c r="B84" s="180" t="s">
+      <c r="B84" s="182" t="s">
         <v>489</v>
       </c>
-      <c r="C84" s="180"/>
-      <c r="D84" s="180"/>
-      <c r="E84" s="180"/>
-      <c r="F84" s="179"/>
-      <c r="G84" s="179"/>
-      <c r="H84" s="179"/>
+      <c r="C84" s="182"/>
+      <c r="D84" s="182"/>
+      <c r="E84" s="182"/>
+      <c r="F84" s="183"/>
+      <c r="G84" s="183"/>
+      <c r="H84" s="183"/>
       <c r="I84" s="106" t="s">
         <v>131</v>
       </c>
@@ -6097,15 +6106,15 @@
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86" s="93"/>
-      <c r="B86" s="180" t="s">
+      <c r="B86" s="182" t="s">
         <v>497</v>
       </c>
-      <c r="C86" s="180"/>
-      <c r="D86" s="180"/>
-      <c r="E86" s="180"/>
-      <c r="F86" s="179"/>
-      <c r="G86" s="179"/>
-      <c r="H86" s="179"/>
+      <c r="C86" s="182"/>
+      <c r="D86" s="182"/>
+      <c r="E86" s="182"/>
+      <c r="F86" s="183"/>
+      <c r="G86" s="183"/>
+      <c r="H86" s="183"/>
       <c r="I86" s="106" t="s">
         <v>131</v>
       </c>
@@ -6190,8 +6199,8 @@
       <c r="A91" s="95" t="s">
         <v>530</v>
       </c>
-      <c r="B91" s="125" t="s">
-        <v>179</v>
+      <c r="B91" s="92" t="s">
+        <v>124</v>
       </c>
       <c r="C91" s="117" t="s">
         <v>141</v>
@@ -6203,7 +6212,9 @@
       <c r="F91" s="117" t="s">
         <v>223</v>
       </c>
-      <c r="G91" s="117"/>
+      <c r="G91" s="177" t="s">
+        <v>149</v>
+      </c>
       <c r="H91" s="117" t="s">
         <v>224</v>
       </c>
@@ -6219,444 +6230,433 @@
       <c r="R91" s="117"/>
       <c r="S91" s="117"/>
     </row>
-    <row r="92" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="95" t="s">
+    <row r="92" spans="1:19" s="177" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="93"/>
+      <c r="B92" s="182" t="s">
+        <v>707</v>
+      </c>
+      <c r="C92" s="182"/>
+      <c r="D92" s="182"/>
+      <c r="E92" s="182"/>
+      <c r="F92" s="183"/>
+      <c r="G92" s="183"/>
+      <c r="H92" s="183"/>
+      <c r="I92" s="178"/>
+    </row>
+    <row r="93" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="95" t="s">
         <v>530</v>
       </c>
-      <c r="B92" s="116" t="s">
+      <c r="B93" s="116" t="s">
         <v>222</v>
       </c>
-      <c r="C92" s="117" t="s">
+      <c r="C93" s="117" t="s">
         <v>188</v>
       </c>
-      <c r="D92" s="117" t="s">
+      <c r="D93" s="117" t="s">
         <v>526</v>
       </c>
-      <c r="E92" s="117"/>
-      <c r="F92" s="117" t="s">
+      <c r="E93" s="117"/>
+      <c r="F93" s="117" t="s">
         <v>223</v>
       </c>
-      <c r="G92" s="117"/>
-      <c r="H92" s="117" t="s">
+      <c r="G93" s="177" t="s">
+        <v>149</v>
+      </c>
+      <c r="H93" s="117" t="s">
         <v>224</v>
       </c>
-      <c r="I92" s="117"/>
-      <c r="J92" s="117"/>
-      <c r="K92" s="117"/>
-      <c r="L92" s="117"/>
-      <c r="M92" s="117"/>
-      <c r="N92" s="117"/>
-      <c r="O92" s="117"/>
-      <c r="P92" s="117"/>
-      <c r="Q92" s="117"/>
-      <c r="R92" s="117"/>
-      <c r="S92" s="117"/>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A93" s="93"/>
-      <c r="B93" s="180" t="s">
+      <c r="I93" s="117"/>
+      <c r="J93" s="117"/>
+      <c r="K93" s="117"/>
+      <c r="L93" s="117"/>
+      <c r="M93" s="117"/>
+      <c r="N93" s="117"/>
+      <c r="O93" s="117"/>
+      <c r="P93" s="117"/>
+      <c r="Q93" s="117"/>
+      <c r="R93" s="117"/>
+      <c r="S93" s="117"/>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A94" s="93"/>
+      <c r="B94" s="182" t="s">
         <v>543</v>
       </c>
-      <c r="C93" s="180"/>
-      <c r="D93" s="180"/>
-      <c r="E93" s="180"/>
-      <c r="F93" s="179"/>
-      <c r="G93" s="179"/>
-      <c r="H93" s="179"/>
-      <c r="I93" s="106" t="s">
+      <c r="C94" s="182"/>
+      <c r="D94" s="182"/>
+      <c r="E94" s="182"/>
+      <c r="F94" s="183"/>
+      <c r="G94" s="183"/>
+      <c r="H94" s="183"/>
+      <c r="I94" s="106" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A94" s="95" t="s">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A95" s="95" t="s">
         <v>531</v>
       </c>
-      <c r="B94" s="116" t="s">
+      <c r="B95" s="116" t="s">
         <v>518</v>
       </c>
-      <c r="C94" s="117"/>
-      <c r="D94" s="117" t="s">
+      <c r="C95" s="117"/>
+      <c r="D95" s="117" t="s">
         <v>486</v>
       </c>
-      <c r="E94" s="117"/>
-      <c r="F94" s="117" t="s">
+      <c r="E95" s="117"/>
+      <c r="F95" s="117" t="s">
         <v>542</v>
       </c>
-      <c r="G94" s="117"/>
-      <c r="H94" s="117" t="s">
+      <c r="G95" s="117"/>
+      <c r="H95" s="117" t="s">
         <v>224</v>
       </c>
-      <c r="I94" s="117"/>
-      <c r="J94" s="117"/>
-      <c r="K94" s="117"/>
-      <c r="L94" s="117"/>
-      <c r="M94" s="117"/>
-      <c r="N94" s="117"/>
-      <c r="O94" s="117"/>
-      <c r="P94" s="117"/>
-      <c r="Q94" s="117"/>
-      <c r="R94" s="117"/>
-      <c r="S94" s="117"/>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A95" s="93"/>
-      <c r="B95" s="180" t="s">
+      <c r="I95" s="117"/>
+      <c r="J95" s="117"/>
+      <c r="K95" s="117"/>
+      <c r="L95" s="117"/>
+      <c r="M95" s="117"/>
+      <c r="N95" s="117"/>
+      <c r="O95" s="117"/>
+      <c r="P95" s="117"/>
+      <c r="Q95" s="117"/>
+      <c r="R95" s="117"/>
+      <c r="S95" s="117"/>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A96" s="93"/>
+      <c r="B96" s="182" t="s">
         <v>541</v>
       </c>
-      <c r="C95" s="180"/>
-      <c r="D95" s="180"/>
-      <c r="E95" s="180"/>
-      <c r="F95" s="180"/>
-      <c r="G95" s="180"/>
-      <c r="H95" s="180"/>
-      <c r="I95" s="106" t="s">
+      <c r="C96" s="182"/>
+      <c r="D96" s="182"/>
+      <c r="E96" s="182"/>
+      <c r="F96" s="182"/>
+      <c r="G96" s="182"/>
+      <c r="H96" s="182"/>
+      <c r="I96" s="106" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A96" s="102" t="s">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="102" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" s="93" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="93" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="93" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A99" s="92" t="s">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" s="92" t="s">
         <v>279</v>
       </c>
-      <c r="B99" s="102" t="s">
+      <c r="B100" s="102" t="s">
         <v>518</v>
       </c>
-      <c r="C99" s="102" t="s">
+      <c r="C100" s="102" t="s">
         <v>188</v>
       </c>
-      <c r="D99" s="102" t="s">
+      <c r="D100" s="102" t="s">
         <v>284</v>
       </c>
-      <c r="F99" s="105" t="s">
+      <c r="F100" s="105" t="s">
         <v>280</v>
       </c>
-      <c r="H99" s="118" t="s">
+      <c r="H100" s="118" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A100" s="93"/>
-      <c r="B100" s="180" t="s">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" s="93"/>
+      <c r="B101" s="182" t="s">
         <v>282</v>
       </c>
-      <c r="C100" s="180"/>
-      <c r="D100" s="180"/>
-      <c r="E100" s="180"/>
-      <c r="F100" s="179"/>
-      <c r="G100" s="179"/>
-      <c r="H100" s="179"/>
-      <c r="I100" s="106" t="s">
+      <c r="C101" s="182"/>
+      <c r="D101" s="182"/>
+      <c r="E101" s="182"/>
+      <c r="F101" s="183"/>
+      <c r="G101" s="183"/>
+      <c r="H101" s="183"/>
+      <c r="I101" s="106" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A101" s="93" t="s">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="B101" s="102" t="s">
+      <c r="B102" s="102" t="s">
         <v>179</v>
       </c>
-      <c r="F101" s="102" t="s">
+      <c r="F102" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="G101" s="102" t="s">
+      <c r="G102" s="102" t="s">
         <v>149</v>
       </c>
-      <c r="H101" s="102" t="s">
+      <c r="H102" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="I101" s="106"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A102" s="93"/>
-      <c r="B102" s="180" t="s">
+      <c r="I102" s="106"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" s="93"/>
+      <c r="B103" s="182" t="s">
         <v>498</v>
       </c>
-      <c r="C102" s="180"/>
-      <c r="D102" s="180"/>
-      <c r="E102" s="180"/>
-      <c r="F102" s="179"/>
-      <c r="G102" s="179"/>
-      <c r="H102" s="179"/>
-      <c r="I102" s="106"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A103" s="93" t="s">
+      <c r="C103" s="182"/>
+      <c r="D103" s="182"/>
+      <c r="E103" s="182"/>
+      <c r="F103" s="183"/>
+      <c r="G103" s="183"/>
+      <c r="H103" s="183"/>
+      <c r="I103" s="106"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" s="93" t="s">
         <v>218</v>
       </c>
-      <c r="B103" s="102" t="s">
+      <c r="B104" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="F103" s="102" t="s">
+      <c r="F104" s="102" t="s">
         <v>80</v>
       </c>
-      <c r="G103" s="102" t="s">
+      <c r="G104" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="I103" s="106"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A104" s="93"/>
-      <c r="B104" s="180" t="s">
+      <c r="I104" s="106"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" s="93"/>
+      <c r="B105" s="182" t="s">
         <v>82</v>
       </c>
-      <c r="C104" s="180"/>
-      <c r="D104" s="180"/>
-      <c r="E104" s="180"/>
-      <c r="F104" s="179"/>
-      <c r="G104" s="179"/>
-      <c r="H104" s="179"/>
-      <c r="I104" s="106"/>
-    </row>
-    <row r="105" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="92" t="s">
+      <c r="C105" s="182"/>
+      <c r="D105" s="182"/>
+      <c r="E105" s="182"/>
+      <c r="F105" s="183"/>
+      <c r="G105" s="183"/>
+      <c r="H105" s="183"/>
+      <c r="I105" s="106"/>
+    </row>
+    <row r="106" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="92" t="s">
         <v>663</v>
       </c>
-      <c r="B105" s="156" t="s">
+      <c r="B106" s="156" t="s">
         <v>179</v>
       </c>
-      <c r="C105" s="156" t="s">
+      <c r="C106" s="156" t="s">
         <v>188</v>
       </c>
-      <c r="D105" s="156" t="s">
+      <c r="D106" s="156" t="s">
         <v>526</v>
       </c>
-      <c r="F105" s="156" t="s">
+      <c r="F106" s="156" t="s">
         <v>656</v>
       </c>
-      <c r="G105" s="156" t="s">
+      <c r="G106" s="156" t="s">
         <v>641</v>
       </c>
-      <c r="H105" s="156" t="s">
+      <c r="H106" s="156" t="s">
         <v>79</v>
       </c>
-      <c r="I105" s="157" t="s">
+      <c r="I106" s="157" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="106" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="93"/>
-      <c r="B106" s="178" t="s">
+    <row r="107" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="93"/>
+      <c r="B107" s="184" t="s">
         <v>655</v>
       </c>
-      <c r="C106" s="178"/>
-      <c r="D106" s="178"/>
-      <c r="E106" s="178"/>
-      <c r="F106" s="179"/>
-      <c r="G106" s="179"/>
-      <c r="H106" s="179"/>
-      <c r="I106" s="179"/>
-    </row>
-    <row r="107" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="156" t="s">
+      <c r="C107" s="184"/>
+      <c r="D107" s="184"/>
+      <c r="E107" s="184"/>
+      <c r="F107" s="183"/>
+      <c r="G107" s="183"/>
+      <c r="H107" s="183"/>
+      <c r="I107" s="183"/>
+    </row>
+    <row r="108" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="156" t="s">
         <v>55</v>
       </c>
-      <c r="B107" s="156" t="s">
+      <c r="B108" s="156" t="s">
         <v>179</v>
       </c>
-      <c r="F107" s="156" t="s">
+      <c r="F108" s="156" t="s">
         <v>650</v>
       </c>
-      <c r="H107" s="156" t="s">
+      <c r="H108" s="156" t="s">
         <v>79</v>
       </c>
-      <c r="I107" s="155"/>
-    </row>
-    <row r="108" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="93"/>
-      <c r="B108" s="180" t="s">
+      <c r="I108" s="155"/>
+    </row>
+    <row r="109" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="93"/>
+      <c r="B109" s="182" t="s">
         <v>664</v>
       </c>
-      <c r="C108" s="180"/>
-      <c r="D108" s="180"/>
-      <c r="E108" s="180"/>
-      <c r="F108" s="179"/>
-      <c r="G108" s="179"/>
-      <c r="H108" s="179"/>
-      <c r="I108" s="155" t="s">
+      <c r="C109" s="182"/>
+      <c r="D109" s="182"/>
+      <c r="E109" s="182"/>
+      <c r="F109" s="183"/>
+      <c r="G109" s="183"/>
+      <c r="H109" s="183"/>
+      <c r="I109" s="155" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A109" s="102" t="s">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" s="102" t="s">
         <v>248</v>
       </c>
-      <c r="B109" s="102" t="s">
+      <c r="B110" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="F109" s="102" t="s">
+      <c r="F110" s="102" t="s">
         <v>246</v>
       </c>
-      <c r="H109" s="102" t="s">
+      <c r="H110" s="102" t="s">
         <v>79</v>
       </c>
-      <c r="I109" s="106"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" s="93"/>
-      <c r="B110" s="180" t="s">
+      <c r="I110" s="106"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" s="93"/>
+      <c r="B111" s="182" t="s">
         <v>247</v>
       </c>
-      <c r="C110" s="180"/>
-      <c r="D110" s="180"/>
-      <c r="E110" s="180"/>
-      <c r="F110" s="179"/>
-      <c r="G110" s="179"/>
-      <c r="H110" s="179"/>
-      <c r="I110" s="106" t="s">
+      <c r="C111" s="182"/>
+      <c r="D111" s="182"/>
+      <c r="E111" s="182"/>
+      <c r="F111" s="183"/>
+      <c r="G111" s="183"/>
+      <c r="H111" s="183"/>
+      <c r="I111" s="106" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="111" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="156" t="s">
+    <row r="112" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="156" t="s">
         <v>649</v>
       </c>
-      <c r="B111" s="156" t="s">
+      <c r="B112" s="156" t="s">
         <v>179</v>
       </c>
-      <c r="F111" s="156" t="s">
+      <c r="F112" s="156" t="s">
         <v>645</v>
       </c>
-      <c r="H111" s="156" t="s">
+      <c r="H112" s="156" t="s">
         <v>79</v>
       </c>
-      <c r="I111" s="155"/>
-    </row>
-    <row r="112" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="93"/>
-      <c r="B112" s="180" t="s">
+      <c r="I112" s="155"/>
+    </row>
+    <row r="113" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="93"/>
+      <c r="B113" s="182" t="s">
         <v>93</v>
       </c>
-      <c r="C112" s="180"/>
-      <c r="D112" s="180"/>
-      <c r="E112" s="180"/>
-      <c r="F112" s="179"/>
-      <c r="G112" s="179"/>
-      <c r="H112" s="179"/>
-      <c r="I112" s="155" t="s">
+      <c r="C113" s="182"/>
+      <c r="D113" s="182"/>
+      <c r="E113" s="182"/>
+      <c r="F113" s="183"/>
+      <c r="G113" s="183"/>
+      <c r="H113" s="183"/>
+      <c r="I113" s="155" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A113" s="93" t="s">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" s="93" t="s">
         <v>186</v>
       </c>
-      <c r="B113" s="106" t="s">
+      <c r="B114" s="106" t="s">
         <v>114</v>
       </c>
-      <c r="C113" s="106"/>
-      <c r="D113" s="104" t="s">
+      <c r="C114" s="106"/>
+      <c r="D114" s="104" t="s">
         <v>283</v>
       </c>
-      <c r="E113" s="106"/>
-      <c r="F113" s="102" t="s">
+      <c r="E114" s="106"/>
+      <c r="F114" s="102" t="s">
         <v>187</v>
       </c>
-      <c r="G113" s="102" t="s">
+      <c r="G114" s="102" t="s">
         <v>175</v>
       </c>
-      <c r="I113" s="106"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A114" s="93"/>
-      <c r="B114" s="180" t="s">
+      <c r="I114" s="106"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" s="93"/>
+      <c r="B115" s="182" t="s">
         <v>612</v>
       </c>
-      <c r="C114" s="180"/>
-      <c r="D114" s="180"/>
-      <c r="E114" s="179"/>
-      <c r="F114" s="179"/>
-      <c r="G114" s="179"/>
-      <c r="H114" s="179"/>
-      <c r="I114" s="106"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A115" s="102" t="s">
+      <c r="C115" s="182"/>
+      <c r="D115" s="182"/>
+      <c r="E115" s="183"/>
+      <c r="F115" s="183"/>
+      <c r="G115" s="183"/>
+      <c r="H115" s="183"/>
+      <c r="I115" s="106"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" s="102" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A116" s="96" t="s">
+    <row r="117" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A117" s="96" t="s">
         <v>260</v>
       </c>
-      <c r="B116" s="92" t="s">
+      <c r="B117" s="92" t="s">
         <v>307</v>
       </c>
-      <c r="C116" s="102" t="s">
+      <c r="C117" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="D116" s="102" t="s">
+      <c r="D117" s="102" t="s">
         <v>285</v>
       </c>
-      <c r="F116" s="105" t="s">
+      <c r="F117" s="105" t="s">
         <v>275</v>
       </c>
-      <c r="G116" s="102" t="s">
+      <c r="G117" s="102" t="s">
         <v>258</v>
       </c>
-      <c r="H116" s="118" t="s">
+      <c r="H117" s="118" t="s">
         <v>276</v>
       </c>
-      <c r="I116" s="102" t="s">
+      <c r="I117" s="102" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A117" s="93"/>
-      <c r="B117" s="178" t="s">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" s="93"/>
+      <c r="B118" s="184" t="s">
         <v>490</v>
       </c>
-      <c r="C117" s="178"/>
-      <c r="D117" s="178"/>
-      <c r="E117" s="178"/>
-      <c r="F117" s="179"/>
-      <c r="G117" s="179"/>
-      <c r="H117" s="179"/>
-      <c r="I117" s="106"/>
-    </row>
-    <row r="118" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A118" s="96" t="s">
-        <v>260</v>
-      </c>
-      <c r="B118" s="92" t="s">
-        <v>613</v>
-      </c>
-      <c r="C118" s="102" t="s">
-        <v>188</v>
-      </c>
-      <c r="D118" s="102" t="s">
-        <v>285</v>
-      </c>
-      <c r="F118" s="105" t="s">
-        <v>275</v>
-      </c>
-      <c r="G118" s="102" t="s">
-        <v>258</v>
-      </c>
-      <c r="H118" s="118" t="s">
-        <v>276</v>
-      </c>
-      <c r="I118" s="102" t="s">
-        <v>306</v>
-      </c>
+      <c r="C118" s="184"/>
+      <c r="D118" s="184"/>
+      <c r="E118" s="184"/>
+      <c r="F118" s="183"/>
+      <c r="G118" s="183"/>
+      <c r="H118" s="183"/>
+      <c r="I118" s="106"/>
     </row>
     <row r="119" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A119" s="96" t="s">
-        <v>615</v>
+        <v>260</v>
       </c>
       <c r="B119" s="92" t="s">
         <v>613</v>
@@ -6668,7 +6668,7 @@
         <v>285</v>
       </c>
       <c r="F119" s="105" t="s">
-        <v>536</v>
+        <v>275</v>
       </c>
       <c r="G119" s="102" t="s">
         <v>258</v>
@@ -6680,304 +6680,304 @@
         <v>306</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A120" s="93"/>
-      <c r="B120" s="178" t="s">
+    <row r="120" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A120" s="96" t="s">
+        <v>615</v>
+      </c>
+      <c r="B120" s="92" t="s">
+        <v>613</v>
+      </c>
+      <c r="C120" s="102" t="s">
+        <v>188</v>
+      </c>
+      <c r="D120" s="102" t="s">
+        <v>285</v>
+      </c>
+      <c r="F120" s="105" t="s">
+        <v>536</v>
+      </c>
+      <c r="G120" s="102" t="s">
+        <v>258</v>
+      </c>
+      <c r="H120" s="118" t="s">
+        <v>276</v>
+      </c>
+      <c r="I120" s="102" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" s="93"/>
+      <c r="B121" s="184" t="s">
         <v>539</v>
       </c>
-      <c r="C120" s="178"/>
-      <c r="D120" s="178"/>
-      <c r="E120" s="178"/>
-      <c r="F120" s="179"/>
-      <c r="G120" s="179"/>
-      <c r="H120" s="179"/>
-      <c r="I120" s="106"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A121" s="102" t="s">
+      <c r="C121" s="184"/>
+      <c r="D121" s="184"/>
+      <c r="E121" s="184"/>
+      <c r="F121" s="183"/>
+      <c r="G121" s="183"/>
+      <c r="H121" s="183"/>
+      <c r="I121" s="106"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" s="102" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A122" s="93" t="s">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A123" s="93" t="s">
         <v>90</v>
       </c>
-      <c r="B122" s="102" t="s">
+      <c r="B123" s="102" t="s">
         <v>76</v>
       </c>
-      <c r="F122" s="102" t="s">
+      <c r="F123" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="G122" s="113" t="s">
+      <c r="G123" s="113" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A123" s="93"/>
-      <c r="B123" s="180" t="s">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" s="93"/>
+      <c r="B124" s="182" t="s">
         <v>92</v>
       </c>
-      <c r="C123" s="180"/>
-      <c r="D123" s="180"/>
-      <c r="E123" s="180"/>
-      <c r="F123" s="179"/>
-      <c r="G123" s="179"/>
-      <c r="H123" s="179"/>
-    </row>
-    <row r="124" spans="1:9" s="168" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="93" t="s">
+      <c r="C124" s="182"/>
+      <c r="D124" s="182"/>
+      <c r="E124" s="182"/>
+      <c r="F124" s="183"/>
+      <c r="G124" s="183"/>
+      <c r="H124" s="183"/>
+    </row>
+    <row r="125" spans="1:9" s="168" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="93" t="s">
         <v>687</v>
       </c>
-      <c r="B124" s="116" t="s">
+      <c r="B125" s="116" t="s">
         <v>613</v>
       </c>
-      <c r="C124" s="167" t="s">
+      <c r="C125" s="167" t="s">
         <v>188</v>
       </c>
-      <c r="D124" s="171" t="s">
+      <c r="D125" s="171" t="s">
         <v>284</v>
       </c>
-      <c r="E124" s="167"/>
-      <c r="F124" s="168" t="s">
+      <c r="E125" s="167"/>
+      <c r="F125" s="168" t="s">
         <v>690</v>
       </c>
-      <c r="G124" s="170" t="s">
+      <c r="G125" s="170" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A125" s="93" t="s">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" s="93" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A126" s="102" t="s">
-        <v>60</v>
-      </c>
-      <c r="B126" s="102" t="s">
-        <v>139</v>
-      </c>
-      <c r="D126" s="104" t="s">
-        <v>283</v>
-      </c>
-      <c r="F126" s="102" t="s">
-        <v>126</v>
-      </c>
-      <c r="H126" s="118" t="s">
-        <v>127</v>
-      </c>
-      <c r="I126" s="102" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="102" t="s">
+        <v>60</v>
+      </c>
+      <c r="B127" s="102" t="s">
+        <v>139</v>
+      </c>
+      <c r="D127" s="104" t="s">
+        <v>283</v>
+      </c>
+      <c r="F127" s="102" t="s">
+        <v>126</v>
+      </c>
+      <c r="H127" s="118" t="s">
+        <v>127</v>
+      </c>
+      <c r="I127" s="102" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A128" s="102" t="s">
         <v>117</v>
       </c>
-      <c r="B127" s="102" t="s">
+      <c r="B128" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="F127" s="102" t="s">
+      <c r="F128" s="102" t="s">
         <v>95</v>
       </c>
-      <c r="H127" s="102" t="s">
+      <c r="H128" s="102" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A128" s="93"/>
-      <c r="B128" s="180" t="s">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" s="93"/>
+      <c r="B129" s="182" t="s">
         <v>96</v>
       </c>
-      <c r="C128" s="180"/>
-      <c r="D128" s="180"/>
-      <c r="E128" s="180"/>
-      <c r="F128" s="179"/>
-      <c r="G128" s="179"/>
-      <c r="H128" s="179"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A129" s="93" t="s">
+      <c r="C129" s="182"/>
+      <c r="D129" s="182"/>
+      <c r="E129" s="182"/>
+      <c r="F129" s="183"/>
+      <c r="G129" s="183"/>
+      <c r="H129" s="183"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A130" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="B129" s="102" t="s">
+      <c r="B130" s="102" t="s">
         <v>76</v>
       </c>
-      <c r="F129" s="102" t="s">
+      <c r="F130" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="G129" s="102" t="s">
+      <c r="G130" s="102" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A130" s="102"/>
-      <c r="B130" s="180" t="s">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A131" s="102"/>
+      <c r="B131" s="182" t="s">
         <v>491</v>
       </c>
-      <c r="C130" s="180"/>
-      <c r="D130" s="180"/>
-      <c r="E130" s="180"/>
-      <c r="F130" s="179"/>
-      <c r="G130" s="179"/>
-      <c r="H130" s="179"/>
-      <c r="I130" s="179"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A131" s="97" t="s">
+      <c r="C131" s="182"/>
+      <c r="D131" s="182"/>
+      <c r="E131" s="182"/>
+      <c r="F131" s="183"/>
+      <c r="G131" s="183"/>
+      <c r="H131" s="183"/>
+      <c r="I131" s="183"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A132" s="97" t="s">
         <v>205</v>
       </c>
-      <c r="B131" s="106"/>
-      <c r="C131" s="106"/>
-      <c r="D131" s="106"/>
-      <c r="E131" s="106"/>
-      <c r="F131" s="102" t="s">
+      <c r="B132" s="106"/>
+      <c r="C132" s="106"/>
+      <c r="D132" s="106"/>
+      <c r="E132" s="106"/>
+      <c r="F132" s="102" t="s">
         <v>206</v>
       </c>
-      <c r="H131" s="105" t="s">
+      <c r="H132" s="105" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A132" s="93" t="s">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A133" s="93" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A133" s="102" t="s">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A134" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="B133" s="92" t="s">
+      <c r="B134" s="92" t="s">
         <v>144</v>
       </c>
-      <c r="C133" s="92"/>
-      <c r="D133" s="92"/>
-      <c r="E133" s="92" t="s">
+      <c r="C134" s="92"/>
+      <c r="D134" s="92"/>
+      <c r="E134" s="92" t="s">
         <v>145</v>
       </c>
-      <c r="F133" s="102" t="s">
+      <c r="F134" s="102" t="s">
         <v>132</v>
       </c>
-      <c r="H133" s="102" t="s">
+      <c r="H134" s="102" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A134" s="93"/>
-      <c r="B134" s="182" t="s">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A135" s="93"/>
+      <c r="B135" s="185" t="s">
         <v>488</v>
       </c>
-      <c r="C134" s="182"/>
-      <c r="D134" s="182"/>
-      <c r="E134" s="182"/>
-      <c r="F134" s="179"/>
-      <c r="G134" s="179"/>
-      <c r="H134" s="179"/>
-      <c r="I134" s="179"/>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A135" s="102" t="s">
-        <v>143</v>
-      </c>
-      <c r="B135" s="92" t="s">
-        <v>139</v>
-      </c>
-      <c r="C135" s="92"/>
-      <c r="D135" s="119" t="s">
-        <v>283</v>
-      </c>
-      <c r="E135" s="92"/>
-      <c r="F135" s="102" t="s">
-        <v>132</v>
-      </c>
-      <c r="H135" s="102" t="s">
-        <v>133</v>
-      </c>
+      <c r="C135" s="185"/>
+      <c r="D135" s="185"/>
+      <c r="E135" s="185"/>
+      <c r="F135" s="183"/>
+      <c r="G135" s="183"/>
+      <c r="H135" s="183"/>
+      <c r="I135" s="183"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="102" t="s">
-        <v>64</v>
+        <v>143</v>
+      </c>
+      <c r="B136" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="C136" s="92"/>
+      <c r="D136" s="119" t="s">
+        <v>283</v>
+      </c>
+      <c r="E136" s="92"/>
+      <c r="F136" s="102" t="s">
+        <v>132</v>
+      </c>
+      <c r="H136" s="102" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="102" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="102" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A139" s="102" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A139" s="123" t="s">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A140" s="123" t="s">
         <v>534</v>
       </c>
-      <c r="B139" s="125" t="s">
+      <c r="B140" s="125" t="s">
         <v>606</v>
       </c>
-      <c r="C139" s="102" t="s">
+      <c r="C140" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="D139" s="102" t="s">
+      <c r="D140" s="102" t="s">
         <v>285</v>
       </c>
-      <c r="F139" s="105" t="s">
+      <c r="F140" s="105" t="s">
         <v>607</v>
       </c>
-      <c r="G139" s="102" t="s">
+      <c r="G140" s="102" t="s">
         <v>258</v>
       </c>
-      <c r="H139" s="118" t="s">
+      <c r="H140" s="118" t="s">
         <v>533</v>
       </c>
-      <c r="I139" s="102" t="s">
+      <c r="I140" s="102" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A140" s="93"/>
-      <c r="B140" s="178"/>
-      <c r="C140" s="178"/>
-      <c r="D140" s="178"/>
-      <c r="E140" s="178"/>
-      <c r="F140" s="179"/>
-      <c r="G140" s="179"/>
-      <c r="H140" s="179"/>
-      <c r="I140" s="106"/>
-    </row>
-    <row r="141" spans="1:9" s="125" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="123" t="s">
-        <v>608</v>
-      </c>
-      <c r="B141" s="125" t="s">
-        <v>518</v>
-      </c>
-      <c r="C141" s="125" t="s">
-        <v>188</v>
-      </c>
-      <c r="D141" s="125" t="s">
-        <v>285</v>
-      </c>
-      <c r="F141" s="105" t="s">
-        <v>605</v>
-      </c>
-      <c r="G141" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="H141" s="118" t="s">
-        <v>533</v>
-      </c>
-      <c r="I141" s="125" t="s">
-        <v>306</v>
-      </c>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A141" s="93"/>
+      <c r="B141" s="184"/>
+      <c r="C141" s="184"/>
+      <c r="D141" s="184"/>
+      <c r="E141" s="184"/>
+      <c r="F141" s="183"/>
+      <c r="G141" s="183"/>
+      <c r="H141" s="183"/>
+      <c r="I141" s="106"/>
     </row>
     <row r="142" spans="1:9" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="123" t="s">
-        <v>604</v>
-      </c>
-      <c r="B142" s="92" t="s">
-        <v>277</v>
+        <v>608</v>
+      </c>
+      <c r="B142" s="125" t="s">
+        <v>518</v>
       </c>
       <c r="C142" s="125" t="s">
         <v>188</v>
@@ -6986,7 +6986,7 @@
         <v>285</v>
       </c>
       <c r="F142" s="105" t="s">
-        <v>540</v>
+        <v>605</v>
       </c>
       <c r="G142" s="125" t="s">
         <v>258</v>
@@ -6999,465 +6999,502 @@
       </c>
     </row>
     <row r="143" spans="1:9" s="125" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="93"/>
-      <c r="B143" s="178" t="s">
+      <c r="A143" s="123" t="s">
+        <v>604</v>
+      </c>
+      <c r="B143" s="92" t="s">
+        <v>277</v>
+      </c>
+      <c r="C143" s="125" t="s">
+        <v>188</v>
+      </c>
+      <c r="D143" s="125" t="s">
+        <v>285</v>
+      </c>
+      <c r="F143" s="105" t="s">
+        <v>540</v>
+      </c>
+      <c r="G143" s="125" t="s">
+        <v>258</v>
+      </c>
+      <c r="H143" s="118" t="s">
+        <v>533</v>
+      </c>
+      <c r="I143" s="125" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" s="125" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="93"/>
+      <c r="B144" s="184" t="s">
         <v>538</v>
       </c>
-      <c r="C143" s="178"/>
-      <c r="D143" s="178"/>
-      <c r="E143" s="178"/>
-      <c r="F143" s="179"/>
-      <c r="G143" s="179"/>
-      <c r="H143" s="179"/>
-      <c r="I143" s="124"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A144" s="123" t="s">
+      <c r="C144" s="184"/>
+      <c r="D144" s="184"/>
+      <c r="E144" s="184"/>
+      <c r="F144" s="183"/>
+      <c r="G144" s="183"/>
+      <c r="H144" s="183"/>
+      <c r="I144" s="124"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A145" s="123" t="s">
         <v>537</v>
       </c>
-      <c r="B144" s="92" t="s">
+      <c r="B145" s="92" t="s">
         <v>277</v>
       </c>
-      <c r="C144" s="102" t="s">
+      <c r="C145" s="102" t="s">
         <v>188</v>
       </c>
-      <c r="D144" s="102" t="s">
+      <c r="D145" s="102" t="s">
         <v>285</v>
       </c>
-      <c r="F144" s="105" t="s">
+      <c r="F145" s="105" t="s">
         <v>532</v>
       </c>
-      <c r="G144" s="102" t="s">
+      <c r="G145" s="102" t="s">
         <v>258</v>
       </c>
-      <c r="H144" s="118" t="s">
+      <c r="H145" s="118" t="s">
         <v>533</v>
       </c>
-      <c r="I144" s="102" t="s">
+      <c r="I145" s="102" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A145" s="93"/>
-      <c r="B145" s="180" t="s">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A146" s="93"/>
+      <c r="B146" s="182" t="s">
         <v>282</v>
       </c>
-      <c r="C145" s="180"/>
-      <c r="D145" s="180"/>
-      <c r="E145" s="180"/>
-      <c r="F145" s="180"/>
-      <c r="G145" s="180"/>
-      <c r="H145" s="180"/>
-      <c r="I145" s="106" t="s">
+      <c r="C146" s="182"/>
+      <c r="D146" s="182"/>
+      <c r="E146" s="182"/>
+      <c r="F146" s="182"/>
+      <c r="G146" s="182"/>
+      <c r="H146" s="182"/>
+      <c r="I146" s="106" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A146" s="102" t="s">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A147" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="B146" s="102" t="s">
+      <c r="B147" s="102" t="s">
         <v>509</v>
       </c>
-      <c r="C146" s="102" t="s">
+      <c r="C147" s="102" t="s">
         <v>208</v>
       </c>
-      <c r="D146" s="104" t="s">
+      <c r="D147" s="104" t="s">
         <v>511</v>
       </c>
-      <c r="F146" s="102" t="s">
+      <c r="F147" s="102" t="s">
         <v>501</v>
       </c>
-      <c r="G146" s="102" t="s">
+      <c r="G147" s="102" t="s">
         <v>149</v>
       </c>
-      <c r="I146" s="102" t="s">
+      <c r="I147" s="102" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A147" s="93"/>
-      <c r="B147" s="180" t="s">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A148" s="93"/>
+      <c r="B148" s="182" t="s">
         <v>510</v>
       </c>
-      <c r="C147" s="180"/>
-      <c r="D147" s="180"/>
-      <c r="E147" s="180"/>
-      <c r="F147" s="179"/>
-      <c r="G147" s="179"/>
-      <c r="H147" s="179"/>
-      <c r="I147" s="179"/>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A148" s="102" t="s">
+      <c r="C148" s="182"/>
+      <c r="D148" s="182"/>
+      <c r="E148" s="182"/>
+      <c r="F148" s="183"/>
+      <c r="G148" s="183"/>
+      <c r="H148" s="183"/>
+      <c r="I148" s="183"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A149" s="102" t="s">
         <v>506</v>
       </c>
-      <c r="B148" s="102" t="s">
+      <c r="B149" s="102" t="s">
         <v>507</v>
       </c>
-      <c r="F148" s="102" t="s">
+      <c r="F149" s="102" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A149" s="93"/>
-      <c r="B149" s="180" t="s">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A150" s="93"/>
+      <c r="B150" s="182" t="s">
         <v>505</v>
       </c>
-      <c r="C149" s="180"/>
-      <c r="D149" s="180"/>
-      <c r="E149" s="180"/>
-      <c r="F149" s="179"/>
-      <c r="G149" s="179"/>
-      <c r="H149" s="179"/>
-      <c r="I149" s="179"/>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A150" s="93" t="s">
-        <v>68</v>
-      </c>
+      <c r="C150" s="182"/>
+      <c r="D150" s="182"/>
+      <c r="E150" s="182"/>
+      <c r="F150" s="183"/>
+      <c r="G150" s="183"/>
+      <c r="H150" s="183"/>
+      <c r="I150" s="183"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="93" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A152" s="93" t="s">
         <v>192</v>
       </c>
-      <c r="B151" s="102" t="s">
+      <c r="B152" s="102" t="s">
         <v>518</v>
       </c>
-      <c r="D151" s="102" t="s">
+      <c r="D152" s="102" t="s">
         <v>284</v>
       </c>
-      <c r="F151" s="102" t="s">
+      <c r="F152" s="102" t="s">
         <v>525</v>
       </c>
-      <c r="G151" s="102" t="s">
+      <c r="G152" s="102" t="s">
         <v>149</v>
       </c>
-      <c r="H151" s="92" t="s">
+      <c r="H152" s="92" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A152" s="102" t="s">
-        <v>147</v>
-      </c>
-      <c r="B152" s="102" t="s">
-        <v>136</v>
-      </c>
-      <c r="F152" s="102" t="s">
-        <v>135</v>
-      </c>
-      <c r="H152" s="102" t="s">
-        <v>142</v>
-      </c>
-      <c r="I152" s="106"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="102" t="s">
+        <v>147</v>
+      </c>
+      <c r="B153" s="102" t="s">
+        <v>136</v>
+      </c>
+      <c r="F153" s="102" t="s">
+        <v>135</v>
+      </c>
+      <c r="H153" s="102" t="s">
+        <v>142</v>
+      </c>
+      <c r="I153" s="106"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A154" s="102" t="s">
         <v>146</v>
       </c>
-      <c r="B153" s="102" t="s">
+      <c r="B154" s="102" t="s">
         <v>210</v>
       </c>
-      <c r="C153" s="102" t="s">
+      <c r="C154" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="F153" s="102" t="s">
+      <c r="F154" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="G153" s="102" t="s">
+      <c r="G154" s="102" t="s">
         <v>149</v>
       </c>
-      <c r="I153" s="106"/>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A154" s="93"/>
-      <c r="B154" s="180" t="s">
+      <c r="I154" s="106"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A155" s="93"/>
+      <c r="B155" s="182" t="s">
         <v>123</v>
       </c>
-      <c r="C154" s="180"/>
-      <c r="D154" s="180"/>
-      <c r="E154" s="180"/>
-      <c r="F154" s="179"/>
-      <c r="G154" s="179"/>
-      <c r="H154" s="179"/>
-      <c r="I154" s="179"/>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A155" s="102" t="s">
-        <v>69</v>
-      </c>
-      <c r="B155" s="102" t="s">
-        <v>136</v>
-      </c>
-      <c r="C155" s="102" t="s">
-        <v>188</v>
-      </c>
-      <c r="F155" s="102" t="s">
-        <v>148</v>
-      </c>
-      <c r="G155" s="102" t="s">
-        <v>149</v>
-      </c>
-      <c r="I155" s="106"/>
+      <c r="C155" s="182"/>
+      <c r="D155" s="182"/>
+      <c r="E155" s="182"/>
+      <c r="F155" s="183"/>
+      <c r="G155" s="183"/>
+      <c r="H155" s="183"/>
+      <c r="I155" s="183"/>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="102" t="s">
         <v>69</v>
       </c>
       <c r="B156" s="102" t="s">
-        <v>190</v>
+        <v>136</v>
       </c>
       <c r="C156" s="102" t="s">
-        <v>208</v>
-      </c>
-      <c r="F156" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="F156" s="102" t="s">
         <v>148</v>
       </c>
       <c r="G156" s="102" t="s">
         <v>149</v>
       </c>
-      <c r="I156" s="106" t="s">
+      <c r="I156" s="106"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A157" s="102" t="s">
+        <v>69</v>
+      </c>
+      <c r="B157" s="102" t="s">
+        <v>190</v>
+      </c>
+      <c r="C157" s="102" t="s">
+        <v>208</v>
+      </c>
+      <c r="F157" s="120" t="s">
+        <v>148</v>
+      </c>
+      <c r="G157" s="102" t="s">
+        <v>149</v>
+      </c>
+      <c r="I157" s="106" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A157" s="93"/>
-      <c r="B157" s="180" t="s">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A158" s="93"/>
+      <c r="B158" s="182" t="s">
         <v>237</v>
       </c>
-      <c r="C157" s="180"/>
-      <c r="D157" s="180"/>
-      <c r="E157" s="180"/>
-      <c r="F157" s="180"/>
-      <c r="G157" s="180"/>
-      <c r="H157" s="180"/>
-      <c r="I157" s="106"/>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A158" s="102" t="s">
+      <c r="C158" s="182"/>
+      <c r="D158" s="182"/>
+      <c r="E158" s="182"/>
+      <c r="F158" s="182"/>
+      <c r="G158" s="182"/>
+      <c r="H158" s="182"/>
+      <c r="I158" s="106"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A159" s="102" t="s">
         <v>450</v>
       </c>
-      <c r="B158" s="102" t="s">
+      <c r="B159" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="C158" s="102" t="s">
+      <c r="C159" s="102" t="s">
         <v>188</v>
       </c>
-      <c r="F158" s="102" t="s">
+      <c r="F159" s="102" t="s">
         <v>166</v>
       </c>
-      <c r="G158" s="102" t="s">
+      <c r="G159" s="102" t="s">
         <v>149</v>
       </c>
-      <c r="I158" s="106"/>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A159" s="93"/>
-      <c r="B159" s="180" t="s">
+      <c r="I159" s="106"/>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A160" s="93"/>
+      <c r="B160" s="182" t="s">
         <v>215</v>
       </c>
-      <c r="C159" s="180"/>
-      <c r="D159" s="180"/>
-      <c r="E159" s="180"/>
-      <c r="F159" s="180"/>
-      <c r="G159" s="180"/>
-      <c r="H159" s="180"/>
-      <c r="I159" s="106"/>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A160" s="102" t="s">
+      <c r="C160" s="182"/>
+      <c r="D160" s="182"/>
+      <c r="E160" s="182"/>
+      <c r="F160" s="182"/>
+      <c r="G160" s="182"/>
+      <c r="H160" s="182"/>
+      <c r="I160" s="106"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A161" s="102" t="s">
         <v>174</v>
       </c>
-      <c r="B160" s="102" t="s">
+      <c r="B161" s="102" t="s">
         <v>171</v>
       </c>
-      <c r="D160" s="104" t="s">
+      <c r="D161" s="104" t="s">
         <v>283</v>
       </c>
-      <c r="F160" s="102" t="s">
+      <c r="F161" s="102" t="s">
         <v>169</v>
       </c>
-      <c r="G160" s="102" t="s">
+      <c r="G161" s="102" t="s">
         <v>149</v>
       </c>
-      <c r="H160" s="102" t="s">
+      <c r="H161" s="102" t="s">
         <v>170</v>
       </c>
-      <c r="I160" s="106"/>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A161" s="93"/>
-      <c r="B161" s="180" t="s">
+      <c r="I161" s="106"/>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A162" s="93"/>
+      <c r="B162" s="182" t="s">
         <v>172</v>
       </c>
-      <c r="C161" s="180"/>
-      <c r="D161" s="180"/>
-      <c r="E161" s="180"/>
-      <c r="F161" s="180"/>
-      <c r="G161" s="180"/>
-      <c r="H161" s="180"/>
-      <c r="I161" s="106"/>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A162" s="102" t="s">
-        <v>70</v>
-      </c>
-      <c r="B162" s="102" t="s">
-        <v>136</v>
-      </c>
-      <c r="C162" s="102" t="s">
-        <v>188</v>
-      </c>
-      <c r="F162" s="102" t="s">
-        <v>166</v>
-      </c>
-      <c r="G162" s="102" t="s">
-        <v>149</v>
-      </c>
-      <c r="I162" s="106" t="s">
-        <v>471</v>
-      </c>
+      <c r="C162" s="182"/>
+      <c r="D162" s="182"/>
+      <c r="E162" s="182"/>
+      <c r="F162" s="182"/>
+      <c r="G162" s="182"/>
+      <c r="H162" s="182"/>
+      <c r="I162" s="106"/>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="102" t="s">
-        <v>165</v>
+        <v>70</v>
       </c>
       <c r="B163" s="102" t="s">
-        <v>244</v>
+        <v>136</v>
+      </c>
+      <c r="C163" s="102" t="s">
+        <v>188</v>
       </c>
       <c r="F163" s="102" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
       <c r="G163" s="102" t="s">
         <v>149</v>
       </c>
-      <c r="I163" s="106"/>
+      <c r="I163" s="106" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A164" s="121" t="s">
+      <c r="A164" s="102" t="s">
+        <v>165</v>
+      </c>
+      <c r="B164" s="102" t="s">
+        <v>244</v>
+      </c>
+      <c r="F164" s="102" t="s">
+        <v>84</v>
+      </c>
+      <c r="G164" s="102" t="s">
+        <v>149</v>
+      </c>
+      <c r="I164" s="106"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A165" s="121" t="s">
         <v>193</v>
       </c>
-      <c r="B164" s="102" t="s">
+      <c r="B165" s="102" t="s">
         <v>136</v>
       </c>
-      <c r="F164" s="102" t="s">
+      <c r="F165" s="102" t="s">
         <v>195</v>
       </c>
-      <c r="H164" s="102" t="s">
+      <c r="H165" s="102" t="s">
         <v>194</v>
       </c>
-      <c r="I164" s="106"/>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B165" s="106" t="s">
+      <c r="I165" s="106"/>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B166" s="106" t="s">
         <v>287</v>
       </c>
-      <c r="C165" s="106"/>
-      <c r="D165" s="106"/>
-      <c r="E165" s="106"/>
-    </row>
-    <row r="166" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A166" s="96" t="s">
+      <c r="C166" s="106"/>
+      <c r="D166" s="106"/>
+      <c r="E166" s="106"/>
+    </row>
+    <row r="167" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A167" s="96" t="s">
         <v>199</v>
       </c>
-      <c r="B166" s="102" t="s">
+      <c r="B167" s="102" t="s">
         <v>136</v>
       </c>
-      <c r="F166" s="102" t="s">
+      <c r="F167" s="102" t="s">
         <v>197</v>
       </c>
-      <c r="H166" s="102" t="s">
+      <c r="H167" s="102" t="s">
         <v>194</v>
       </c>
-      <c r="I166" s="106"/>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B167" s="106" t="s">
+      <c r="I167" s="106"/>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B168" s="106" t="s">
         <v>287</v>
       </c>
-      <c r="C167" s="106"/>
-      <c r="D167" s="106"/>
-      <c r="E167" s="106"/>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A168" s="121" t="s">
+      <c r="C168" s="106"/>
+      <c r="D168" s="106"/>
+      <c r="E168" s="106"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A169" s="121" t="s">
         <v>201</v>
       </c>
-      <c r="B168" s="102" t="s">
+      <c r="B169" s="102" t="s">
         <v>190</v>
       </c>
-      <c r="F168" s="102" t="s">
+      <c r="F169" s="102" t="s">
         <v>195</v>
       </c>
-      <c r="H168" s="102" t="s">
+      <c r="H169" s="102" t="s">
         <v>194</v>
       </c>
-      <c r="I168" s="106"/>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B169" s="180" t="s">
+      <c r="I169" s="106"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B170" s="182" t="s">
         <v>200</v>
       </c>
-      <c r="C169" s="180"/>
-      <c r="D169" s="180"/>
-      <c r="E169" s="180"/>
-      <c r="F169" s="179"/>
-      <c r="G169" s="179"/>
-      <c r="H169" s="179"/>
-      <c r="I169" s="179"/>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A170" s="102" t="s">
+      <c r="C170" s="182"/>
+      <c r="D170" s="182"/>
+      <c r="E170" s="182"/>
+      <c r="F170" s="183"/>
+      <c r="G170" s="183"/>
+      <c r="H170" s="183"/>
+      <c r="I170" s="183"/>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A171" s="102" t="s">
         <v>71</v>
-      </c>
-      <c r="B170" s="102" t="s">
-        <v>136</v>
-      </c>
-      <c r="F170" s="102" t="s">
-        <v>85</v>
-      </c>
-      <c r="G170" s="102" t="s">
-        <v>149</v>
-      </c>
-      <c r="I170" s="106"/>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A171" s="121" t="s">
-        <v>268</v>
       </c>
       <c r="B171" s="102" t="s">
         <v>136</v>
       </c>
       <c r="F171" s="102" t="s">
+        <v>85</v>
+      </c>
+      <c r="G171" s="102" t="s">
+        <v>149</v>
+      </c>
+      <c r="I171" s="106"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A172" s="121" t="s">
+        <v>268</v>
+      </c>
+      <c r="B172" s="102" t="s">
+        <v>136</v>
+      </c>
+      <c r="F172" s="102" t="s">
         <v>266</v>
       </c>
-      <c r="G171" s="113" t="s">
+      <c r="G172" s="113" t="s">
         <v>258</v>
       </c>
-      <c r="H171" s="102" t="s">
+      <c r="H172" s="102" t="s">
         <v>267</v>
       </c>
-      <c r="I171" s="106"/>
+      <c r="I172" s="106"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="B169:I169"/>
-    <mergeCell ref="B130:I130"/>
-    <mergeCell ref="B64:I64"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B66:H66"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="B60:H60"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="B39:I39"/>
-    <mergeCell ref="B102:H102"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="B70:H70"/>
-    <mergeCell ref="B134:I134"/>
-    <mergeCell ref="B86:H86"/>
-    <mergeCell ref="B75:I75"/>
+  <mergeCells count="54">
+    <mergeCell ref="B92:H92"/>
+    <mergeCell ref="B144:H144"/>
+    <mergeCell ref="B113:H113"/>
+    <mergeCell ref="B141:H141"/>
+    <mergeCell ref="B96:H96"/>
+    <mergeCell ref="B94:H94"/>
+    <mergeCell ref="B101:H101"/>
+    <mergeCell ref="B105:H105"/>
+    <mergeCell ref="B111:H111"/>
+    <mergeCell ref="B109:H109"/>
+    <mergeCell ref="B107:I107"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B150:I150"/>
+    <mergeCell ref="B162:H162"/>
+    <mergeCell ref="B160:H160"/>
+    <mergeCell ref="B115:H115"/>
+    <mergeCell ref="B129:H129"/>
+    <mergeCell ref="B124:H124"/>
+    <mergeCell ref="B158:H158"/>
+    <mergeCell ref="B121:H121"/>
+    <mergeCell ref="B155:I155"/>
+    <mergeCell ref="B118:H118"/>
+    <mergeCell ref="B148:I148"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B146:H146"/>
     <mergeCell ref="B79:H79"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B10:H10"/>
@@ -7469,66 +7506,56 @@
     <mergeCell ref="B73:H73"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B149:I149"/>
-    <mergeCell ref="B161:H161"/>
-    <mergeCell ref="B159:H159"/>
-    <mergeCell ref="B114:H114"/>
-    <mergeCell ref="B128:H128"/>
-    <mergeCell ref="B123:H123"/>
-    <mergeCell ref="B157:H157"/>
-    <mergeCell ref="B120:H120"/>
-    <mergeCell ref="B154:I154"/>
-    <mergeCell ref="B117:H117"/>
-    <mergeCell ref="B147:I147"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B145:H145"/>
-    <mergeCell ref="B143:H143"/>
-    <mergeCell ref="B112:H112"/>
-    <mergeCell ref="B140:H140"/>
-    <mergeCell ref="B95:H95"/>
-    <mergeCell ref="B93:H93"/>
-    <mergeCell ref="B100:H100"/>
-    <mergeCell ref="B104:H104"/>
-    <mergeCell ref="B110:H110"/>
-    <mergeCell ref="B108:H108"/>
-    <mergeCell ref="B106:I106"/>
+    <mergeCell ref="B170:I170"/>
+    <mergeCell ref="B131:I131"/>
+    <mergeCell ref="B64:I64"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B66:H66"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B60:H60"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="B39:I39"/>
+    <mergeCell ref="B103:H103"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="B70:H70"/>
+    <mergeCell ref="B135:I135"/>
+    <mergeCell ref="B86:H86"/>
+    <mergeCell ref="B75:I75"/>
   </mergeCells>
   <phoneticPr fontId="39" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A166" r:id="rId1" display="ZEL"/>
-    <hyperlink ref="A164" r:id="rId2" display="ZEL-CBL"/>
-    <hyperlink ref="A168" r:id="rId3" display="ZEL-CBL"/>
+    <hyperlink ref="A167" r:id="rId1" display="ZEL"/>
+    <hyperlink ref="A165" r:id="rId2" display="ZEL-CBL"/>
+    <hyperlink ref="A169" r:id="rId3" display="ZEL-CBL"/>
     <hyperlink ref="H23" r:id="rId4"/>
-    <hyperlink ref="A131" r:id="rId5"/>
-    <hyperlink ref="H131" r:id="rId6"/>
+    <hyperlink ref="A132" r:id="rId5"/>
+    <hyperlink ref="H132" r:id="rId6"/>
     <hyperlink ref="B1" r:id="rId7"/>
     <hyperlink ref="F42" r:id="rId8" location="/"/>
     <hyperlink ref="A74" r:id="rId9"/>
-    <hyperlink ref="A171" r:id="rId10" display="ZEN"/>
-    <hyperlink ref="A118" r:id="rId11"/>
-    <hyperlink ref="F118" r:id="rId12"/>
-    <hyperlink ref="F99" r:id="rId13"/>
+    <hyperlink ref="A172" r:id="rId10" display="ZEN"/>
+    <hyperlink ref="A119" r:id="rId11"/>
+    <hyperlink ref="F119" r:id="rId12"/>
+    <hyperlink ref="F100" r:id="rId13"/>
     <hyperlink ref="A17" r:id="rId14"/>
     <hyperlink ref="H17" r:id="rId15" display="Desktop Wallet"/>
     <hyperlink ref="F17" r:id="rId16"/>
-    <hyperlink ref="F116" r:id="rId17"/>
-    <hyperlink ref="A116" r:id="rId18"/>
+    <hyperlink ref="F117" r:id="rId17"/>
+    <hyperlink ref="A117" r:id="rId18"/>
     <hyperlink ref="A9" r:id="rId19" display="BTCP"/>
     <hyperlink ref="A11" r:id="rId20"/>
-    <hyperlink ref="A119" r:id="rId21" display="RVN"/>
-    <hyperlink ref="F119" r:id="rId22"/>
-    <hyperlink ref="F144" r:id="rId23" display="stratum+tcp://&lt;algo&gt;.eu1.unimining.net:&lt;PORT&gt;"/>
-    <hyperlink ref="A144" r:id="rId24" display="MTN"/>
-    <hyperlink ref="A139" r:id="rId25" display="MTN"/>
+    <hyperlink ref="A120" r:id="rId21" display="RVN"/>
+    <hyperlink ref="F120" r:id="rId22"/>
+    <hyperlink ref="F145" r:id="rId23" display="stratum+tcp://&lt;algo&gt;.eu1.unimining.net:&lt;PORT&gt;"/>
+    <hyperlink ref="A145" r:id="rId24" display="MTN"/>
+    <hyperlink ref="A140" r:id="rId25" display="MTN"/>
     <hyperlink ref="A7" r:id="rId26"/>
     <hyperlink ref="A82" r:id="rId27"/>
-    <hyperlink ref="A142" r:id="rId28" display="MTN"/>
-    <hyperlink ref="F142" r:id="rId29" display="stratum+tcp://mine.icemining.ca:3636"/>
-    <hyperlink ref="A141" r:id="rId30" display="MTN"/>
-    <hyperlink ref="F141" r:id="rId31"/>
+    <hyperlink ref="A143" r:id="rId28" display="MTN"/>
+    <hyperlink ref="F143" r:id="rId29" display="stratum+tcp://mine.icemining.ca:3636"/>
+    <hyperlink ref="A142" r:id="rId30" display="MTN"/>
+    <hyperlink ref="F142" r:id="rId31"/>
     <hyperlink ref="F36" r:id="rId32" location="/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7542,7 +7569,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7624,7 +7651,7 @@
         <v>1400</v>
       </c>
       <c r="I3" s="44">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -7650,7 +7677,7 @@
         <v>1400</v>
       </c>
       <c r="I4" s="44">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -7668,7 +7695,7 @@
         <v>160</v>
       </c>
       <c r="F5" s="44">
-        <v>1100</v>
+        <v>1150</v>
       </c>
       <c r="G5" s="44">
         <v>160</v>
@@ -7695,7 +7722,7 @@
         <v>160</v>
       </c>
       <c r="F6" s="44">
-        <v>1100</v>
+        <v>1150</v>
       </c>
       <c r="G6" s="44">
         <v>160</v>
@@ -7722,7 +7749,7 @@
         <v>160</v>
       </c>
       <c r="F7" s="44">
-        <v>1100</v>
+        <v>1150</v>
       </c>
       <c r="G7" s="44">
         <v>160</v>
@@ -7749,7 +7776,7 @@
         <v>160</v>
       </c>
       <c r="F8" s="44">
-        <v>1100</v>
+        <v>1150</v>
       </c>
       <c r="G8" s="44">
         <v>160</v>
@@ -7775,7 +7802,7 @@
         <v>160</v>
       </c>
       <c r="F9" s="44">
-        <v>1100</v>
+        <v>800</v>
       </c>
       <c r="G9" s="44">
         <v>160</v>
@@ -7801,7 +7828,7 @@
         <v>160</v>
       </c>
       <c r="F10" s="44">
-        <v>1100</v>
+        <v>1150</v>
       </c>
       <c r="G10" s="44">
         <v>160</v>
@@ -8062,7 +8089,7 @@
       <c r="I23" s="175">
         <v>140</v>
       </c>
-      <c r="J23" s="191"/>
+      <c r="J23" s="179"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="43"/>
@@ -8171,7 +8198,7 @@
         <v>140</v>
       </c>
       <c r="F30" s="44">
-        <v>1300</v>
+        <v>1100</v>
       </c>
       <c r="G30" s="175">
         <v>160</v>
@@ -8182,7 +8209,7 @@
       <c r="I30" s="175">
         <v>140</v>
       </c>
-      <c r="J30" s="191"/>
+      <c r="J30" s="179"/>
     </row>
     <row r="31" spans="1:10" s="176" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="43" t="s">
@@ -8201,7 +8228,7 @@
         <v>150</v>
       </c>
       <c r="F31" s="44">
-        <v>1300</v>
+        <v>1100</v>
       </c>
       <c r="G31" s="175">
         <v>160</v>
@@ -8212,7 +8239,7 @@
       <c r="I31" s="175">
         <v>150</v>
       </c>
-      <c r="J31" s="192"/>
+      <c r="J31" s="180"/>
     </row>
     <row r="32" spans="1:10" s="176" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="43" t="s">
@@ -8231,7 +8258,7 @@
         <v>140</v>
       </c>
       <c r="F32" s="44">
-        <v>1150</v>
+        <v>1100</v>
       </c>
       <c r="G32" s="175">
         <v>130</v>
@@ -8242,7 +8269,7 @@
       <c r="I32" s="175">
         <v>140</v>
       </c>
-      <c r="J32" s="191"/>
+      <c r="J32" s="179"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="43"/>
@@ -8689,7 +8716,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="38" x14ac:dyDescent="0.2">
-      <c r="A2" s="188" t="s">
+      <c r="A2" s="192" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -8700,7 +8727,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="38" x14ac:dyDescent="0.2">
-      <c r="A3" s="189"/>
+      <c r="A3" s="193"/>
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
@@ -8716,7 +8743,7 @@
       <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="188" t="s">
+      <c r="A5" s="192" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="5"/>
@@ -8725,32 +8752,32 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="189"/>
-      <c r="B6" s="183" t="s">
+      <c r="A6" s="193"/>
+      <c r="B6" s="187" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="183"/>
+      <c r="C6" s="187"/>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="189"/>
+      <c r="A7" s="193"/>
       <c r="B7" s="6"/>
       <c r="C7" s="31" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="189"/>
+      <c r="A8" s="193"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="189"/>
-      <c r="B9" s="184" t="s">
+      <c r="A9" s="193"/>
+      <c r="B9" s="188" t="s">
         <v>601</v>
       </c>
-      <c r="C9" s="185"/>
+      <c r="C9" s="189"/>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -8774,7 +8801,7 @@
       <c r="C12" s="29"/>
     </row>
     <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="190" t="s">
+      <c r="A13" s="194" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -8785,25 +8812,25 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="189"/>
+      <c r="A14" s="193"/>
       <c r="B14" s="5"/>
       <c r="C14" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A15" s="189"/>
+      <c r="A15" s="193"/>
       <c r="B15" s="5"/>
       <c r="C15" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="189"/>
-      <c r="B16" s="186" t="s">
+      <c r="A16" s="193"/>
+      <c r="B16" s="190" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="187"/>
+      <c r="C16" s="191"/>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">

</xml_diff>

<commit_message>
InstallMiners will automatically apply 'sudo' if required.
</commit_message>
<xml_diff>
--- a/miners.xlsx
+++ b/miners.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="1740" windowWidth="25540" windowHeight="10900" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="60" yWindow="1740" windowWidth="25540" windowHeight="10900" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="711">
   <si>
     <t>Miners (AMD)</t>
   </si>
@@ -1667,9 +1667,6 @@
     <t>stratum+tcp://lyra2re.usa.nicehash.com:3347</t>
   </si>
   <si>
-    <t>--verbosity 3 -SP 2 -U -S $URL_PORT -O $WALLET.$WORKER_NAME:x</t>
-  </si>
-  <si>
     <t>-l  &lt;URL_PORT&gt; -u &lt;WALLET&gt;.&lt;WORKER_NAME&gt; -t 0  -e 0 $GPUS</t>
   </si>
   <si>
@@ -2159,7 +2156,19 @@
     <t>https://whattomine.com/coins?utf8=%E2%9C%93&amp;adapt_q_280x=0&amp;adapt_q_380=0&amp;adapt_q_fury=0&amp;adapt_q_470=0&amp;adapt_q_480=0&amp;adapt_q_570=0&amp;adapt_q_580=0&amp;adapt_q_vega56=0&amp;adapt_q_vega64=0&amp;adapt_q_750Ti=0&amp;adapt_q_1050Ti=0&amp;adapt_q_10606=0&amp;adapt_q_1070=0&amp;adapt_q_1070Ti=3&amp;adapt_1070Ti=true&amp;adapt_q_1080=0&amp;adapt_q_1080Ti=1&amp;adapt_1080Ti=true&amp;eth=true&amp;factor%5Beth_hr%5D=126.50&amp;factor%5Beth_p%5D=545.00&amp;grof=true&amp;factor%5Bgro_hr%5D=167.50&amp;factor%5Bgro_p%5D=570.00&amp;phi=true&amp;factor%5Bphi_hr%5D=99.00&amp;factor%5Bphi_p%5D=590.00&amp;cn=true&amp;factor%5Bcn_hr%5D=2720.00&amp;factor%5Bcn_p%5D=410.00&amp;cn7=true&amp;factor%5Bcn7_hr%5D=2720.00&amp;factor%5Bcn7_p%5D=410.00&amp;eq=true&amp;factor%5Beq_hr%5D=2095.00&amp;factor%5Beq_p%5D=550.00&amp;lre=true&amp;factor%5Blrev2_hr%5D=187000.00&amp;factor%5Blrev2_p%5D=550.00&amp;ns=true&amp;factor%5Bns_hr%5D=4550.00&amp;factor%5Bns_p%5D=550.00&amp;tt10=true&amp;factor%5Btt10_hr%5D=88.50&amp;factor%5Btt10_p%5D=560.00&amp;x16r=true&amp;factor%5Bx16r_hr%5D=45.00&amp;factor%5Bx16r_p%5D=565.00&amp;factor%5Bl2z_hr%5D=9.00&amp;factor%5Bl2z_p%5D=500.00&amp;n5=true&amp;factor%5Bn5_hr%5D=225.00&amp;factor%5Bn5_p%5D=550.00&amp;xn=true&amp;factor%5Bxn_hr%5D=16.10&amp;factor%5Bxn_p%5D=550.00&amp;factor%5Bcost%5D=0.0945&amp;sort=Profitability24&amp;volume=0&amp;revenue=24h&amp;factor%5Bexchanges%5D%5B%5D=&amp;factor%5Bexchanges%5D%5B%5D=binance&amp;factor%5Bexchanges%5D%5B%5D=bitfinex&amp;factor%5Bexchanges%5D%5B%5D=bittrex&amp;factor%5Bexchanges%5D%5B%5D=cryptobridge&amp;factor%5Bexchanges%5D%5B%5D=cryptopia&amp;factor%5Bexchanges%5D%5B%5D=hitbtc&amp;factor%5Bexchanges%5D%5B%5D=poloniex&amp;factor%5Bexchanges%5D%5B%5D=yobit&amp;dataset=Titans&amp;commit=Calculate</t>
   </si>
   <si>
-    <t xml:space="preserve"> $GPUS -epool $URL_PORT -ewal $WALLET.$WORKER_NAME -eworker $WALLET.$WORKER_NAME -esm 2 -epsw $PSW -allpools 1 -allcoins 1 -mode 1 -lidag 0 -asm 0 -mport 0</t>
+    <t>Repeatedly crashes everyone else on rig-Nvidia, so has been unplugged from here.</t>
+  </si>
+  <si>
+    <t>stratum+tcp://daggerhashimoto.usa.nicehash.com:3353</t>
+  </si>
+  <si>
+    <t>--farm-recheck 200 -U --pool $URL_PORT -O &lt;WALLET&gt;.$WORKER_NAME:x $GPUS</t>
+  </si>
+  <si>
+    <t>NH-ET-ethminer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -epool $URL_PORT -ewal $WALLET -eworker $WORKER_NAME -esm 2 -epsw $PSW -allpools 1 -allcoins 1 -mode 1 -lidag 0 -asm 0 -mport 0 $GPUS</t>
   </si>
 </sst>
 </file>
@@ -2169,7 +2178,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="69" x14ac:knownFonts="1">
+  <fonts count="70" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2591,6 +2600,12 @@
       <sz val="12"/>
       <name val="Microsoft Sans Serif"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <name val="MicrosoftSansSerif"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -2670,7 +2685,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3186,12 +3201,12 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
@@ -3216,6 +3231,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3559,10 +3578,10 @@
     </row>
     <row r="3" spans="1:14" s="66" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="66" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B3" s="66" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C3" s="129"/>
       <c r="D3" s="129"/>
@@ -3613,7 +3632,7 @@
         <v>281</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D6" s="56" t="s">
         <v>527</v>
@@ -3634,18 +3653,18 @@
         <v>283</v>
       </c>
       <c r="J6" s="56" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="K6" s="56" t="s">
         <v>285</v>
       </c>
       <c r="L6" s="56" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L7" s="56" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -3688,57 +3707,57 @@
         <v>153</v>
       </c>
       <c r="B1" s="143" t="s">
+        <v>549</v>
+      </c>
+      <c r="C1" s="143" t="s">
+        <v>551</v>
+      </c>
+      <c r="D1" s="143" t="s">
         <v>550</v>
       </c>
-      <c r="C1" s="143" t="s">
+      <c r="E1" s="142" t="s">
+        <v>555</v>
+      </c>
+      <c r="F1" s="142" t="s">
+        <v>554</v>
+      </c>
+      <c r="G1" s="144" t="s">
         <v>552</v>
       </c>
-      <c r="D1" s="143" t="s">
-        <v>551</v>
-      </c>
-      <c r="E1" s="142" t="s">
-        <v>556</v>
-      </c>
-      <c r="F1" s="142" t="s">
-        <v>555</v>
-      </c>
-      <c r="G1" s="144" t="s">
+      <c r="H1" s="143" t="s">
+        <v>598</v>
+      </c>
+      <c r="I1" s="159" t="s">
+        <v>666</v>
+      </c>
+      <c r="J1" s="165" t="s">
+        <v>645</v>
+      </c>
+      <c r="K1" s="158" t="s">
+        <v>646</v>
+      </c>
+      <c r="L1" s="142" t="s">
+        <v>596</v>
+      </c>
+      <c r="M1" s="146" t="s">
+        <v>602</v>
+      </c>
+      <c r="N1" s="146" t="s">
+        <v>667</v>
+      </c>
+      <c r="O1" s="144" t="s">
+        <v>599</v>
+      </c>
+      <c r="P1" s="143" t="s">
         <v>553</v>
-      </c>
-      <c r="H1" s="143" t="s">
-        <v>599</v>
-      </c>
-      <c r="I1" s="159" t="s">
-        <v>667</v>
-      </c>
-      <c r="J1" s="165" t="s">
-        <v>646</v>
-      </c>
-      <c r="K1" s="158" t="s">
-        <v>647</v>
-      </c>
-      <c r="L1" s="142" t="s">
-        <v>597</v>
-      </c>
-      <c r="M1" s="146" t="s">
-        <v>603</v>
-      </c>
-      <c r="N1" s="146" t="s">
-        <v>668</v>
-      </c>
-      <c r="O1" s="144" t="s">
-        <v>600</v>
-      </c>
-      <c r="P1" s="143" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="145" customFormat="1" ht="33" x14ac:dyDescent="0.2">
       <c r="A2" s="138" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B2" s="139" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C2" s="140"/>
       <c r="D2" s="140"/>
@@ -3757,7 +3776,7 @@
     </row>
     <row r="3" spans="1:16" s="133" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="133" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B3" s="132"/>
       <c r="C3" s="130"/>
@@ -3797,25 +3816,25 @@
     </row>
     <row r="5" spans="1:16" s="136" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="136" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B5" s="137"/>
       <c r="D5" s="136" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="H5" s="136" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L5" s="136" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="O5" s="136" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="133" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="133" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B6" s="132"/>
       <c r="C6" s="130"/>
@@ -3855,7 +3874,7 @@
     </row>
     <row r="8" spans="1:16" s="133" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="133" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B8" s="132"/>
       <c r="C8" s="130"/>
@@ -3885,7 +3904,7 @@
       <c r="G9" s="130"/>
       <c r="H9" s="130"/>
       <c r="J9" s="131" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="K9" s="130"/>
       <c r="L9" s="130"/>
@@ -3899,22 +3918,22 @@
         <v>30</v>
       </c>
       <c r="B10" s="133" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C10" s="131" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D10" s="131" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E10" s="131" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F10" s="131" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G10" s="131" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H10" s="131"/>
       <c r="I10" s="131"/>
@@ -3925,12 +3944,12 @@
       <c r="N10" s="131"/>
       <c r="O10" s="131"/>
       <c r="P10" s="131" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="133" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -3945,36 +3964,36 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="133" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I14" s="132" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="N14" s="132" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="O14" s="132" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="133" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="133" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="160" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="133" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -3984,7 +4003,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="133" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -3992,17 +4011,17 @@
         <v>35</v>
       </c>
       <c r="J21" s="132" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="133" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="133" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -4010,12 +4029,12 @@
         <v>42</v>
       </c>
       <c r="J24" s="132" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="133" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -4023,12 +4042,12 @@
         <v>45</v>
       </c>
       <c r="J26" s="132" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="133" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -4036,17 +4055,17 @@
         <v>249</v>
       </c>
       <c r="J28" s="132" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="133" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="133" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -4061,12 +4080,12 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="133" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="133" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -4076,12 +4095,12 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="133" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="133" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -4089,22 +4108,22 @@
         <v>55</v>
       </c>
       <c r="J38" s="132" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="133" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="133" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="133" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -4112,57 +4131,57 @@
         <v>260</v>
       </c>
       <c r="I42" s="132" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="133" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="135" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="134" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="133" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="133" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="133" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="133" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="133" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="133" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="133" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -4170,7 +4189,7 @@
         <v>69</v>
       </c>
       <c r="J53" s="132" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -4201,7 +4220,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4246,52 +4265,52 @@
         <v>188</v>
       </c>
       <c r="C2" s="78" t="s">
+        <v>637</v>
+      </c>
+      <c r="D2" s="78" t="s">
         <v>638</v>
-      </c>
-      <c r="D2" s="78" t="s">
-        <v>639</v>
       </c>
       <c r="E2" s="80"/>
       <c r="F2" s="81" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="79" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="77" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B3" s="45" t="s">
         <v>141</v>
       </c>
       <c r="C3" s="78" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D3" s="78" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E3" s="80"/>
       <c r="F3" s="81" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="100" customFormat="1" ht="50" x14ac:dyDescent="0.2">
       <c r="A4" s="152" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B4" s="39" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="100" t="s">
+        <v>617</v>
+      </c>
+      <c r="D4" s="100" t="s">
         <v>618</v>
       </c>
-      <c r="D4" s="100" t="s">
+      <c r="E4" s="153" t="s">
         <v>619</v>
       </c>
-      <c r="E4" s="153" t="s">
-        <v>620</v>
-      </c>
       <c r="F4" s="99" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="79" customFormat="1" ht="19" x14ac:dyDescent="0.2">
@@ -4302,16 +4321,16 @@
         <v>188</v>
       </c>
       <c r="C5" s="78" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D5" s="79" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E5" s="82" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F5" s="79" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="100" customFormat="1" ht="50" x14ac:dyDescent="0.2">
@@ -4346,7 +4365,7 @@
       </c>
       <c r="E7" s="84"/>
       <c r="F7" s="41" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G7" s="85"/>
     </row>
@@ -4404,7 +4423,7 @@
         <v>140</v>
       </c>
       <c r="F11" s="99" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -4418,7 +4437,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="99" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G12" s="51" t="s">
         <v>212</v>
@@ -4432,10 +4451,10 @@
         <v>208</v>
       </c>
       <c r="C13" s="51" t="s">
+        <v>545</v>
+      </c>
+      <c r="D13" s="51" t="s">
         <v>546</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="33" x14ac:dyDescent="0.2">
@@ -4457,7 +4476,7 @@
     </row>
     <row r="15" spans="1:7" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="100" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B15" s="39" t="s">
         <v>188</v>
@@ -4466,7 +4485,7 @@
         <v>176</v>
       </c>
       <c r="D15" s="100" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E15" s="83"/>
       <c r="F15" s="181" t="s">
@@ -4568,7 +4587,7 @@
         <v>519</v>
       </c>
       <c r="B1" s="164" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C1" s="149" t="s">
         <v>520</v>
@@ -4577,79 +4596,79 @@
         <v>523</v>
       </c>
       <c r="E1" s="148" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G1" s="150" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I1" s="36" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="K1" s="150" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="L1" s="42" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B2" t="s">
+        <v>656</v>
+      </c>
+      <c r="C2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D2" t="s">
+        <v>628</v>
+      </c>
+      <c r="F2" t="s">
+        <v>661</v>
+      </c>
+      <c r="G2" t="s">
         <v>657</v>
       </c>
-      <c r="C2" t="s">
-        <v>633</v>
-      </c>
-      <c r="D2" t="s">
-        <v>629</v>
-      </c>
-      <c r="F2" t="s">
-        <v>662</v>
-      </c>
-      <c r="G2" t="s">
-        <v>658</v>
-      </c>
       <c r="H2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>684</v>
+      </c>
+      <c r="I3" s="162" t="s">
         <v>685</v>
-      </c>
-      <c r="I3" s="162" t="s">
-        <v>686</v>
       </c>
       <c r="J3" s="162"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D5" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -4657,7 +4676,7 @@
         <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D6" s="147"/>
       <c r="E6" s="147"/>
@@ -4670,11 +4689,11 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C7" s="147"/>
       <c r="D7" s="147" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E7" s="147"/>
       <c r="F7" s="147"/>
@@ -4686,10 +4705,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D8" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -4697,7 +4716,7 @@
         <v>35</v>
       </c>
       <c r="H9" s="162" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I9" s="162"/>
       <c r="J9" s="162"/>
@@ -4708,7 +4727,7 @@
       </c>
       <c r="C10" s="147"/>
       <c r="D10" s="147" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E10" s="147"/>
       <c r="F10" s="147"/>
@@ -4724,7 +4743,7 @@
       </c>
       <c r="C11" s="147"/>
       <c r="D11" s="147" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E11" s="147"/>
       <c r="F11" s="147"/>
@@ -4740,7 +4759,7 @@
       </c>
       <c r="C12" s="147"/>
       <c r="D12" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E12" s="147"/>
       <c r="F12" s="147"/>
@@ -4755,19 +4774,19 @@
         <v>55</v>
       </c>
       <c r="B13" s="162" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C13" s="147"/>
       <c r="D13" s="147"/>
       <c r="E13" s="147" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F13" s="147"/>
       <c r="G13" s="162" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H13" s="162" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I13" s="162"/>
       <c r="J13" s="162"/>
@@ -4780,20 +4799,20 @@
       <c r="C14" s="147"/>
       <c r="D14" s="147"/>
       <c r="E14" s="147" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F14" s="147"/>
       <c r="G14" s="147"/>
       <c r="H14" s="147"/>
       <c r="I14" s="169" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="J14" s="169"/>
       <c r="K14" s="147"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C15" s="147"/>
       <c r="D15" s="147"/>
@@ -4803,7 +4822,7 @@
       <c r="H15" s="147"/>
       <c r="I15" s="169"/>
       <c r="J15" s="169" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="K15" s="147"/>
     </row>
@@ -4812,7 +4831,7 @@
         <v>63</v>
       </c>
       <c r="D16" s="147" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -4820,10 +4839,10 @@
         <v>534</v>
       </c>
       <c r="E17" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I17" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -4831,37 +4850,37 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D18" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C19" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D20" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -4889,9 +4908,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S172"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4981,7 +5000,7 @@
     </row>
     <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="128" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B7" s="125" t="s">
         <v>216</v>
@@ -4990,7 +5009,7 @@
         <v>291</v>
       </c>
       <c r="F7" s="102" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G7" s="113" t="s">
         <v>258</v>
@@ -5229,7 +5248,7 @@
     </row>
     <row r="26" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="92" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B26" s="156" t="s">
         <v>139</v>
@@ -5238,7 +5257,7 @@
         <v>283</v>
       </c>
       <c r="F26" s="156" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -5262,7 +5281,7 @@
     </row>
     <row r="29" spans="1:9" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="92" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B29" s="173" t="s">
         <v>179</v>
@@ -5274,13 +5293,13 @@
         <v>526</v>
       </c>
       <c r="F29" s="173" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G29" s="173" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H29" s="172" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="I29" s="174" t="s">
         <v>471</v>
@@ -5289,7 +5308,7 @@
     <row r="30" spans="1:9" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="93"/>
       <c r="B30" s="184" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C30" s="184"/>
       <c r="D30" s="184"/>
@@ -5301,7 +5320,7 @@
     </row>
     <row r="31" spans="1:9" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="92" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B31" s="173" t="s">
         <v>124</v>
@@ -5313,13 +5332,13 @@
         <v>526</v>
       </c>
       <c r="F31" s="173" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G31" s="173" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H31" s="172" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="I31" s="174" t="s">
         <v>471</v>
@@ -5327,7 +5346,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="93" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B32" s="156" t="s">
         <v>124</v>
@@ -5339,7 +5358,7 @@
         <v>526</v>
       </c>
       <c r="F32" s="125" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G32" s="125" t="s">
         <v>149</v>
@@ -5359,10 +5378,10 @@
         <v>526</v>
       </c>
       <c r="F33" s="173" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G33" s="173" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H33" s="172"/>
       <c r="I33" s="174" t="s">
@@ -5371,7 +5390,7 @@
     </row>
     <row r="34" spans="1:19" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="92" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B34" s="173" t="s">
         <v>179</v>
@@ -5383,10 +5402,10 @@
         <v>526</v>
       </c>
       <c r="F34" s="173" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="G34" s="173" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H34" s="172"/>
       <c r="I34" s="174" t="s">
@@ -5408,7 +5427,7 @@
     </row>
     <row r="36" spans="1:19" s="173" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="92" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B36" s="173" t="s">
         <v>179</v>
@@ -5417,7 +5436,7 @@
         <v>208</v>
       </c>
       <c r="F36" s="152" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G36" s="173" t="s">
         <v>149</v>
@@ -5499,7 +5518,7 @@
         <v>72</v>
       </c>
       <c r="G40" s="102" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H40" s="106"/>
       <c r="I40" s="107" t="s">
@@ -5695,7 +5714,7 @@
     </row>
     <row r="57" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="93" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B57" s="156" t="s">
         <v>139</v>
@@ -5704,7 +5723,7 @@
         <v>283</v>
       </c>
       <c r="F57" s="156" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G57" s="156" t="s">
         <v>121</v>
@@ -5717,7 +5736,7 @@
     <row r="58" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="93"/>
       <c r="B58" s="184" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C58" s="184"/>
       <c r="D58" s="184"/>
@@ -5738,7 +5757,7 @@
         <v>283</v>
       </c>
       <c r="F59" s="109" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="H59" s="102" t="s">
         <v>77</v>
@@ -5748,7 +5767,7 @@
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="93"/>
       <c r="B60" s="184" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C60" s="184"/>
       <c r="D60" s="184"/>
@@ -5760,7 +5779,7 @@
     </row>
     <row r="61" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="156" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B61" s="156" t="s">
         <v>114</v>
@@ -5769,7 +5788,7 @@
         <v>283</v>
       </c>
       <c r="F61" s="109" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G61" s="156" t="s">
         <v>115</v>
@@ -5794,7 +5813,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="93" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B63" s="156" t="s">
         <v>139</v>
@@ -5813,7 +5832,7 @@
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="93"/>
       <c r="B64" s="184" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C64" s="184"/>
       <c r="D64" s="184"/>
@@ -5834,7 +5853,7 @@
         <v>283</v>
       </c>
       <c r="F65" s="102" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G65" s="102" t="s">
         <v>115</v>
@@ -5966,12 +5985,12 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75" s="93"/>
-      <c r="B75" s="185" t="s">
+      <c r="B75" s="186" t="s">
         <v>286</v>
       </c>
-      <c r="C75" s="185"/>
-      <c r="D75" s="185"/>
-      <c r="E75" s="185"/>
+      <c r="C75" s="186"/>
+      <c r="D75" s="186"/>
+      <c r="E75" s="186"/>
       <c r="F75" s="183"/>
       <c r="G75" s="183"/>
       <c r="H75" s="183"/>
@@ -6019,7 +6038,7 @@
     </row>
     <row r="79" spans="1:19" s="113" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="93"/>
-      <c r="B79" s="186" t="s">
+      <c r="B79" s="185" t="s">
         <v>289</v>
       </c>
       <c r="C79" s="183"/>
@@ -6051,7 +6070,7 @@
     </row>
     <row r="82" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="121" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.2">
@@ -6134,7 +6153,7 @@
         <v>528</v>
       </c>
       <c r="B89" s="117" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C89" s="117"/>
       <c r="D89" s="122" t="s">
@@ -6142,7 +6161,7 @@
       </c>
       <c r="E89" s="117"/>
       <c r="F89" s="117" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G89" s="125" t="s">
         <v>149</v>
@@ -6203,7 +6222,7 @@
         <v>124</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>141</v>
+        <v>208</v>
       </c>
       <c r="D91" s="117" t="s">
         <v>526</v>
@@ -6233,19 +6252,19 @@
     <row r="92" spans="1:19" s="177" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="93"/>
       <c r="B92" s="182" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="C92" s="182"/>
       <c r="D92" s="182"/>
       <c r="E92" s="182"/>
-      <c r="F92" s="183"/>
-      <c r="G92" s="183"/>
-      <c r="H92" s="183"/>
+      <c r="F92" s="182"/>
+      <c r="G92" s="182"/>
+      <c r="H92" s="182"/>
       <c r="I92" s="178"/>
     </row>
     <row r="93" spans="1:19" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="95" t="s">
-        <v>530</v>
+        <v>709</v>
       </c>
       <c r="B93" s="116" t="s">
         <v>222</v>
@@ -6258,7 +6277,7 @@
       </c>
       <c r="E93" s="117"/>
       <c r="F93" s="117" t="s">
-        <v>223</v>
+        <v>707</v>
       </c>
       <c r="G93" s="177" t="s">
         <v>149</v>
@@ -6281,7 +6300,7 @@
     <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94" s="93"/>
       <c r="B94" s="182" t="s">
-        <v>543</v>
+        <v>708</v>
       </c>
       <c r="C94" s="182"/>
       <c r="D94" s="182"/>
@@ -6450,7 +6469,7 @@
     </row>
     <row r="106" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="92" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B106" s="156" t="s">
         <v>179</v>
@@ -6462,10 +6481,10 @@
         <v>526</v>
       </c>
       <c r="F106" s="156" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G106" s="156" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H106" s="156" t="s">
         <v>79</v>
@@ -6477,7 +6496,7 @@
     <row r="107" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="93"/>
       <c r="B107" s="184" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C107" s="184"/>
       <c r="D107" s="184"/>
@@ -6495,7 +6514,7 @@
         <v>179</v>
       </c>
       <c r="F108" s="156" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="H108" s="156" t="s">
         <v>79</v>
@@ -6505,7 +6524,7 @@
     <row r="109" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="93"/>
       <c r="B109" s="182" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C109" s="182"/>
       <c r="D109" s="182"/>
@@ -6549,13 +6568,13 @@
     </row>
     <row r="112" spans="1:9" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="156" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B112" s="156" t="s">
         <v>179</v>
       </c>
       <c r="F112" s="156" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="H112" s="156" t="s">
         <v>79</v>
@@ -6600,7 +6619,7 @@
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="93"/>
       <c r="B115" s="182" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C115" s="182"/>
       <c r="D115" s="182"/>
@@ -6659,7 +6678,7 @@
         <v>260</v>
       </c>
       <c r="B119" s="92" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C119" s="102" t="s">
         <v>188</v>
@@ -6682,10 +6701,10 @@
     </row>
     <row r="120" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A120" s="96" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B120" s="92" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C120" s="102" t="s">
         <v>188</v>
@@ -6752,10 +6771,10 @@
     </row>
     <row r="125" spans="1:9" s="168" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="93" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B125" s="116" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C125" s="167" t="s">
         <v>188</v>
@@ -6765,7 +6784,7 @@
       </c>
       <c r="E125" s="167"/>
       <c r="F125" s="168" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G125" s="170" t="s">
         <v>258</v>
@@ -6890,12 +6909,12 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="93"/>
-      <c r="B135" s="185" t="s">
+      <c r="B135" s="186" t="s">
         <v>488</v>
       </c>
-      <c r="C135" s="185"/>
-      <c r="D135" s="185"/>
-      <c r="E135" s="185"/>
+      <c r="C135" s="186"/>
+      <c r="D135" s="186"/>
+      <c r="E135" s="186"/>
       <c r="F135" s="183"/>
       <c r="G135" s="183"/>
       <c r="H135" s="183"/>
@@ -6940,7 +6959,7 @@
         <v>534</v>
       </c>
       <c r="B140" s="125" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C140" s="102" t="s">
         <v>141</v>
@@ -6949,7 +6968,7 @@
         <v>285</v>
       </c>
       <c r="F140" s="105" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G140" s="102" t="s">
         <v>258</v>
@@ -6974,7 +6993,7 @@
     </row>
     <row r="142" spans="1:9" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="123" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B142" s="125" t="s">
         <v>518</v>
@@ -6986,7 +7005,7 @@
         <v>285</v>
       </c>
       <c r="F142" s="105" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G142" s="125" t="s">
         <v>258</v>
@@ -7000,7 +7019,7 @@
     </row>
     <row r="143" spans="1:9" s="125" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="123" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B143" s="92" t="s">
         <v>277</v>
@@ -7468,17 +7487,33 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B92:H92"/>
-    <mergeCell ref="B144:H144"/>
-    <mergeCell ref="B113:H113"/>
-    <mergeCell ref="B141:H141"/>
-    <mergeCell ref="B96:H96"/>
-    <mergeCell ref="B94:H94"/>
-    <mergeCell ref="B101:H101"/>
-    <mergeCell ref="B105:H105"/>
-    <mergeCell ref="B111:H111"/>
-    <mergeCell ref="B109:H109"/>
-    <mergeCell ref="B107:I107"/>
+    <mergeCell ref="B170:I170"/>
+    <mergeCell ref="B131:I131"/>
+    <mergeCell ref="B64:I64"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B66:H66"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B60:H60"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="B39:I39"/>
+    <mergeCell ref="B103:H103"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="B70:H70"/>
+    <mergeCell ref="B135:I135"/>
+    <mergeCell ref="B86:H86"/>
+    <mergeCell ref="B75:I75"/>
+    <mergeCell ref="B79:H79"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B58:I58"/>
+    <mergeCell ref="B62:H62"/>
+    <mergeCell ref="B37:I37"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B73:H73"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B35:I35"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B150:I150"/>
     <mergeCell ref="B162:H162"/>
@@ -7495,33 +7530,17 @@
     <mergeCell ref="B45:H45"/>
     <mergeCell ref="B41:I41"/>
     <mergeCell ref="B146:H146"/>
-    <mergeCell ref="B79:H79"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B58:I58"/>
-    <mergeCell ref="B62:H62"/>
-    <mergeCell ref="B37:I37"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B73:H73"/>
-    <mergeCell ref="B30:I30"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B170:I170"/>
-    <mergeCell ref="B131:I131"/>
-    <mergeCell ref="B64:I64"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B66:H66"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="B60:H60"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="B39:I39"/>
-    <mergeCell ref="B103:H103"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="B70:H70"/>
-    <mergeCell ref="B135:I135"/>
-    <mergeCell ref="B86:H86"/>
-    <mergeCell ref="B75:I75"/>
+    <mergeCell ref="B92:H92"/>
+    <mergeCell ref="B144:H144"/>
+    <mergeCell ref="B113:H113"/>
+    <mergeCell ref="B141:H141"/>
+    <mergeCell ref="B96:H96"/>
+    <mergeCell ref="B94:H94"/>
+    <mergeCell ref="B101:H101"/>
+    <mergeCell ref="B105:H105"/>
+    <mergeCell ref="B111:H111"/>
+    <mergeCell ref="B109:H109"/>
+    <mergeCell ref="B107:I107"/>
   </mergeCells>
   <phoneticPr fontId="39" type="noConversion"/>
   <hyperlinks>
@@ -7567,9 +7586,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29:F32"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7586,7 +7605,7 @@
     <col min="10" max="10" width="77.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>225</v>
       </c>
@@ -7603,10 +7622,10 @@
         <v>296</v>
       </c>
       <c r="F1" s="40" t="s">
+        <v>699</v>
+      </c>
+      <c r="G1" s="40" t="s">
         <v>700</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>701</v>
       </c>
       <c r="H1" s="40" t="s">
         <v>308</v>
@@ -7615,9 +7634,9 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B2" s="72"/>
       <c r="C2" s="52"/>
@@ -7628,7 +7647,7 @@
       <c r="H2" s="47"/>
       <c r="I2" s="47"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="43" t="s">
         <v>297</v>
       </c>
@@ -7654,7 +7673,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="43" t="s">
         <v>298</v>
       </c>
@@ -7680,7 +7699,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="43" t="s">
         <v>230</v>
       </c>
@@ -7707,7 +7726,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="43" t="s">
         <v>229</v>
       </c>
@@ -7734,7 +7753,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="43" t="s">
         <v>231</v>
       </c>
@@ -7761,7 +7780,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="43" t="s">
         <v>233</v>
       </c>
@@ -7788,33 +7807,37 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+    <row r="9" spans="1:10" s="70" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="67" t="s">
         <v>299</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="B9" s="195"/>
+      <c r="C9" s="68" t="s">
         <v>235</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="69">
         <v>1350</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="69">
         <v>160</v>
       </c>
-      <c r="F9" s="44">
+      <c r="F9" s="69">
         <v>800</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="69">
         <v>160</v>
       </c>
-      <c r="H9" s="44">
+      <c r="H9" s="69">
         <v>1350</v>
       </c>
-      <c r="I9" s="44">
+      <c r="I9" s="69">
         <v>160</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="196" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="43" t="s">
         <v>300</v>
       </c>
@@ -7840,10 +7863,10 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="43"/>
     </row>
-    <row r="12" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
         <v>464</v>
       </c>
@@ -7856,7 +7879,7 @@
       <c r="H12" s="47"/>
       <c r="I12" s="47"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="43" t="s">
         <v>226</v>
       </c>
@@ -7883,7 +7906,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="43" t="s">
         <v>227</v>
       </c>
@@ -7910,7 +7933,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="43" t="s">
         <v>228</v>
       </c>
@@ -7937,7 +7960,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="43" t="s">
         <v>232</v>
       </c>
@@ -8135,7 +8158,7 @@
         <v>225</v>
       </c>
       <c r="J26" s="71" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -8144,7 +8167,7 @@
     </row>
     <row r="28" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="46" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B28" s="72"/>
       <c r="C28" s="52"/>
@@ -8175,7 +8198,7 @@
         <v>140</v>
       </c>
       <c r="H29" s="44">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="I29" s="44">
         <v>140</v>
@@ -8203,11 +8226,11 @@
       <c r="G30" s="175">
         <v>160</v>
       </c>
-      <c r="H30" s="175">
-        <v>1000</v>
+      <c r="H30" s="44">
+        <v>1100</v>
       </c>
       <c r="I30" s="175">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="J30" s="179"/>
     </row>
@@ -8233,11 +8256,11 @@
       <c r="G31" s="175">
         <v>160</v>
       </c>
-      <c r="H31" s="175">
-        <v>1000</v>
+      <c r="H31" s="44">
+        <v>1100</v>
       </c>
       <c r="I31" s="175">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="J31" s="180"/>
     </row>
@@ -8263,8 +8286,8 @@
       <c r="G32" s="175">
         <v>130</v>
       </c>
-      <c r="H32" s="175">
-        <v>1200</v>
+      <c r="H32" s="44">
+        <v>1000</v>
       </c>
       <c r="I32" s="175">
         <v>140</v>
@@ -8775,7 +8798,7 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="193"/>
       <c r="B9" s="188" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C9" s="189"/>
     </row>
@@ -8931,7 +8954,7 @@
         <v>470</v>
       </c>
       <c r="F1" s="126" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -9143,7 +9166,7 @@
         <v>512</v>
       </c>
       <c r="G1" s="42" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="64" customFormat="1" ht="14" x14ac:dyDescent="0.2">
@@ -9160,10 +9183,10 @@
         <v>478</v>
       </c>
       <c r="F2" s="65" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="G2" s="64" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>